<commit_message>
new file:   Dev/Calendar_LambdaModule.xlsx 	renamed:    Resources/ISO_8601_FormatHashTables.xlsx -> Dev/ISO_8601_FormatHashTables.xlsx 	deleted:    ISO_8601_LambdaModule.xlsx 	modified:   Release/ISO_8601_LambdaModule.xlsx 	new file:   Source/CALENDAR.lambda 	modified:   Source/ISO_8601.lambda
</commit_message>
<xml_diff>
--- a/Release/ISO_8601_LambdaModule.xlsx
+++ b/Release/ISO_8601_LambdaModule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbb3931c8741440f/Projects/Datachord/Excel-Lambda-Calendar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbb3931c8741440f/Projects/Datachord/Excel-Lambda-Calendar/Release/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7850" documentId="8_{19407E84-97AB-407A-B069-4931D05A9863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6462BBE8-1B64-4DF8-A050-D14C4B1D7FC1}"/>
+  <xr:revisionPtr revIDLastSave="9458" documentId="8_{19407E84-97AB-407A-B069-4931D05A9863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DEC1751-93E0-4903-986C-78D70D796430}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="771" firstSheet="2" activeTab="4" xr2:uid="{E51D3FA6-F220-43B2-A131-7A848E5BABC5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="771" firstSheet="2" activeTab="3" xr2:uid="{E51D3FA6-F220-43B2-A131-7A848E5BABC5}"/>
   </bookViews>
   <sheets>
     <sheet name="ISO_8601_Logical" sheetId="1" r:id="rId1"/>
@@ -41,8 +41,8 @@
     <definedName name="ISO_8601.IS_VALID_WEEK_DATE">_xlfn.LAMBDA(_xlpm.YearCE,_xlpm.Week,_xlpm.DayOfWeek,_xlop.DayOfWeekMandatory, IF(NOT(ISO_8601.IS_VALID_YEAR(_xlpm.YearCE)) + NOT(ISNUMBER(_xlpm.Week)), FALSE, _xlfn.LET(_xlpm._ommitDoW, NOT(ISNUMBER(_xlpm.DayOfWeek)), IF((N(_xlpm.DayOfWeekMandatory) &lt;&gt; 0) * _xlpm._ommitDoW, FALSE, _xlfn.LET(_xlpm._week, INT(_xlpm.Week), IF(((_xlpm._week &gt;= 1) * (_xlpm._week &lt;= ISO_8601.YEAR_WEEK_COUNT(_xlpm.YearCE))) = 0, FALSE, IF(_xlpm._ommitDoW, TRUE, IF(_xlpm.Week &lt;&gt; _xlpm._week, FALSE, _xlfn.LET(_xlpm._dow, INT(_xlpm.DayOfWeek), ((_xlpm._dow &gt;= 1) * (_xlpm._dow &lt;= 7)) &lt;&gt; 0)))))))))</definedName>
     <definedName name="ISO_8601.IS_VALID_YEAR">_xlfn.LAMBDA(_xlpm.YearCE,_xlop.AllowDecimal, _xlfn.IFS(NOT(ISNUMBER(_xlpm.YearCE)), FALSE, (N(_xlpm.AllowDecimal) = 0) * (_xlpm.YearCE &lt;&gt; INT(_xlpm.YearCE)), FALSE, TRUE, ABS(_xlpm.YearCE) &lt; 100000))</definedName>
     <definedName name="ISO_8601.PARSE_DATE">_xlfn.LAMBDA(_xlpm.Text, _xlfn.LET(_xlpm._fmtHashTable, {16384,1,3,1,4,0,0,0;20480,1,3,1,5,0,0,0;28672,3,1,2,4,0,0,3;28677,2,1,3,4,6,2,0;29952,2,2,1,4,6,2,0;32768,3,1,1,4,5,2,2;32773,3,1,3,4,6,2,1;32774,2,1,3,5,7,2,0;34048,3,2,2,4,0,0,3;34054,2,2,3,4,7,2,0;34304,2,2,1,5,7,2,0;36864,3,1,1,5,6,2,2;36870,3,1,3,5,7,2,1;38400,3,2,2,5,0,0,3;38407,2,2,3,5,8,2,0;42368,3,2,1,4,6,2,2;42390,3,2,3,4,7,2,1;46736,3,2,1,5,7,2,2;46759,3,2,3,5,8,2,1}, _xlpm.fnException, _xlfn.LAMBDA(_xlpm._exception,_xlop._precision,_xlop._extended,_xlop._dateType, _xlfn.IFS(_xlpm._exception = "N/A", {FALSE,"","","","","",""}, _xlpm._exception = "VALUE", _xlfn.IFS(_xlpm._precision = 1, _xlfn.HSTACK(FALSE, 0, N(_xlpm._extended), N(_xlpm._dateType), {#VALUE!,"",""}), _xlpm._precision = 2, _xlfn.HSTACK(FALSE, 0, N(_xlpm._extended), N(_xlpm._dateType), {#VALUE!,#VALUE!,""}), TRUE, _xlfn.HSTACK(FALSE, 0, N(_xlpm._extended), N(_xlpm._dateType), {#VALUE!,#VALUE!,#VALUE!})), TRUE, {"","","","","","",""})), IF(_xlpm.Text = "", _xlpm.fnException(""), IF(NOT(ISO_8601.VALIDATE_CHARACTERS(_xlpm.Text, 1)), _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._hasSign, _xlfn.IFS(LEFT(_xlpm.Text, 1) = "+", TRUE, LEFT(_xlpm.Text, 1) = "-", TRUE, _xlfn.UNICODE(LEFT(_xlpm.Text, 1)) = 8722, TRUE, TRUE, FALSE), _xlpm._yearSign, _xlfn.IFS(LEFT(_xlpm.Text, 1) = "-", -1, _xlfn.UNICODE(LEFT(_xlpm.Text, 1)) = 8722, -1, TRUE, 1), _xlpm._len, LEN(_xlpm.Text) - N(_xlpm._hasSign), _xlpm._sDate, IF(_xlpm._hasSign, RIGHT(_xlpm.Text, _xlpm._len), _xlpm.Text), _xlpm._Hyph1Pos, IFERROR(FIND("-", _xlpm._sDate), 0), _xlpm._Hyph2Pos, IFERROR(FIND("-", _xlpm._sDate, _xlpm._Hyph1Pos + 1), 0), _xlpm._Wpos, IFERROR(FIND("W", _xlpm._sDate), 0), _xlpm._hash, (_xlpm._len * 4096) + (_xlpm._Hyph1Pos * 256) + (_xlpm._Hyph2Pos * 16) + _xlpm._Wpos, _xlpm._hashLkup, _xlfn.IFNA(_xlfn.XMATCH(_xlpm._hash, _xlfn.CHOOSECOLS(_xlpm._fmtHashTable, 1), 0), 0), IF(_xlpm._hashLkup = 0, _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._defn, _xlfn.CHOOSEROWS(_xlpm._fmtHashTable, _xlpm._hashLkup), _xlpm._precision, INDEX(_xlpm._defn, 1, 2), _xlpm._extended, INDEX(_xlpm._defn, 1, 3), _xlpm._dateType, INDEX(_xlpm._defn, 1, 4), _xlpm._yearCE, _xlpm._yearSign * VALUE(LEFT(_xlpm._sDate, INDEX(_xlpm._defn, 1, 5))), _xlpm._dArg1, IF((_xlpm._precision &lt; 2) + (INDEX(_xlpm._defn, 1, 6) = 0), "", VALUE(MID(_xlpm._sDate, INDEX(_xlpm._defn, 1, 6), INDEX(_xlpm._defn, 1, 7)))), _xlpm._dArg2, IF(_xlpm._precision &lt; 3, "", VALUE(RIGHT(_xlpm._sDate, INDEX(_xlpm._defn, 1, 8)))), _xlpm._valid, _xlfn.IFS(_xlpm._dateType = 1, ISO_8601.IS_VALID_DATE(_xlpm._yearCE, _xlpm._dArg1, _xlpm._dArg2), _xlpm._dateType = 2, ISO_8601.IS_VALID_ORDINAL_DATE(_xlpm._yearCE, _xlpm._dArg2), _xlpm._dateType = 3, ISO_8601.IS_VALID_WEEK_DATE(_xlpm._yearCE, _xlpm._dArg1, _xlpm._dArg2), TRUE, TRUE), IF(_xlpm._valid, _xlfn.HSTACK(TRUE, _xlpm._precision, _xlpm._extended, _xlpm._dateType, _xlpm._yearCE, _xlpm._dArg1, _xlpm._dArg2), _xlpm.fnException("VALUE", _xlpm._precision, _xlpm._extended, _xlpm._dateType)))))))))</definedName>
-    <definedName name="ISO_8601.PARSE_ISO8601">_xlfn.LAMBDA(_xlpm.Text, _xlfn.LET(_xlpm.fnException, _xlfn.LAMBDA(_xlpm._exception, IF(_xlpm._exception = "N/A", {FALSE,0,"","","","","","","","","",""}, {"","","","","","","","","","","",""})), _xlpm.fnPartsFlag, _xlfn.LAMBDA(_xlpm._pDate,_xlpm._pTime,_xlpm._pTZ, _xlfn.LET(_xlpm._datePart, N(INDEX(_xlpm._pDate, 1, 1)) * 4, _xlpm._timePart, N(INDEX(_xlpm._pTime, 1, 1)) * 2, _xlpm._tzPart, N(INDEX(_xlpm._pTZ, 1, 1)) * 1, _xlpm._datePart + _xlpm._timePart + _xlpm._tzPart)), _xlpm.fnISOValueCompliance, _xlfn.LAMBDA(_xlpm._pDate,_xlpm._pTime,_xlpm._pTZ, _xlfn.LET(_xlpm._dateISOCompliant, IF(INDEX(_xlpm._pDate, 1, 1) = "", TRUE, INDEX(_xlpm._pDate, 1, 1)), _xlpm._timeISOCompliant, IF(INDEX(_xlpm._pTime, 1, 1) = "", TRUE, INDEX(_xlpm._pTime, 1, 1)), _xlpm._tzISOCompliant, IF(INDEX(_xlpm._pTZ, 1, 1) = "", TRUE, INDEX(_xlpm._pTZ, 1, 1)), (_xlpm._dateISOCompliant * _xlpm._timeISOCompliant * _xlpm._tzISOCompliant) &lt;&gt; 0)), _xlpm.fnISOFormatCompliance, _xlfn.LAMBDA(_xlpm._pDate,_xlpm._pTime,_xlpm._pTZ, _xlfn.LET(_xlpm._dateFmt, N(INDEX(_xlpm._pDate, 1, 3)), _xlpm._timeFmt, N(INDEX(_xlpm._pTime, 1, 3)), _xlpm._tzoFmt, N(INDEX(_xlpm._pTZ, 1, 3)), _xlpm._resolveFmt, _xlfn.IFS((_xlpm._dateFmt = 3) * (_xlpm._timeFmt = 0) * (_xlpm._tzoFmt = 0), 3, (_xlpm._dateFmt = 0) * (_xlpm._timeFmt = 3) * (_xlpm._tzoFmt = 0), 3, (_xlpm._dateFmt = 0) * (_xlpm._timeFmt = 0) * (_xlpm._tzoFmt = 3), 3, (_xlpm._dateFmt &lt;&gt; 2) * (_xlpm._timeFmt &lt;&gt; 2) * (_xlpm._tzoFmt &lt;&gt; 2), 1, (_xlpm._dateFmt &lt;&gt; 1) * (_xlpm._timeFmt &lt;&gt; 1) * (_xlpm._tzoFmt &lt;&gt; 1), 2, TRUE, 0), _xlfn.HSTACK(N(_xlpm._resolveFmt &lt;&gt; 0), _xlpm._resolveFmt))), _xlpm.fnISOPrecisionCompliance, _xlfn.LAMBDA(_xlpm._pDate,_xlpm._pTime,_xlpm._pTZ, _xlfn.LET(_xlpm._datePrec, N(INDEX(_xlpm._pDate, 1, 2)), _xlpm._timePrec, N(INDEX(_xlpm._pTime, 1, 2)), _xlpm._tzPrec, N(INDEX(_xlpm._pTZ, 1, 2)), _xlfn.IFS(_xlpm._datePrec = 0, IF(_xlpm._timePrec = 0, IF(_xlpm._tzPrec = 0, _xlfn.HSTACK(FALSE, 0), _xlfn.HSTACK(TRUE, _xlpm._tzPrec + 3)), _xlfn.HSTACK(TRUE, _xlpm._timePrec + 3)), _xlpm._datePrec &lt; 3, _xlfn.HSTACK((_xlpm._timePrec = 0), _xlpm._datePrec), TRUE, _xlfn.HSTACK(TRUE, _xlpm._timePrec + 3)))), IF(_xlpm.Text = "", _xlpm.fnException(""), _xlfn.LET(_xlpm._parts, ISO_8601.PARSE_PARTS(_xlpm.Text), IF(N(INDEX(_xlpm._parts, 1, 2)) = 0, _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._isoPartsCompliance, N(INDEX(_xlpm._parts, 1, 1)), _xlpm._pDate, ISO_8601.PARSE_DATE(INDEX(_xlpm._parts, 1, 3)), _xlpm._pTime, ISO_8601.PARSE_TIME(INDEX(_xlpm._parts, 1, 4)), _xlpm._pTZ, ISO_8601.PARSE_TIME_ZONE(INDEX(_xlpm._parts, 1, 5)), _xlpm._isoValueCompliance, _xlpm.fnISOValueCompliance(_xlpm._pDate, _xlpm._pTime, _xlpm._pTZ), _xlpm._isoFormatCompliance, _xlpm.fnISOFormatCompliance(_xlpm._pDate, _xlpm._pTime, _xlpm._pTZ), _xlpm._isoPrecisionCompliance, _xlpm.fnISOPrecisionCompliance(_xlpm._pDate, _xlpm._pTime, _xlpm._pTZ), _xlpm._outISOcompliance, (_xlpm._isoValueCompliance * _xlpm._isoPartsCompliance * INDEX(_xlpm._isoFormatCompliance, 1, 1) * INDEX(_xlpm._isoPrecisionCompliance, 1, 1)) &lt;&gt; 0, _xlpm._outDateType, N(INDEX(_xlpm._pDate, 1, 4)), _xlpm._outDate, _xlfn.DROP(_xlpm._pDate, , 4), _xlpm._outTime, _xlfn.DROP(_xlpm._pTime, , 3), _xlpm._outTZ, _xlfn.DROP(_xlpm._pTZ, , 3), _xlpm._outPartsFlag, _xlpm.fnPartsFlag(_xlpm._pDate, _xlpm._pTime, _xlpm._pTZ), _xlfn.HSTACK(_xlpm._outISOcompliance, _xlpm._outPartsFlag, INDEX(_xlpm._isoPrecisionCompliance, 1, 2), INDEX(_xlpm._isoFormatCompliance, 1, 2), _xlpm._outDateType, _xlpm._outDate, _xlpm._outTime, _xlpm._outTZ)))))))</definedName>
-    <definedName name="ISO_8601.PARSE_PARTS">_xlfn.LAMBDA(_xlpm.Text, _xlfn.LET(_xlpm.fnException, _xlfn.LAMBDA(_xlpm._exception, IF(_xlpm._exception = "N/A", {FALSE,0,"","",""}, {"","","","",""})), _xlpm.fnCountChars, _xlfn.LAMBDA(_xlpm.CharArray,_xlpm.Text, IF(_xlpm.Text = "", 0, _xlfn.LET(_xlpm._removed, _xlfn.REDUCE(_xlpm.Text, _xlpm.CharArray, _xlfn.LAMBDA(_xlpm._acc,_xlpm._curr, SUBSTITUTE(_xlpm._acc, _xlpm._curr, ""))), LEN(_xlpm.Text) - LEN(_xlpm._removed)))), _xlpm.fnFindNthCharPos, _xlfn.LAMBDA(_xlpm.Chars,_xlpm.Text,_xlpm.N, _xlfn.LET(_xlpm._charCount, LEN(_xlpm.Chars), _xlpm._n, INT(N(_xlpm.N)), IF((_xlpm._charCount = 0) + (_xlpm._n = 0), 0, _xlfn.LET(_xlpm._chars, MID(_xlpm.Chars, _xlfn.SEQUENCE(1, _xlpm._charCount), 1), _xlpm._findCount, _xlpm.fnCountChars(_xlpm._chars, _xlpm.Text), IF(_xlpm._findCount &lt; ABS(_xlpm._n), 0, _xlfn.LET(_xlpm._nth, IF(_xlpm._n &gt; 0, _xlpm._n, _xlpm._findCount + _xlpm._n + 1), _xlpm._nthPos, _xlfn.REDUCE(0, _xlfn.SEQUENCE(1, _xlpm._nth), _xlfn.LAMBDA(_xlpm._acc,_xlpm._curr, IF(_xlpm._acc &lt; 0, -1, _xlfn.LET(_xlpm._nextPosChars, IFERROR(FIND(_xlpm._chars, _xlpm.Text, _xlpm._acc + 1), 0), _xlpm._nextPos, MIN(_xlfn._xlws.FILTER(_xlpm._nextPosChars, _xlpm._nextPosChars &gt; 0, 0)), IF(_xlpm._nextPos = 0, -1, _xlpm._nextPos))))), MAX(_xlpm._nthPos, 0))))))), _xlpm.WithT_Logic, {1,0,2;1,1,1;1,2,3;2,0,6;2,1,5;2,2,7}, _xlpm.WithoutT_Logic, {0,0,0,0,4;0,0,0,1,2;0,0,1,0,2;1,0,0,0,4;1,0,0,1,1;1,0,1,0,1;1,1,0,0,1;2,0,0,0,4;2,0,0,1,3;2,0,1,0,3;2,0,1,1,3;2,1,0,1,3;2,1,1,0,3}, _xlpm.fnWithT_PartsLen, _xlfn.LAMBDA(_xlpm._Tpos,_xlpm._Tfirst, _xlfn.LET(_xlpm._len, LEN(_xlpm.Text), _xlpm._afterT, RIGHT(_xlpm.Text, _xlpm._len - _xlpm._Tpos), _xlpm._TZmarkerPos, _xlpm.fnFindNthCharPos("Z+-" &amp; _xlfn.UNICHAR(8722), _xlpm._afterT, 1), _xlpm._TZmarkFirst, IF(_xlpm._TZmarkerPos &gt; 1, 2, _xlpm._TZmarkerPos), _xlpm._partsFlag, _xlfn._xlws.FILTER(_xlfn.CHOOSECOLS(_xlpm.WithT_Logic, 3), (_xlfn.CHOOSECOLS(_xlpm.WithT_Logic, 1) = _xlpm._Tfirst) * (_xlfn.CHOOSECOLS(_xlpm.WithT_Logic, 2) = _xlpm._TZmarkFirst), #N/A), IF(ISNA(_xlpm._partsFlag), _xlfn.HSTACK(#N/A, 0, 0, 0), _xlfn.LET(_xlpm._dateLen, _xlpm._Tpos - 1, _xlpm._timeLen, IF(_xlfn.BITAND(_xlpm._partsFlag, 2) = 2, IF(_xlfn.BITAND(_xlpm._partsFlag, 1) = 1, _xlpm._TZmarkerPos - 1, _xlpm._len - _xlpm._Tpos), 0), _xlpm._tzLen, _xlpm._len - _xlpm._Tpos - _xlpm._timeLen, _xlfn.HSTACK(_xlpm._partsFlag, _xlpm._dateLen, _xlpm._timeLen, _xlpm._tzLen))))), _xlpm.fnWithoutT_PartsLen, _xlfn.LAMBDA(_xlfn.LET(_xlpm._len, LEN(_xlpm.Text), _xlpm._TZmarkPos, _xlpm.fnFindNthCharPos("Z+-" &amp; _xlfn.UNICHAR(8722), _xlpm.Text, -1), _xlpm._TZmarkFirst, IF(_xlpm._TZmarkPos &gt; 1, 2, _xlpm._TZmarkPos), _xlpm._TZmarkIsZ, IF(_xlpm._TZmarkPos &gt; 0, N(CODE(MID(_xlpm.Text, _xlpm._TZmarkPos, 1)) = 90), 0), _xlpm._HasColon, N(IFERROR(FIND(":", _xlpm.Text), 0) &gt; 0), _xlpm._lenBeforeTZ, IF(_xlpm._TZmarkFirst = 0, _xlpm._len, _xlpm._TZmarkPos - 1), _xlpm._timeConditional, IF(_xlpm._TZmarkFirst = 1, _xlfn.LET(_xlpm._lenAfterTZ, _xlpm._len - _xlpm._TZmarkPos, _xlfn.IFS(_xlpm._lenAfterTZ = 2, 1, _xlpm._lenAfterTZ = 6, 1, TRUE, 0)), N(_xlpm._lenBeforeTZ = 2)), _xlpm._match, ((_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 1) = _xlpm._TZmarkFirst) * (_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 2) = _xlpm._TZmarkIsZ) * (_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 3) = _xlpm._HasColon) * (_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 4) = _xlpm._timeConditional)), _xlpm._partsFlag, _xlfn._xlws.FILTER(_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 5), _xlpm._match, #N/A), _xlpm._dateLen, IF(_xlfn.BITAND(_xlpm._partsFlag, 4) = 4, _xlpm._len, 0), _xlpm._timeLen, IF(_xlfn.BITAND(_xlpm._partsFlag, 2) = 2, _xlpm._lenBeforeTZ, 0), _xlpm._tzLen, IF(_xlfn.BITAND(_xlpm._partsFlag, 1) = 1, _xlpm._len - _xlpm._TZmarkPos + 1, 0), _xlfn.HSTACK(_xlpm._partsFlag, _xlpm._dateLen, _xlpm._timeLen, _xlpm._tzLen))), IF(_xlpm.Text = "", _xlpm.fnException(""), IF(NOT(ISO_8601.VALIDATE_CHARACTERS(_xlpm.Text, 0)), _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._Tpos, IFERROR(FIND("T", _xlpm.Text), 0), IF(_xlpm._Tpos = LEN(_xlpm.Text), _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._hasT, IF(_xlpm._Tpos &gt; 1, 2, _xlpm._Tpos), _xlpm._partsLen, IF(_xlpm._hasT, _xlpm.fnWithT_PartsLen(_xlpm._Tpos, _xlpm._hasT), _xlpm.fnWithoutT_PartsLen()), _xlpm._partsFlag, INDEX(_xlpm._partsLen, 1, 1), IF(ISNA(_xlpm._partsFlag), _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._isoCompliant, _xlfn.IFS(_xlpm._partsFlag = 1, FALSE, _xlpm._partsFlag = 5, FALSE, _xlpm._partsFlag = 4, TRUE, TRUE, (_xlpm._hasT &gt; 0)), _xlpm._datePart, IF(_xlfn.BITAND(_xlpm._partsFlag, 4) = 4, LEFT(_xlpm.Text, INDEX(_xlpm._partsLen, 1, 2)), ""), _xlpm._timePart, IF(_xlfn.BITAND(_xlpm._partsFlag, 2) = 2, "T" &amp; MID(_xlpm.Text, _xlpm._Tpos + 1, INDEX(_xlpm._partsLen, 1, 3)), ""), _xlpm._tzPart, IF(_xlfn.BITAND(_xlpm._partsFlag, 1) = 1, RIGHT(_xlpm.Text, INDEX(_xlpm._partsLen, 1, 4)), ""), _xlfn.HSTACK(_xlpm._isoCompliant, _xlpm._partsFlag, _xlpm._datePart, _xlpm._timePart, _xlpm._tzPart))))))))))</definedName>
+    <definedName name="ISO_8601.PARSE_ISO8601">_xlfn.LAMBDA(_xlpm.Text,_xlop.AllowMixedFormat, _xlfn.LET(_xlpm.fnException, _xlfn.LAMBDA(_xlpm._exception, IF(_xlpm._exception = "N/A", {FALSE,0,"","","","","","","","","",""}, {"","","","","","","","","","","",""})), _xlpm.fnPartsFlag, _xlfn.LAMBDA(_xlpm._pDate,_xlpm._pTime,_xlpm._pTZ, _xlfn.LET(_xlpm._datePart, N(INDEX(_xlpm._pDate, 1, 1)) * 4, _xlpm._timePart, N(INDEX(_xlpm._pTime, 1, 1)) * 2, _xlpm._tzPart, N(INDEX(_xlpm._pTZ, 1, 1)) * 1, _xlpm._datePart + _xlpm._timePart + _xlpm._tzPart)), _xlpm.fnISOValueCompliance, _xlfn.LAMBDA(_xlpm._pDate,_xlpm._pTime,_xlpm._pTZ, _xlfn.LET(_xlpm._dateISOCompliant, IF(INDEX(_xlpm._pDate, 1, 1) = "", TRUE, INDEX(_xlpm._pDate, 1, 1)), _xlpm._timeISOCompliant, IF(INDEX(_xlpm._pTime, 1, 1) = "", TRUE, INDEX(_xlpm._pTime, 1, 1)), _xlpm._tzISOCompliant, IF(INDEX(_xlpm._pTZ, 1, 1) = "", TRUE, INDEX(_xlpm._pTZ, 1, 1)), (_xlpm._dateISOCompliant * _xlpm._timeISOCompliant * _xlpm._tzISOCompliant) &lt;&gt; 0)), _xlpm.fnISOFormatCompliance, _xlfn.LAMBDA(_xlpm._pDate,_xlpm._pTime,_xlpm._pTZ,_xlpm._allowMixedFormat, _xlfn.LET(_xlpm._dateFmt, N(INDEX(_xlpm._pDate, 1, 3)), _xlpm._timeFmt, N(INDEX(_xlpm._pTime, 1, 3)), _xlpm._tzoFmt, N(INDEX(_xlpm._pTZ, 1, 3)), _xlpm._resolveFmt, _xlfn.IFS((_xlpm._dateFmt = 3) * (_xlpm._timeFmt = 0) * (_xlpm._tzoFmt = 0), 3, (_xlpm._dateFmt = 0) * (_xlpm._timeFmt = 3) * (_xlpm._tzoFmt = 0), 3, (_xlpm._dateFmt = 0) * (_xlpm._timeFmt = 0) * (_xlpm._tzoFmt = 3), 3, (_xlpm._dateFmt &lt;&gt; 2) * (_xlpm._timeFmt &lt;&gt; 2) * (_xlpm._tzoFmt &lt;&gt; 2), 1, (_xlpm._dateFmt &lt;&gt; 1) * (_xlpm._timeFmt &lt;&gt; 1) * (_xlpm._tzoFmt &lt;&gt; 1), 2, TRUE, 4), _xlpm._formatCompliant, IF(_xlpm._allowMixedFormat, 1, N(_xlpm._resolveFmt &lt; 4)), _xlfn.HSTACK(_xlpm._formatCompliant, _xlpm._resolveFmt))), _xlpm.fnISOPrecisionCompliance, _xlfn.LAMBDA(_xlpm._pDate,_xlpm._pTime,_xlpm._pTZ, _xlfn.LET(_xlpm._datePrec, N(INDEX(_xlpm._pDate, 1, 2)), _xlpm._timePrec, N(INDEX(_xlpm._pTime, 1, 2)), _xlpm._tzPrec, N(INDEX(_xlpm._pTZ, 1, 2)), _xlfn.IFS(_xlpm._datePrec = 0, IF(_xlpm._timePrec = 0, IF(_xlpm._tzPrec = 0, _xlfn.HSTACK(FALSE, 0), _xlfn.HSTACK(TRUE, _xlpm._tzPrec + 3)), _xlfn.HSTACK(TRUE, _xlpm._timePrec + 3)), _xlpm._datePrec &lt; 3, _xlfn.HSTACK((_xlpm._timePrec = 0), _xlpm._datePrec), TRUE, _xlfn.HSTACK(TRUE, _xlpm._timePrec + 3)))), IF(_xlpm.Text = "", _xlpm.fnException(""), _xlfn.LET(_xlpm._parts, ISO_8601.PARSE_PARTS(_xlpm.Text), IF(N(INDEX(_xlpm._parts, 1, 2)) = 0, _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._allowMixedFormat, N(_xlpm.AllowMixedFormat) &lt;&gt; 0, _xlpm._isoPartsCompliance, N(INDEX(_xlpm._parts, 1, 1)), _xlpm._pDate, ISO_8601.PARSE_DATE(INDEX(_xlpm._parts, 1, 3)), _xlpm._pTime, ISO_8601.PARSE_TIME(INDEX(_xlpm._parts, 1, 4)), _xlpm._pTZ, ISO_8601.PARSE_TIME_ZONE(INDEX(_xlpm._parts, 1, 5)), _xlpm._isoValueCompliance, _xlpm.fnISOValueCompliance(_xlpm._pDate, _xlpm._pTime, _xlpm._pTZ), _xlpm._isoFormatCompliance, _xlpm.fnISOFormatCompliance(_xlpm._pDate, _xlpm._pTime, _xlpm._pTZ, _xlpm._allowMixedFormat), _xlpm._isoPrecisionCompliance, _xlpm.fnISOPrecisionCompliance(_xlpm._pDate, _xlpm._pTime, _xlpm._pTZ), _xlpm._outISOcompliance, (_xlpm._isoValueCompliance * _xlpm._isoPartsCompliance * INDEX(_xlpm._isoFormatCompliance, 1, 1) * INDEX(_xlpm._isoPrecisionCompliance, 1, 1)) &lt;&gt; 0, _xlpm._outDateType, N(INDEX(_xlpm._pDate, 1, 4)), _xlpm._outDate, _xlfn.DROP(_xlpm._pDate, , 4), _xlpm._outTime, _xlfn.DROP(_xlpm._pTime, , 3), _xlpm._outTZ, _xlfn.DROP(_xlpm._pTZ, , 3), _xlpm._outPartsFlag, _xlpm.fnPartsFlag(_xlpm._pDate, _xlpm._pTime, _xlpm._pTZ), _xlfn.HSTACK(_xlpm._outISOcompliance, _xlpm._outPartsFlag, INDEX(_xlpm._isoPrecisionCompliance, 1, 2), INDEX(_xlpm._isoFormatCompliance, 1, 2), _xlpm._outDateType, _xlpm._outDate, _xlpm._outTime, _xlpm._outTZ)))))))</definedName>
+    <definedName name="ISO_8601.PARSE_PARTS">_xlfn.LAMBDA(_xlpm.Text, _xlfn.LET(_xlpm.fnException, _xlfn.LAMBDA(_xlpm._exception, IF(_xlpm._exception = "N/A", {FALSE,0,"","",""}, {"","","","",""})), _xlpm.fnCountChars, _xlfn.LAMBDA(_xlpm.CharArray,_xlpm.Text, IF(_xlpm.Text = "", 0, _xlfn.LET(_xlpm._removed, _xlfn.REDUCE(_xlpm.Text, _xlpm.CharArray, _xlfn.LAMBDA(_xlpm._acc,_xlpm._curr, SUBSTITUTE(_xlpm._acc, _xlpm._curr, ""))), LEN(_xlpm.Text) - LEN(_xlpm._removed)))), _xlpm.fnFindNthCharPos, _xlfn.LAMBDA(_xlpm.Chars,_xlpm.Text,_xlpm.N,_xlop.StartPos, IF(N(_xlpm.StartPos) &gt; LEN(_xlpm.Text), 0, _xlfn.LET(_xlpm._fromPos, IF(N(_xlpm.StartPos) &lt;= 0, 0, N(_xlpm.StartPos) - 1), _xlpm._text, IF(_xlpm._fromPos = 0, _xlpm.Text, RIGHT(_xlpm.Text, LEN(_xlpm.Text) - _xlpm._fromPos)), _xlpm._charCount, LEN(_xlpm.Chars), _xlpm._n, INT(N(_xlpm.N)), IF((_xlpm._charCount = 0) + (_xlpm._n = 0), 0, _xlfn.LET(_xlpm._chars, MID(_xlpm.Chars, _xlfn.SEQUENCE(1, _xlpm._charCount), 1), _xlpm._findCount, _xlpm.fnCountChars(_xlpm._chars, _xlpm._text), IF(_xlpm._findCount &lt; ABS(_xlpm._n), 0, _xlfn.LET(_xlpm._nth, IF(_xlpm._n &gt; 0, _xlpm._n, _xlpm._findCount + _xlpm._n + 1), _xlpm._nthPos, _xlfn.REDUCE(0, _xlfn.SEQUENCE(1, _xlpm._nth), _xlfn.LAMBDA(_xlpm._acc,_xlpm._curr, IF(_xlpm._acc &lt; 0, -1, _xlfn.LET(_xlpm._nextPosChars, IFERROR(FIND(_xlpm._chars, _xlpm._text, _xlpm._acc + 1), 0), _xlpm._nextPos, MIN(_xlfn._xlws.FILTER(_xlpm._nextPosChars, _xlpm._nextPosChars &gt; 0, 0)), IF(_xlpm._nextPos = 0, -1, _xlpm._nextPos))))), IF(_xlpm._nthPos &gt; 0, _xlpm._nthPos + _xlpm._fromPos, 0)))))))), _xlpm.WithT_Logic, {1,0,2;1,1,1;1,2,3;2,0,6;2,1,5;2,2,7}, _xlpm.WithoutT_Logic, {0,0,0,0,4;0,0,0,1,2;0,0,1,0,2;1,0,0,0,4;1,0,0,1,1;1,0,1,0,1;1,1,0,0,1;2,0,0,0,4;2,0,0,1,3;2,0,1,0,3;2,0,1,1,3;2,1,0,1,3;2,1,1,0,3}, _xlpm.fnWithT_PartsLen, _xlfn.LAMBDA(_xlpm._Tpos,_xlpm._Tfirst, _xlfn.LET(_xlpm._len, LEN(_xlpm.Text), _xlpm._afterT, RIGHT(_xlpm.Text, _xlpm._len - _xlpm._Tpos), _xlpm._TZmarkerPos, _xlpm.fnFindNthCharPos("Z+-" &amp; _xlfn.UNICHAR(8722), _xlpm._afterT, 1), _xlpm._TZmarkFirst, IF(_xlpm._TZmarkerPos &gt; 1, 2, _xlpm._TZmarkerPos), _xlpm._partsFlag, _xlfn._xlws.FILTER(_xlfn.CHOOSECOLS(_xlpm.WithT_Logic, 3), (_xlfn.CHOOSECOLS(_xlpm.WithT_Logic, 1) = _xlpm._Tfirst) * (_xlfn.CHOOSECOLS(_xlpm.WithT_Logic, 2) = _xlpm._TZmarkFirst), #N/A), IF(ISNA(_xlpm._partsFlag), _xlfn.HSTACK(#N/A, 0, 0, 0), _xlfn.LET(_xlpm._dateLen, _xlpm._Tpos - 1, _xlpm._timeLen, IF(_xlfn.BITAND(_xlpm._partsFlag, 2) = 2, IF(_xlfn.BITAND(_xlpm._partsFlag, 1) = 1, _xlpm._TZmarkerPos - 1, _xlpm._len - _xlpm._Tpos), 0), _xlpm._tzLen, _xlpm._len - _xlpm._Tpos - _xlpm._timeLen, _xlfn.HSTACK(_xlpm._partsFlag, _xlpm._dateLen, _xlpm._timeLen, _xlpm._tzLen))))), _xlpm.fnWithoutT_PartsLen, _xlfn.LAMBDA(_xlfn.LET(_xlpm._len, LEN(_xlpm.Text), _xlpm._TZmarkPos, _xlpm.fnFindNthCharPos("Z+-" &amp; _xlfn.UNICHAR(8722), _xlpm.Text, -1), _xlpm._TZmarkFirst, IF(_xlpm._TZmarkPos &gt; 1, 2, _xlpm._TZmarkPos), _xlpm._TZmarkIsZ, IF(_xlpm._TZmarkPos &gt; 0, N(CODE(MID(_xlpm.Text, _xlpm._TZmarkPos, 1)) = 90), 0), _xlpm._HasColon, N(IFERROR(FIND(":", _xlpm.Text), 0) &gt; 0), _xlpm._lenBeforeTZ, IF(_xlpm._TZmarkFirst = 0, _xlpm._len, _xlpm._TZmarkPos - 1), _xlpm._timeConditional, IF(_xlpm._TZmarkFirst = 1, _xlfn.LET(_xlpm._lenAfterTZ, _xlpm._len - _xlpm._TZmarkPos, _xlfn.IFS(_xlpm._lenAfterTZ = 2, 1, _xlpm._lenAfterTZ = 6, 1, TRUE, 0)), N(_xlpm._lenBeforeTZ = 2)), _xlpm._match, ((_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 1) = _xlpm._TZmarkFirst) * (_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 2) = _xlpm._TZmarkIsZ) * (_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 3) = _xlpm._HasColon) * (_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 4) = _xlpm._timeConditional)), _xlpm._partsFlag, _xlfn._xlws.FILTER(_xlfn.CHOOSECOLS(_xlpm.WithoutT_Logic, 5), _xlpm._match, #N/A), _xlpm._dateLen, IF(_xlfn.BITAND(_xlpm._partsFlag, 4) = 4, _xlpm._len, 0), _xlpm._timeLen, IF(_xlfn.BITAND(_xlpm._partsFlag, 2) = 2, _xlpm._lenBeforeTZ, 0), _xlpm._tzLen, IF(_xlfn.BITAND(_xlpm._partsFlag, 1) = 1, _xlpm._len - _xlpm._TZmarkPos + 1, 0), _xlfn.HSTACK(_xlpm._partsFlag, _xlpm._dateLen, _xlpm._timeLen, _xlpm._tzLen))), IF(_xlpm.Text = "", _xlpm.fnException(""), IF(NOT(ISO_8601.VALIDATE_CHARACTERS(_xlpm.Text, 0)), _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._Tpos, IFERROR(FIND("T", _xlpm.Text), 0), IF(_xlpm._Tpos = LEN(_xlpm.Text), _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._hasT, IF(_xlpm._Tpos &gt; 1, 2, _xlpm._Tpos), _xlpm._partsLen, IF(_xlpm._hasT, _xlpm.fnWithT_PartsLen(_xlpm._Tpos, _xlpm._hasT), _xlpm.fnWithoutT_PartsLen()), _xlpm._partsFlag, INDEX(_xlpm._partsLen, 1, 1), IF(ISNA(_xlpm._partsFlag), _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._isoCompliant, _xlfn.IFS(_xlpm._partsFlag = 1, FALSE, _xlpm._partsFlag = 5, FALSE, _xlpm._partsFlag = 4, TRUE, TRUE, (_xlpm._hasT &gt; 0)), _xlpm._datePart, IF(_xlfn.BITAND(_xlpm._partsFlag, 4) = 4, LEFT(_xlpm.Text, INDEX(_xlpm._partsLen, 1, 2)), ""), _xlpm._timePart, IF(_xlfn.BITAND(_xlpm._partsFlag, 2) = 2, "T" &amp; MID(_xlpm.Text, _xlpm._Tpos + 1, INDEX(_xlpm._partsLen, 1, 3)), ""), _xlpm._tzPart, IF(_xlfn.BITAND(_xlpm._partsFlag, 1) = 1, RIGHT(_xlpm.Text, INDEX(_xlpm._partsLen, 1, 4)), ""), _xlfn.HSTACK(_xlpm._isoCompliant, _xlpm._partsFlag, _xlpm._datePart, _xlpm._timePart, _xlpm._tzPart))))))))))</definedName>
     <definedName name="ISO_8601.PARSE_TIME">_xlfn.LAMBDA(_xlpm.Text, _xlfn.LET(_xlpm._fmtHashTable, {8192,1,3,0,0;16384,2,1,3,0;24576,3,1,3,2;32775,4,1,3,4;36871,5,1,3,5;40967,6,1,3,6;21248,2,2,4,0;33632,3,2,4,2;41833,4,2,4,4;45929,5,2,4,5;50025,6,2,4,6}, _xlpm.fnException, _xlfn.LAMBDA(_xlpm._exception,_xlop._precision,_xlop._extended, _xlfn.IFS(_xlpm._exception = "N/A", {FALSE,"","","","",""}, _xlpm._exception = "VALUE", _xlfn.IFS(_xlpm._precision = 1, _xlfn.HSTACK(FALSE, 0, N(_xlpm._extended), {#VALUE!,"",""}), _xlpm._precision = 2, _xlfn.HSTACK(FALSE, 0, N(_xlpm._extended), {#VALUE!,#VALUE!,""}), TRUE, _xlfn.HSTACK(FALSE, 0, N(_xlpm._extended), {#VALUE!,#VALUE!,#VALUE!})), TRUE, {"","","","","",""})), _xlpm.fnCountChars, _xlfn.LAMBDA(_xlpm.CharArray,_xlpm.Text, IF(_xlpm.Text = "", 0, _xlfn.LET(_xlpm._removed, _xlfn.REDUCE(_xlpm.Text, _xlpm.CharArray, _xlfn.LAMBDA(_xlpm._acc,_xlpm._curr, SUBSTITUTE(_xlpm._acc, _xlpm._curr, ""))), LEN(_xlpm.Text) - LEN(_xlpm._removed)))), _xlpm.fnFindNthCharPos, _xlfn.LAMBDA(_xlpm.Chars,_xlpm.Text,_xlpm.N, _xlfn.LET(_xlpm._charCount, LEN(_xlpm.Chars), _xlpm._n, INT(N(_xlpm.N)), IF((_xlpm._charCount = 0) + (_xlpm._n = 0), 0, _xlfn.LET(_xlpm._chars, MID(_xlpm.Chars, _xlfn.SEQUENCE(1, _xlpm._charCount), 1), _xlpm._findCount, _xlpm.fnCountChars(_xlpm._chars, _xlpm.Text), IF(_xlpm._findCount &lt; ABS(_xlpm._n), 0, _xlfn.LET(_xlpm._nth, IF(_xlpm._n &gt; 0, _xlpm._n, _xlpm._findCount + _xlpm._n + 1), _xlpm._nthPos, _xlfn.REDUCE(0, _xlfn.SEQUENCE(1, _xlpm._nth), _xlfn.LAMBDA(_xlpm._acc,_xlpm._curr, IF(_xlpm._acc &lt; 0, -1, _xlfn.LET(_xlpm._nextPosChars, IFERROR(FIND(_xlpm._chars, _xlpm.Text, _xlpm._acc + 1), 0), _xlpm._nextPos, MIN(_xlfn._xlws.FILTER(_xlpm._nextPosChars, _xlpm._nextPosChars &gt; 0, 0)), IF(_xlpm._nextPos = 0, -1, _xlpm._nextPos))))), MAX(_xlpm._nthPos, 0))))))), IF(_xlpm.Text = "", _xlpm.fnException(""), IF(NOT(ISO_8601.VALIDATE_CHARACTERS(_xlpm.Text, 2)), _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._Tpos, IFERROR(FIND("T", _xlpm.Text), 0), IF(_xlpm._Tpos &gt; 1, _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._sTime, IF(_xlpm._Tpos = 1, RIGHT(_xlpm.Text, LEN(_xlpm.Text) - 1), _xlpm.Text), _xlpm._len, LEN(_xlpm._sTime), _xlpm._colon1Pos, IFERROR(FIND(":", _xlpm._sTime), 0), _xlpm._colon2Pos, IFERROR(FIND(":", _xlpm._sTime, _xlpm._colon1Pos + 1), 0), _xlpm._decimalPos, _xlpm.fnFindNthCharPos(".,", _xlpm._sTime, 1), _xlpm._hash, (_xlpm._len * 4096) + (_xlpm._colon1Pos * 256) + (_xlpm._colon2Pos * 16) + _xlpm._decimalPos, _xlpm._hashLkup, _xlfn.IFNA(_xlfn.XMATCH(_xlpm._hash, _xlfn.CHOOSECOLS(_xlpm._fmtHashTable, 1), 0), 0), IF(_xlpm._hashLkup = 0, _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._defn, _xlfn.CHOOSEROWS(_xlpm._fmtHashTable, _xlpm._hashLkup), _xlpm._precision, INDEX(_xlpm._defn, 1, 2), _xlpm._extended, INDEX(_xlpm._defn, 1, 3), _xlpm._hour, VALUE(LEFT(_xlpm._sTime, 2)), _xlpm._minute, IF(_xlpm._precision &lt; 2, "", VALUE(MID(_xlpm._sTime, INDEX(_xlpm._defn, 1, 4), 2))), _xlpm._secLen, INDEX(_xlpm._defn, 1, 5), _xlpm._second, _xlfn.IFS(_xlpm._precision &lt; 3, "", _xlpm._precision = 3, VALUE(RIGHT(_xlpm._sTime, _xlpm._secLen)), TRUE, _xlfn.LET(_xlpm._sSec, RIGHT(_xlpm._sTime, _xlpm._secLen), _xlpm._intSec, VALUE(LEFT(_xlpm._sSec, 2)), _xlpm._fracSec, VALUE(RIGHT(_xlpm._sSec, _xlpm._secLen - 3)), _xlpm._decimalBase, INDEX({10,100,1000}, 1, _xlpm._precision - 3), _xlpm._intSec + (_xlpm._fracSec / _xlpm._decimalBase))), IF(NOT(ISO_8601.IS_VALID_TIME(_xlpm._hour, _xlpm._minute, _xlpm._second)), _xlpm.fnException("VALUE", _xlpm._precision, _xlpm._extended), _xlfn.HSTACK((_xlpm._Tpos = 1), _xlpm._precision, _xlpm._extended, _xlpm._hour, _xlpm._minute, _xlpm._second)))))))))))</definedName>
     <definedName name="ISO_8601.PARSE_TIME_ZONE">_xlfn.LAMBDA(_xlpm.Text, _xlfn.LET(_xlpm._fmtHashTable, {1536,3,3,1,0;3328,1,3,0,0;5376,2,1,0,4;6464,2,2,0,5;7424,3,1,0,4;9543,3,2,0,5}, _xlpm.fnException, _xlfn.LAMBDA(_xlpm._exception,_xlop._extended, _xlfn.IFS(_xlpm._exception = "N/A", {FALSE,"","",""}, _xlpm._exception = "VALUE", _xlfn.HSTACK(FALSE, 0, N(_xlpm._extended), {#VALUE!}), TRUE, {"","","",""})), _xlpm.fnCountChars, _xlfn.LAMBDA(_xlpm.CharArray,_xlpm.Text, IF(_xlpm.Text = "", 0, _xlfn.LET(_xlpm._removed, _xlfn.REDUCE(_xlpm.Text, _xlpm.CharArray, _xlfn.LAMBDA(_xlpm._acc,_xlpm._curr, SUBSTITUTE(_xlpm._acc, _xlpm._curr, ""))), LEN(_xlpm.Text) - LEN(_xlpm._removed)))), _xlpm.fnFindNthCharPos, _xlfn.LAMBDA(_xlpm.Chars,_xlpm.Text,_xlpm.N, _xlfn.LET(_xlpm._charCount, LEN(_xlpm.Chars), _xlpm._n, INT(N(_xlpm.N)), IF((_xlpm._charCount = 0) + (_xlpm._n = 0), 0, _xlfn.LET(_xlpm._chars, MID(_xlpm.Chars, _xlfn.SEQUENCE(1, _xlpm._charCount), 1), _xlpm._findCount, _xlpm.fnCountChars(_xlpm._chars, _xlpm.Text), IF(_xlpm._findCount &lt; ABS(_xlpm._n), 0, _xlfn.LET(_xlpm._nth, IF(_xlpm._n &gt; 0, _xlpm._n, _xlpm._findCount + _xlpm._n + 1), _xlpm._nthPos, _xlfn.REDUCE(0, _xlfn.SEQUENCE(1, _xlpm._nth), _xlfn.LAMBDA(_xlpm._acc,_xlpm._curr, IF(_xlpm._acc &lt; 0, -1, _xlfn.LET(_xlpm._nextPosChars, IFERROR(FIND(_xlpm._chars, _xlpm.Text, _xlpm._acc + 1), 0), _xlpm._nextPos, MIN(_xlfn._xlws.FILTER(_xlpm._nextPosChars, _xlpm._nextPosChars &gt; 0, 0)), IF(_xlpm._nextPos = 0, -1, _xlpm._nextPos))))), MAX(_xlpm._nthPos, 0))))))), IF(_xlpm.Text = "", _xlpm.fnException(""), IF(NOT(ISO_8601.VALIDATE_CHARACTERS(_xlpm.Text, 3)), _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._len, LEN(_xlpm.Text), _xlpm._Zonly, N((_xlpm._len = 1) * (IFERROR(FIND("Z", _xlpm.Text), 0) = 1)), _xlpm._lastSignPosAt1, N(_xlpm.fnFindNthCharPos("+-" &amp; _xlfn.UNICHAR(8722), _xlpm.Text, -1) = 1), _xlpm._colon1Pos, IFERROR(FIND(":", _xlpm.Text), 0), _xlpm._colon2Pos, IFERROR(FIND(":", _xlpm.Text, _xlpm._colon1Pos + 1), 0), _xlpm._hash, (_xlpm._len * 1024) + (_xlpm._Zonly * 512) + (_xlpm._lastSignPosAt1 * 256) + (_xlpm._colon1Pos * 16) + _xlpm._colon2Pos, _xlpm._hashLkup, _xlfn.IFNA(_xlfn.XMATCH(_xlpm._hash, _xlfn.CHOOSECOLS(_xlpm._fmtHashTable, 1), 0), 0), IF(_xlpm._hashLkup = 0, _xlpm.fnException("N/A"), _xlfn.LET(_xlpm._defn, _xlfn.CHOOSEROWS(_xlpm._fmtHashTable, _xlpm._hashLkup), _xlpm._precision, INDEX(_xlpm._defn, 1, 2), _xlpm._extended, INDEX(_xlpm._defn, 1, 3), IF(INDEX(_xlpm._defn, 1, 4) &gt; 0, _xlfn.HSTACK(TRUE, _xlpm._precision, _xlpm._extended, 0), _xlfn.LET(_xlpm._sign, _xlfn.IFS(LEFT(_xlpm.Text, 1) = "-", -1, _xlfn.UNICODE(LEFT(_xlpm.Text, 1)) = 8722, -1, TRUE, 1), _xlpm._hour, _xlpm._sign * VALUE(MID(_xlpm.Text, 2, 2)), _xlpm._minute, IF(_xlpm._precision &lt; 2, "", VALUE(MID(_xlpm.Text, INDEX(_xlpm._defn, 1, 5), 2))), _xlpm._second, IF(_xlpm._precision &lt; 3, "", VALUE(RIGHT(_xlpm.Text, 2))), _xlpm._tzoMinutes, INT((N(_xlpm._hour) * 3600) + (N(_xlpm._minute) * 60) + N(_xlpm._second)) / 60, IF(NOT(ISO_8601.IS_VALID_TIME_ZONE(_xlpm._tzoMinutes)), _xlpm.fnException("VALUE", _xlpm._extended), _xlfn.HSTACK(TRUE, _xlpm._precision, _xlpm._extended, _xlpm._tzoMinutes)))))))))))</definedName>
     <definedName name="ISO_8601.TO_WEEK_DATE">_xlfn.LAMBDA(_xlpm.YearCE,_xlpm.Month,_xlpm.Day, IF(ISNUMBER(_xlpm.Month), IF(NOT(ISO_8601.IS_VALID_DATE(_xlpm.YearCE, _xlpm.Month, _xlpm.Day, 1)), #VALUE!, _xlfn.LET(_xlpm._fracDay, _xlpm.Day - INT(_xlpm.Day), _xlpm._dow, ISO_8601.DAY_OF_WEEK(_xlpm.YearCE, _xlpm.Month, _xlpm.Day), _xlpm._week, ISO_8601.WEEK_NUMBER(_xlpm.YearCE, _xlpm.Month, _xlpm.Day), _xlpm._yearCE, INT(_xlpm.YearCE) + _xlfn.IFS((_xlpm._week = 1) * (_xlpm.Month = 12), 1, (_xlpm._week &gt;= 52) * (_xlpm.Month = 1), -1, TRUE, 0), _xlfn.HSTACK(_xlpm._yearCE, _xlpm._week, _xlpm._dow + _xlpm._fracDay))), IF(NOT(ISO_8601.IS_VALID_ORDINAL_DATE(_xlpm.YearCE, _xlpm.Day)), #VALUE!, _xlfn.LET(_xlpm._fracDay, _xlpm.Day - INT(_xlpm.Day), _xlpm._dow, ISO_8601.DAY_OF_WEEK_FROM_ORDINAL(_xlpm.YearCE, _xlpm.Day), _xlpm._week, ISO_8601.WEEK_NUMBER_FROM_ORDINAL(_xlpm.YearCE, _xlpm.Day), _xlpm._yearCE, INT(_xlpm.YearCE) + _xlfn.IFS((_xlpm._week = 1) * (_xlpm.Month = 12), 1, (_xlpm._week &gt;= 52) * (_xlpm.Month = 1), -1, TRUE, 0), _xlfn.HSTACK(_xlpm._yearCE, _xlpm._week, _xlpm._dow + _xlpm._fracDay)))))</definedName>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="172">
   <si>
     <t>IS_VALID_YEAR(YearCE)</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>ISO8601</t>
+  </si>
+  <si>
+    <t>AllowMixedFormat</t>
   </si>
 </sst>
 </file>
@@ -894,7 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -955,7 +958,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -967,8 +969,10 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -1764,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A7EFF7-D7B6-49F8-9B8B-8E9959D1B63D}">
   <dimension ref="A1:V58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,24 +1793,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58" t="s">
+      <c r="A1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2007,34 +2011,34 @@
       <c r="A16" s="26"/>
     </row>
     <row r="18" spans="1:22" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58" t="s">
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="58" t="s">
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="58"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="60"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2528,25 +2532,25 @@
       <c r="S38" s="25"/>
     </row>
     <row r="41" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="58" t="s">
+      <c r="A41" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="58"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58" t="s">
+      <c r="B41" s="60"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="58"/>
-      <c r="L41" s="58"/>
-      <c r="M41" s="58"/>
-      <c r="N41" s="58"/>
-      <c r="O41" s="58"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
+      <c r="K41" s="60"/>
+      <c r="L41" s="60"/>
+      <c r="M41" s="60"/>
+      <c r="N41" s="60"/>
+      <c r="O41" s="60"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -2926,21 +2930,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -3109,22 +3113,22 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="58" t="s">
+      <c r="H16" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
-      <c r="L16" s="58"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
       <c r="M16" s="2"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -3384,22 +3388,22 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="H30" s="58" t="s">
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="H30" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -3563,24 +3567,24 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="58" t="s">
+      <c r="A42" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="58"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="58" t="s">
+      <c r="H42" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="I42" s="58"/>
-      <c r="J42" s="58"/>
-      <c r="K42" s="58"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="58"/>
-      <c r="N42" s="58"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="60"/>
+      <c r="L42" s="60"/>
+      <c r="M42" s="60"/>
+      <c r="N42" s="60"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -3782,25 +3786,25 @@
       </c>
     </row>
     <row r="55" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A55" s="58" t="s">
+      <c r="A55" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="58"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="60"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="58" t="s">
+      <c r="H55" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="I55" s="58"/>
-      <c r="J55" s="58"/>
-      <c r="K55" s="58"/>
-      <c r="L55" s="58"/>
-      <c r="M55" s="58"/>
-      <c r="N55" s="58"/>
-      <c r="O55" s="58"/>
+      <c r="I55" s="60"/>
+      <c r="J55" s="60"/>
+      <c r="K55" s="60"/>
+      <c r="L55" s="60"/>
+      <c r="M55" s="60"/>
+      <c r="N55" s="60"/>
+      <c r="O55" s="60"/>
     </row>
     <row r="57" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
@@ -4426,31 +4430,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D209D5E7-E650-490C-9B1C-E77B3A161125}">
-  <dimension ref="A1:S134"/>
+  <dimension ref="A1:T134"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4461,7 +4467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -4470,7 +4476,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -4482,7 +4488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>43</v>
       </c>
@@ -4494,7 +4500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>44</v>
       </c>
@@ -4506,7 +4512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>45</v>
       </c>
@@ -4518,7 +4524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>46</v>
       </c>
@@ -4530,7 +4536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>47</v>
       </c>
@@ -4542,7 +4548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>48</v>
       </c>
@@ -4554,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>48</v>
       </c>
@@ -4566,7 +4572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>49</v>
       </c>
@@ -4578,7 +4584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>50</v>
       </c>
@@ -4590,7 +4596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>51</v>
       </c>
@@ -4603,12 +4609,13 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -4958,7 +4965,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
         <v>67</v>
       </c>
@@ -4985,7 +4992,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
         <v>64</v>
       </c>
@@ -5012,7 +5019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
         <v>68</v>
       </c>
@@ -5039,7 +5046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
         <v>69</v>
       </c>
@@ -5066,7 +5073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
         <v>70</v>
       </c>
@@ -5093,7 +5100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="36" t="s">
         <v>63</v>
       </c>
@@ -5120,7 +5127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="s">
         <v>120</v>
       </c>
@@ -5147,7 +5154,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="36" t="s">
         <v>133</v>
       </c>
@@ -5174,7 +5181,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>135</v>
       </c>
@@ -5201,15 +5208,16 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="58" t="s">
+    <row r="44" spans="1:17" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A44" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-    </row>
-    <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="60"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="60"/>
+    </row>
+    <row r="46" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>1</v>
       </c>
@@ -5231,9 +5239,9 @@
       <c r="G46" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="P46" s="43"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q46" s="43"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="32"/>
       <c r="B47" s="8" t="str" cm="1">
         <f t="array" ref="B47:G47">ISO_8601.PARSE_TIME(A47)</f>
@@ -5255,7 +5263,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>1</v>
       </c>
@@ -5279,7 +5287,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="34" t="s">
         <v>71</v>
       </c>
@@ -5303,7 +5311,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
         <v>128</v>
       </c>
@@ -5327,7 +5335,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
         <v>123</v>
       </c>
@@ -5351,7 +5359,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
         <v>75</v>
       </c>
@@ -5375,7 +5383,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
         <v>76</v>
       </c>
@@ -5399,7 +5407,7 @@
         <v>35.677999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
         <v>124</v>
       </c>
@@ -5423,7 +5431,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
         <v>125</v>
       </c>
@@ -5447,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
         <v>77</v>
       </c>
@@ -5470,10 +5478,10 @@
       <c r="G56" s="12">
         <v>34</v>
       </c>
-      <c r="N56" s="40"/>
-      <c r="S56" s="40"/>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O56" s="40"/>
+      <c r="T56" s="40"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
         <v>78</v>
       </c>
@@ -5496,9 +5504,9 @@
       <c r="G57" s="9">
         <v>54.012</v>
       </c>
-      <c r="N57" s="40"/>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O57" s="40"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
         <v>92</v>
       </c>
@@ -5521,9 +5529,9 @@
       <c r="G58" s="3">
         <v>12.34</v>
       </c>
-      <c r="N58" s="40"/>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O58" s="40"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
         <v>126</v>
       </c>
@@ -5546,10 +5554,10 @@
       <c r="G59" s="9" t="str">
         <v/>
       </c>
-      <c r="N59" s="40"/>
-      <c r="R59" s="40"/>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O59" s="40"/>
+      <c r="S59" s="40"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="36" t="s">
         <v>79</v>
       </c>
@@ -5572,10 +5580,10 @@
       <c r="G60" s="3" t="str">
         <v/>
       </c>
-      <c r="N60" s="40"/>
-      <c r="Q60" s="40"/>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O60" s="40"/>
+      <c r="R60" s="40"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
         <v>80</v>
       </c>
@@ -5598,10 +5606,10 @@
       <c r="G61" s="9" t="str">
         <v/>
       </c>
-      <c r="N61" s="40"/>
-      <c r="R61" s="40"/>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O61" s="40"/>
+      <c r="S61" s="40"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="36" t="s">
         <v>127</v>
       </c>
@@ -5624,31 +5632,32 @@
       <c r="G62" s="3" t="str">
         <v/>
       </c>
-      <c r="N62" s="40"/>
-      <c r="Q62" s="40"/>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N63" s="40"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N64" s="40"/>
-      <c r="R64" s="40"/>
-    </row>
-    <row r="65" spans="1:18" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="58" t="s">
+      <c r="O62" s="40"/>
+      <c r="R62" s="40"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O63" s="40"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O64" s="40"/>
+      <c r="S64" s="40"/>
+    </row>
+    <row r="65" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A65" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="B65" s="58"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-      <c r="N65" s="40"/>
-      <c r="Q65" s="40"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N66" s="40"/>
-      <c r="R66" s="40"/>
-    </row>
-    <row r="67" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B65" s="60"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="60"/>
+      <c r="O65" s="40"/>
+      <c r="R65" s="40"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O66" s="40"/>
+      <c r="S66" s="40"/>
+    </row>
+    <row r="67" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>1</v>
       </c>
@@ -5664,9 +5673,9 @@
       <c r="E67" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="L67" s="40"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M67" s="40"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="32"/>
       <c r="B68" s="8" t="str" cm="1">
         <f t="array" ref="B68:E68">ISO_8601.PARSE_TIME_ZONE(A68)</f>
@@ -5681,10 +5690,10 @@
       <c r="E68" s="37" t="str">
         <v/>
       </c>
-      <c r="L68" s="40"/>
-      <c r="Q68" s="40"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M68" s="40"/>
+      <c r="R68" s="40"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
         <v>1</v>
       </c>
@@ -5702,7 +5711,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="34" t="s">
         <v>90</v>
       </c>
@@ -5720,7 +5729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="35" t="s">
         <v>82</v>
       </c>
@@ -5738,7 +5747,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="32" t="s">
         <v>83</v>
       </c>
@@ -5756,7 +5765,7 @@
         <v>-720</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
         <v>84</v>
       </c>
@@ -5774,7 +5783,7 @@
         <v>-720</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="32" t="s">
         <v>85</v>
       </c>
@@ -5792,7 +5801,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
         <v>86</v>
       </c>
@@ -5810,7 +5819,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="32" t="s">
         <v>87</v>
       </c>
@@ -5828,7 +5837,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="35" t="s">
         <v>88</v>
       </c>
@@ -5846,7 +5855,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="32" t="s">
         <v>89</v>
       </c>
@@ -5864,7 +5873,7 @@
         <v>570.36666666666667</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="36" t="s">
         <v>91</v>
       </c>
@@ -5882,7 +5891,7 @@
         <v>-519.63333333333333</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="41" t="s">
         <v>93</v>
       </c>
@@ -5919,12 +5928,13 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A84" s="58" t="s">
+      <c r="A84" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="B84" s="58"/>
-      <c r="C84" s="58"/>
-      <c r="D84" s="58"/>
+      <c r="B84" s="60"/>
+      <c r="C84" s="60"/>
+      <c r="D84" s="60"/>
+      <c r="E84" s="60"/>
     </row>
     <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
@@ -6154,7 +6164,7 @@
         <v>Z</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="32" t="s">
         <v>138</v>
       </c>
@@ -6175,7 +6185,7 @@
         <v>+930</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="36" t="s">
         <v>137</v>
       </c>
@@ -6196,7 +6206,7 @@
         <v>Z</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="41" t="s">
         <v>107</v>
       </c>
@@ -6217,7 +6227,7 @@
         <v>+09</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="36" t="s">
         <v>80</v>
       </c>
@@ -6238,7 +6248,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="44" t="s">
         <v>114</v>
       </c>
@@ -6259,7 +6269,7 @@
         <v>+15</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="36" t="s">
         <v>133</v>
       </c>
@@ -6280,7 +6290,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="44" t="s">
         <v>139</v>
       </c>
@@ -6301,62 +6311,64 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A106" s="58" t="s">
+    <row r="106" spans="1:17" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A106" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="B106" s="58"/>
-      <c r="C106" s="58"/>
-      <c r="D106" s="58"/>
-    </row>
-    <row r="108" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="B106" s="60"/>
+      <c r="C106" s="60"/>
+      <c r="D106" s="60"/>
+      <c r="E106" s="60"/>
+    </row>
+    <row r="108" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B108" s="31" t="s">
+      <c r="B108" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C108" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="C108" s="31" t="s">
+      <c r="D108" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="D108" s="31" t="s">
+      <c r="E108" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="E108" s="31" t="s">
+      <c r="F108" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="F108" s="31" t="s">
+      <c r="G108" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="G108" s="31" t="s">
+      <c r="H108" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H108" s="31" t="s">
+      <c r="I108" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="I108" s="31" t="s">
+      <c r="J108" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="J108" s="31" t="s">
+      <c r="K108" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="K108" s="31" t="s">
+      <c r="L108" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="L108" s="31" t="s">
+      <c r="M108" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="M108" s="31" t="s">
+      <c r="N108" s="31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="32"/>
-      <c r="B109" s="8" t="str" cm="1">
-        <f t="array" ref="B109:M109">ISO_8601.PARSE_ISO8601(A109)</f>
-        <v/>
-      </c>
-      <c r="C109" s="8" t="str">
+      <c r="B109" s="8"/>
+      <c r="C109" s="8" t="str" cm="1">
+        <f t="array" ref="C109:N109">ISO_8601.PARSE_ISO8601(A109,B109)</f>
         <v/>
       </c>
       <c r="D109" s="8" t="str">
@@ -6386,24 +6398,25 @@
       <c r="L109" s="8" t="str">
         <v/>
       </c>
-      <c r="M109" s="37" t="str">
-        <v/>
-      </c>
-      <c r="P109" s="1"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M109" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N109" s="37" t="str">
+        <v/>
+      </c>
+      <c r="Q109" s="1"/>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B110" s="11" t="b" cm="1">
-        <f t="array" ref="B110:M110">ISO_8601.PARSE_ISO8601(A110)</f>
-        <v>0</v>
-      </c>
-      <c r="C110" s="11">
-        <v>0</v>
-      </c>
-      <c r="D110" s="11" t="str">
-        <v/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="11" t="b" cm="1">
+        <f t="array" ref="C110:N110">ISO_8601.PARSE_ISO8601(A110,B110)</f>
+        <v>0</v>
+      </c>
+      <c r="D110" s="11">
+        <v>0</v>
       </c>
       <c r="E110" s="11" t="str">
         <v/>
@@ -6429,23 +6442,24 @@
       <c r="L110" s="11" t="str">
         <v/>
       </c>
-      <c r="M110" s="38" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M110" s="11" t="str">
+        <v/>
+      </c>
+      <c r="N110" s="38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="B111" s="8" t="b" cm="1">
-        <f t="array" ref="B111:M111">ISO_8601.PARSE_ISO8601(A111)</f>
-        <v>0</v>
-      </c>
-      <c r="C111" s="8">
-        <v>0</v>
-      </c>
-      <c r="D111" s="8" t="str">
-        <v/>
+      <c r="B111" s="57"/>
+      <c r="C111" s="8" t="b" cm="1">
+        <f t="array" ref="C111:N111">ISO_8601.PARSE_ISO8601(A111,B111)</f>
+        <v>0</v>
+      </c>
+      <c r="D111" s="8">
+        <v>0</v>
       </c>
       <c r="E111" s="8" t="str">
         <v/>
@@ -6471,23 +6485,24 @@
       <c r="L111" s="8" t="str">
         <v/>
       </c>
-      <c r="M111" s="37" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M111" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N111" s="37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B112" s="11" t="b" cm="1">
-        <f t="array" ref="B112:M112">ISO_8601.PARSE_ISO8601(A112)</f>
-        <v>0</v>
-      </c>
-      <c r="C112" s="11">
-        <v>0</v>
-      </c>
-      <c r="D112" s="11" t="str">
-        <v/>
+      <c r="B112" s="58"/>
+      <c r="C112" s="11" t="b" cm="1">
+        <f t="array" ref="C112:N112">ISO_8601.PARSE_ISO8601(A112,B112)</f>
+        <v>0</v>
+      </c>
+      <c r="D112" s="11">
+        <v>0</v>
       </c>
       <c r="E112" s="11" t="str">
         <v/>
@@ -6513,35 +6528,36 @@
       <c r="L112" s="11" t="str">
         <v/>
       </c>
-      <c r="M112" s="38" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M112" s="11" t="str">
+        <v/>
+      </c>
+      <c r="N112" s="38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B113" s="8" t="b" cm="1">
-        <f t="array" ref="B113:M113">ISO_8601.PARSE_ISO8601(A113)</f>
-        <v>0</v>
-      </c>
-      <c r="C113" s="8">
+      <c r="B113" s="57"/>
+      <c r="C113" s="8" t="b" cm="1">
+        <f t="array" ref="C113:N113">ISO_8601.PARSE_ISO8601(A113,B113)</f>
+        <v>0</v>
+      </c>
+      <c r="D113" s="8">
         <v>5</v>
       </c>
-      <c r="D113" s="8">
-        <v>1</v>
-      </c>
       <c r="E113" s="8">
+        <v>1</v>
+      </c>
+      <c r="F113" s="8">
         <v>2</v>
       </c>
-      <c r="F113" s="8">
-        <v>1</v>
-      </c>
       <c r="G113" s="8">
-        <v>2023</v>
-      </c>
-      <c r="H113" s="8" t="str">
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="H113" s="8">
+        <v>2023</v>
       </c>
       <c r="I113" s="8" t="str">
         <v/>
@@ -6555,39 +6571,40 @@
       <c r="L113" s="8" t="str">
         <v/>
       </c>
-      <c r="M113" s="37">
+      <c r="M113" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N113" s="37">
         <v>570.36666666666667</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="B114" s="11" t="b" cm="1">
-        <f t="array" ref="B114:M114">ISO_8601.PARSE_ISO8601(A114)</f>
-        <v>0</v>
-      </c>
-      <c r="C114" s="11">
+      <c r="B114" s="58"/>
+      <c r="C114" s="11" t="b" cm="1">
+        <f t="array" ref="C114:N114">ISO_8601.PARSE_ISO8601(A114,B114)</f>
+        <v>0</v>
+      </c>
+      <c r="D114" s="11">
         <v>5</v>
-      </c>
-      <c r="D114" s="11">
-        <v>2</v>
       </c>
       <c r="E114" s="11">
         <v>2</v>
       </c>
       <c r="F114" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G114" s="11">
+        <v>1</v>
+      </c>
+      <c r="H114" s="11">
         <v>99999</v>
       </c>
-      <c r="H114" s="11">
+      <c r="I114" s="11">
         <v>10</v>
       </c>
-      <c r="I114" s="11" t="str">
-        <v/>
-      </c>
       <c r="J114" s="11" t="str">
         <v/>
       </c>
@@ -6597,74 +6614,76 @@
       <c r="L114" s="11" t="str">
         <v/>
       </c>
-      <c r="M114" s="38">
+      <c r="M114" s="11" t="str">
+        <v/>
+      </c>
+      <c r="N114" s="38">
         <v>570.36666666666667</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="B115" s="8" t="b" cm="1">
-        <f t="array" ref="B115:M115">ISO_8601.PARSE_ISO8601(A115)</f>
-        <v>1</v>
-      </c>
-      <c r="C115" s="8">
+      <c r="B115" s="57"/>
+      <c r="C115" s="8" t="b" cm="1">
+        <f t="array" ref="C115:N115">ISO_8601.PARSE_ISO8601(A115,B115)</f>
+        <v>1</v>
+      </c>
+      <c r="D115" s="8">
         <v>7</v>
       </c>
-      <c r="D115" s="8">
+      <c r="E115" s="8">
         <v>9</v>
       </c>
-      <c r="E115" s="8">
+      <c r="F115" s="8">
         <v>2</v>
       </c>
-      <c r="F115" s="8">
+      <c r="G115" s="8">
         <v>3</v>
       </c>
-      <c r="G115" s="8">
+      <c r="H115" s="8">
         <v>99999</v>
       </c>
-      <c r="H115" s="8">
+      <c r="I115" s="8">
         <v>15</v>
       </c>
-      <c r="I115" s="8">
+      <c r="J115" s="8">
         <v>2</v>
       </c>
-      <c r="J115" s="8">
+      <c r="K115" s="8">
         <v>14</v>
       </c>
-      <c r="K115" s="8">
+      <c r="L115" s="8">
         <v>25</v>
       </c>
-      <c r="L115" s="8">
+      <c r="M115" s="8">
         <v>21.123000000000001</v>
       </c>
-      <c r="M115" s="37">
+      <c r="N115" s="37">
         <v>570.36666666666667</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="B116" s="11" t="b" cm="1">
-        <f t="array" ref="B116:M116">ISO_8601.PARSE_ISO8601(A116)</f>
-        <v>1</v>
-      </c>
-      <c r="C116" s="11">
+      <c r="B116" s="58"/>
+      <c r="C116" s="11" t="b" cm="1">
+        <f t="array" ref="C116:N116">ISO_8601.PARSE_ISO8601(A116,B116)</f>
+        <v>1</v>
+      </c>
+      <c r="D116" s="11">
         <v>3</v>
       </c>
-      <c r="D116" s="11">
+      <c r="E116" s="11">
         <v>5</v>
       </c>
-      <c r="E116" s="11">
+      <c r="F116" s="11">
         <v>2</v>
       </c>
-      <c r="F116" s="11">
-        <v>0</v>
-      </c>
-      <c r="G116" s="11" t="str">
-        <v/>
+      <c r="G116" s="11">
+        <v>0</v>
       </c>
       <c r="H116" s="11" t="str">
         <v/>
@@ -6672,83 +6691,85 @@
       <c r="I116" s="11" t="str">
         <v/>
       </c>
-      <c r="J116" s="11">
+      <c r="J116" s="11" t="str">
+        <v/>
+      </c>
+      <c r="K116" s="11">
         <v>12</v>
       </c>
-      <c r="K116" s="11">
+      <c r="L116" s="11">
         <v>35</v>
       </c>
-      <c r="L116" s="11" t="str">
-        <v/>
-      </c>
-      <c r="M116" s="38">
+      <c r="M116" s="11" t="str">
+        <v/>
+      </c>
+      <c r="N116" s="38">
         <v>570</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="B117" s="8" t="b" cm="1">
-        <f t="array" ref="B117:M117">ISO_8601.PARSE_ISO8601(A117)</f>
-        <v>1</v>
-      </c>
-      <c r="C117" s="8">
+      <c r="B117" s="57"/>
+      <c r="C117" s="8" t="b" cm="1">
+        <f t="array" ref="C117:N117">ISO_8601.PARSE_ISO8601(A117,B117)</f>
+        <v>1</v>
+      </c>
+      <c r="D117" s="8">
         <v>6</v>
       </c>
-      <c r="D117" s="8">
+      <c r="E117" s="8">
         <v>5</v>
       </c>
-      <c r="E117" s="8">
+      <c r="F117" s="8">
         <v>2</v>
       </c>
-      <c r="F117" s="8">
+      <c r="G117" s="8">
         <v>3</v>
       </c>
-      <c r="G117" s="8">
-        <v>2023</v>
-      </c>
       <c r="H117" s="8">
+        <v>2023</v>
+      </c>
+      <c r="I117" s="8">
         <v>15</v>
       </c>
-      <c r="I117" s="8">
+      <c r="J117" s="8">
         <v>2</v>
       </c>
-      <c r="J117" s="8">
+      <c r="K117" s="8">
         <v>14</v>
       </c>
-      <c r="K117" s="8">
+      <c r="L117" s="8">
         <v>25</v>
       </c>
-      <c r="L117" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M117" s="37" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M117" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N117" s="37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B118" s="11" t="b" cm="1">
-        <f t="array" ref="B118:M118">ISO_8601.PARSE_ISO8601(A118)</f>
-        <v>1</v>
-      </c>
-      <c r="C118" s="11">
+      <c r="B118" s="58"/>
+      <c r="C118" s="11" t="b" cm="1">
+        <f t="array" ref="C118:N118">ISO_8601.PARSE_ISO8601(A118,B118)</f>
+        <v>1</v>
+      </c>
+      <c r="D118" s="11">
         <v>2</v>
       </c>
-      <c r="D118" s="11">
+      <c r="E118" s="11">
         <v>9</v>
       </c>
-      <c r="E118" s="11">
+      <c r="F118" s="11">
         <v>2</v>
       </c>
-      <c r="F118" s="11">
-        <v>0</v>
-      </c>
-      <c r="G118" s="11" t="str">
-        <v/>
+      <c r="G118" s="11">
+        <v>0</v>
       </c>
       <c r="H118" s="11" t="str">
         <v/>
@@ -6756,41 +6777,42 @@
       <c r="I118" s="11" t="str">
         <v/>
       </c>
-      <c r="J118" s="11">
+      <c r="J118" s="11" t="str">
+        <v/>
+      </c>
+      <c r="K118" s="11">
         <v>12</v>
       </c>
-      <c r="K118" s="11">
+      <c r="L118" s="11">
         <v>35</v>
       </c>
-      <c r="L118" s="11">
+      <c r="M118" s="11">
         <v>12</v>
       </c>
-      <c r="M118" s="38" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N118" s="38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="B119" s="8" t="b" cm="1">
-        <f t="array" ref="B119:M119">ISO_8601.PARSE_ISO8601(A119)</f>
-        <v>1</v>
-      </c>
-      <c r="C119" s="8">
+      <c r="B119" s="57"/>
+      <c r="C119" s="8" t="b" cm="1">
+        <f t="array" ref="C119:N119">ISO_8601.PARSE_ISO8601(A119,B119)</f>
+        <v>1</v>
+      </c>
+      <c r="D119" s="8">
         <v>3</v>
       </c>
-      <c r="D119" s="8">
+      <c r="E119" s="8">
         <v>9</v>
       </c>
-      <c r="E119" s="8">
-        <v>1</v>
-      </c>
       <c r="F119" s="8">
-        <v>0</v>
-      </c>
-      <c r="G119" s="8" t="str">
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="G119" s="8">
+        <v>0</v>
       </c>
       <c r="H119" s="8" t="str">
         <v/>
@@ -6798,41 +6820,42 @@
       <c r="I119" s="8" t="str">
         <v/>
       </c>
-      <c r="J119" s="8">
+      <c r="J119" s="8" t="str">
+        <v/>
+      </c>
+      <c r="K119" s="8">
         <v>12</v>
       </c>
-      <c r="K119" s="8">
+      <c r="L119" s="8">
         <v>35</v>
       </c>
-      <c r="L119" s="8">
+      <c r="M119" s="8">
         <v>12</v>
       </c>
-      <c r="M119" s="37">
+      <c r="N119" s="37">
         <v>540</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B120" s="11" t="b" cm="1">
-        <f t="array" ref="B120:M120">ISO_8601.PARSE_ISO8601(A120)</f>
-        <v>0</v>
-      </c>
-      <c r="C120" s="11">
-        <v>1</v>
+      <c r="B120" s="58"/>
+      <c r="C120" s="11" t="b" cm="1">
+        <f t="array" ref="C120:N120">ISO_8601.PARSE_ISO8601(A120,B120)</f>
+        <v>0</v>
       </c>
       <c r="D120" s="11">
+        <v>1</v>
+      </c>
+      <c r="E120" s="11">
         <v>6</v>
       </c>
-      <c r="E120" s="11">
+      <c r="F120" s="11">
         <v>3</v>
       </c>
-      <c r="F120" s="11">
-        <v>0</v>
-      </c>
-      <c r="G120" s="11" t="str">
-        <v/>
+      <c r="G120" s="11">
+        <v>0</v>
       </c>
       <c r="H120" s="11" t="str">
         <v/>
@@ -6849,35 +6872,36 @@
       <c r="L120" s="11" t="str">
         <v/>
       </c>
-      <c r="M120" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M120" s="11" t="str">
+        <v/>
+      </c>
+      <c r="N120" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B121" s="8" t="b" cm="1">
-        <f t="array" ref="B121:M121">ISO_8601.PARSE_ISO8601(A121)</f>
-        <v>1</v>
-      </c>
-      <c r="C121" s="8">
+      <c r="B121" s="57"/>
+      <c r="C121" s="8" t="b" cm="1">
+        <f t="array" ref="C121:N121">ISO_8601.PARSE_ISO8601(A121,B121)</f>
+        <v>1</v>
+      </c>
+      <c r="D121" s="8">
         <v>4</v>
       </c>
-      <c r="D121" s="8">
-        <v>1</v>
-      </c>
       <c r="E121" s="8">
+        <v>1</v>
+      </c>
+      <c r="F121" s="8">
         <v>3</v>
       </c>
-      <c r="F121" s="8">
-        <v>1</v>
-      </c>
       <c r="G121" s="8">
-        <v>2023</v>
-      </c>
-      <c r="H121" s="8" t="str">
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="H121" s="8">
+        <v>2023</v>
       </c>
       <c r="I121" s="8" t="str">
         <v/>
@@ -6891,116 +6915,121 @@
       <c r="L121" s="8" t="str">
         <v/>
       </c>
-      <c r="M121" s="37" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M121" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N121" s="37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="B122" s="11" t="b" cm="1">
-        <f t="array" ref="B122:M122">ISO_8601.PARSE_ISO8601(A122)</f>
-        <v>0</v>
-      </c>
-      <c r="C122" s="11">
+      <c r="B122" s="58">
+        <v>1</v>
+      </c>
+      <c r="C122" s="11" t="b" cm="1">
+        <f t="array" ref="C122:N122">ISO_8601.PARSE_ISO8601(A122,B122)</f>
+        <v>1</v>
+      </c>
+      <c r="D122" s="11">
         <v>6</v>
       </c>
-      <c r="D122" s="11">
+      <c r="E122" s="11">
         <v>5</v>
       </c>
-      <c r="E122" s="11">
-        <v>0</v>
-      </c>
       <c r="F122" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G122" s="11">
-        <v>2023</v>
+        <v>1</v>
       </c>
       <c r="H122" s="11">
+        <v>2023</v>
+      </c>
+      <c r="I122" s="11">
         <v>2</v>
       </c>
-      <c r="I122" s="11">
+      <c r="J122" s="11">
         <v>23</v>
       </c>
-      <c r="J122" s="11">
+      <c r="K122" s="11">
         <v>14</v>
       </c>
-      <c r="K122" s="11">
+      <c r="L122" s="11">
         <v>35</v>
       </c>
-      <c r="L122" s="11" t="str">
-        <v/>
-      </c>
-      <c r="M122" s="38" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M122" s="11" t="str">
+        <v/>
+      </c>
+      <c r="N122" s="38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="B123" s="8" t="b" cm="1">
-        <f t="array" ref="B123:M123">ISO_8601.PARSE_ISO8601(A123)</f>
-        <v>1</v>
-      </c>
-      <c r="C123" s="8">
+      <c r="B123" s="57"/>
+      <c r="C123" s="8" t="b" cm="1">
+        <f t="array" ref="C123:N123">ISO_8601.PARSE_ISO8601(A123,B123)</f>
+        <v>1</v>
+      </c>
+      <c r="D123" s="8">
         <v>7</v>
       </c>
-      <c r="D123" s="8">
+      <c r="E123" s="8">
         <v>5</v>
       </c>
-      <c r="E123" s="8">
+      <c r="F123" s="8">
         <v>2</v>
       </c>
-      <c r="F123" s="8">
-        <v>1</v>
-      </c>
       <c r="G123" s="8">
-        <v>2023</v>
+        <v>1</v>
       </c>
       <c r="H123" s="8">
+        <v>2023</v>
+      </c>
+      <c r="I123" s="8">
         <v>2</v>
       </c>
-      <c r="I123" s="8">
+      <c r="J123" s="8">
         <v>23</v>
       </c>
-      <c r="J123" s="8">
+      <c r="K123" s="8">
         <v>14</v>
       </c>
-      <c r="K123" s="8">
+      <c r="L123" s="8">
         <v>35</v>
       </c>
-      <c r="L123" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M123" s="37">
+      <c r="M123" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N123" s="37">
         <v>900</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B124" s="11" t="b" cm="1">
-        <f t="array" ref="B124:M124">ISO_8601.PARSE_ISO8601(A124)</f>
-        <v>0</v>
-      </c>
-      <c r="C124" s="11">
-        <v>1</v>
+      <c r="B124" s="58"/>
+      <c r="C124" s="11" t="b" cm="1">
+        <f t="array" ref="C124:N124">ISO_8601.PARSE_ISO8601(A124,B124)</f>
+        <v>0</v>
       </c>
       <c r="D124" s="11">
+        <v>1</v>
+      </c>
+      <c r="E124" s="11">
         <v>4</v>
       </c>
-      <c r="E124" s="11">
+      <c r="F124" s="11">
         <v>2</v>
       </c>
-      <c r="F124" s="11">
-        <v>1</v>
-      </c>
-      <c r="G124" s="11" t="e">
-        <v>#VALUE!</v>
+      <c r="G124" s="11">
+        <v>1</v>
       </c>
       <c r="H124" s="11" t="e">
         <v>#VALUE!</v>
@@ -7008,8 +7037,8 @@
       <c r="I124" s="11" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="J124" s="11" t="str">
-        <v/>
+      <c r="J124" s="11" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="K124" s="11" t="str">
         <v/>
@@ -7017,80 +7046,82 @@
       <c r="L124" s="11" t="str">
         <v/>
       </c>
-      <c r="M124" s="38">
+      <c r="M124" s="11" t="str">
+        <v/>
+      </c>
+      <c r="N124" s="38">
         <v>540</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="B125" s="8" t="b" cm="1">
-        <f t="array" ref="B125:M125">ISO_8601.PARSE_ISO8601(A125)</f>
-        <v>0</v>
-      </c>
-      <c r="C125" s="8">
+      <c r="B125" s="57"/>
+      <c r="C125" s="8" t="b" cm="1">
+        <f t="array" ref="C125:N125">ISO_8601.PARSE_ISO8601(A125,B125)</f>
+        <v>0</v>
+      </c>
+      <c r="D125" s="8">
         <v>6</v>
-      </c>
-      <c r="D125" s="8">
-        <v>2</v>
       </c>
       <c r="E125" s="8">
         <v>2</v>
       </c>
       <c r="F125" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G125" s="8">
-        <v>2023</v>
+        <v>1</v>
       </c>
       <c r="H125" s="8">
+        <v>2023</v>
+      </c>
+      <c r="I125" s="8">
         <v>2</v>
       </c>
-      <c r="I125" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J125" s="8">
+      <c r="J125" s="8" t="str">
+        <v/>
+      </c>
+      <c r="K125" s="8">
         <v>14</v>
       </c>
-      <c r="K125" s="8">
+      <c r="L125" s="8">
         <v>35</v>
       </c>
-      <c r="L125" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M125" s="37" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M125" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N125" s="37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="B126" s="11" t="b" cm="1">
-        <f t="array" ref="B126:M126">ISO_8601.PARSE_ISO8601(A126)</f>
-        <v>0</v>
-      </c>
-      <c r="C126" s="11">
+      <c r="B126" s="58"/>
+      <c r="C126" s="11" t="b" cm="1">
+        <f t="array" ref="C126:N126">ISO_8601.PARSE_ISO8601(A126,B126)</f>
         <v>0</v>
       </c>
       <c r="D126" s="11">
         <v>0</v>
       </c>
       <c r="E126" s="11">
+        <v>0</v>
+      </c>
+      <c r="F126" s="11">
         <v>2</v>
       </c>
-      <c r="F126" s="11">
-        <v>1</v>
-      </c>
-      <c r="G126" s="11" t="e">
-        <v>#VALUE!</v>
+      <c r="G126" s="11">
+        <v>1</v>
       </c>
       <c r="H126" s="11" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="I126" s="11" t="str">
-        <v/>
+      <c r="I126" s="11" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="J126" s="11" t="str">
         <v/>
@@ -7101,32 +7132,33 @@
       <c r="L126" s="11" t="str">
         <v/>
       </c>
-      <c r="M126" s="38" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M126" s="11" t="str">
+        <v/>
+      </c>
+      <c r="N126" s="38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B127" s="8" t="b" cm="1">
-        <f t="array" ref="B127:M127">ISO_8601.PARSE_ISO8601(A127)</f>
-        <v>0</v>
-      </c>
-      <c r="C127" s="8">
+      <c r="B127" s="57"/>
+      <c r="C127" s="8" t="b" cm="1">
+        <f t="array" ref="C127:N127">ISO_8601.PARSE_ISO8601(A127,B127)</f>
         <v>0</v>
       </c>
       <c r="D127" s="8">
         <v>0</v>
       </c>
       <c r="E127" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F127" s="8">
-        <v>0</v>
-      </c>
-      <c r="G127" s="8" t="str">
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="G127" s="8">
+        <v>0</v>
       </c>
       <c r="H127" s="8" t="str">
         <v/>
@@ -7143,162 +7175,166 @@
       <c r="L127" s="8" t="str">
         <v/>
       </c>
-      <c r="M127" s="37" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M127" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N127" s="37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="B128" s="11" t="b" cm="1">
-        <f t="array" ref="B128:M128">ISO_8601.PARSE_ISO8601(A128)</f>
-        <v>0</v>
-      </c>
-      <c r="C128" s="11">
+      <c r="B128" s="58"/>
+      <c r="C128" s="11" t="b" cm="1">
+        <f t="array" ref="C128:N128">ISO_8601.PARSE_ISO8601(A128,B128)</f>
+        <v>0</v>
+      </c>
+      <c r="D128" s="11">
         <v>4</v>
       </c>
-      <c r="D128" s="11">
+      <c r="E128" s="11">
         <v>3</v>
       </c>
-      <c r="E128" s="11">
+      <c r="F128" s="11">
         <v>2</v>
       </c>
-      <c r="F128" s="11">
-        <v>1</v>
-      </c>
       <c r="G128" s="11">
-        <v>2023</v>
+        <v>1</v>
       </c>
       <c r="H128" s="11">
+        <v>2023</v>
+      </c>
+      <c r="I128" s="11">
         <v>2</v>
       </c>
-      <c r="I128" s="11">
+      <c r="J128" s="11">
         <v>23</v>
-      </c>
-      <c r="J128" s="11" t="e">
-        <v>#VALUE!</v>
       </c>
       <c r="K128" s="11" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="L128" s="11" t="str">
-        <v/>
-      </c>
-      <c r="M128" s="38" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L128" s="11" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M128" s="11" t="str">
+        <v/>
+      </c>
+      <c r="N128" s="38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="B129" s="8" t="b" cm="1">
-        <f t="array" ref="B129:M129">ISO_8601.PARSE_ISO8601(A129)</f>
-        <v>1</v>
-      </c>
-      <c r="C129" s="8">
+      <c r="B129" s="57"/>
+      <c r="C129" s="8" t="b" cm="1">
+        <f t="array" ref="C129:N129">ISO_8601.PARSE_ISO8601(A129,B129)</f>
+        <v>1</v>
+      </c>
+      <c r="D129" s="8">
         <v>7</v>
       </c>
-      <c r="D129" s="8">
+      <c r="E129" s="8">
         <v>5</v>
       </c>
-      <c r="E129" s="8">
+      <c r="F129" s="8">
         <v>2</v>
       </c>
-      <c r="F129" s="8">
-        <v>1</v>
-      </c>
       <c r="G129" s="8">
-        <v>2023</v>
+        <v>1</v>
       </c>
       <c r="H129" s="8">
+        <v>2023</v>
+      </c>
+      <c r="I129" s="8">
         <v>2</v>
       </c>
-      <c r="I129" s="8">
+      <c r="J129" s="8">
         <v>23</v>
       </c>
-      <c r="J129" s="8">
+      <c r="K129" s="8">
         <v>14</v>
       </c>
-      <c r="K129" s="8">
+      <c r="L129" s="8">
         <v>55</v>
       </c>
-      <c r="L129" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M129" s="37">
+      <c r="M129" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N129" s="37">
         <v>900</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="B130" s="14" t="b" cm="1">
-        <f t="array" ref="B130:M130">ISO_8601.PARSE_ISO8601(A130)</f>
-        <v>0</v>
-      </c>
-      <c r="C130" s="14">
+      <c r="B130" s="59"/>
+      <c r="C130" s="14" t="b" cm="1">
+        <f t="array" ref="C130:N130">ISO_8601.PARSE_ISO8601(A130,B130)</f>
+        <v>0</v>
+      </c>
+      <c r="D130" s="14">
         <v>6</v>
       </c>
-      <c r="D130" s="14">
+      <c r="E130" s="14">
         <v>5</v>
       </c>
-      <c r="E130" s="14">
+      <c r="F130" s="14">
         <v>2</v>
       </c>
-      <c r="F130" s="14">
-        <v>1</v>
-      </c>
       <c r="G130" s="14">
-        <v>2023</v>
+        <v>1</v>
       </c>
       <c r="H130" s="14">
+        <v>2023</v>
+      </c>
+      <c r="I130" s="14">
         <v>2</v>
       </c>
-      <c r="I130" s="14">
+      <c r="J130" s="14">
         <v>23</v>
       </c>
-      <c r="J130" s="14">
+      <c r="K130" s="14">
         <v>14</v>
       </c>
-      <c r="K130" s="14">
+      <c r="L130" s="14">
         <v>55</v>
       </c>
-      <c r="L130" s="14" t="str">
-        <v/>
-      </c>
-      <c r="M130" s="47" t="e">
+      <c r="M130" s="14" t="str">
+        <v/>
+      </c>
+      <c r="N130" s="47" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="B131" s="8" t="b" cm="1">
-        <f t="array" ref="B131:M131">ISO_8601.PARSE_ISO8601(A131)</f>
-        <v>1</v>
-      </c>
-      <c r="C131" s="8">
+      <c r="B131" s="57"/>
+      <c r="C131" s="8" t="b" cm="1">
+        <f t="array" ref="C131:N131">ISO_8601.PARSE_ISO8601(A131,B131)</f>
+        <v>1</v>
+      </c>
+      <c r="D131" s="8">
         <v>4</v>
       </c>
-      <c r="D131" s="8">
-        <v>1</v>
-      </c>
       <c r="E131" s="8">
+        <v>1</v>
+      </c>
+      <c r="F131" s="8">
         <v>3</v>
       </c>
-      <c r="F131" s="8">
-        <v>1</v>
-      </c>
       <c r="G131" s="8">
+        <v>1</v>
+      </c>
+      <c r="H131" s="8">
         <v>99999</v>
       </c>
-      <c r="H131" s="8" t="str">
-        <v/>
-      </c>
       <c r="I131" s="8" t="str">
         <v/>
       </c>
@@ -7311,24 +7347,25 @@
       <c r="L131" s="8" t="str">
         <v/>
       </c>
-      <c r="M131" s="37" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M131" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N131" s="37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="B132" s="14" t="b" cm="1">
-        <f t="array" ref="B132:M132">ISO_8601.PARSE_ISO8601(A132)</f>
-        <v>0</v>
-      </c>
-      <c r="C132" s="14">
+      <c r="B132" s="59"/>
+      <c r="C132" s="14" t="b" cm="1">
+        <f t="array" ref="C132:N132">ISO_8601.PARSE_ISO8601(A132,B132)</f>
+        <v>0</v>
+      </c>
+      <c r="D132" s="14">
         <v>6</v>
       </c>
-      <c r="D132" s="14">
-        <v>1</v>
-      </c>
       <c r="E132" s="14">
         <v>1</v>
       </c>
@@ -7336,49 +7373,50 @@
         <v>1</v>
       </c>
       <c r="G132" s="14">
+        <v>1</v>
+      </c>
+      <c r="H132" s="14">
         <v>99999</v>
       </c>
-      <c r="H132" s="14" t="str">
-        <v/>
-      </c>
       <c r="I132" s="14" t="str">
         <v/>
       </c>
-      <c r="J132" s="14">
+      <c r="J132" s="14" t="str">
+        <v/>
+      </c>
+      <c r="K132" s="14">
         <v>9</v>
       </c>
-      <c r="K132" s="14" t="str">
-        <v/>
-      </c>
       <c r="L132" s="14" t="str">
         <v/>
       </c>
-      <c r="M132" s="47" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M132" s="14" t="str">
+        <v/>
+      </c>
+      <c r="N132" s="47" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="B133" s="8" t="b" cm="1">
-        <f t="array" ref="B133:M133">ISO_8601.PARSE_ISO8601(A133)</f>
-        <v>0</v>
-      </c>
-      <c r="C133" s="8">
+      <c r="B133" s="57"/>
+      <c r="C133" s="8" t="b" cm="1">
+        <f t="array" ref="C133:N133">ISO_8601.PARSE_ISO8601(A133,B133)</f>
         <v>0</v>
       </c>
       <c r="D133" s="8">
         <v>0</v>
       </c>
       <c r="E133" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F133" s="8">
-        <v>0</v>
-      </c>
-      <c r="G133" s="8" t="str">
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="G133" s="8">
+        <v>0</v>
       </c>
       <c r="H133" s="8" t="str">
         <v/>
@@ -7395,32 +7433,33 @@
       <c r="L133" s="8" t="str">
         <v/>
       </c>
-      <c r="M133" s="37" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M133" s="8" t="str">
+        <v/>
+      </c>
+      <c r="N133" s="37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="B134" s="14" t="b" cm="1">
-        <f t="array" ref="B134:M134">ISO_8601.PARSE_ISO8601(A134)</f>
-        <v>0</v>
-      </c>
-      <c r="C134" s="14">
+      <c r="B134" s="59"/>
+      <c r="C134" s="14" t="b" cm="1">
+        <f t="array" ref="C134:N134">ISO_8601.PARSE_ISO8601(A134,B134)</f>
         <v>0</v>
       </c>
       <c r="D134" s="14">
         <v>0</v>
       </c>
       <c r="E134" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F134" s="14">
-        <v>0</v>
-      </c>
-      <c r="G134" s="14" t="str">
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="G134" s="14">
+        <v>0</v>
       </c>
       <c r="H134" s="14" t="str">
         <v/>
@@ -7437,18 +7476,21 @@
       <c r="L134" s="14" t="str">
         <v/>
       </c>
-      <c r="M134" s="47" t="str">
+      <c r="M134" s="14" t="str">
+        <v/>
+      </c>
+      <c r="N134" s="47" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A106:E106"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A84:E84"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7462,8 +7504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA07EFA6-CBC4-406A-9EC3-A2F16F1825C8}">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7479,33 +7521,32 @@
     <col min="22" max="22" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:22" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="I1" s="48" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="Q1" s="59" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="Q1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+    </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
@@ -7522,7 +7563,7 @@
       <c r="E3" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="48" t="s">
         <v>144</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -7540,7 +7581,7 @@
       <c r="M3" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="N3" s="49" t="s">
+      <c r="N3" s="48" t="s">
         <v>144</v>
       </c>
       <c r="Q3" s="5" t="s">
@@ -7555,7 +7596,7 @@
       <c r="T3" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="U3" s="49" t="s">
+      <c r="U3" s="48" t="s">
         <v>144</v>
       </c>
     </row>
@@ -7817,7 +7858,7 @@
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
-      <c r="F10" s="50" t="str" cm="1">
+      <c r="F10" s="49" t="str" cm="1">
         <f t="array" ref="F10">ISO_8601.FORMAT_DATE(A10,B10,C10,D10,E10)</f>
         <v>−0500-05-02</v>
       </c>
@@ -7837,26 +7878,26 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="59" t="s">
+    <row r="14" spans="1:22" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="I14" s="48" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="I14" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>3</v>
@@ -7870,7 +7911,7 @@
       <c r="D16" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="E16" s="49" t="s">
+      <c r="E16" s="48" t="s">
         <v>144</v>
       </c>
       <c r="I16" s="5" t="s">
@@ -7888,7 +7929,7 @@
       <c r="M16" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="N16" s="49" t="s">
+      <c r="N16" s="48" t="s">
         <v>144</v>
       </c>
     </row>
@@ -8066,28 +8107,27 @@
         <v>−0500-W12-3</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="59" t="s">
+    <row r="25" spans="1:17" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
     <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>153</v>
@@ -8128,7 +8168,7 @@
       <c r="M27" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="N27" s="49" t="s">
+      <c r="N27" s="48" t="s">
         <v>144</v>
       </c>
     </row>
@@ -8349,12 +8389,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A25:Q25"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="Q1:V1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8363,9 +8397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052D9A64-AEFD-4F90-BDF6-19F88196B125}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8379,14 +8411,11 @@
     <col min="8" max="8" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
@@ -8397,14 +8426,14 @@
       <c r="C3" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="48" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="52" t="str" cm="1">
+      <c r="C4" s="51" t="str" cm="1">
         <f t="array" ref="C4:D4">ISO_8601.CONVERT_TO_DATE(A4,B4)</f>
         <v/>
       </c>
@@ -8417,7 +8446,7 @@
         <v>161</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="51" cm="1">
+      <c r="C5" s="50" cm="1">
         <f t="array" ref="C5:D5">ISO_8601.CONVERT_TO_DATE(A5,B5)</f>
         <v>45058.604166666664</v>
       </c>
@@ -8430,7 +8459,7 @@
         <v>163</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="52" t="e" cm="1">
+      <c r="C6" s="51" t="e" cm="1">
         <f t="array" ref="C6:D6">ISO_8601.CONVERT_TO_DATE(A6,B6)</f>
         <v>#NUM!</v>
       </c>
@@ -8443,7 +8472,7 @@
         <v>164</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="51" cm="1">
+      <c r="C7" s="50" cm="1">
         <f t="array" ref="C7:D7">ISO_8601.CONVERT_TO_DATE(A7,B7)</f>
         <v>0.52444444444444438</v>
       </c>
@@ -8456,7 +8485,7 @@
         <v>114</v>
       </c>
       <c r="B8" s="8"/>
-      <c r="C8" s="52" cm="1">
+      <c r="C8" s="51" cm="1">
         <f t="array" ref="C8:D8">ISO_8601.CONVERT_TO_DATE(A8,B8)</f>
         <v>44980.607638888891</v>
       </c>
@@ -8469,7 +8498,7 @@
         <v>165</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="53" cm="1">
+      <c r="C9" s="52" cm="1">
         <f t="array" ref="C9:D9">ISO_8601.CONVERT_TO_DATE(A9,B9)</f>
         <v>44938.607708333337</v>
       </c>
@@ -8482,11 +8511,11 @@
         <v>166</v>
       </c>
       <c r="B10" s="19"/>
-      <c r="C10" s="54" cm="1">
+      <c r="C10" s="53" cm="1">
         <f t="array" ref="C10:D10">ISO_8601.CONVERT_TO_DATE(A10,B10)</f>
         <v>45275.274305555555</v>
       </c>
-      <c r="D10" s="50" t="str">
+      <c r="D10" s="49" t="str">
         <v/>
       </c>
     </row>
@@ -8497,7 +8526,7 @@
       <c r="B11" s="14">
         <v>1</v>
       </c>
-      <c r="C11" s="53" t="e" cm="1">
+      <c r="C11" s="52" t="e" cm="1">
         <f t="array" ref="C11:D11">ISO_8601.CONVERT_TO_DATE(A11,B11)</f>
         <v>#N/A</v>
       </c>
@@ -8505,19 +8534,18 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="59" t="s">
+    <row r="14" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>169</v>
@@ -8545,7 +8573,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="55">
+      <c r="A17" s="54">
         <v>45071</v>
       </c>
       <c r="B17" s="8"/>
@@ -8560,7 +8588,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="56">
+      <c r="A18" s="55">
         <v>45141.608303900466</v>
       </c>
       <c r="B18" s="11">
@@ -8583,7 +8611,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="55">
+      <c r="A19" s="54">
         <v>36892</v>
       </c>
       <c r="B19" s="8">
@@ -8606,7 +8634,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="57">
+      <c r="A20" s="56">
         <v>36892</v>
       </c>
       <c r="B20" s="14">
@@ -8625,16 +8653,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A14:H14"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAiAH0ALAB7ACIAcABhAHQAaAAiADoAIgAvAHAAcgBvAGoAZQBjAHQAcwAvAEkAUwBPAF8AOAA2ADAAMQAiACwAIgB0AGUAeAB0ACIAOgAiAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABJAFMATwBfADgANgAwADEAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAIAAgACAAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABUAGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAHMAdABhAG4AZABhAHIAZAAgAGQAZQBmAGkAbgBlAHMAIABhACAAdQBuAGkAdgBlAHIAcwBhAGwAIABuAG8AdABhAHQAaQBvAG4AIABvAGYAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABEAGEAdABlAHMAIABhAHIAZQAgAGkAbgAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIAIABhAG4AZAAgAHQAaQBtAGUAcwAgAGEAcgBlACAAYgBhAHMAZQBkACAAbwBuACAAdABoAGUAIAAyADQAIABoAG8AdQByACAAdABpAG0AZQBrAGUAZQBwAGkAbgBnACAAcwB5AHMAdABlAG0AIAB3AGkAdABoACAAYQBuACAAIAAgACAAIAAgACMAXABuACMAIABvAHAAdABpAG8AbgBhAGwAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAZgByAG8AbQAgAFUAVABDAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABNAG8AZAB1AGwAZQAgAEQAZQBwAGUAbgBkAGUAbgBjAGkAZQBzADoAIABOAG8AbgBlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABMAG8AZwBpAGMAYQBsACAARgB1AG4AYwB0AGkAbwBuAHMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBZAEUAQQBSACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQBzAHQAcwAgAGkAZgAgAGEAIAB5AGUAYQByACAAaQBzACAAdgBhAGwAaQBkACAAZgBvAHIAIABJAFMATwAgADgANgAwADEALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAIABcAG4AIwAgAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAHkAZQBhAHIAIABpAG4AYwBsAHUAZABlAHMAIABhACAAbABlAGEAcAAgAGQAYQB5ACAAaQBuACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAGQAYQB0AGUAIABpAHMAIAB2AGEAbABpAGQAIABmAG8AcgAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwAgAFwAbgAjACAASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAGUAcwB0AHMAIABpAGYAIABhACAAdABpAG0AZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIAAyADQAIABoAG8AdQByACAAdABpAG0AZQBrAGUAZQBwAGkAbgBnACAAcwB5AHMAdABlAG0ALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjACAAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBUAEkATQBFAF8AWgBPAE4ARQAgACAAIAAgACAAIAAgAFQAZQBzAHQAcwAgAGkAZgAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAaQBzACAAaQBuACAAdgBhAGwAaQBkACAAcgBhAG4AZwBlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAgACAAIAAgAFQAZQBzAHQAcwAgAGkAZgAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlACAAaQBzACAAdgBhAGwAaQBkACAAZgBvAHIAIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBXAEUARQBLAF8ARABBAFQARQAgACAAIAAgACAAIAAgAFQAZQBzAHQAcwAgAGkAZgAgAGEAIAB3AGUAZQBrACAAZABhAHQAZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAIABcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEMAYQBsAGUAbgBkAGEAcgAgAEYAdQBuAGMAdABpAG8AbgBzACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACAAIwBcAG4AIwAgAFkARQBBAFIAXwBEAEEAWQBfAEMATwBVAE4AVAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBvAHUAbgB0ACAAbwBmACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5AHMAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIAB5AGUAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFkARQBBAFIAXwBXAEUARQBLAF8AQwBPAFUATgBUACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBvAHUAbgB0ACAAbwBmACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawBzACAAaQBuACAAYQAgAGcAaQB2AGUAbgAgAHkAZQBhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEQAQQBZAF8ATwBSAEQASQBOAEEATAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbgB1AG0AYgBlAHIAIABvAGYAIABhACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAZgByAG8AbQAgAGEAIABnAGkAdgBlAG4AIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABkAGEAdABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAuACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFcARQBFAEsAXwBOAFUATQBCAEUAUgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFcARQBFAEsAXwBOAFUATQBCAEUAUgBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFQATwBfAFcARQBFAEsAXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAYQBuAGQAIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYAUgBPAE0AXwBXAEUARQBLAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAZQBpAHQAaABlAHIAIABhACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAbwByACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdwBlAGUAawAgAGEAbgBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFAAYQByAHMAaQBuAGcAIABGAHUAbgBjAHQAaQBvAG4AcwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACAAIwBcAG4AIwAgAFYAQQBMAEkARABBAFQARQBfAEMASABBAFIAQQBDAFQARQBSAFMAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAdABlAHgAdAAgAGMAbwBuAHQAYQBpAG4AcwAgAG8AbgBsAHkAIABjAGgAYQByAGEAYwB0AGUAcgBzACAAdABoAGEAdAAgAGEAcgBlACAAdgBhAGwAaQBkACAAZgBvAHIAIABJAFMATwAgADgANgAwADEALgAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACAAYQBuAGQAIABkAGEAeQAgAG8AZgAgAGEAIABkAGEAdABlACAAZgByAG8AbQAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AIAAgACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAFQASQBNAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAaABvAHUAcgAsACAAbQBpAG4AdQB0AGUAIABhAG4AZAAgAHMAZQBjAG8AbgBkACAAbwBmACAAdABpAG0AZQAgAGYAcgBvAG0AIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAFQASQBNAEUAXwBaAE8ATgBFACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAFAAQQBSAFQAUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUwBwAGwAaQB0AHMAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAB0AGUAZAAgAHQAZQB4AHQAIAB2AGEAbAB1AGUAIABpAG4AdABvACAAaQBuAHQAbwAgAHIAZQBzAHAAZQBjAHQAaQB2AGUAIABwAGEAcgB0AHMAIABvAGYAIABkAGEAdABlACwAIAAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAEkAUwBPADgANgAwADEAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAGMAbwBtAHAAbABpAGMAYQB0AGkAbwBuAHMAIABmAHIAbwBtACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYAbwByAG0AYQB0AHQAaQBuAGcAIABGAHUAbgBjAHQAaQBvAG4AcwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIABkAGEAdABlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8AVABJAE0ARQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIAB0AGkAbQBlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8AVABJAE0ARQBfAFoATwBOAEUAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIAB0AGkAbQBlACAAegBvAG4AZQAgAGEAcwAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8AVwBFAEUASwBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIAB3AGUAZQBrACAAZABhAHQAZQAgAGEAcwAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8ASQBTAE8AOAA2ADAAMQAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABjAG8AbQBwAGwAaQBjAGEAdABpAG8AbgBzACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEMAbwBuAHYAZQByAHMAaQBvAG4AIABGAHUAbgBjAHQAaQBvAG4AcwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACAAIwBcAG4AIwAgAEMATwBOAFYARQBSAFQAXwBUAE8AXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgACAAQwBvAG4AdgBlAHIAdABzACAAdABlAHgAdAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQAIAB0AG8AIABhAG4AIABFAHgAYwBlAGwAIABkAGEAdABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEMATwBOAFYARQBSAFQAXwBGAFIATwBNAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAQwBvAG4AdgBlAHIAdABzACAAYQBuACAARQB4AGMAZQBsACAAZABhAHQAZQAgAHQAbwAgAEkAUwBPACAAZgBvAHIAbQBhAHQAdABlAGQAIAB0AGUAeAB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBfAFYAQQBMAEkARABfAFkARQBBAFIAXABuAFwAbgBUAGUAcwB0AHMAIABpAGYAIABhACAAeQBlAGEAcgAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAASQBTAE8AIAA4ADYAMAAxAC4AXABuAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABiAG8AbwBsAGUAYQBuAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBBAGwAbABvAHcARABlAGMAaQBtAGEAbAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEEAbABsAG8AdwAgAGQAZQBjAGkAbQBhAGwAIAB2AGEAbAB1AGUAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBfAFYAQQBMAEkARABfAFkARQBBAFIAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAAWwBBAGwAbABvAHcARABlAGMAaQBtAGEAbABdACwAXABuACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACwAXABuACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACgATgAoAEEAbABsAG8AdwBEAGUAYwBpAG0AYQBsACkAIAA9ACAAMAApACAAKgAgACgAWQBlAGEAcgBDAEUAIAA8AD4AIABJAE4AVAAoAFkAZQBhAHIAQwBFACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIABBAEIAUwAoAFkAZQBhAHIAQwBFACkAIAA8ACAAMQAwADAAMAAwADAAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAF8ATABFAEEAUABfAFkARQBBAFIAXABuAFwAbgBUAGUAcwB0AHMAIABpAGYAIABhACAAeQBlAGEAcgAgAGkAbgBjAGwAdQBkAGUAcwAgAGEAIABsAGUAYQBwACAAZABhAHkAIABpAG4AIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAYgBvAG8AbABlAGEAbgAuAFwAbgAjAFYAQQBMAFUARQAhACAAaQBmACAAbgBvAHQAIABhACAAdgBhAGwAaQBkACAAeQBlAGEAcgAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASQBTAF8ATABFAEEAUABfAFkARQBBAFIAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAE4AVAAoAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATQBPAEQAKABfAHkAZQBhAHIAQwBFACwAIAA0ADAAMAApACAAPQAgADAALAAgAFQAUgBVAEUALAAgAEkARgAoAE0ATwBEACgAXwB5AGUAYQByAEMARQAsACAAMQAwADAAKQAgAD0AIAAwACwAIABGAEEATABTAEUALAAgAE0ATwBEACgAXwB5AGUAYQByAEMARQAsACAANAApACAAPQAgADAAKQApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFAFwAbgBcAG4AVABlAHMAdABzACAAaQBmACAAYQAgAGQAYQB0AGUAIABpAHMAIAB2AGEAbABpAGQAIABmAG8AcgAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIALgBcAG4ASQBmACAAbQBvAG4AdABoACAAYQBuAGQAIABkAGEAeQAgAG0AaQBzAHMAaQBuAGcALAAgAGMAbwBuAHMAaQBkAGUAcgBlAGQAIABhACAAeQBlAGEAcgAgAG8AbgBsAHkAIABkAGEAdABlAC4AXABuAEkAZgAgAG8AbgBsAHkAIABkAGEAeQAgAGkAcwAgAG0AaQBzAHMAaQBuAGcALAAgAGMAbwBuAHMAaQBkAGUAcgBlAGQAIABhACAAeQBlAGEAcgAgAGEAbgBkACAAbQBvAG4AdABoACAAZABhAHQAZQAuAFwAbgBPAG4AbAB5ACAAdABoAGUAIABsAGEAcwB0ACAAcAByAG8AdgBpAGQAZQBkACAAZQBsAGUAbQBlAG4AdAAgAGMAYQBuACAAaABhAHYAZQAgAGEAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAdgBhAGwAdQBlAC4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAYgBvAG8AbABlAGEAbgAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAE0AbwBuAHQAaAAgAG8AZgAgAHkAZQBhAHIAXABuAEQAYQB5ACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAYQB5ACAAbwBmACAAbQBvAG4AdABoAFwAbgBbAEEAbABsAE0AYQBuAGQAYQB0AG8AcgB5AF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABEAGkAcwBhAGwAbABvAHcAIABzAGgAbwByAHQAIABmAG8AcgBtAHMAOgAgAFkAZQBhAHIALAAgAFkAZQBhAHIAIABhAG4AZAAgAE0AbwBuAHQAaABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABbAEEAbABsAE0AYQBuAGQAYQB0AG8AcgB5AF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAXwBlAGwAZQBtAGUAbgB0AHMALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACAAKgAgAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkAIAAqACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBlAGwAZQBtAGUAbgB0AHMAIAA9ACAAMAApACAAKwAgACgAKABOACgAQQBsAGwATQBhAG4AZABhAHQAbwByAHkAKQAgADwAPgAgADAAKQAgACoAIAAoAF8AZQBsAGUAbQBlAG4AdABzACAAPAAgADMAKQApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHkAZQBhAHIAIABpAHMAIABtAGEAbgBkAGEAdABvAHIAeQAsACAAYQBuAGQAIABhAGwAbAAgAGUAbABlAG0AZQBuAHQAcwAgAG0AYQBuAGQAYQB0AG8AcgB5ACAAaQBmACAAQQBsAGwATQBhAG4AZABhAHQAbwByAHkAIABzAHcAaQB0AGMAaAAgAGkAcwAgAHMAZQB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAbABlAG0AZQBuAHQAcwAgAD0AIAAzACwAIAAvAC8AIAB5AGUAYQByACwAIABtAG8AbgB0AGgAIABhAG4AZAAgAGQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAG8AbgB0AGgAIAA8AD4AIABJAE4AVAAoAE0AbwBuAHQAaAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG0AbwBuAHQAaAAgAGMAYQBuAG4AbwB0ACAAYgBlACAAZgByAGEAYwB0AGkAbwBuAGEAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABmAG8AcgAgAG0AbwBuAHQAaAAgAHIAYQBuAGcAZQAgADEALgAuADEAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKAAoAE0AbwBuAHQAaAAgAD4APQAgADEAKQAgACoAIAAoAE0AbwBuAHQAaAAgADwAPQAgADEAMgApACkAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABJAE4AVAAoAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgATQBvAG4AdABoACAAPQAgADIAKQAsACAALwAvACAARgBlAGIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAGQAYQB5ACAAPgA9ACAAMQApACAAKgAgACgAXwBkAGEAeQAgADwAPQAgACgAMgA4ACAAKwAgAE4AKABJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACkAKQApACkAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABNAG8AbgB0AGgAIAA8AD0AIAA3ACkALAAgAC8ALwAgAEoAYQBuACwAIABNAGEAcgAsACAAQQBwAHIALAAgAE0AYQB5ACwAIABKAHUAbgAsACAASgB1AGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAGQAYQB5ACAAPgA9ACAAMQApACAAKgAgACgAXwBkAGEAeQAgADwAPQAgACgAMwAwACAAKwAgAE0ATwBEACgATQBvAG4AdABoACwAIAAyACkAKQApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgATQBvAG4AdABoACAAPgA9ACAAOAApACwAIAAvAC8AIABBAHUAZwAsACAAUwBlAHAALAAgAE8AYwB0ACwAIABOAG8AdgAsACAARABlAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBkAGEAeQAgAD4APQAgADEAKQAgACoAIAAoAF8AZABhAHkAIAA8AD0AIAAoADMAMQAgAC0AIABNAE8ARAAoAE0AbwBuAHQAaAAsACAAMgApACkAKQAgADwAPgAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAbABlAG0AZQBuAHQAcwAgAD0AIAAyACwAIAAvAC8AIAB5AGUAYQByACAAYQBuAGQAIABtAG8AbgB0AGgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFkARQBBAFIAKABZAGUAYQByAEMARQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAEkATgBUACgATQBvAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAGYAbwByACAAbQBvAG4AdABoACAAcgBhAG4AZwBlACAAMQAuAC4AMQAyAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBtAG8AbgB0AGgAIAA+AD0AIAAxACkAIAAqACAAKABfAG0AbwBuAHQAaAAgADwAPQAgADEAMgApACkAIAA8AD4AIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAGwAZQBtAGUAbgB0AHMAIAA9ACAAMQAsACAALwAvACAAeQBlAGEAcgAgAG8AbgBsAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACwAIAAxACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAXABuAFwAbgBUAGUAcwB0AHMAIABpAGYAIABhACAAdABpAG0AZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIAAyADQAIABoAG8AdQByACAAdABpAG0AZQBrAGUAZQBwAGkAbgBnACAAcwB5AHMAdABlAG0ALgBcAG4ATwBuAGwAeQAgAHQAaABlACAAbABhAHMAdAAgAHAAcgBvAHYAaQBkAGUAZAAgAGUAbABlAG0AZQBuAHQAIABjAGEAbgAgAGgAYQB2AGUAIABhACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHYAYQBsAHUAZQAuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAGIAbwBvAGwAZQBhAG4ALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEgAbwB1AHIAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADAALgAuADIANABcAG4ATQBpAG4AdQB0AGUAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAMAAuAC4ANQA5AC4AOQA5ADkAXABuAFMAZQBjAG8AbgBkACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADAALgAuADUAOQAuADkAOQA5AFwAbgBbAEEAbABsAE0AYQBuAGQAYQB0AG8AcgB5AF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABEAGkAcwBhAGwAbABvAHcAIABzAGgAbwByAHQAIABmAG8AcgBtAHMAOgAgAEgAbwB1AHIALAAgAEgAbwB1AHIAIABhAG4AZAAgAE0AaQBuAHUAdABlAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBJAFMAXwBWAEEATABJAEQAXwBUAEkATQBFACAAPQAgAEwAQQBNAEIARABBACgASABvAHUAcgAsACAATQBpAG4AdQB0AGUALAAgAFMAZQBjAG8AbgBkACwAIABbAEEAbABsAE0AYQBuAGQAYQB0AG8AcgB5AF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAXwBlAGwAZQBtAGUAbgB0AHMALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgASABvAHUAcgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AaQBuAHUAdABlACkAKQAgACoAIABJAFMATgBVAE0AQgBFAFIAKABTAGUAYwBvAG4AZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAGkAbgB1AHQAZQApACkAIAAqACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABTAGUAYwBvAG4AZAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFMAZQBjAG8AbgBkACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBlAGwAZQBtAGUAbgB0AHMAIAA9ACAAMAApACAAKwAgACgAKABOACgAQQBsAGwATQBhAG4AZABhAHQAbwByAHkAKQAgADwAPgAgADAAKQAgACoAIAAoAF8AZQBsAGUAbQBlAG4AdABzACAAPAAgADMAKQApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGgAbwB1AHIAIABpAHMAIABtAGEAbgBkAGEAdABvAHIAeQAsACAAYQBuAGQAIABhAGwAbAAgAGUAbABlAG0AZQBuAHQAcwAgAG0AYQBuAGQAYQB0AG8AcgB5ACAAaQBmACAAQQBsAGwATQBhAG4AZABhAHQAbwByAHkAIABzAHcAaQB0AGMAaAAgAGkAcwAgAHMAZQB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAbABlAG0AZQBuAHQAcwAgAD0AIAAzACwAIAAvAC8AIABoAG8AdQByACwAIABtAGkAbgB1AHQAZQAsACAAcwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQAWAAsACAAUgBPAFUATgBEAEQATwBXAE4AKABTAGUAYwBvAG4AZAAgACoAIAAxADAAMAAwADAALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAGgAbwB1AHIAIABpAHMAIABuAG8AdAAgAGYAcgBhAGMAdABpAG8AbgBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAbwB1AHIAIAA8AD4AIABJAE4AVAAoAEgAbwB1AHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABoAG8AdQByACAAaQBuACAAcgBhAG4AZwBlACAAMAAuAC4AMgA0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgASABvAHUAcgAgAD4APQAgADAAKQAgACoAIAAoAEgAbwB1AHIAIAA8AD0AIAAyADQAKQApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGUAcwB0ACAAbQBpAG4AdQB0AGUAIABpAHMAIABuAG8AdAAgAGYAcgBhAGMAdABpAG8AbgBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0AaQBuAHUAdABlACAAPAA+ACAASQBOAFQAKABNAGkAbgB1AHQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAG0AaQBuAHUAdABlACAAaQBuACAAcgBhAG4AZwBlACAAMAAuAC4ANQA5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgATQBpAG4AdQB0AGUAIAA+AD0AIAAwACkAIAAqACAAKABNAGkAbgB1AHQAZQAgADwAPQAgADUAOQApACkAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIAB6AGUAcgBvACAAbQBpAG4AdQB0AGUAIABhAG4AZAAgAHMAZQBjAG8AbgBkACAAZgBvAHIAIAAyADQAIABoAG8AdQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgASABvAHUAcgAgAD0AIAAyADQAKQAgACoAIAAoACgATQBpAG4AdQB0AGUAIAA8AD4AIAAwACkAIAArACAAKABfAHMAZQBjAG8AbgBkAFgAIAA8AD4AIAAwACkAKQApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABzAGUAYwBvAG4AZAAgAGkAbgAgAHIAYQBuAGcAZQAgADAALgAuADUAOQAuADkAOQA5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBzAGUAYwBvAG4AZABYACAAPgA9ACAAMAApACAAKgAgACgAXwBzAGUAYwBvAG4AZABYACAAPAAgADYAMAAwADAAMAAwACkAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAbABlAG0AZQBuAHQAcwAgAD0AIAAyACwAIAAvAC8AIABoAG8AdQByACAAYQBuAGQAIABtAGkAbgB1AHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAGkAbgB1AHQAZQBYACwAIABSAE8AVQBOAEQARABPAFcATgAoAE0AaQBuAHUAdABlACAAKgAgADYAMAAwADAAMAAwACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABoAG8AdQByACAAaQBzACAAbgBvAHQAIABmAHIAYQBjAHQAaQBvAG4AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAG8AdQByACAAPAA+ACAASQBOAFQAKABIAG8AdQByACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGUAcwB0ACAAaABvAHUAcgAgAGkAbgAgAHIAYQBuAGcAZQAgADAALgAuADIANABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKAAoAEgAbwB1AHIAIAA+AD0AIAAwACkAIAAqACAAKABIAG8AdQByACAAPAA9ACAAMgA0ACkAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAHoAZQByAG8AIABtAGkAbgB1AHQAZQAgAGYAbwByACAAMgA0ACAAaABvAHUAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKAAoAEgAbwB1AHIAIAA9ACAAMgA0ACkAIAAqACAAKABfAG0AaQBuAHUAdABlAFgAIAA8AD4AIAAwACkAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGUAcwB0ACAAbQBpAG4AdQB0AGUAIABpAG4AIAByAGEAbgBnAGUAIAAwAC4ALgA1ADkALgA5ADkAOQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKAAoAF8AbQBpAG4AdQB0AGUAWAAgAD4APQAgADAAKQAgACoAIAAoAF8AbQBpAG4AdQB0AGUAWAAgADwAIAAzADYAMAAwADAAMAAwADAAKQApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBsAGUAbQBlAG4AdABzACAAPQAgADEALAAgAC8ALwAgAGgAbwB1AHIAIABvAG4AbAB5ACAAdABpAG0AZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByAFgALAAgAFIATwBVAE4ARABEAE8AVwBOACgASABvAHUAcgAgACoAIAAzADYAMAAwADAAMAAwADAALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAGgAbwB1AHIAIABpAG4AIAByAGEAbgBnAGUAIAAwAC4ALgAyADQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBoAG8AdQByAFgAIAA+AD0AIAAwACkAIAAqACAAKABfAGgAbwB1AHIAWAAgADwAPQAgADgANgA0ADAAMAAwADAAMAAwACkAKQAgADwAPgAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQBfAFoATwBOAEUAXABuAFwAbgBUAGUAcwB0AHMAIABpAGYAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGkAcwAgAGkAbgAgAHYAYQBsAGkAZAAgAHIAYQBuAGcAZQAuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAGIAbwBvAGwAZQBhAG4ALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAE8AZgBmAHMAZQB0AE0AaQBuAHUAdABlAHMAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABSAGEAbgBnAGUAIABpAHMAIAAtADkAMAAwAC4ALgArADkAMAAwACAALQA+ACAALQAxADUAOgAwADAALgAuACsAMQA1ADoAMAAwAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBJAFMAXwBWAEEATABJAEQAXwBUAEkATQBFAF8AWgBPAE4ARQAgAD0AIABMAEEATQBCAEQAQQAoAE8AZgBmAHMAZQB0AE0AaQBuAHUAdABlAHMALABcAG4AIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE8AZgBmAHMAZQB0AE0AaQBuAHUAdABlAHMAKQApACwAIABGAEEATABTAEUALAAgACgAKABPAGYAZgBzAGUAdABNAGkAbgB1AHQAZQBzACAAPgA9ACAALQA5ADAAMAApACAAKgAgACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwAgADwAPQAgADkAMAAwACkAKQAgADwAPgAgADAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAF8AVgBBAEwASQBEAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAXABuAFwAbgBUAGUAcwB0AHMAIABpAGYAIABhAG4AIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAGIAbwBvAGwAZQBhAG4ALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAE8AcgBkAGkAbgBhAGwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAATwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASQBTAF8AVgBBAEwASQBEAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbAAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABPAHIAZABpAG4AYQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAIAAvAC8AIABPAHIAZABpAG4AYQBsACAAaQBzACAAbQBhAG4AZABhAHQAbwByAHkAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwByAGQAaQBuAGEAbAAsACAASQBOAFQAKABPAHIAZABpAG4AYQBsACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBhAHAARABhAHkALAAgAE4AKABJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABmAG8AcgAgAHYAYQBsAGkAZAAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAG8AcgBkAGkAbgBhAGwAIAA+AD0AIAAxACkAIAAqACAAKABfAG8AcgBkAGkAbgBhAGwAIAA8AD0AIAAoADMANgA1ACAAKwAgAF8AbABlAGEAcABEAGEAeQApACkAKQAgADwAPgAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBfAFYAQQBMAEkARABfAFcARQBFAEsAXwBEAEEAVABFAFwAbgBcAG4AVABlAHMAdABzACAAaQBmACAAYQAgAHcAZQBlAGsAIABkAGEAdABlACAAaQBzACAAdgBhAGwAaQBkACAAZgBvAHIAIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAYgBvAG8AbABlAGEAbgAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAFcAZQBlAGsAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAG8AZgAgAHQAaABlACAAeQBlAGEAcgBcAG4ARABhAHkATwBmAFcAZQBlAGsAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIAB3AGgAZQByAGUAIAAxAC4ALgA3ACAALQA+ACAATQBvAG4ALgAuAFMAdQBuAFwAbgBbAEQAYQB5AE8AZgBXAGUAZQBrAE0AYQBuAGQAYQB0AG8AcgB5AF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABEAGEAeQBPAGYAVwBlAGUAawAgAG0AdQBzAHQAIABiAGUAIABwAHIAbwB2AGkAZABlAGQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBfAFYAQQBMAEkARABfAFcARQBFAEsAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAFcAZQBlAGsALAAgAEQAYQB5AE8AZgBXAGUAZQBrACwAIABbAEQAYQB5AE8AZgBXAGUAZQBrAE0AYQBuAGQAYQB0AG8AcgB5AF0ALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFcAZQBlAGsAKQApACwAXABuACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALAAgAC8ALwAgAFkAZQBhAHIAIABhAG4AZAAgAFcAZQBlAGsAIABtAGEAbgBkAGEAdABvAHIAeQBcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwBtAG0AaQB0AEQAbwBXACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5AE8AZgBXAGUAZQBrACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAE4AKABEAGEAeQBPAGYAVwBlAGUAawBNAGEAbgBkAGEAdABvAHIAeQApACAAPAA+ACAAMAApACAAKgAgAF8AbwBtAG0AaQB0AEQAbwBXACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAIAAvAC8AIABEAGEAeQBPAGYAVwBlAGUAawBNAGEAbgBkAGEAdABvAHIAeQAgAHMAZQB0ACAAYQBuAGQAIABEAGEAeQBPAGYAVwBlAGUAawAgAGkAcwAgAG8AbQBtAGkAdABlAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABpAGYAIAB3AGUAZQBrACAAaQBuACAAcgBhAG4AZwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrACwAIABJAE4AVAAoAFcAZQBlAGsAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAHcAZQBlAGsAIAA+AD0AIAAxACkAIAAqACAAKABfAHcAZQBlAGsAIAA8AD0AIABZAEUAQQBSAF8AVwBFAEUASwBfAEMATwBVAE4AVAAoAFkAZQBhAHIAQwBFACkAKQApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwBtAG0AaQB0AEQAbwBXACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAALwAvACAAeQBlAGEAcgAgAGEAbgBkACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFcAZQBlAGsAIAA8AD4AIABfAHcAZQBlAGsALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsACAALwAvACAAdwBlAGUAawAgAGgAYQBzACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHYAYQBsAHUAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABpAGYAIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABpAG4AIAByAGEAbgBnAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcALAAgAEkATgBUACgARABhAHkATwBmAFcAZQBlAGsAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBkAG8AdwAgAD4APQAgADEAKQAgACoAIAAoAF8AZABvAHcAIAA8AD0AIAA3ACkAKQAgADwAPgAgADAAIAAvAC8AIABUAGUAcwB0ACAAZgBvAHIAIABEAGEAeQBPAGYAVwBlAGUAawAgADEALgAuADcAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkARQBBAFIAXwBEAEEAWQBfAEMATwBVAE4AVABcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGMAbwB1AG4AdAAgAG8AZgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAeQBzACAAZgBvAHIAIABhACAAZwBpAHYAZQBuACAAeQBlAGEAcgAuAFwAbgBJAG4AdABlAGcAZQByACAAdwBpAHQAaAAgAHIAYQBuAGcAZQAgADMANgA1AC4ALgAzADYANgBcAG4AIwBWAEEATABVAEUAIQAgAGkAZgAgAG4AbwB0ACAAYQAgAHYAYQBsAGkAZAAgAHkAZQBhAHIALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFkARQBBAFIAXwBEAEEAWQBfAEMATwBVAE4AVAAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAXABuACAAIAAgACAASQBGACgATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUALAAgADEAKQApACwAIAAjAFYAQQBMAFUARQAhACwAIABJAEYAKABJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACkALAAgADMANgA2ACwAIAAzADYANQApACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkARQBBAFIAXwBXAEUARQBLAF8AQwBPAFUATgBUAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBvAHUAbgB0ACAAbwBmACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawBzACAAaQBuACAAYQAgAGcAaQB2AGUAbgAgAHkAZQBhAHIALgBcAG4ASQBuAHQAZQBnAGUAcgAgAHcAaQB0AGgAIAByAGEAbgBnAGUAIAA1ADIALgAuADUAMwBcAG4AIwBWAEEATABVAEUAIQAgAGkAZgAgAG4AbwB0ACAAYQAgAHYAYQBsAGkAZAAgAHkAZQBhAHIALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFkARQBBAFIAXwBXAEUARQBLAF8AQwBPAFUATgBUACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcATABhAHMAdABEAGEAeQAsACAATQBPAEQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACAAKwAgAEkATgBUACgAXwB5AGUAYQByAEMARQAgAC8AIAA0ACkAIAAtACAASQBOAFQAKABfAHkAZQBhAHIAQwBFACAALwAgADEAMAAwACkAIAArACAASQBOAFQAKABfAHkAZQBhAHIAQwBFACAALwAgADQAMAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAA3AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcATABhAHMAdABEAGEAeQAgAD0AIAA0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAaQBmACAAbABhAHMAdAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgAgAGkAcwAgAGEAIABUAGgAdQByAHMAZABhAHkALAAgAHQAaABlAG4AIABoAGEAcwAgAGEAbgAgAGUAeAB0AHIAYQAgAHcAZQBlAGsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAANQAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABhAHMAdABZAGUAYQByACwAIABfAHkAZQBhAHIAQwBFACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcATABhAHMAdABEAGEAeQBQAHIAZQB2ACwAIABNAE8ARAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAYQBzAHQAWQBlAGEAcgAgACsAIABJAE4AVAAoAF8AbABhAHMAdABZAGUAYQByACAALwAgADQAKQAgAC0AIABJAE4AVAAoAF8AbABhAHMAdABZAGUAYQByACAALwAgADEAMAAwACkAIAArAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBUACgAXwBsAGEAcwB0AFkAZQBhAHIAIAAvACAANAAwADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAA3AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcATABhAHMAdABEAGEAeQBQAHIAZQB2ACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAaQBmACAAbABhAHMAdAAgAGQAYQB5ACAAbwBmACAAcAByAGUAdgBpAG8AdQBzACAAeQBlAGEAcgAgAGkAcwAgAGEAIABXAGUAZABuAGUAcwBkAGEAeQAsACAAdABoAGUAbgAgAGgAYQBzACAAYQBuACAAZQB4AHQAcgBhACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAANQAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG8AdABoAGUAcgB3AGkAegBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAA1ADIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAQQBZAF8ATwBSAEQASQBOAEEATABcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAG8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG4AdQBtAGIAZQByACAAbwBmACAAYQAgAGQAYQB0AGUAIABpAG4AIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAEkAbgB0AGUAZwBlAHIAIAB3AGkAdABoACAAcgBhAG4AZwBlACAAMQAuAC4AMwA2ADYAXABuACMAVgBBAEwAVQBFACEAIABpAGYAIABuAG8AdAAgAGEAIAB2AGEAbABpAGQAIABkAGEAdABlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBNAG8AbgB0AGgAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAE0AbwBuAHQAaAAgAG8AZgAgAHkAZQBhAHIAXABuAEQAYQB5ACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARABhAHkAIABvAGYAIABtAG8AbgB0AGgAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQAQQBZAF8ATwBSAEQASQBOAEEATAAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIAB7ADAALAAgADMAMQAsACAANQA5ACwAIAA5ADAALAAgADEAMgAwACwAIAAxADUAMQAsACAAMQA4ADEALAAgADIAMQAyACwAIAAyADQAMwAsACAAMgA3ADMALAAgADMAMAA0ACwAIAAzADMANAB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAIABJAE4AVAAoAE0AbwBuAHQAaAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEQAYQB5ACAAKwAgAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAE8AZgBmAHMAZQB0ACwAIAAsACAAXwBtAG8AbgB0AGgAKQAgACsAIABJAEYAKABfAG0AbwBuAHQAaAAgADwAPQAgADIALAAgADAALAAgAE4AKABJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAFIATwBNAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB0AGUAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlAC4AXABuACMAVgBBAEwAVQBFACEAIABpAGYAIABuAG8AdAAgAHYAYQBsAGkAZAAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlAC4AXABuAFwAbgBDAG8AbAB1AG0AbgBzADoAXABuACAAIAAxACAAfAAgAFkAZQBhAHIAIABDAEUAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuACAAIAAyACAAfAAgAE0AbwBuAHQAaAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxAC4ALgAxADIAXABuACAAIAAzACAAfAAgAEQAYQB5ACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIAAxAC4ALgAzADEAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAE8AcgBkAGkAbgBhAGwAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABPAHIAZABpAG4AYQBsACAAZABhAHkAIABvAGYAIAB5AGUAYQByAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBGAFIATwBNAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbAAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABPAHIAZABpAG4AYQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgARgBpAHIAcwB0AE8AcgBkAGkAbgBhAGwALAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAMQAsACAAMwAyACwAIAA2ADEALAAgADkAMgAsACAAMQAyADIALAAgADEANQAzACwAIAAxADgAMwAsACAAMgAxADQALAAgADIANAA1ACwAIAAyADcANQAsACAAMwAwADYALAAgADMAMwA2AH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7ADEALAAgADMAMgAsACAANgAwACwAIAA5ADEALAAgADEAMgAxACwAIAAxADUAMgAsACAAMQA4ADIALAAgADIAMQAzACwAIAAyADQANAAsACAAMgA3ADQALAAgADMAMAA1ACwAIAAzADMANQB9AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwByAGQAaQBuAGEAbAAsACAASQBOAFQAKABPAHIAZABpAG4AYQBsACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAFgATQBBAFQAQwBIACgAXwBvAHIAZABpAG4AYQBsACwAIABfAG0AbwBuAHQAaABGAGkAcgBzAHQATwByAGQAaQBuAGEAbAAsACAALQAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AZgBmAHMAZQB0ACwAIABJAE4ARABFAFgAKABfAG0AbwBuAHQAaABGAGkAcgBzAHQATwByAGQAaQBuAGEAbAAsACAAXwBtAG8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABPAHIAZABpAG4AYQBsACAALQAgAF8AbwBmAGYAcwBlAHQAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFkAZQBhAHIAQwBFACwAIABfAG0AbwBuAHQAaAAsACAAXwBkAGEAeQApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBEAEEAWQBfAE8ARgBfAFcARQBFAEsAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB0AGUALgBcAG4AIAAgADEAIAAtACAATQBvAG4AZABhAHkAXABuACAAIAAyACAALQAgAFQAdQBlAHMAZABhAHkAXABuACAAIAAzACAALQAgAFcAZQBkAG4AZQBzAGQAYQB5AFwAbgAgACAANAAgAC0AIABUAGgAdQByAGQAYQB5AFwAbgAgACAANQAgAC0AIABGAHIAaQBkAGEAeQBcAG4AIAAgADYAIAAtACAAUwBhAHQAdQByAGQAYQB5AFwAbgAgACAANwAgAC0AIABTAHUAbgBkAGEAeQBcAG4AIwBWAEEATABVAEUAIQAgAGkAZgAgAG4AbwB0ACAAYQAgAHYAYQBsAGkAZAAgAGQAYQB0AGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAE0AbwBuAHQAaAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATQBvAG4AdABoACAAbwBmACAAeQBlAGEAcgBcAG4ARABhAHkAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGEAeQAgAG8AZgAgAG0AbwBuAHQAaABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABBAFkAXwBPAEYAXwBXAEUARQBLACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAVQBzAGkAbgBnACAAWgBlAGwAbABlAHIAIABDAG8AbgBnAHIAdQBlAG4AYwBlACwAIABjAGYALgAgAGgAdAB0AHAAcwA6AC8ALwBlAG4ALgB3AGkAawBpAHAAZQBkAGkAYQAuAG8AcgBnAC8AdwBpAGsAaQAvAFoAZQBsAGwAZQByACUAMgA3AHMAXwBjAG8AbgBnAHIAdQBlAG4AYwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAATQBhAHAAIABtAG8AbgB0AGgAcwAgAE0AYQByAC4ALgBGAGUAYgAgAC0APgAgADMALgAuADEANABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB6AGUAbABsAGUAcgBNAG8AbgB0AGgALAAgAE0ATwBEACgASQBOAFQAKABNAG8AbgB0AGgAKQAgAC0AIAAzACwAIAAxADIAKQAgACsAIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABKAGEAbgAsACAARgBlAGIAIABjAG8AbgBzAGkAZABlAHIAZQBkACAAYgBlAGwAbwBuAGcAaQBuAGcAIAB0AG8AIABwAHIAZQB2AGkAbwB1AHMAIAB5AGUAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHoAZQBsAGwAZQByAFkAZQBhAHIALAAgAEkATgBUACgAWQBlAGEAcgBDAEUAKQAgAC0AIABJAE4AVAAoAF8AegBlAGwAbABlAHIATQBvAG4AdABoACAALwAgADEAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBPAGYAQwBlAG4AdAAsACAATQBPAEQAKABfAHoAZQBsAGwAZQByAFkAZQBhAHIALAAgADEAMAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB6AGUAcgBvAEIAYQBzAGUAZABDAGUAbgB0ACwAIABJAE4AVAAoAF8AegBlAGwAbABlAHIAWQBlAGEAcgAgAC8AIAAxADAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABaAGUAbABsAGUAcgAgAEMAbwBuAGcAcgB1AGUAbgBjAGUAIABmAG8AcgAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAZQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAByAGUAdAB1AHIAbgBzACAAdwBlAGUAawBkAGEAeQBzACAAMAAuAC4ANgAgAC0APgAgAFMAYQB0AC4ALgBGAHIAaQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB6AGUAbABsAGUAcgBXAGUAZQBrAEQAYQB5ACwAIABNAE8ARAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBUACgARABhAHkAKQAgACsAIABJAE4AVAAoADEAMwAgACoAIAAoAF8AegBlAGwAbABlAHIATQBvAG4AdABoACAAKwAgADEAKQAgAC8AIAA1ACkAIAArACAAXwB5AGUAYQByAE8AZgBDAGUAbgB0ACAAKwAgAEkATgBUACgAXwB5AGUAYQByAE8AZgBDAGUAbgB0ACAALwAgADQAKQAgACsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4AVAAoAF8AegBlAHIAbwBCAGEAcwBlAGQAQwBlAG4AdAAgAC8AIAA0ACkAIAAtACAAMgAgACoAIABfAHoAZQByAG8AQgBhAHMAZQBkAEMAZQBuAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAA3AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABUAHIAYQBuAHMAbABhAHQAZQAgAHQAbwAgAEkAUwBPACAAbgB1AG0AYgBlAHIAaQBuAGcAIAAxAC4ALgA3ACAALQA+ACAATQBvAG4ALgAuAFMAdQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AegBlAGwAbABlAHIAVwBlAGUAawBEAGEAeQAgACsAIAA1ACwAIAA3ACkAIAArACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABBAFkAXwBPAEYAXwBXAEUARQBLAF8ARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlAC4AXABuACAAIAAxACAALQAgAE0AbwBuAGQAYQB5AFwAbgAgACAAMgAgAC0AIABUAHUAZQBzAGQAYQB5AFwAbgAgACAAMwAgAC0AIABXAGUAZABuAGUAcwBkAGEAeQBcAG4AIAAgADQAIAAtACAAVABoAHUAcgBkAGEAeQBcAG4AIAAgADUAIAAtACAARgByAGkAZABhAHkAXABuACAAIAA2ACAALQAgAFMAYQB0AHUAcgBkAGEAeQBcAG4AIAAgADcAIAAtACAAUwB1AG4AZABhAHkAXABuACMAVgBBAEwAVQBFACEAIABpAGYAIABuAG8AdAAgAGEAIAB2AGEAbABpAGQAIABkAGEAdABlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAE8AcgBkAGkAbgBhAGwAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABPAHIAZABpAG4AYQBsACAAZABhAHkAIABvAGYAIAB5AGUAYQByAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEEAWQBfAE8ARgBfAFcARQBFAEsAXwBGAFIATwBNAF8ATwBSAEQASQBOAEEATAAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABPAHIAZABpAG4AYQBsACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAE8AcgBkAGkAbgBhAGwAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQByAHMAdABEAGEAeQBPAGYAWQBlAGEAcgAsACAARABBAFkAXwBPAEYAXwBXAEUARQBLACgAWQBlAGEAcgBDAEUALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAVAByAGEAbgBzAGwAYQB0AGUAIAB0AG8AIABJAFMATwAgAG4AdQBtAGIAZQByAGkAbgBnACAAMQAuAC4ANwAgAC0APgAgAE0AbwBuAC4ALgBTAHUAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBPAEQAKABfAGYAaQByAHMAdABEAGEAeQBPAGYAWQBlAGEAcgAgACsAIABJAE4AVAAoAE8AcgBkAGkAbgBhAGwAKQAgAC0AIAAyACwAIAA3ACkAIAArACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVwBFAEUASwBfAE4AVQBNAEIARQBSAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB0AGUALgBcAG4ASQBuAHQAZQBnAGUAcgAgAHcAaQB0AGgAIAByAGEAbgBnAGUAIAAxAC4ALgA1ADMAXABuACMAVgBBAEwAVQBFACEAIABpAGYAIABuAG8AdAAgAGEAIAB2AGEAbABpAGQAIABkAGEAdABlAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBNAG8AbgB0AGgAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAE0AbwBuAHQAaAAgAG8AZgAgAHkAZQBhAHIAXABuAEQAYQB5ACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARABhAHkAIABvAGYAIABtAG8AbgB0AGgAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFcARQBFAEsAXwBOAFUATQBCAEUAUgAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwByAGQAaQBuAGEAbAAsACAARABBAFkAXwBPAFIARABJAE4AQQBMACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5AE8AZgBXAGUAZQBrACwAIABEAEEAWQBfAE8ARgBfAFcARQBFAEsAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABXAGUAZQBrACwAIABJAE4AVAAoACgASQBOAFQAKABfAG8AcgBkAGkAbgBhAGwAKQAgAC0AIABfAGQAYQB5AE8AZgBXAGUAZQBrACAAKwAgADEAMAApACAALwAgADcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABXAGUAZQBrACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABsAGEAcwB0ACAAdwBlAGUAawAgAG8AZgAgAHAAcgBlAHYAaQBvAHUAcwAgAHkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWQBFAEEAUgBfAFcARQBFAEsAXwBDAE8AVQBOAFQAKABZAGUAYQByAEMARQAgAC0AIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawAgAD0AIAA1ADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAGYAIAB0AGgAaQBzACAAeQBlAGEAcgAgAGQAbwBlAHMAIABuAG8AdAAgAGgAYQB2AGUAIAA1ADMAIAB3AGUAZQBrAHMALAAgAHQAaABlAG4AIABpAHMAIAB0AGgAZQAgAGYAaQByAHMAdAAgAHcAZQBlAGsAIABvAGYAIABmAG8AbABsAG8AdwBpAG4AZwAgAHkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAWQBFAEEAUgBfAFcARQBFAEsAXwBDAE8AVQBOAFQAKABZAGUAYQByAEMARQApACAAPQAgADUAMwAsACAANQAzACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAG8AbQBpAG4AYQBsAFcAZQBlAGsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFcARQBFAEsAXwBOAFUATQBCAEUAUgBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlAC4AXABuAEkAbgB0AGUAZwBlAHIAIAB3AGkAdABoACAAcgBhAG4AZwBlACAAMQAuAC4ANQAzAFwAbgAjAFYAQQBMAFUARQAhACAAaQBmACAAbgBvAHQAIABhACAAdgBhAGwAaQBkACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4ATwByAGQAaQBuAGEAbAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAE8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG8AZgAgAHkAZQBhAHIAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFcARQBFAEsAXwBOAFUATQBCAEUAUgBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE8AcgBkAGkAbgBhAGwALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFcAZQBlAGsALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACgAWQBlAGEAcgBDAEUALAAgAE8AcgBkAGkAbgBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawAsACAASQBOAFQAKAAoAEkATgBUACgATwByAGQAaQBuAGEAbAApACAALQAgAF8AZABhAHkATwBmAFcAZQBlAGsAIAArACAAMQAwACkAIAAvACAANwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAG8AbQBpAG4AYQBsAFcAZQBlAGsAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGwAYQBzAHQAIAB3AGUAZQBrACAAbwBmACAAcAByAGUAdgBpAG8AdQBzACAAeQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABZAEUAQQBSAF8AVwBFAEUASwBfAEMATwBVAE4AVAAoAFkAZQBhAHIAQwBFACAALQAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABXAGUAZQBrACAAPQAgADUAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGkAZgAgAHQAaABpAHMAIAB5AGUAYQByACAAZABvAGUAcwAgAG4AbwB0ACAAaABhAHYAZQAgADUAMwAgAHcAZQBlAGsAcwAsACAAdABoAGUAbgAgAGkAcwAgADEAcwB0ACAAdwBlAGUAawAgAG8AZgAgAGYAbwBsAGwAbwB3AGkAbgBnACAAeQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABZAEUAQQBSAF8AVwBFAEUASwBfAEMATwBVAE4AVAAoAFkAZQBhAHIAQwBFACkAIAA9ACAANQAzACwAIAA1ADMALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVABPAF8AVwBFAEUASwBfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABhAG4AZAAgAGQAYQB5ACAAbwBmACAAdwBlAGUAawAgAGYAcgBvAG0AIABhACAAZwBpAHYAZQBuACAAZABhAHQAZQAuACAAVABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABkAGEAdABlACAAYwBhAG4AIABpAG0AcABsAGkAYwBpAHQAbAB5AFwAbgBiAGUAIABlAGkAdABoAGUAcgAgAGEAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAbwByACAAbwByAGQAaQBuAGkAbgBhAGwAIABkAGEAdABlAC4AXABuACMAVgBBAEwAVQBFACEAIABpAGYAIABuAG8AdAAgAGEAIAB2AGEAbABpAGQAIABkAGEAdABlAC4AXABuAFwAbgBDAG8AbAB1AG0AbgBzADoAXABuACAAIAAxACAAfAAgAFkAZQBhAHIAIABDAEUAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4AIAAgADIAIAB8ACAAVwBlAGUAawAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMQAuAC4ANQAzAFwAbgAgACAAMwAgAHwAIABEAGEAeQAgAG8AZgAgAHcAZQBlAGsAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIAAxAC4ALgA3ACAATQBvAG4ALgAuAHMAdQBuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBNAG8AbgB0AGgAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATQBvAG4AdABoACAAbwBmACAAdABoAGUAIAB5AGUAYQByAC4AIABJAGYAIABvAG0AbQBpAHQAdABlAGQALAAgAGQAYQB5ACAAaQBzACAAYQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAG8AcgBkAGkAbgBhAGwALgBcAG4ARABhAHkAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAYQB5ACAAbwBmACAAdABoAGUAIABtAG8AbgB0AGgAIAB3AGgAZQBuACAAbQBvAG4AdABoACAAcAByAG8AdgBpAGQAZQBkACwAIABvAHQAaABlAHIAdwBpAHMAZQAgAG8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG8AZgAgAHQAaABlACAAeQBlAGEAcgAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBUAE8AXwBXAEUARQBLAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABwAGEAcgBhAG0AZQB0AGUAcgBzACAAYQByAGUAIABhACAAZABhAHQAZQBcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgByAGEAYwBEAGEAeQAsACAARABhAHkAIAAtACAASQBOAFQAKABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwAsACAARABBAFkAXwBPAEYAXwBXAEUARQBLACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdwBlAGUAawAsACAAVwBFAEUASwBfAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAEkATgBUACgAWQBlAGEAcgBDAEUAKQAgACsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoACgAXwB3AGUAZQBrACAAPQAgADEAKQAgACoAIAAoAE0AbwBuAHQAaAAgAD0AIAAxADIAKQAsACAAMQAsACAAKABfAHcAZQBlAGsAIAA+AD0AIAA1ADIAKQAgACoAIAAoAE0AbwBuAHQAaAAgAD0AIAAxACkALAAgAC0AMQAsACAAVABSAFUARQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHkAZQBhAHIAQwBFACwAIABfAHcAZQBlAGsALAAgAF8AZABvAHcAIAArACAAXwBmAHIAYQBjAEQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAHAAYQByAGEAbQBlAHQAZQByAHMAIABhAHIAZQAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAARABhAHkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAcgBhAGMARABhAHkALAAgAEQAYQB5ACAALQAgAEkATgBUACgARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACgAWQBlAGEAcgBDAEUALAAgAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHcAZQBlAGsALAAgAFcARQBFAEsAXwBOAFUATQBCAEUAUgBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACgAWQBlAGEAcgBDAEUALAAgAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAE4AVAAoAFkAZQBhAHIAQwBFACkAIAArAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKAAoAF8AdwBlAGUAawAgAD0AIAAxACkAIAAqACAAKABNAG8AbgB0AGgAIAA9ACAAMQAyACkALAAgADEALAAgACgAXwB3AGUAZQBrACAAPgA9ACAANQAyACkAIAAqACAAKABNAG8AbgB0AGgAIAA9ACAAMQApACwAIAAtADEALAAgAFQAUgBVAEUALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwB5AGUAYQByAEMARQAsACAAXwB3AGUAZQBrACwAIABfAGQAbwB3ACAAKwAgAF8AZgByAGEAYwBEAGEAeQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAFIATwBNAF8AVwBFAEUASwBfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABlAGkAdABoAGUAcgAgAGEAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB0AGUAIABvAHIAIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAgAGYAcgBvAG0AIABhACAAZwBpAHYAZQBuACAAdwBlAGUAawAgAGEAbgBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFwAbgAjAFYAQQBMAFUARQAhACAAaQBmACAAbgBvAHQAIABhACAAdgBhAGwAaQBkACAAdwBlAGUAawAgAGQAYQB0AGUALgBcAG4AXABuAEMAbwBsAHUAbQBuAHMAOgBcAG4AUgBlAHQAdQByAG4ATwByAGQAaQBuAGEAbAAgAD0AIABGAEEATABTAEUAXABuACAAIAAxACAAfAAgAFkAZQBhAHIAIABDAEUAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuACAAIAAyACAAfAAgAE0AbwBuAHQAaAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxAC4ALgAxADIAXABuACAAIAAzACAAfAAgAEQAYQB5ACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIAAxAC4ALgAzADEAXABuAFIAZQB0AHUAcgBuAE8AcgBkAGkAbgBhAGwAIAA9ACAAVABSAFUARQBcAG4AIAAgADEAIAB8ACAAWQBlAGEAcgAgAEMARQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4AIAAgADIAIAB8ACAATwByAGQAaQBuAGEAbAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADEALgAuADMANgA2AFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4AVwBlAGUAawAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABvAGYAIAB0AGgAZQAgAHkAZQBhAHIAXABuAEQAYQB5AE8AZgBXAGUAZQBrACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIAB3AGgAZQByAGUAIAAxAC4ALgA3ACAALQA+ACAATQBvAG4ALgAuAFMAdQBuACAAXABuAFsAUgBlAHQAdQByAG4ATwByAGQAaQBuAGEAbABdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAUgBlAHQAdQByAG4AIAByAGUAcwB1AGwAdAAgAGEAcwAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBGAFIATwBNAF8AVwBFAEUASwBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAAVwBlAGUAawAsACAARABhAHkATwBmAFcAZQBlAGsALAAgAFsAUgBlAHQAdQByAG4ATwByAGQAaQBuAGEAbABdACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFcARQBFAEsAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAFcAZQBlAGsALAAgAEQAYQB5AE8AZgBXAGUAZQBrACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AEMAbwByAHIAZQBjAHQAaQBvAG4ALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAoAFkAZQBhAHIAQwBFACwAIAAxACwAIAA0ACkAIAArACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AcgBkAGkAbgBhAGwARABhAHkALAAgAEkATgBUACgAVwBlAGUAawApACAAKgAgADcAIAArACAARABhAHkATwBmAFcAZQBlAGsAIAAtACAAXwB5AEMAbwByAHIAZQBjAHQAaQBvAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAG4AdABPAHIAZABpAG4AYQBsACwAIABJAE4AVAAoAF8AbwByAGQAaQBuAGEAbABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAG4AdABPAHIAZABpAG4AYQBsACAAPAAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQB2AFkAZQBhAHIALAAgAFkAZQBhAHIAQwBFACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAdgBZAGUAYQByAEQAYQB5AEMAbwB1AG4AdAAsACAAWQBFAEEAUgBfAEQAQQBZAF8AQwBPAFUATgBUACgAXwBwAHIAZQB2AFkAZQBhAHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGQAagB1AHMAdABlAGQATwByAGQAaQBuAGEAbABEAGEAeQAsACAAXwBwAHIAZQB2AFkAZQBhAHIARABhAHkAQwBvAHUAbgB0ACAAKwAgAF8AbwByAGQAaQBuAGEAbABEAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AKABSAGUAdAB1AHIAbgBPAHIAZABpAG4AYQBsACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwBwAHIAZQB2AFkAZQBhAHIALAAgAF8AYQBkAGoAdQBzAHQAZQBkAE8AcgBkAGkAbgBhAGwARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAFIATwBNAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABfAHAAcgBlAHYAWQBlAGEAcgAsACAAXwBhAGQAagB1AHMAdABlAGQATwByAGQAaQBuAGEAbABEAGEAeQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAG4AdABPAHIAZABpAG4AYQBsACAAPAA9ACAAMwA2ADUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AKABSAGUAdAB1AHIAbgBPAHIAZABpAG4AYQBsACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFkAZQBhAHIAQwBFACwAIABfAG8AcgBkAGkAbgBhAGwARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAF8AbwByAGQAaQBuAGEAbABEAGEAeQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABoAGkAcwBZAGUAYQByAEQAYQB5AEMAbwB1AG4AdAAsACAAWQBFAEEAUgBfAEQAQQBZAF8AQwBPAFUATgBUACgAWQBlAGEAcgBDAEUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBuAHQATwByAGQAaQBuAGEAbAAgAD4AIABfAHQAaABpAHMAWQBlAGEAcgBEAGEAeQBDAG8AdQBuAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AZQB4AHQAWQBlAGEAcgAsACAAWQBlAGEAcgBDAEUAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBkAGoAdQBzAHQAZQBkAE8AcgBkAGkAbgBhAGwARABhAHkALAAgAF8AbwByAGQAaQBuAGEAbABEAGEAeQAgAC0AIABfAHQAaABpAHMAWQBlAGEAcgBEAGEAeQBDAG8AdQBuAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AKABSAGUAdAB1AHIAbgBPAHIAZABpAG4AYQBsACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AbgBlAHgAdABZAGUAYQByACwAIABfAGEAZABqAHUAcwB0AGUAZABPAHIAZABpAG4AYQBsAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAF8AbgBlAHgAdABZAGUAYQByACwAIABfAGEAZABqAHUAcwB0AGUAZABPAHIAZABpAG4AYQBsAEQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbABhAHMAdAAgAGQAYQB5ACAAbwBmACAAYQAgAGwAZQBhAHAAIAB5AGUAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgAUgBlAHQAdQByAG4ATwByAGQAaQBuAGEAbAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAWQBlAGEAcgBDAEUALAAgAF8AbwByAGQAaQBuAGEAbABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAF8AbwByAGQAaQBuAGEAbABEAGEAeQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBWAEEATABJAEQAQQBUAEUAXwBDAEgAQQBSAEEAQwBUAEUAUgBTAFwAbgBcAG4AVABlAHMAdABzACAAaQBmACAAdABlAHgAdAAgAGMAbwBuAHQAYQBpAG4AcwAgAG8AbgBsAHkAIABjAGgAYQByAGEAYwB0AGUAcgBzACAAdABoAGEAdAAgAGEAcgBlACAAdgBhAGwAaQBkACAAZgBvAHIAIABJAFMATwAgADgANgAwADEALgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABiAG8AbwBsAGUAYQBuAC4AIABBAG4AIABlAG0AcAB0AHkAIABzAHQAcgBpAG4AZwAgAHIAZQB0AHUAcgBuAHMAIABuAHUAbABsAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBUAGUAeAB0ACAAIAAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAAgAHwAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAB0AGUAZAAgAHQAZQB4AHQALgBcAG4AWwBTAHUAYgBzAGUAdABdACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUwB1AGIAcwBlAHQAIABmAG8AcgBtAGEAdAAgAHQAbwAgAG0AYQB0AGMAaABcAG4AIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQB6AG8AbgBlACAAIAArACwALQAuADAAMQAyADMANAA1ADYANwA4ADkAOgBUAFcAWgASIiAAKABkAGUAZgBhAHUAbAB0ACkAXABuACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAxACAALQAgAGQAYQB0AGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAtADAAMQAyADMANAA1ADYANwA4ADkAVwASIlwAbgAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMgAgAC0AIAB0AGkAbQBlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACwALgAwADEAMgAzADQANQA2ADcAOAA5ADoAVABcAG4AIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAAdABpAG0AZQAgAHoAbwBuAGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAArAC0AMAAxADIAMwA0ADUANgA3ADgAOQA6AFoAEiJcAG4AIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADQAIAAtACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAArACwALQAuADAAMQAyADMANAA1ADYANwA4ADkAOgBUAFcAEiJcAG4AIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADUAIAAtACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAIAAgACAAIAAgACAAIAArACwALQAuADAAMQAyADMANAA1ADYANwA4ADkAOgBUAFoAEiJcAG4AIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADYAIAAtACAAZAB1AHIAYQB0AGkAbwBuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAsAC0ALgAwADEAMgAzADQANQA2ADcAOAA5ADoARABIAE0AUABTAFQAVwBZAFwAbgAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANwAgAC0AIABpAG4AdABlAHIAdgBhAGwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsALAAtAC4ALwAwADEAMgAzADQANQA2ADcAOAA5ADoARABIAE0AUABTAFQAVwBZAFoAEiJcAG4AIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADgAIAAtACAAZgB1AGwAbAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAArACwALQAuAC8AMAAxADIAMwA0ADUANgA3ADgAOQA6AEQASABNAFAAUgBTAFQAVwBZAFoAEiJcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AVgBBAEwASQBEAEEAVABFAF8AQwBIAEEAUgBBAEMAVABFAFIAUwAgAD0AIABMAEEATQBCAEQAQQAoAFQAZQB4AHQALAAgAFsAUwB1AGIAcwBlAHQAXQAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAVABlAHgAdAAgAD0AIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAZAB4ACwAIABJAE4AVAAoAE4AKABTAHUAYgBzAGUAdAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByAFMAZQB0ACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBkAHgAIAA8AD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAZABhAHQAZQAsACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsALAAtAC4AMAAxADIAMwA0ADUANgA3ADgAOQA6AFQAVwBaAFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAGQAeAAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAZABhAHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAKwAtADAAMQAyADMANAA1ADYANwA4ADkAVwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBkAHgAIAA9ACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAaQBtAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACwALgAwADEAMgAzADQANQA2ADcAOAA5ADoAVABcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAZAB4ACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGkAbQBlACAAegBvAG4AZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAKwAtADAAMQAyADMANAA1ADYANwA4ADkAOgBaAFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAGQAeAAgAD0AIAA0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAKwAsAC0ALgAwADEAMgAzADQANQA2ADcAOAA5ADoAVABXAFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAGQAeAAgAD0AIAA1ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsALAAtAC4AMAAxADIAMwA0ADUANgA3ADgAOQA6AFQAWgBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBkAHgAIAA9ACAANgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGQAdQByAGEAdABpAG8AbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIALAAtAC4AMAAxADIAMwA0ADUANgA3ADgAOQA6AEQASABNAFAAUwBUAFcAWQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAZAB4ACAAPQAgADcALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAG4AdABlAHIAdgBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsALAAtAC4ALwAwADEAMgAzADQANQA2ADcAOAA5ADoARABIAE0AUABTAFQAVwBZAFoAXAAiACAAJgAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAZAB4ACAAPgA9ACAAOAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGYAdQBsAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsALAAtAC4ALwAwADEAMgAzADQANQA2ADcAOAA5ADoARABIAE0AUABSAFMAVABXAFkAWgBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAcwBjAGEAcABlAFQAZQB4AHQALAAgAFMAVQBCAFMAVABJAFQAVQBUAEUAKABTAFUAQgBTAFQASQBUAFUAVABFACgAVABlAHgAdAAsACAAXAAiACYAXAAiACwAIABcACIAJgBhAG0AcAA7AFwAIgApACwAIABcACIAPABcACIALAAgAFwAIgAmAGwAdAA7AFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeABtAGwALAAgAFwAIgA8AHQAPgA8AHMAPgBcACIAIAAmACAAXwBlAHMAYwBhAHAAZQBUAGUAeAB0ACAAJgAgAFwAIgA8AC8AcwA+ADwALwB0AD4AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeABwAGEAdABoACwAIABcACIALwAvAHMAWwB0AHIAYQBuAHMAbABhAHQAZQAoAC4ALAAnAFwAIgAgACYAIABfAGMAaABhAHIAUwBlAHQAIAAmACAAXAAiACcALAAnACcAKQA9ACcAJwBdAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBFAFIAUgBPAFIAKABGAEkATABUAEUAUgBYAE0ATAAoAF8AeABtAGwALAAgAF8AeABwAGEAdABoACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACAAYQBuAGQAIABkAGEAeQAgAG8AZgAgAGEAIABkAGEAdABlACAAZgByAG8AbQAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AXABuAE4AbwB0AGUAIABZAFkAWQBZAE0ATQAgAGkAcwAgAGkAbgB2AGEAbABpAGQALAAgAGQAdQBlACAAdABvACAAYwBvAGwAbABpAHMAaQBvAG4AIAB3AGkAdABoACAAdAByAHUAbgBjAGEAdABlAGQAIABmAG8AcgBtAGEAdAAgAFkAWQBNAE0ARABEACAAaQBuACAAZQBhAHIAbABpAGUAcgAgAHYAZQByAHMAaQBvAG4AcwAgAG8AZgAgAEkAUwBPACAAOAA2ADAAMQAuAFwAbgBcAG4AQwBvAGwAdQBtAG4AcwA6AFwAbgAgACAAMQAgAHwAIABJAFMATwBDAG8AbQBwAGwAaQBhAG4AdAAgAHwAIABiAG8AbwBsAGUAYQBuACAAfAAgAEYAbABhAGcAIABpAGYAIABjAG8AbQBwAGwAaQBhAG4AdAAgAHQAbwAgAEkAUwBPACAAOAA2ADAAMQAgAHMAdABhAG4AZABhAHIAZABcAG4AIAAgADIAIAB8ACAAUAByAGUAYwBpAHMAaQBvAG4AIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAwACAALQAgAGkAbgB2AGEAbABpAGQAIAB2AGEAbAB1AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMQAgAC0AIAB5AGUAYQByAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADIAIAAtACAAbQBvAG4AdABoAC8AdwBlAGUAawBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAzACAALQAgAGQAYQB5AFwAbgAgACAAMwAgAHwAIABGAG8AcgBtAGEAdAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADEAIAAtACAAYgBhAHMAaQBjAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADIAIAAtACAAZQB4AHQAZQBuAGQAZQBkAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADMAIAAtACAAYwBvAG4AcwBpAHMAdABlAG4AdAAgAHcAaQB0AGgAIABiAGEAcwBpAGMAIABvAHIAIABlAHgAdABlAG4AZABlAGQAXABuACAAIAA0ACAAfAAgAEQAYQB0AGUAVAB5AHAAZQAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMQAgAC0AIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADIAIAAtACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMwAgAC0AIAB3AGUAZQBrACAAZABhAHQAZQBcAG4AIAAgADUAIAB8ACAAWQBlAGEAcgAgAEMARQAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuACAAIAA2ACAAfAAgAEQAYQB0AGUAQQByAGcAMQAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATQBvAG4AdABoACAAMQAuAC4AMQAyACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAxAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAEUAbQBwAHQAeQAgAHcAaABlAG4AIABEAGEAdABlAFQAeQBwAGUAIAA9ACAAMgBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABXAGUAZQBrACAAMQAuAC4ANQAzACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAzAFwAbgAgACAANwAgAHwAIABEAGEAdABlAEEAcgBnADIAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEQAYQB5ACAAMQAuAC4AMwAxACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAxAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE8AcgBkAGkAbgBhAGwAIAAxAC4ALgAzADYANgAgAHcAaABlAG4AIABEAGEAdABlAFQAeQBwAGUAIAA9ACAAMgBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABEAGEAeQAgAG8AZgAgAFcAZQBlAGsAIAAxAC4ALgA3ACAALQA+ACAATQBvAG4ALgAuAFMAdQBuACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAzAFwAbgAgACAAIAAgACAAIAAgACAAXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFQAZQB4AHQAIAAgACAAIAAgACAAIAAgAHwAIABzAHQAcgBpAG4AZwAgAHwAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAB0AGUAZAAgAGQAYQB0AGUALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAfAAgAEUAeABhAG0AcABsAGUAIABmAG8AcgBtAGEAdABzADoAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgAHwAIAArAFkAWQBZAFkAWQAtAE0ATQAtAEQARAAsACAALQBZAFkAWQBZAC0ATQBNAC0ARABEACwAIABZAFkAWQBZAC0ATQBNAC0ARABEACwAIABZAFkAWQBZAC0ATQBNACwAIABZAFkAWQBZAE0ATQBEAEQALAAgAFkAWQBZAFkAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABUAGUAeAB0ACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBsAHUAbQBuAHMAOgAgAEgAYQBzAGgALAAgAFAAcgBlAGMAaQBzAGkAbwBuACwAIABGAG8AcgBtAGEAdAAsACAARABhAHQAZQBUAHkAcABlACwAIABZAGUAYQByAEwAZQBuACwAIABEAGEAdABlAEEAcgBnADEAUABvAHMALAAgAEQAYQB0AGUAQQByAGcAMQBMAGUAbgAsACAARABhAHQAZQBBAHIAZwAyAEwAZQBuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAdwBoAGUAcgBlACAASABhAHMAaAAgAD0AIAAoAEwARQBOACAAKgAgADQAMAA5ADYAKQAgACsAIAAoAEgAeQBwAGgAZQBuAFAAbwBzACAAKgAgADIANQA2ACkAIAArACAAKABIAHkAcABoAGUAbgAyAFAAbwBzACAAKgAgADEANgApACAAKwAgAFcAUABvAHMAIABcAG4AIAAgACAAIAAgACAAIAAgAF8AZgBtAHQASABhAHMAaABUAGEAYgBsAGUALAAgAHsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEANgAzADgANAAsACAAMQAsACAAMwAsACAAMQAsACAANAAsACAAMAAsACAAMAAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyADAANAA4ADAALAAgADEALAAgADMALAAgADEALAAgADUALAAgADAALAAgADAALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgA4ADYANwAyACwAIAAzACwAIAAxACwAIAAyACwAIAA0ACwAIAAwACwAIAAwACwAIAAzADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIAOAA2ADcANwAsACAAMgAsACAAMQAsACAAMwAsACAANAAsACAANgAsACAAMgAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyADkAOQA1ADIALAAgADIALAAgADIALAAgADEALAAgADQALAAgADYALAAgADIALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwAyADcANgA4ACwAIAAzACwAIAAxACwAIAAxACwAIAA0ACwAIAA1ACwAIAAyACwAIAAyADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMAMgA3ADcAMwAsACAAMwAsACAAMQAsACAAMwAsACAANAAsACAANgAsACAAMgAsACAAMQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADIANwA3ADQALAAgADIALAAgADEALAAgADMALAAgADUALAAgADcALAAgADIALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwA0ADAANAA4ACwAIAAzACwAIAAyACwAIAAyACwAIAA0ACwAIAAwACwAIAAwACwAIAAzADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMANAAwADUANAAsACAAMgAsACAAMgAsACAAMwAsACAANAAsACAANwAsACAAMgAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADQAMwAwADQALAAgADIALAAgADIALAAgADEALAAgADUALAAgADcALAAgADIALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwA2ADgANgA0ACwAIAAzACwAIAAxACwAIAAxACwAIAA1ACwAIAA2ACwAIAAyACwAIAAyADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMANgA4ADcAMAAsACAAMwAsACAAMQAsACAAMwAsACAANQAsACAANwAsACAAMgAsACAAMQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADgANAAwADAALAAgADMALAAgADIALAAgADIALAAgADUALAAgADAALAAgADAALAAgADMAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwA4ADQAMAA3ACwAIAAyACwAIAAyACwAIAAzACwAIAA1ACwAIAA4ACwAIAAyACwAIAAwADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADQAMgAzADYAOAAsACAAMwAsACAAMgAsACAAMQAsACAANAAsACAANgAsACAAMgAsACAAMgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAA0ADIAMwA5ADAALAAgADMALAAgADIALAAgADMALAAgADQALAAgADcALAAgADIALAAgADEAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAANAA2ADcAMwA2ACwAIAAzACwAIAAyACwAIAAxACwAIAA1ACwAIAA3ACwAIAAyACwAIAAyADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADQANgA3ADUAOQAsACAAMwAsACAAMgAsACAAMwAsACAANQAsACAAOAAsACAAMgAsACAAMQBcAG4AIAAgACAAIAAgACAAIAAgAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAsACAATABBAE0AQgBEAEEAKABfAGUAeABjAGUAcAB0AGkAbwBuACwAIABbAF8AcAByAGUAYwBpAHMAaQBvAG4AXQAsACAAWwBfAGUAeAB0AGUAbgBkAGUAZABdACwAIABbAF8AZABhAHQAZQBUAHkAcABlAF0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgACAAfAAgAHMAdAByAGkAbgBnACAAIAB8ACAAbgB1AGwAbAAgACAARQBtAHAAdAB5ACAAdABlAHgAdABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAATgAvAEEAIAAgACAAVQBuAGEAYgBsAGUAIAB0AG8AIABwAGEAcgBzAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAFYAQQBMAFUARQAgAEkAbgB2AGEAbABpAGQAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUAByAGUAYwBpAHMAaQBvAG4AIABvAGYAIABwAGEAcgBzAGUAZAAgAHYAYQBsAHUAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABfAGUAeAB0AGUAbgBkAGUAZAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABQAGEAcgBzAGUAZAAgAGUAeAB0AGUAbgBkAGUAZAAgAGYAbwByAG0AYQB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABfAGQAYQB0AGUAVAB5AHAAZQAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABDAGEAbABlAG4AZABhAHIAIABkAGEAdABlACwAIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAsACAAbwByACAAdwBlAGUAawAgAGQAYQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIATgAvAEEAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AEYAQQBMAFMARQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIAVgBBAEwAVQBFAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABGAEEATABTAEUALAAgADAALAAgAE4AKABfAGUAeAB0AGUAbgBkAGUAZAApACwAIABOACgAXwBkAGEAdABlAFQAeQBwAGUAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIABcACIAXAAiACwAIABcACIAXAAiAH0AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAEYAQQBMAFMARQAsACAAMAAsACAATgAoAF8AZQB4AHQAZQBuAGQAZQBkACkALAAgAE4AKABfAGQAYQB0AGUAVAB5AHAAZQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgAFwAIgBcACIAfQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAC8ALwBfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABGAEEATABTAEUALAAgADAALAAgAE4AKABfAGUAeAB0AGUAbgBkAGUAZAApACwAIABOACgAXwBkAGEAdABlAFQAeQBwAGUAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0AKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABJAEYAKABUAGUAeAB0ACAAPQAgAFwAIgBcACIALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAFYAQQBMAEkARABBAFQARQBfAEMASABBAFIAQQBDAFQARQBSAFMAKABUAGUAeAB0ACwAIAAxACkAKQAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAUwBpAGcAbgAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAEYAVAAoAFQAZQB4AHQALAAgADEAKQAgAD0AIABcACIAKwBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUARgBUACgAVABlAHgAdAAsACAAMQApACAAPQAgAFwAIgAtAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFUATgBJAEMATwBEAEUAKABMAEUARgBUACgAVABlAHgAdAAsACAAMQApACkAIAA9ACAAOAA3ADIAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAFMAaQBnAG4ALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBGAFQAKABUAGUAeAB0ACwAIAAxACkAIAA9ACAAXAAiAC0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABVAE4ASQBDAE8ARABFACgATABFAEYAVAAoAFQAZQB4AHQALAAgADEAKQApACAAPQAgADgANwAyADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4ALAAgAEwARQBOACgAVABlAHgAdAApACAALQAgAE4AKABfAGgAYQBzAFMAaQBnAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAEQAYQB0AGUALAAgAEkARgAoAF8AaABhAHMAUwBpAGcAbgAsACAAUgBJAEcASABUACgAVABlAHgAdAAsACAAXwBsAGUAbgApACwAIABUAGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ASAB5AHAAaAAxAFAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgAtAFwAIgAsACAAXwBzAEQAYQB0AGUAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEgAeQBwAGgAMgBQAG8AcwAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIALQBcACIALAAgAF8AcwBEAGEAdABlACwAIABfAEgAeQBwAGgAMQBQAG8AcwAgACsAIAAxACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBXAHAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgBXAFwAIgAsACAAXwBzAEQAYQB0AGUAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAGgALAAgACgAXwBsAGUAbgAgACoAIAA0ADAAOQA2ACkAIAArACAAKABfAEgAeQBwAGgAMQBQAG8AcwAgACoAIAAyADUANgApACAAKwAgACgAXwBIAHkAcABoADIAUABvAHMAIAAqACAAMQA2ACkAIAArACAAXwBXAHAAbwBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAGgATABrAHUAcAAsACAASQBGAE4AQQAoAFgATQBBAFQAQwBIACgAXwBoAGEAcwBoACwAIABDAEgATwBPAFMARQBDAE8ATABTACgAXwBmAG0AdABIAGEAcwBoAFQAYQBiAGwAZQAsACAAMQApACwAIAAwACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBoAGEAcwBoAEwAawB1AHAAIAA9ACAAMAAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAZgBuACwAIABDAEgATwBPAFMARQBSAE8AVwBTACgAXwBmAG0AdABIAGEAcwBoAFQAYQBiAGwAZQAsACAAXwBoAGEAcwBoAEwAawB1AHAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAdABlAG4AZABlAGQALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFQAeQBwAGUALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAAXwB5AGUAYQByAFMAaQBnAG4AIAAqACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8AcwBEAGEAdABlACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADUAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAQQByAGcAMQAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA8ACAAMgApACAAKwAgACgASQBOAEQARQBYACgAXwBkAGUAZgBuACwAIAAxACwAIAA2ACkAIAA9ACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABNAEkARAAoAF8AcwBEAGEAdABlACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADYAKQAsACAASQBOAEQARQBYACgAXwBkAGUAZgBuACwAIAAxACwAIAA3ACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAQQByAGcAMgAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPAAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AcwBEAGEAdABlACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADgAKQApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdgBhAGwAaQBkACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFQAeQBwAGUAIAA9ACAAMQAsACAASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAF8AeQBlAGEAcgBDAEUALAAgAF8AZABBAHIAZwAxACwAIABfAGQAQQByAGcAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAVAB5AHAAZQAgAD0AIAAyACwAIABJAFMAXwBWAEEATABJAEQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAF8AeQBlAGEAcgBDAEUALAAgAF8AZABBAHIAZwAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBUAHkAcABlACAAPQAgADMALAAgAEkAUwBfAFYAQQBMAEkARABfAFcARQBFAEsAXwBEAEEAVABFACgAXwB5AGUAYQByAEMARQAsACAAXwBkAEEAcgBnADEALAAgAF8AZABBAHIAZwAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAFQAUgBVAEUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AdgBhAGwAaQBkACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFQAUgBVAEUALAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAF8AZQB4AHQAZQBuAGQAZQBkACwAIABfAGQAYQB0AGUAVAB5AHAAZQAsACAAXwB5AGUAYQByAEMARQAsACAAXwBkAEEAcgBnADEALAAgAF8AZABBAHIAZwAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBWAEEATABVAEUAXAAiACwAIABfAHAAcgBlAGMAaQBzAGkAbwBuACwAIABfAGUAeAB0AGUAbgBkAGUAZAAsACAAXwBkAGEAdABlAFQAeQBwAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBUAEkATQBFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAaABvAHUAcgAsACAAbQBpAG4AdQB0AGUAIABhAG4AZAAgAHMAZQBjAG8AbgBkACAAbwBmACAAdABpAG0AZQAgAGYAcgBvAG0AIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuAFwAbgBcAG4AQwBvAGwAdQBtAG4AcwA6AFwAbgAgACAAMQAgAHwAIABJAFMATwBDAG8AbQBwAGwAaQBhAG4AdAAgAHwAIABiAG8AbwBsAGUAYQBuACAAfAAgAEYAbABhAGcAIABpAGYAIABjAG8AbQBwAGwAaQBhAG4AdAAgAHQAbwAgAEkAUwBPACAAOAA2ADAAMQAgAHMAdABhAG4AZABhAHIAZABcAG4AIAAgADIAIAB8ACAAUAByAGUAYwBpAHMAaQBvAG4AIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAwACAALQAgAGkAbgB2AGEAbABpAGQAIAB2AGEAbAB1AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMQAgAC0AIABoAG8AdQByAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADIAIAAtACAAbQBpAG4AdQB0AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMwAgAC0AIABpAG4AdABlAGcAZQByACAAcwBlAGMAbwBuAGQAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAANAAgAC0AIABzAGUAYwBvAG4AZAAgADAALgAwAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADUAIAAtACAAcwBlAGMAbwBuAGQAIAAwAC4AMAAwAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADYAIAAtACAAcwBlAGMAbwBuAGQAIAAwAC4AMAAwADAAXABuACAAIAAzACAAfAAgAEYAbwByAG0AYQB0ACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMQAgAC0AIABiAGEAcwBpAGMAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMgAgAC0AIABlAHgAdABlAG4AZABlAGQAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMwAgAC0AIABjAG8AbgBzAGkAcwB0AGUAbgB0ACAAdwBpAHQAaAAgAGIAYQBzAGkAYwAgAG8AcgAgAGUAeAB0AGUAbgBkAGUAZABcAG4AIAAgADQAIAB8ACAASABvAHUAcgAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAwAC4ALgAyADQAXABuACAAIAA1ACAAfAAgAE0AaQBuAHUAdABlACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMAAuAC4ANQA5AFwAbgAgACAANgAgAHwAIABTAGUAYwBvAG4AZAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADAALgAuADUAOQAuADkAOQA5AFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVABlAHgAdAAgACAAIAAgACAAIAAgACAAfAAgAHMAdAByAGkAbgBnACAAfAAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AHQAZQBkACAAdABpAG0AZQAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAARQB4AGEAbQBwAGwAZQAgAGYAbwByAG0AYQB0AHMAOgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAfAAgAFQAaABoADoAbQBtADoAcwBzAC4AcwBzAHMALAAgAFQAaABoADoAbQBtADoAcwBzACwAIABUAGgAaABtAG0ALAAgAFQAaABoAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBQAEEAUgBTAEUAXwBUAEkATQBFACAAPQAgAEwAQQBNAEIARABBACgAVABlAHgAdAAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABDAG8AbAB1AG0AbgBzADoAIABIAGEAcwBoACwAIABQAHIAZQBjAGkAcwBpAG8AbgAsACAARgBvAHIAbQBhAHQALAAgAE0AaQBuAHUAdABlAFAAbwBzACwAIABTAGUAYwBvAG4AZABMAGUAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAHcAaABlAHIAZQAgAEgAYQBzAGgAIAA9ACAAKABMAEUATgAgACoAIAA0ADAAOQA2ACkAIAArACAAKABDAG8AbABvAG4AMQBQAG8AcwAgACoAIAAyADUANgApACAAKwAgACgAQwBvAGwAbwBuADIAUABvAHMAIAAqACAAMQA2ACkAIAArACAARABlAGMAaQBtAGEAbABQAG8AcwAgAFwAbgAgACAAIAAgACAAIAAgACAAXwBmAG0AdABIAGEAcwBoAFQAYQBiAGwAZQAsACAAewBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAOAAxADkAMgAsACAAMQAsACAAMwAsACAAMAAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxADYAMwA4ADQALAAgADIALAAgADEALAAgADMALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgA0ADUANwA2ACwAIAAzACwAIAAxACwAIAAzACwAIAAyADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMAMgA3ADcANQAsACAANAAsACAAMQAsACAAMwAsACAANAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADYAOAA3ADEALAAgADUALAAgADEALAAgADMALAAgADUAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAANAAwADkANgA3ACwAIAA2ACwAIAAxACwAIAAzACwAIAA2ADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIAMQAyADQAOAAsACAAMgAsACAAMgAsACAANAAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADMANgAzADIALAAgADMALAAgADIALAAgADQALAAgADIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAANAAxADgAMwAzACwAIAA0ACwAIAAyACwAIAA0ACwAIAA0ADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADQANQA5ADIAOQAsACAANQAsACAAMgAsACAANAAsACAANQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAA1ADAAMAAyADUALAAgADYALAAgADIALAAgADQALAAgADYAXABuACAAIAAgACAAIAAgACAAIAB9ACwAXABuACAAIAAgACAAIAAgACAAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4ALAAgAEwAQQBNAEIARABBACgAXwBlAHgAYwBlAHAAdABpAG8AbgAsACAAWwBfAHAAcgBlAGMAaQBzAGkAbwBuAF0ALAAgAFsAXwBlAHgAdABlAG4AZABlAGQAXQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABfAGUAeABjAGUAcAB0AGkAbwBuACAAIAB8ACAAcwB0AHIAaQBuAGcAIAAgAHwAIABuAHUAbABsACAAIABFAG0AcAB0AHkAIAB0AGUAeAB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABOAC8AQQAgACAAIABVAG4AYQBiAGwAZQAgAHQAbwAgAHAAYQByAHMAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAVgBBAEwAVQBFACAASQBuAHYAYQBsAGkAZAAgAHYAYQBsAHUAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABQAHIAZQBjAGkAcwBpAG8AbgAgAG8AZgAgAHAAYQByAHMAZQBkACAAdgBhAGwAdQBlAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAF8AZQB4AHQAZQBuAGQAZQBkACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFAAYQByAHMAZQBkACAAZQB4AHQAZQBuAGQAZQBkACAAZgBvAHIAbQBhAHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIATgAvAEEAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AEYAQQBMAFMARQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIAVgBBAEwAVQBFAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABGAEEATABTAEUALAAgADAALAAgAE4AKABfAGUAeAB0AGUAbgBkAGUAZAApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgARgBBAEwAUwBFACwAIAAwACwAIABOACgAXwBlAHgAdABlAG4AZABlAGQAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIABcACIAXAAiAH0AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAAvAC8AXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgARgBBAEwAUwBFACwAIAAwACwAIABOACgAXwBlAHgAdABlAG4AZABlAGQAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0AKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBDAG8AdQBuAHQAQwBoAGEAcgBzACwAIABMAEEATQBCAEQAQQAoAEMAaABhAHIAQQByAHIAYQB5ACwAIABUAGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQAIAA9ACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAGUAbQBvAHYAZQBkACwAIABSAEUARABVAEMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEMAaABhAHIAQQByAHIAYQB5ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwAQQBNAEIARABBACgAXwBhAGMAYwAsACAAXwBjAHUAcgByACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAXwBhAGMAYwAsACAAXwBjAHUAcgByACwAIABcACIAXAAiACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBOACgAVABlAHgAdAApACAALQAgAEwARQBOACgAXwByAGUAbQBvAHYAZQBkACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBGAGkAbgBkAE4AdABoAEMAaABhAHIAUABvAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBzACwAIABUAGUAeAB0ACwAIABOACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByAEMAbwB1AG4AdAAsACAATABFAE4AKABDAGgAYQByAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgAsACAASQBOAFQAKABOACgATgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBjAGgAYQByAEMAbwB1AG4AdAAgAD0AIAAwACkAIAArACAAKABfAG4AIAA9ACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAcwAsACAATQBJAEQAKABDAGgAYQByAHMALAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AYwBoAGEAcgBDAG8AdQBuAHQAKQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAG4AZABDAG8AdQBuAHQALAAgAGYAbgBDAG8AdQBuAHQAQwBoAGEAcgBzACgAXwBjAGgAYQByAHMALAAgAFQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQBuAGQAQwBvAHUAbgB0ACAAPAAgAEEAQgBTACgAXwBuACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG4AdABoACAAYwBhAG4AIABjAG8AdQBuAHQAIABmAHIAbwBtACAAZQBuAGQAIABiAGEAYwBrAHcAYQByAGQAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgB0AGgALAAgAEkARgAoAF8AbgAgAD4AIAAwACwAIABfAG4ALAAgAF8AZgBpAG4AZABDAG8AdQBuAHQAIAArACAAXwBuACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAHQAaABQAG8AcwAsACAAUgBFAEQAVQBDAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAUQBVAEUATgBDAEUAKAAxACwAIABfAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABfAGEAYwBjACwAIABfAGMAdQByAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBjAGMAIAA8ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABJAEYARQBSAFIATwBSACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAE4ARAAoAF8AYwBoAGEAcgBzACwAIABUAGUAeAB0ACwAIABfAGEAYwBjACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAeAB0AFAAbwBzACwAIABNAEkATgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBMAFQARQBSACgAXwBuAGUAeAB0AFAAbwBzAEMAaABhAHIAcwAsACAAXwBuAGUAeAB0AFAAbwBzAEMAaABhAHIAcwAgAD4AIAAwACwAIAAwACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBuAGUAeAB0AFAAbwBzACAAPQAgADAALAAgAC0AMQAsACAAXwBuAGUAeAB0AFAAbwBzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAEEAWAAoAF8AbgB0AGgAUABvAHMALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAVABlAHgAdAAgAD0AIABcACIAXAAiACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABWAEEATABJAEQAQQBUAEUAXwBDAEgAQQBSAEEAQwBUAEUAUgBTACgAVABlAHgAdAAsACAAMgApACkALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBOAC8AQQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFQAcABvAHMALAAgAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXAAiAFQAXAAiACwAIABUAGUAeAB0ACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBUAHAAbwBzACAAPgAgADEALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBOAC8AQQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBUAGkAbQBlACwAIABJAEYAKABfAFQAcABvAHMAIAA9ACAAMQAsACAAUgBJAEcASABUACgAVABlAHgAdAAsACAATABFAE4AKABUAGUAeAB0ACkAIAAtACAAMQApACwAIABUAGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACwAIABMAEUATgAoAF8AcwBUAGkAbQBlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAbwBsAG8AbgAxAFAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgA6AFwAIgAsACAAXwBzAFQAaQBtAGUAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAG8AbABvAG4AMgBQAG8AcwAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAOgBcACIALAAgAF8AcwBUAGkAbQBlACwAIABfAGMAbwBsAG8AbgAxAFAAbwBzACAAKwAgADEAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAYwBpAG0AYQBsAFAAbwBzACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiAC4ALABcACIALAAgAF8AcwBUAGkAbQBlACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAGgALAAgACgAXwBsAGUAbgAgACoAIAA0ADAAOQA2ACkAIAArACAAKABfAGMAbwBsAG8AbgAxAFAAbwBzACAAKgAgADIANQA2ACkAIAArACAAKABfAGMAbwBsAG8AbgAyAFAAbwBzACAAKgAgADEANgApACAAKwAgAF8AZABlAGMAaQBtAGEAbABQAG8AcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAaABMAGsAdQBwACwAIABJAEYATgBBACgAWABNAEEAVABDAEgAKABfAGgAYQBzAGgALAAgAEMASABPAE8AUwBFAEMATwBMAFMAKABfAGYAbQB0AEgAYQBzAGgAVABhAGIAbABlACwAIAAxACkALAAgADAAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBoAGEAcwBoAEwAawB1AHAAIAA9ACAAMAAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBmAG4ALAAgAEMASABPAE8AUwBFAFIATwBXAFMAKABfAGYAbQB0AEgAYQBzAGgAVABhAGIAbABlACwAIABfAGgAYQBzAGgATABrAHUAcAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQB4AHQAZQBuAGQAZQBkACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIALAAgAFYAQQBMAFUARQAoAEwARQBGAFQAKABfAHMAVABpAG0AZQAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAGkAbgB1AHQAZQAsACAASQBGACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgADwAIAAyACwAIABcACIAXAAiACwAIABWAEEATABVAEUAKABNAEkARAAoAF8AcwBUAGkAbQBlACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADQAKQAsACAAMgApACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAEwAZQBuACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA8ACAAMwAsACAAXAAiAFwAIgAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AcwBUAGkAbQBlACwAIABfAHMAZQBjAEwAZQBuACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAC8ALwAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA+ACAAMwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGMAYQBuAG8AdAAgAGEAcwBzAHUAbQBlACAAVgBBAEwAVQBFACAAZgB1AG4AYwB0AGkAbwBuACAAdwBpAGwAbAAgAHUAcwBlACAAZABlAGMAaQBtAGEAbAAgAGMAaABhAHIAYQBjAHQAZQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB3AGgAZQBuACAARQB4AGMAZQBsACAAaABhAHMAIABuAG8AbgAtAGUAbgBnAGwAaQBzAGgAIABSAGUAZwBpAG8AbgBhAGwAIABzAGUAdAB0AGkAbgBnAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBTAGUAYwAsACAAUgBJAEcASABUACgAXwBzAFQAaQBtAGUALAAgAF8AcwBlAGMATABlAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAbgB0AFMAZQBjACwAIABWAEEATABVAEUAKABMAEUARgBUACgAXwBzAFMAZQBjACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAcgBhAGMAUwBlAGMALAAgAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AcwBTAGUAYwAsACAAXwBzAGUAYwBMAGUAbgAgAC0AIAAzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBjAGkAbQBhAGwAQgBhAHMAZQAsACAASQBOAEQARQBYACgAewAxADAALAAgADEAMAAwACwAIAAxADAAMAAwAH0ALAAgADEAIAAsAF8AcAByAGUAYwBpAHMAaQBvAG4AIAAtACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBuAHQAUwBlAGMAIAArACAAKABfAGYAcgBhAGMAUwBlAGMAIAAvACAAXwBkAGUAYwBpAG0AYQBsAEIAYQBzAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBUAEkATQBFACgAXwBoAG8AdQByACwAIABfAG0AaQBuAHUAdABlACwAIABfAHMAZQBjAG8AbgBkACkAKQAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAFYAQQBMAFUARQBcACIALAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAF8AZQB4AHQAZQBuAGQAZQBkACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoACgAXwBUAHAAbwBzACAAPQAgADEAKQAsACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAsACAAXwBlAHgAdABlAG4AZABlAGQALAAgAF8AaABvAHUAcgAsACAAXwBtAGkAbgB1AHQAZQAsACAAXwBzAGUAYwBvAG4AZAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBUAEkATQBFAF8AWgBPAE4ARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AXABuAFwAbgBDAG8AbAB1AG0AbgBzADoAXABuACAAIAAxACAAfAAgAEkAUwBPAEMAbwBtAHAAbABpAGEAbgB0ACAAIAB8ACAAYgBvAG8AbABlAGEAbgAgAHwAIABGAGwAYQBnACAAaQBmACAAYwBvAG0AcABsAGkAYQBuAHQAIAB0AG8AIABJAFMATwAgADgANgAwADEAIABzAHQAYQBuAGQAYQByAGQAXABuACAAIAAyACAAfAAgAFAAcgBlAGMAaQBzAGkAbwBuACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAwACAALQAgAGkAbgB2AGEAbABpAGQAIAB2AGEAbAB1AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAxACAALQAgAGgAbwB1AHIAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAyACAALQAgAG0AaQBuAHUAdABlAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMwAgAC0AIABzAGUAYwBvAG4AZABcAG4AIAAgADMAIAB8ACAARgBvAHIAbQBhAHQAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADEAIAAtACAAYgBhAHMAaQBjAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMgAgAC0AIABlAHgAdABlAG4AZABlAGQAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAzACAALQAgAGMAbwBuAHMAaQBzAHQAZQBuAHQAIAB3AGkAdABoACAAYgBhAHMAaQBjACAAbwByACAAZQB4AHQAZQBuAGQAZQBkAFwAbgAgACAANQAgAHwAIABPAGYAZgBzAGUAdABNAGkAbgB1AHQAZQBzACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAALQA5ADAAMAAuAC4AKwA5ADAAMABcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFQAZQB4AHQAIAAgACAAIAAgACAAIAAgAHwAIABzAHQAcgBpAG4AZwAgAHwAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAB0AGUAZAAgAHQAaQBtAGUAIAB6AG8AbgBlAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgAHwAIABFAHgAYQBtAHAAbABlACAAZgBvAHIAbQBhAHQAcwA6AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAAKwBoAGgAOgBtAG0ALAAgACsAaABoAG0AbQAsACAALQBoAGgALAAgAFoAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAFQASQBNAEUAXwBaAE8ATgBFACAAPQAgAEwAQQBNAEIARABBACgAVABlAHgAdAAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABDAG8AbAB1AG0AbgBzADoAIABIAGEAcwBoACwAIABQAHIAZQBjAGkAcwBpAG8AbgAsACAARQB4AHQAZQBuAGQAZQBkACwAIABaACwAIABNAGkAbgBQAG8AcwBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAHcAaABlAHIAZQAgAGgAYQBzAGgAIAA9ACAATABFAE4AIAAqACAAMQAwADIANAAgACsAIABaAG8AbgBsAHkAIAAqACAANQAxADIAIAArACAATABhAHMAdABTAGkAZwBuAFAAbwBzAEEAdAAxACAAKgAyADUANgAgACsAIABDAG8AbABvAG4AMQBQAG8AcwAgACoAIAAxADYAIAArACAAQwBvAGwAbwBuADIAUABvAHMAXABuACAAIAAgACAAIAAgACAAIABfAGYAbQB0AEgAYQBzAGgAVABhAGIAbABlACwAIAB7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxADUAMwA2ACwAIAAzACwAIAAzACwAIAAxACwAIAAwADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMAMwAyADgALAAgADEALAAgADMALAAgADAALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAANQAzADcANgAsACAAMgAsACAAMQAsACAAMAAsACAANAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAA2ADQANgA0ACwAIAAyACwAIAAyACwAIAAwACwAIAA1ADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADcANAAyADQALAAgADMALAAgADEALAAgADAALAAgADQAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAOQA1ADQAMwAsACAAMwAsACAAMgAsACAAMAAsACAANQBcAG4AIAAgACAAIAAgACAAIAAgAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAsACAATABBAE0AQgBEAEEAKABfAGUAeABjAGUAcAB0AGkAbwBuACwAIABbAF8AZQB4AHQAZQBuAGQAZQBkAF0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgACAAfAAgAHMAdAByAGkAbgBnACAAIAB8ACAAbgB1AGwAbAAgACAARQBtAHAAdAB5ACAAdABlAHgAdABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAATgAvAEEAIAAgACAAVQBuAGEAYgBsAGUAIAB0AG8AIABwAGEAcgBzAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAFYAQQBMAFUARQAgAEkAbgB2AGEAbABpAGQAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAdABlAG4AZABlAGQAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUABhAHIAcwBlAGQAIABlAHgAdABlAG4AZABlAGQAIABmAG8AcgBtAGEAdABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBOAC8AQQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsARgBBAEwAUwBFACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBWAEEATABVAEUAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAEYAQQBMAFMARQAsACAAMAAsACAATgAoAF8AZQB4AHQAZQBuAGQAZQBkACkALAAgAHsAIwBWAEEATABVAEUAIQB9ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBBAHIAcgBhAHkALAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHgAdAAgAD0AIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIAZQBtAG8AdgBlAGQALAAgAFIARQBEAFUAQwBFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBoAGEAcgBBAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABfAGEAYwBjACwAIABfAGMAdQByAHIALAAgAFMAVQBCAFMAVABJAFQAVQBUAEUAKABfAGEAYwBjACwAIABfAGMAdQByAHIALAAgAFwAIgBcACIAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAE4AKABUAGUAeAB0ACkAIAAtACAATABFAE4AKABfAHIAZQBtAG8AdgBlAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEYAaQBuAGQATgB0AGgAQwBoAGEAcgBQAG8AcwAsACAATABBAE0AQgBEAEEAKABDAGgAYQByAHMALAAgAFQAZQB4AHQALAAgAE4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAQwBvAHUAbgB0ACwAIABMAEUATgAoAEMAaABhAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuACwAIABJAE4AVAAoAE4AKABOACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABfAGMAaABhAHIAQwBvAHUAbgB0ACAAPQAgADAAKQAgACsAIAAoAF8AbgAgAD0AIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgBzACwAIABNAEkARAAoAEMAaABhAHIAcwAsACAAUwBFAFEAVQBFAE4AQwBFACgAMQAsACAAXwBjAGgAYQByAEMAbwB1AG4AdAApACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAbgBkAEMAbwB1AG4AdAAsACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMAKABfAGMAaABhAHIAcwAsACAAVABlAHgAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAG4AZABDAG8AdQBuAHQAIAA8ACAAQQBCAFMAKABfAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbgB0AGgAIABjAGEAbgAgAGMAbwB1AG4AdAAgAGYAcgBvAG0AIABlAG4AZAAgAGIAYQBjAGsAdwBhAHIAZABzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAHQAaAAsACAASQBGACgAXwBuACAAPgAgADAALAAgAF8AbgAsACAAXwBmAGkAbgBkAEMAbwB1AG4AdAAgACsAIABfAG4AIAArACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AdABoAFAAbwBzACwAIABSAEUARABVAEMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEEATQBCAEQAQQAoAF8AYQBjAGMALAAgAF8AYwB1AHIAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGMAYwAgADwAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAtADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBlAHgAdABQAG8AcwBDAGgAYQByAHMALAAgAEkARgBFAFIAUgBPAFIAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEkATgBEACgAXwBjAGgAYQByAHMALAAgAFQAZQB4AHQALAAgAF8AYQBjAGMAIAArACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AZQB4AHQAUABvAHMALAAgAE0ASQBOACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAEwAVABFAFIAKABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACAAPgAgADAALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAG4AZQB4AHQAUABvAHMAIAA9ACAAMAAsACAALQAxACwAIABfAG4AZQB4AHQAUABvAHMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0AQQBYACgAXwBuAHQAaABQAG8AcwAsACAAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAVABlAHgAdAAgAD0AIABcACIAXAAiACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABWAEEATABJAEQAQQBUAEUAXwBDAEgAQQBSAEEAQwBUAEUAUgBTACgAVABlAHgAdAAsACAAMwApACkALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBOAC8AQQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACwAIABMAEUATgAoAFQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBaAG8AbgBsAHkALAAgAE4AKAAoAF8AbABlAG4AIAA9ACAAMQApACAAKgAgACgASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAWgBcACIALAAgAFQAZQB4AHQAKQAsACAAMAApACAAPQAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAYQBzAHQAUwBpAGcAbgBQAG8AcwBBAHQAMQAsACAATgAoAGYAbgBGAGkAbgBkAE4AdABoAEMAaABhAHIAUABvAHMAKABcACIAKwAtAFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAIABUAGUAeAB0ACwAIAAtADEAKQAgAD0AIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGwAbwBuADEAUABvAHMALAAgAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXAAiADoAXAAiACwAIABUAGUAeAB0ACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAG8AbABvAG4AMgBQAG8AcwAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAOgBcACIALAAgAFQAZQB4AHQALAAgAF8AYwBvAGwAbwBuADEAUABvAHMAIAArACAAMQApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAaAAsACAAKABfAGwAZQBuACAAKgAgADEAMAAyADQAKQAgACsAIAAoAF8AWgBvAG4AbAB5ACAAKgAgADUAMQAyACkAIAArACAAKABfAGwAYQBzAHQAUwBpAGcAbgBQAG8AcwBBAHQAMQAgACoAIAAyADUANgApACAAKwAgACgAXwBjAG8AbABvAG4AMQBQAG8AcwAgACoAIAAxADYAKQAgACsAIABfAGMAbwBsAG8AbgAyAFAAbwBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAGgATABrAHUAcAAsACAASQBGAE4AQQAoAFgATQBBAFQAQwBIACgAXwBoAGEAcwBoACwAIABDAEgATwBPAFMARQBDAE8ATABTACgAXwBmAG0AdABIAGEAcwBoAFQAYQBiAGwAZQAsACAAMQApACwAIAAwACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBoAGEAcwBoAEwAawB1AHAAIAA9ACAAMAAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAZgBuACwAIABDAEgATwBPAFMARQBSAE8AVwBTACgAXwBmAG0AdABIAGEAcwBoAFQAYQBiAGwAZQAsACAAXwBoAGEAcwBoAEwAawB1AHAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAdABlAG4AZABlAGQALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASQBOAEQARQBYACgAXwBkAGUAZgBuACwAIAAxACwAIAA0ACkAIAA+ACAAMAAsACAALwAvACAAWgAgAG8AbgBsAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFQAUgBVAEUALAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAF8AZQB4AHQAZQBuAGQAZQBkACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUARgBUACgAVABlAHgAdAAsACAAMQApACAAPQAgAFwAIgAtAFwAIgAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVQBOAEkAQwBPAEQARQAoAEwARQBGAFQAKABUAGUAeAB0ACwAIAAxACkAKQAgAD0AIAA4ADcAMgAyACwAIAAtADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAAxAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgAsACAAXwBzAGkAZwBuACAAKgAgAFYAQQBMAFUARQAoAE0ASQBEACgAVABlAHgAdAAsACAAMgAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAGkAbgB1AHQAZQAsACAASQBGACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgADwAIAAyACwAIABcACIAXAAiACwAIABWAEEATABVAEUAKABNAEkARAAoAFQAZQB4AHQALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAANQApACwAIAAyACkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQALAAgAEkARgAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA8ACAAMwAsACAAXAAiAFwAIgAsACAAVgBBAEwAVQBFACgAUgBJAEcASABUACgAVABlAHgAdAAsACAAMgApACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAE0AaQBuAHUAdABlAHMALAAgAEkATgBUACgAKABOACgAXwBoAG8AdQByACkAIAAqACAAMwA2ADAAMAApACAAKwAgACgATgAoAF8AbQBpAG4AdQB0AGUAKQAgACoAIAA2ADAAKQAgACsAIABOACgAXwBzAGUAYwBvAG4AZAApACkAIAAvACAANgAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQBfAFoATwBOAEUAKABfAHQAegBvAE0AaQBuAHUAdABlAHMAKQApACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIAVgBBAEwAVQBFAFwAIgAsACAAXwBlAHgAdABlAG4AZABlAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAVABSAFUARQAsACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAsACAAXwBlAHgAdABlAG4AZABlAGQALAAgAF8AdAB6AG8ATQBpAG4AdQB0AGUAcwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBQAEEAUgBUAFMAXABuAFwAbgBTAHAAbABpAHQAcwAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AHQAZQBkACAAdABlAHgAdAAgAHYAYQBsAHUAZQAgAGkAbgB0AG8AIABpAG4AdABvACAAcgBlAHMAcABlAGMAdABpAHYAZQAgAHAAYQByAHQAcwAgAG8AZgAgAGQAYQB0AGUALAAgAHQAaQBtAGUAIABhAG4AZAAgAHQAaQBtAGUAIAB6AG8AbgBlAC4AXABuAFwAbgBDAG8AbAB1AG0AbgBzADoAXABuACAAIAAxACAAfAAgAEkAUwBPAEMAbwBtAHAAbABpAGEAbgB0ACAAfAAgAGIAbwBvAGwAZQBhAG4AIAB8ACAARgBsAGEAZwAgAGkAZgAgAGMAbwBtAHAAbABpAGEAbgB0ACAAdABvACAASQBTAE8AIAA4ADYAMAAxACAAcwB0AGEAbgBkAGEAcgBkAFwAbgAgACAAMgAgAHwAIABQAGEAcgB0AHMAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEIAaQB0AGYAbABhAGcAIABvAGYAIABwAGEAcgB0AHMAIAAwAC4ALgA3AFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADAAeAAwADQAIAAtACAAZABhAHQAZQBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAwAHgAMAAyACAALQAgAHQAaQBtAGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMAB4ADAAMQAgAC0AIAB0AGkAbQBlACAAegBvAG4AZQBcAG4AIAAgADMAIAB8ACAARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAAgAHwAXABuACAAIAA0ACAAfAAgAFQAaQBtAGUAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdAByAGkAbgBnACAAIAB8AFwAbgAgACAANQAgAHwAIABUAGkAbQBlACAAWgBvAG4AZQAgACAAIAAgAHwAIABzAHQAcgBpAG4AZwAgACAAfABcAG4AIAAgACAAIAAgACAAXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFQAZQB4AHQAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdAByAGkAbgBnACAAfAAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AHQAZQBkACAAdgBhAGwAdQBlACAAZgBvAHIAIABkAGEAdABlACwAIAB0AGkAbQBlACAAbwByACAAdABpAG0AZQAgAHoAbwBuAGUALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AUABBAFIAUwBFAF8AUABBAFIAVABTACAAPQAgAEwAQQBNAEIARABBACgAVABlAHgAdAAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAsACAATABBAE0AQgBEAEEAKABfAGUAeABjAGUAcAB0AGkAbwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAF8AZQB4AGMAZQBwAHQAaQBvAG4AIAAgAHwAIABzAHQAcgBpAG4AZwAgACAAfAAgAG4AdQBsAGwAIAAgAEUAbQBwAHQAeQAgAHQAZQB4AHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE4ALwBBACAAIAAgAFUAbgBhAGIAbABlACAAdABvACAAcABhAHIAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBOAC8AQQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AEYAQQBMAFMARQAsACAAMAAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBBAHIAcgBhAHkALAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHgAdAAgAD0AIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIAZQBtAG8AdgBlAGQALAAgAFIARQBEAFUAQwBFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBoAGEAcgBBAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABfAGEAYwBjACwAIABfAGMAdQByAHIALAAgAFMAVQBCAFMAVABJAFQAVQBUAEUAKABfAGEAYwBjACwAIABfAGMAdQByAHIALAAgAFwAIgBcACIAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAE4AKABUAGUAeAB0ACkAIAAtACAATABFAE4AKABfAHIAZQBtAG8AdgBlAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBGAGkAbgBkAE4AdABoAEMAaABhAHIAUABvAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBzACwAIABUAGUAeAB0ACwAIABOACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByAEMAbwB1AG4AdAAsACAATABFAE4AKABDAGgAYQByAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgAsACAASQBOAFQAKABOACgATgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBjAGgAYQByAEMAbwB1AG4AdAAgAD0AIAAwACkAIAArACAAKABfAG4AIAA9ACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAcwAsACAATQBJAEQAKABDAGgAYQByAHMALAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AYwBoAGEAcgBDAG8AdQBuAHQAKQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAG4AZABDAG8AdQBuAHQALAAgAGYAbgBDAG8AdQBuAHQAQwBoAGEAcgBzACgAXwBjAGgAYQByAHMALAAgAFQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQBuAGQAQwBvAHUAbgB0ACAAPAAgAEEAQgBTACgAXwBuACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG4AdABoACAAYwBhAG4AIABjAG8AdQBuAHQAIABmAHIAbwBtACAAZQBuAGQAIABiAGEAYwBrAHcAYQByAGQAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgB0AGgALAAgAEkARgAoAF8AbgAgAD4AIAAwACwAIABfAG4ALAAgAF8AZgBpAG4AZABDAG8AdQBuAHQAIAArACAAXwBuACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAHQAaABQAG8AcwAsACAAUgBFAEQAVQBDAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAUQBVAEUATgBDAEUAKAAxACwAIABfAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABfAGEAYwBjACwAIABfAGMAdQByAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBjAGMAIAA8ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABJAEYARQBSAFIATwBSACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAE4ARAAoAF8AYwBoAGEAcgBzACwAIABUAGUAeAB0ACwAIABfAGEAYwBjACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAeAB0AFAAbwBzACwAIABNAEkATgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBMAFQARQBSACgAXwBuAGUAeAB0AFAAbwBzAEMAaABhAHIAcwAsACAAXwBuAGUAeAB0AFAAbwBzAEMAaABhAHIAcwAgAD4AIAAwACwAIAAwACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBuAGUAeAB0AFAAbwBzACAAPQAgADAALAAgAC0AMQAsACAAXwBuAGUAeAB0AFAAbwBzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAEEAWAAoAF8AbgB0AGgAUABvAHMALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgADEAIAAtACAAVAAgAGYAaQByAHMAdAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEAIAA9ACAAQQB0ACAAZgBpAHIAcwB0ACAAcABvAHMAaQB0AGkAbwBuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAgAD0AIABBAGYAdABlAHIAIABmAGkAcgBzAHQAIABwAG8AcwBpAHQAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAAyACAALQAgAFQAWgAgAG0AYQByAGsAZQByACAAYQBmAHQAZQByACAAVAAgACAAIAAwACAAPQAgAE4AbwAgAHMAaQBnAG4AIABvAHIAIABaAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAgAD0AIABGAGkAcgBzAHQAIABwAG8AcwBpAHQAaQBvAG4AIABmAG8AbABsAG8AdwBpAG4AZwAgAFQAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACAAPQAgAEEAZgB0AGUAcgAgAGYAaQByAHMAdAAgAHAAbwBzAGkAdABpAG8AbgAgAGYAbwBsAGwAbwB3AGkAbgBnACAAVABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgADMAIAAtACAAUABhAHIAdABzACAAYgBpAHQAIABmAGwAYQBnACAAIAAgACAAIAAgADAAeAAwADQAIAAtACAARABhAHQAZQBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAeAAwADIAIAAtACAAVABpAG0AZQBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAeAAwADEAIAAtACAAVABpAG0AZQAgAFoAbwBuAGUAXABuACAAIAAgACAAIAAgACAAIABXAGkAdABoAFQAXwBMAG8AZwBpAGMALAAgAHsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEALAAgADAALAAgADIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsACAAMQAsACAAMQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACwAIAAyACwAIAAzADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIALAAgADAALAAgADYAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAsACAAMQAsACAANQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAIAAyACwAIAA3AFwAbgAgACAAIAAgACAAIAAgACAAfQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgADEAIAAtACAAVABaACAAbQBhAHIAawBlAHIAIABmAGkAcgBzAHQAIAAgACAAIAAgADAAIAA9ACAATgBvACAAcwBpAGcAbgAgAG8AcgAgAFoAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACAAPQAgAEYAaQByAHMAdAAgAHAAbwBzAGkAdABpAG8AbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIAIAA9ACAAQQBmAHQAZQByACAAZgBpAHIAcwB0ACAAcABvAHMAaQB0AGkAbwBuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAMgAgAC0AIABUAFoAIABtAGEAcgBrAGUAcgAgAGkAcwAgAFoAIAAoAGIAbwBvAGwAZQBhAG4AKQBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgADMAIAAtACAASABhAHMAIABDAG8AbABvAG4AIAAoAGIAbwBvAGwAZQBhAG4AKQBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgADQAIAAtACAAVABpAG0AZQAgAGMAbwBuAGQAaQB0AGkAbwBuAHMAIAAoAGIAbwBvAGwAZQBhAG4AKQBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgADUAIAAtACAAUABhAHIAdABzACAAYgBpAHQAIABmAGwAYQBnACAAIAAgACAAIAAgADAAeAAwADQAIAAtACAARABhAHQAZQBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAeAAwADIAIAAtACAAVABpAG0AZQBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAeAAwADEAIAAtACAAVABpAG0AZQAgAFoAbwBuAGUAXABuACAAIAAgACAAIAAgACAAIABXAGkAdABoAG8AdQB0AFQAXwBMAG8AZwBpAGMALAAgAHsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALAAgADAALAAgADAALAAgADAALAAgADQAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsACAAMAAsACAAMAAsACAAMQAsACAAMgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAIAAwACwAIAAxACwAIAAwACwAIAAyADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEALAAgADAALAAgADAALAAgADAALAAgADQAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsACAAMAAsACAAMAAsACAAMQAsACAAMQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACwAIAAwACwAIAAxACwAIAAwACwAIAAxADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEALAAgADEALAAgADAALAAgADAALAAgADEAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAsACAAMAAsACAAMAAsACAAMAAsACAANAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAIAAwACwAIAAwACwAIAAxACwAIAAzADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIALAAgADAALAAgADEALAAgADAALAAgADMAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAsACAAMAAsACAAMQAsACAAMQAsACAAMwA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAIAAxACwAIAAwACwAIAAxACwAIAAzADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIALAAgADEALAAgADEALAAgADAALAAgADMAXABuACAAIAAgACAAIAAgACAAIAB9ACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAFcAaQB0AGgAVABfAFAAYQByAHQAcwBMAGUAbgAsACAATABBAE0AQgBEAEEAKABfAFQAcABvAHMALAAgAF8AVABmAGkAcgBzAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuACwAIABMAEUATgAoAFQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBmAHQAZQByAFQALAAgAFIASQBHAEgAVAAoAFQAZQB4AHQALAAgAF8AbABlAG4AIAAtACAAXwBUAHAAbwBzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFQAWgBtAGEAcgBrAGUAcgBQAG8AcwAsACAAZgBuAEYAaQBuAGQATgB0AGgAQwBoAGEAcgBQAG8AcwAoAFwAIgBaACsALQBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsACAAXwBhAGYAdABlAHIAVAAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBUAFoAbQBhAHIAawBGAGkAcgBzAHQALAAgAEkARgAoAF8AVABaAG0AYQByAGsAZQByAFAAbwBzACAAPgAgADEALAAgADIALAAgAF8AVABaAG0AYQByAGsAZQByAFAAbwBzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAcwBGAGwAYQBnACwAIABGAEkATABUAEUAUgAoAEMASABPAE8AUwBFAEMATwBMAFMAKABXAGkAdABoAFQAXwBMAG8AZwBpAGMALAAgADMAKQAsACAAKABDAEgATwBPAFMARQBDAE8ATABTACgAVwBpAHQAaABUAF8ATABvAGcAaQBjACwAIAAxACkAIAA9ACAAXwBUAGYAaQByAHMAdAApACAAKgAgACgAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAFcAaQB0AGgAVABfAEwAbwBnAGkAYwAsACAAMgApACAAPQAgAF8AVABaAG0AYQByAGsARgBpAHIAcwB0ACkALAAgACMATgAvAEEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBOAEEAKABfAHAAYQByAHQAcwBGAGwAYQBnACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAIwBOAC8AQQAsACAAMAAsACAAMAAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUATABlAG4ALAAgAF8AVABwAG8AcwAgAC0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBMAGUAbgAsACAASQBGACgAQgBJAFQAQQBOAEQAKABfAHAAYQByAHQAcwBGAGwAYQBnACwAIAAyACkAIAA9ACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEIASQBUAEEATgBEACgAXwBwAGEAcgB0AHMARgBsAGEAZwAsACAAMQApACAAPQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AVABaAG0AYQByAGsAZQByAFAAbwBzACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4AIAAtACAAXwBUAHAAbwBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AEwAZQBuACwAIABfAGwAZQBuACAALQAgAF8AVABwAG8AcwAgAC0AIABfAHQAaQBtAGUATABlAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHAAYQByAHQAcwBGAGwAYQBnACwAIABfAGQAYQB0AGUATABlAG4ALAAgAF8AdABpAG0AZQBMAGUAbgAsACAAXwB0AHoATABlAG4AKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABmAG4AVwBpAHQAaABvAHUAdABUAF8AUABhAHIAdABzAEwAZQBuACwAIABMAEEATQBCAEQAQQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4ALAAgAEwARQBOACgAVABlAHgAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBUAFoAbQBhAHIAawBQAG8AcwAsACAAZgBuAEYAaQBuAGQATgB0AGgAQwBoAGEAcgBQAG8AcwAoAFwAIgBaACsALQBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsACAAVABlAHgAdAAsACAALQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFQAWgBtAGEAcgBrAEYAaQByAHMAdAAsACAASQBGACgAXwBUAFoAbQBhAHIAawBQAG8AcwAgAD4AIAAxACwAIAAyACwAIABfAFQAWgBtAGEAcgBrAFAAbwBzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFQAWgBtAGEAcgBrAEkAcwBaACwAIABJAEYAKABfAFQAWgBtAGEAcgBrAFAAbwBzACAAPgAgADAALAAgAE4AKABDAE8ARABFACgATQBJAEQAKABUAGUAeAB0ACwAIABfAFQAWgBtAGEAcgBrAFAAbwBzACwAIAAxACkAKQAgAD0AIAA5ADAAKQAsACAAMAApACwAIAAvAC8AIABDAE8ARABFACgAXAAiAFoAXAAiACkAIAA9ACAAOQAwACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBIAGEAcwBDAG8AbABvAG4ALAAgAE4AKABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgA6AFwAIgAsACAAVABlAHgAdAApACwAIAAwACkAIAA+ACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgBCAGUAZgBvAHIAZQBUAFoALAAgAEkARgAoAF8AVABaAG0AYQByAGsARgBpAHIAcwB0ACAAPQAgADAALAAgAF8AbABlAG4ALAAgAF8AVABaAG0AYQByAGsAUABvAHMAIAAtACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlAEMAbwBuAGQAaQB0AGkAbwBuAGEAbAAsACAASQBGACgAXwBUAFoAbQBhAHIAawBGAGkAcgBzAHQAIAA9ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgBBAGYAdABlAHIAVABaACwAIABfAGwAZQBuACAALQAgAF8AVABaAG0AYQByAGsAUABvAHMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABfAGwAZQBuAEEAZgB0AGUAcgBUAFoAIAA9ACAAMgAsACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4AQQBmAHQAZQByAFQAWgAgAD0AIAA2ACwAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AKABfAGwAZQBuAEIAZQBmAG8AcgBlAFQAWgAgAD0AIAAyACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBhAHQAYwBoACwAIAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABDAEgATwBPAFMARQBDAE8ATABTACgAVwBpAHQAaABvAHUAdABUAF8ATABvAGcAaQBjACwAIAAxACkAIAA9ACAAXwBUAFoAbQBhAHIAawBGAGkAcgBzAHQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACoAIAAoAEMASABPAE8AUwBFAEMATwBMAFMAKABXAGkAdABoAG8AdQB0AFQAXwBMAG8AZwBpAGMALAAgADIAKQAgAD0AIABfAFQAWgBtAGEAcgBrAEkAcwBaACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAqACAAKABDAEgATwBPAFMARQBDAE8ATABTACgAVwBpAHQAaABvAHUAdABUAF8ATABvAGcAaQBjACwAIAAzACkAIAA9ACAAXwBIAGEAcwBDAG8AbABvAG4AKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACoAIAAoAEMASABPAE8AUwBFAEMATwBMAFMAKABXAGkAdABoAG8AdQB0AFQAXwBMAG8AZwBpAGMALAAgADQAKQAgAD0AIABfAHQAaQBtAGUAQwBvAG4AZABpAHQAaQBvAG4AYQBsACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAcwBGAGwAYQBnACwAIABGAEkATABUAEUAUgAoAEMASABPAE8AUwBFAEMATwBMAFMAKABXAGkAdABoAG8AdQB0AFQAXwBMAG8AZwBpAGMALAAgADUAKQAsACAAXwBtAGEAdABjAGgALAAgACMATgAvAEEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBMAGUAbgAsACAASQBGACgAQgBJAFQAQQBOAEQAKABfAHAAYQByAHQAcwBGAGwAYQBnACwAIAA0ACkAIAA9ACAANAAsACAAXwBsAGUAbgAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlAEwAZQBuACwAIABJAEYAKABCAEkAVABBAE4ARAAoAF8AcABhAHIAdABzAEYAbABhAGcALAAgADIAKQAgAD0AIAAyACwAIABfAGwAZQBuAEIAZQBmAG8AcgBlAFQAWgAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoATABlAG4ALAAgAEkARgAoAEIASQBUAEEATgBEACgAXwBwAGEAcgB0AHMARgBsAGEAZwAsACAAMQApACAAPQAgADEALAAgAF8AbABlAG4AIAAtACAAXwBUAFoAbQBhAHIAawBQAG8AcwAgACsAIAAxACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AcABhAHIAdABzAEYAbABhAGcALAAgAF8AZABhAHQAZQBMAGUAbgAsACAAXwB0AGkAbQBlAEwAZQBuACwAIABfAHQAegBMAGUAbgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFQAZQB4AHQAIAA9ACAAXAAiAFwAIgAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgAVgBBAEwASQBEAEEAVABFAF8AQwBIAEEAUgBBAEMAVABFAFIAUwAoAFQAZQB4AHQALAAgADAAKQApACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIATgAvAEEAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBUAHAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgBUAFwAIgAsACAAVABlAHgAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AVABwAG8AcwAgAD0AIABMAEUATgAoAFQAZQB4AHQAKQAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAGEAcwBUACwAIABJAEYAKABfAFQAcABvAHMAIAA+ACAAMQAsACAAMgAsACAAXwBUAHAAbwBzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAcwBMAGUAbgAsACAASQBGACgAXwBoAGEAcwBUACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVwBpAHQAaABUAF8AUABhAHIAdABzAEwAZQBuACgAXwBUAHAAbwBzACwAIABfAGgAYQBzAFQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgBuAFcAaQB0AGgAbwB1AHQAVABfAFAAYQByAHQAcwBMAGUAbgAoACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABzAEYAbABhAGcALAAgAEkATgBEAEUAWAAoAF8AcABhAHIAdABzAEwAZQBuACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMATgBBACgAXwBwAGEAcgB0AHMARgBsAGEAZwApACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIATgAvAEEAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAG8AQwBvAG0AcABsAGkAYQBuAHQALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAGEAcgB0AHMARgBsAGEAZwAgAD0AIAAxACwAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAcwBGAGwAYQBnACAAPQAgADUALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABzAEYAbABhAGcAIAA9ACAANAAsACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgACgAXwBoAGEAcwBUACAAPgAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAUABhAHIAdAAsACAASQBGACgAQgBJAFQAQQBOAEQAKABfAHAAYQByAHQAcwBGAGwAYQBnACwAIAA0ACkAIAA9ACAANAAsACAATABFAEYAVAAoAFQAZQB4AHQALAAgAEkATgBEAEUAWAAoAF8AcABhAHIAdABzAEwAZQBuACwAIAAxACwAIAAyACkAKQAsACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBQAGEAcgB0ACwAIABJAEYAKABCAEkAVABBAE4ARAAoAF8AcABhAHIAdABzAEYAbABhAGcALAAgADIAKQAgAD0AIAAyACwAIABcACIAVABcACIAIAAmACAATQBJAEQAKABUAGUAeAB0ACwAIABfAFQAcABvAHMAIAArACAAMQAsACAASQBOAEQARQBYACgAXwBwAGEAcgB0AHMATABlAG4ALAAgADEALAAgADMAKQApACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAUABhAHIAdAAsACAASQBGACgAQgBJAFQAQQBOAEQAKABfAHAAYQByAHQAcwBGAGwAYQBnACwAIAAxACkAIAA9ACAAMQAsACAAUgBJAEcASABUACgAVABlAHgAdAAsACAASQBOAEQARQBYACgAXwBwAGEAcgB0AHMATABlAG4ALAAgADEALAAgADQAKQApACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAGkAcwBvAEMAbwBtAHAAbABpAGEAbgB0ACwAIABfAHAAYQByAHQAcwBGAGwAYQBnACwAIABfAGQAYQB0AGUAUABhAHIAdAAsACAAXwB0AGkAbQBlAFAAYQByAHQALAAgAF8AdAB6AFAAYQByAHQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFAAQQBSAFMARQBfAEkAUwBPADgANgAwADEAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAYwBvAG0AcABsAGkAYwBhAHQAaQBvAG4AcwAgAG8AZgAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPADgANgAwADEAIABmAG8AcgBtAGEAdAAuAFwAbgBcAG4AQwBvAGwAdQBtAG4AcwA6AFwAbgAgACAAMQAgAHwAIABJAFMATwBDAG8AbQBwAGwAaQBhAG4AdAAgACAAIAB8ACAAYgBvAG8AbABlAGEAbgAgAHwAIABGAGwAYQBnACAAaQBmACAAYwBvAG0AcABsAGkAYQBuAHQAIAB0AG8AIABJAFMATwAgADgANgAwADEAIABzAHQAYQBuAGQAYQByAGQAXABuACAAIAAyACAAfAAgAFAAYQByAHQAcwAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEIAaQB0AGYAbABhAGcAIABvAGYAIABwAGEAcgB0AHMAIAAwAC4ALgA3AFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAwAHgAMAA0ACAALQAgAGQAYQB0AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADAAeAAwADIAIAAtACAAdABpAG0AZQBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMAB4ADAAMQAgAC0AIAB0AGkAbQBlACAAegBvAG4AZQBcAG4AIAAgADMAIAB8ACAAUAByAGUAYwBpAHMAaQBvAG4AIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMQAgAC0AIAB5AGUAYQByAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAyACAALQAgAG0AbwBuAHQAaAAvAHcAZQBlAGsAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADMAIAAtACAAZABhAHkAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADQAIAAtACAAaABvAHUAcgBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAANQAgAC0AIABtAGkAbgB1AHQAZQBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAANgAgAC0AIABpAG4AdABlAGcAZQByACAAcwBlAGMAbwBuAGQAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADcAIAAtACAAcwBlAGMAbwBuAGQAIAAwAC4AMABcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAOAAgAC0AIABzAGUAYwBvAG4AZAAgADAALgAwADAAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADkAIAAtACAAcwBlAGMAbwBuAGQAIAAwAC4AMAAwADAAXABuACAAIAA0ACAAfAAgAEYAbwByAG0AYQB0ACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADAAIAAtACAAbQBpAHgAZQBkAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAxACAALQAgAGIAYQBzAGkAYwBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMgAgAC0AIABlAHgAdABlAG4AZABlAGQAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADMAIAAtACAAYwBvAG4AcwBpAHMAdABlAG4AdAAgAHcAaQB0AGgAIABiAGEAcwBpAGMAIABvAHIAIABlAHgAdABlAG4AZABlAGQAXABuACAAIAA1ACAAfAAgAEQAYQB0AGUAIABUAHkAcABlACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADAAIAAtACAAbgBvACAAZABhAHQAZQAgAHAAcgBlAHMAZQBuAHQAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADEAIAAtACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHQAZQBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMgAgAC0AIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMwAgAC0AIAB3AGUAZQBrACAAZABhAHQAZQBcAG4AIAAgADYAIAB8ACAAWQBlAGEAcgAgAEMARQAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgAgACAANwAgAHwAIABNAG8AbgB0AGgAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxAC4ALgAxADIAXABuACAAIAAgACAAfAAgAFcAZQBlAGsAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADEALgAuADUAMwBcAG4AIAAgADgAIAB8ACAARABhAHkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMQAuAC4AMwAxAFwAbgAgACAAIAAgAHwAIABPAHIAZABpAG4AYQBsACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxAC4ALgAzADYANgBcAG4AIAAgACAAIAB8ACAARABhAHkAIABvAGYAIABXAGUAZQBrACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMQAuAC4ANwAgAC0APgAgAE0AbwBuAC4ALgBTAHUAbgBcAG4AIAAgADkAIAB8ACAASABvAHUAcgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMAAuAC4AMgA0AFwAbgAgADEAMAAgAHwAIABNAGkAbgB1AHQAZQAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAwAC4ALgA1ADkAXABuACAAMQAxACAAfAAgAFMAZQBjAG8AbgBkACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADAALgAuADUAOQAuADkAOQA5AFwAbgAgADEAMgAgAHwAIABNAGkAbgB1AHQAZQBzACAATwBmAGYAcwBlAHQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIAAtADkAMAAwAC4ALgArADkAMAAwAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVABlAHgAdAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAB8ACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQAdABlAGQAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAfAAgAEUAeABhAG0AcABsAGUAIABmAG8AcgBtAGEAdABzADoAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAfAAgACsAWQBZAFkAWQBZAC0ATQBNAC0ARABEAFQAaABoADoAbQBtADoAcwBzAC4AcwBzAHMAKwBoAGgAOgBtAG0AOgBzAHMALAAgAFkAWQBZAFkALQBNAE0ALQBEAEQAVABoAGgAOgBtAG0ALQBoAGgALAAgAFkAWQBZAFkALQBXAHcAdwAtAEQAVABoAGgAOgBtAG0AWgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AUABBAFIAUwBFAF8ASQBTAE8AOAA2ADAAMQAgAD0AIABMAEEATQBCAEQAQQAoAFQAZQB4AHQALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACwAIABMAEEATQBCAEQAQQAoAF8AZQB4AGMAZQBwAHQAaQBvAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAAgAHwAIABuAHUAbABsACAAIABFAG0AcAB0AHkAIAB0AGUAeAB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE4ALwBBACAAIAAgAFUAbgBhAGIAbABlACAAdABvACAAcABhAHIAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBOAC8AQQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AEYAQQBMAFMARQAsACAAMAAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAdABzAEYAbABhAGcALAAgAEwAQQBNAEIARABBACgAXwBwAEQAYQB0AGUALAAgAF8AcABUAGkAbQBlACwAIABfAHAAVABaACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFAAYQByAHQALAAgAE4AKABJAE4ARABFAFgAKABfAHAARABhAHQAZQAsACAAMQAsACAAMQApACkAIAAqACAANAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBQAGEAcgB0ACwAIABOACgASQBOAEQARQBYACgAXwBwAFQAaQBtAGUALAAgADEALAAgADEAKQApACAAKgAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBQAGEAcgB0ACwAIABOACgASQBOAEQARQBYACgAXwBwAFQAWgAsACAAMQAsACAAMQApACkAIAAqACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBQAGEAcgB0ACAAKwAgAF8AdABpAG0AZQBQAGEAcgB0ACAAKwAgAF8AdAB6AFAAYQByAHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBJAFMATwBWAGEAbAB1AGUAQwBvAG0AcABsAGkAYQBuAGMAZQAsACAATABBAE0AQgBEAEEAKABfAHAARABhAHQAZQAsACAAXwBwAFQAaQBtAGUALAAgAF8AcABUAFoALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUASQBTAE8AQwBvAG0AcABsAGkAYQBuAHQALAAgAEkARgAoAEkATgBEAEUAWAAoAF8AcABEAGEAdABlACwAIAAxACwAIAAxACkAIAA9ACAAXAAiAFwAIgAsACAAVABSAFUARQAsACAASQBOAEQARQBYACgAXwBwAEQAYQB0AGUALAAgADEALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlAEkAUwBPAEMAbwBtAHAAbABpAGEAbgB0ACwAIABJAEYAKABJAE4ARABFAFgAKABfAHAAVABpAG0AZQAsACAAMQAsACAAMQApACAAPQAgAFwAIgBcACIALAAgAFQAUgBVAEUALAAgAEkATgBEAEUAWAAoAF8AcABUAGkAbQBlACwAIAAxACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AEkAUwBPAEMAbwBtAHAAbABpAGEAbgB0ACwAIABJAEYAKABJAE4ARABFAFgAKABfAHAAVABaACwAIAAxACwAIAAxACkAIAA9ACAAXAAiAFwAIgAsACAAVABSAFUARQAsACAASQBOAEQARQBYACgAXwBwAFQAWgAsACAAMQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AZABhAHQAZQBJAFMATwBDAG8AbQBwAGwAaQBhAG4AdAAgACoAIABfAHQAaQBtAGUASQBTAE8AQwBvAG0AcABsAGkAYQBuAHQAIAAqACAAXwB0AHoASQBTAE8AQwBvAG0AcABsAGkAYQBuAHQAKQAgADwAPgAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEkAUwBPAEYAbwByAG0AYQB0AEMAbwBtAHAAbABpAGEAbgBjAGUALAAgAEwAQQBNAEIARABBACgAXwBwAEQAYQB0AGUALAAgAF8AcABUAGkAbQBlACwAIABfAHAAVABaACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBsAHUAbQBuAHMAIABPAHUAdAA6ACAASQBTAE8AQwBvAG0AcABsAGkAYQBuAHQALAAgAFIAZQBzAG8AbAB2AGUAZABGAG8AcgBtAGEAdABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUARgBtAHQALAAgAE4AKABJAE4ARABFAFgAKABfAHAARABhAHQAZQAsACAAMQAsACAAMwApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUARgBtAHQALAAgAE4AKABJAE4ARABFAFgAKABfAHAAVABpAG0AZQAsACAAMQAsACAAMwApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBvAEYAbQB0ACwAIABOACgASQBOAEQARQBYACgAXwBwAFQAWgAsACAAMQAsACAAMwApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIAZQBzAG8AbAB2AGUARgBtAHQALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AZABhAHQAZQBGAG0AdAAgAD0AIAAzACkAIAAqACAAKABfAHQAaQBtAGUARgBtAHQAIAA9ACAAMAApACAAKgAgACgAXwB0AHoAbwBGAG0AdAAgAD0AIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG8AbgBsAHkAIABkAGEAdABlACAAcAByAG8AdgBpAGQAZQBkACwAIABjAG8AbgBzAGkAcwB0AGUAbgB0ACAAdwBpAHQAaAAgAGIAYQBzAGkAYwAgAG8AcgAgAGUAeAB0AGUAbgBkAGUAZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AZABhAHQAZQBGAG0AdAAgAD0AIAAwACkAIAAqACAAKABfAHQAaQBtAGUARgBtAHQAIAA9ACAAMwApACAAKgAgACgAXwB0AHoAbwBGAG0AdAAgAD0AIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG8AbgBsAHkAIAB0AGkAbQBlACAAcAByAG8AdgBpAGQAZQBkACwAIABjAG8AbgBzAGkAcwB0AGUAbgB0ACAAdwBpAHQAaAAgAGIAYQBzAGkAYwAgAG8AcgAgAGUAeAB0AGUAbgBkAGUAZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AZABhAHQAZQBGAG0AdAAgAD0AIAAwACkAIAAqACAAKABfAHQAaQBtAGUARgBtAHQAIAA9ACAAMAApACAAKgAgACgAXwB0AHoAbwBGAG0AdAAgAD0AIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG8AbgBsAHkAIAB0AGkAbQBlACAAegBvAG4AZQAgAHAAcgBvAHYAaQBkAGUAZAAsACAAYwBvAG4AcwBpAHMAdABlAG4AdAAgAHcAaQB0AGgAIABiAGEAcwBpAGMAIABvAHIAIABlAHgAdABlAG4AZABlAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABfAGQAYQB0AGUARgBtAHQAIAA8AD4AIAAyACkAIAAqACAAKABfAHQAaQBtAGUARgBtAHQAIAA8AD4AIAAyACkAIAAqACAAKABfAHQAegBvAEYAbQB0ACAAPAA+ACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABhAGwAbAAgAGIAYQBzAGkAYwAgAGYAbwByAG0AYQB0ACAAdwBoAGUAcgBlACAAcAByAGUAcwBlAG4AdABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBkAGEAdABlAEYAbQB0ACAAPAA+ACAAMQApACAAKgAgACgAXwB0AGkAbQBlAEYAbQB0ACAAPAA+ACAAMQApACAAKgAgACgAXwB0AHoAbwBGAG0AdAAgADwAPgAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAYQBsAGwAIABlAHgAdABlAG4AZABlAGQAIABmAG8AcgBtAGEAdAAgAHcAaABlAHIAZQAgAHAAcgBlAHMAZQBuAHQAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABtAGkAeABlAGQAIABmAG8AcgBtAGEAdABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATgAoAF8AcgBlAHMAbwBsAHYAZQBGAG0AdAAgADwAPgAgADAAKQAsACAAXwByAGUAcwBvAGwAdgBlAEYAbQB0ACkAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABmAG4ASQBTAE8AUAByAGUAYwBpAHMAaQBvAG4AQwBvAG0AcABsAGkAYQBuAGMAZQAsACAATABBAE0AQgBEAEEAKABfAHAARABhAHQAZQAsACAAXwBwAFQAaQBtAGUALAAgAF8AcABUAFoALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAQwBvAGwAdQBtAG4AcwAgAE8AdQB0ADoAIABJAFMATwBDAG8AbQBwAGwAaQBhAG4AdAAsACAAUAByAGUAYwBpAHMAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFAAcgBlAGMALAAgAE4AKABJAE4ARABFAFgAKABfAHAARABhAHQAZQAsACAAMQAsACAAMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUAUAByAGUAYwAsACAATgAoAEkATgBEAEUAWAAoAF8AcABUAGkAbQBlACwAIAAxACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AFAAcgBlAGMALAAgAE4AKABJAE4ARABFAFgAKABfAHAAVABaACwAIAAxACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAUAByAGUAYwAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AdABpAG0AZQBQAHIAZQBjACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHQAegBQAHIAZQBjACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgARgBBAEwAUwBFACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAVABSAFUARQAsACAAXwB0AHoAUAByAGUAYwAgACsAIAAzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAVABSAFUARQAsACAAXwB0AGkAbQBlAFAAcgBlAGMAIAArACAAMwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAUAByAGUAYwAgADwAIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAKABfAHQAaQBtAGUAUAByAGUAYwAgAD0AIAAwACkALAAgAF8AZABhAHQAZQBQAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAC8ALwAgAF8AZABhAHQAZQBQAHIAZQBjACAAPQAgADMAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABUAFIAVQBFACwAIABfAHQAaQBtAGUAUAByAGUAYwAgACsAIAAzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAVABlAHgAdAAgAD0AIABcACIAXAAiACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAcwAsACAAUABBAFIAUwBFAF8AUABBAFIAVABTACgAVABlAHgAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATgAoAEkATgBEAEUAWAAoAF8AcABhAHIAdABzACwAIAAxACwAIAAyACkAKQAgAD0AIAAwACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIATgAvAEEAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAG8AUABhAHIAdABzAEMAbwBtAHAAbABpAGEAbgBjAGUALAAgAE4AKABJAE4ARABFAFgAKABfAHAAYQByAHQAcwAsACAAMQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAEQAYQB0AGUALAAgAFAAQQBSAFMARQBfAEQAQQBUAEUAKABJAE4ARABFAFgAKABfAHAAYQByAHQAcwAsACAAMQAsACAAMwApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAFQAaQBtAGUALAAgAFAAQQBSAFMARQBfAFQASQBNAEUAKABJAE4ARABFAFgAKABfAHAAYQByAHQAcwAsACAAMQAsACAANAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAFQAWgAsACAAUABBAFIAUwBFAF8AVABJAE0ARQBfAFoATwBOAEUAKABJAE4ARABFAFgAKABfAHAAYQByAHQAcwAsACAAMQAsACAANQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAHMAbwBWAGEAbAB1AGUAQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAZgBuAEkAUwBPAFYAYQBsAHUAZQBDAG8AbQBwAGwAaQBhAG4AYwBlACgAXwBwAEQAYQB0AGUALAAgAF8AcABUAGkAbQBlACwAIABfAHAAVABaACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAHMAbwBGAG8AcgBtAGEAdABDAG8AbQBwAGwAaQBhAG4AYwBlACwAIABmAG4ASQBTAE8ARgBvAHIAbQBhAHQAQwBvAG0AcABsAGkAYQBuAGMAZQAoAF8AcABEAGEAdABlACwAIABfAHAAVABpAG0AZQAsACAAXwBwAFQAWgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAG8AUAByAGUAYwBpAHMAaQBvAG4AQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAZgBuAEkAUwBPAFAAcgBlAGMAaQBzAGkAbwBuAEMAbwBtAHAAbABpAGEAbgBjAGUAKABfAHAARABhAHQAZQAsACAAXwBwAFQAaQBtAGUALAAgAF8AcABUAFoAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AdQB0AEkAUwBPAGMAbwBtAHAAbABpAGEAbgBjAGUALAAgACgAXwBpAHMAbwBWAGEAbAB1AGUAQwBvAG0AcABsAGkAYQBuAGMAZQAgACoAIABfAGkAcwBvAFAAYQByAHQAcwBDAG8AbQBwAGwAaQBhAG4AYwBlACAAKgAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARgBvAHIAbQBhAHQAQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAMQAsACAAMQApACAAKgAgAEkATgBEAEUAWAAoAF8AaQBzAG8AUAByAGUAYwBpAHMAaQBvAG4AQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAMQAsACAAMQApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwB1AHQARABhAHQAZQBUAHkAcABlACwAIABOACgASQBOAEQARQBYACgAXwBwAEQAYQB0AGUALAAgADEALAAgADQAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwB1AHQARABhAHQAZQAsACAARABSAE8AUAAoAF8AcABEAGEAdABlACwAIAAsACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwB1AHQAVABpAG0AZQAsACAARABSAE8AUAAoAF8AcABUAGkAbQBlACwAIAAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwB1AHQAVABaACwAIABEAFIATwBQACgAXwBwAFQAWgAsACAALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AdQB0AFAAYQByAHQAcwBGAGwAYQBnACwAIABmAG4AUABhAHIAdABzAEYAbABhAGcAKABfAHAARABhAHQAZQAsACAAXwBwAFQAaQBtAGUALAAgAF8AcABUAFoAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AbwB1AHQASQBTAE8AYwBvAG0AcABsAGkAYQBuAGMAZQAsACAAXwBvAHUAdABQAGEAcgB0AHMARgBsAGEAZwAsACAASQBOAEQARQBYACgAXwBpAHMAbwBQAHIAZQBjAGkAcwBpAG8AbgBDAG8AbQBwAGwAaQBhAG4AYwBlACwAIAAxACwAIAAyACkALAAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARgBvAHIAbQBhAHQAQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAMQAsACAAMgApACwAIABfAG8AdQB0AEQAYQB0AGUAVAB5AHAAZQAsACAAXwBvAHUAdABEAGEAdABlACwAIABfAG8AdQB0AFQAaQBtAGUALAAgAF8AbwB1AHQAVABaACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAE8AUgBNAEEAVABfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAGQAYQB0AGUAIABhAHMAIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuAFwAbgBFAHgAYQBtAHAAbABlACAAZgBvAHIAbQBhAHQAcwAgACgAbgBvAHQAIABlAHgAaABhAHUAcwB0AGkAdgBlACkAOgAgACsAWQBZAFkAWQBZAC0ATQBNAC0ARABEACwAIABZAFkAWQBZAC0ATQBNAC0ARABEACwAIABZAFkAWQBZAC0ATQBNACwAIAArAFkAWQBZAFkATQBNACwAIABZAFkAWQBZAFwAbgAjAFYAQQBMAFUARQAhACAAaQBmACAAYQBuACAAaQBuAHYAYQBsAGkAZAAgAGQAYQB0AGUAIABvAHIAIABhAG0AYgBpAGcAdQBvAHUAcwAgAGIAYQBzAGkAYwAgAGYAbwByAG0AYQB0AC4AIABlAGcAIAAyADAAMgAzADAANQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBbAE0AbwBuAHQAaABdACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABNAG8AbgB0AGgAIABvAGYAIAB0AGgAZQAgAHkAZQBhAHIAXABuAFsARABhAHkAXQAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEQAYQB5ACAAbwBmACAAdABoAGUAIABtAG8AbgB0AGgAXABuAFsAQgBhAHMAaQBjAF0AIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAFIAZQB0AHUAcgBuACAAaQBuACAAYgBhAHMAaQBjACAAZgBvAHIAbQBhAHQAIABlAGcAIABZAFkAWQBZAE0ATQBEAEQAXABuAFsAUwBpAGcAbgBlAGQAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEEAbAB3AGEAeQBzACAAcwBpAGcAbgAgAHkAZQBhAHIAIAB2AGEAbAB1AGUAIABlAGcAIAArAFkAWQBZAFkALQBNAE0ALQBEAEQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYATwBSAE0AQQBUAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABbAE0AbwBuAHQAaABdACwAIABbAEQAYQB5AF0ALAAgAFsAQgBhAHMAaQBjAF0ALAAgAFsAUwBpAGcAbgBlAGQAXQAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkAIAAqACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACAAKgAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgARABhAHkAKQApACwAXABuACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGIAYQBzAGkAYwBGAG8AcgBtAGEAdAAsACAATgAoAEIAYQBzAGkAYwApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgBlAGQAWQBlAGEAcgAsACAATgAoAFMAaQBnAG4AZQBkACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACkAIAAqACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBGAG0AdAAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABBAEIAUwAoAF8AeQApACAAPgA9ACAAMQAwADAAMAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAKwAwADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMAAwAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgBlAGQAWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsAMAAwADAAMAA7AFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACAAJgAgAFwAIgAwADAAMAAwADsAKwAwADAAMAAwAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgAwADAAMAAwADsAXAAiACAAJgAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkAIAAmACAAXAAiADAAMAAwADAAOwAwADAAMAAwAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAWQBlAGEAcgAsACAAVABFAFgAVAAoAF8AeQAsACAAXwB5AEYAbQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAE0AbwBuAHQAaAAsACAAVABFAFgAVAAoAEkATgBUACgATQBvAG4AdABoACkALAAgAFwAIgAwADAAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGIAYQBzAGkAYwBGAG8AcgBtAGEAdAAsACAAXwBzAFkAZQBhAHIAIAAmACAAXwBzAE0AbwBuAHQAaAAsACAAXwBzAFkAZQBhAHIAIAAmACAAXAAiAC0AXAAiACAAJgAgAF8AcwBNAG8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBEAGEAeQAsACAAVABFAFgAVAAoAEkATgBUACgARABhAHkAKQAsACAAXAAiADAAMABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACAAJgAgAF8AcwBNAG8AbgB0AGgAIAAmACAAXwBzAEQAYQB5ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAWQBlAGEAcgAgACYAIABcACIALQBcACIAIAAmACAAXwBzAE0AbwBuAHQAaAAgACYAIABcACIALQBcACIAIAAmACAAXwBzAEQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8AVABJAE0ARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAdABpAG0AZQAgAGEAcwAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AXABuAEUAeABhAG0AcABsAGUAIABmAG8AcgBtAGEAdABzACAAKABuAG8AdAAgAGUAeABoAGEAdQBzAHQAaQB2AGUAKQA6ACAAVABoAGgAOgBtAG0AOgBzAHMALgBzAHMAcwAsACAAVABoAGgAOgBtAG0AOgBzAHMALAAgAFQAaABoADoAbQBtACwAIABUAGgAaABtAG0AcwBzACwAIABUAGgAaABcAG4AIwBWAEEATABVAEUAIQAgAGkAZgAgAGEAbgAgAGkAbgB2AGEAbABpAGQAIAB0AGkAbQBlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASABvAHUAcgAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMAAuAC4AMgA0AFwAbgBNAGkAbgB1AHQAZQAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAwAC4ALgA1ADkAXABuAFMAZQBjAG8AbgBkACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADAALgAuADUAOQAuADkAOQA5AFwAbgBbAEIAYQBzAGkAYwBdACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABSAGUAdAB1AHIAbgAgAGkAbgAgAGIAYQBzAGkAYwAgAGYAbwByAG0AYQB0AFwAbgBbAFAAcgBlAGMAaQBzAGkAbwBuAF0AIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABTAGUAbABlAGMAdAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAbABlAHYAZQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMAAgAC0AIABhAHUAdABvAG0AYQB0AGkAYwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADEAIAAtACAAaABvAHUAcgBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMgAgAC0AIABtAGkAbgB1AHQAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIABpAG4AdABlAGcAZQByACAAcwBlAGMAbwBuAGQAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADQAIAAtACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHMAZQBjAG8AbgBkAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYATwBSAE0AQQBUAF8AVABJAE0ARQAgAD0AIABMAEEATQBCAEQAQQAoAEgAbwB1AHIALAAgAE0AaQBuAHUAdABlACwAIABTAGUAYwBvAG4AZAAsACAAWwBCAGEAcwBpAGMAXQAsACAAWwBQAHIAZQBjAGkAcwBpAG8AbgBdACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEgAbwB1AHIAKQApACAAKgAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQApACAAKgAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAUwBlAGMAbwBuAGQAKQApACwAXABuACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBUAEkATQBFACgASABvAHUAcgAsACAATQBpAG4AdQB0AGUALAAgAFMAZQBjAG8AbgBkACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAE4AKABCAGEAcwBpAGMAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMALAAgAFIATwBVAE4ARABEAE8AVwBOACgATgAoAFMAZQBjAG8AbgBkACkALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQAsACAASQBOAFQAKABOACgATQBpAG4AdQB0AGUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoACwAIABJAE4AVAAoAE4AKABIAG8AdQByACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAE0AQQBYACgASQBOAFQAKABOACgAUAByAGUAYwBpAHMAaQBvAG4AKQApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHUAcwBlAFAAcgBlAGMAaQBzAGkAbwBuACwAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABJAFMATgBVAE0AQgBFAFIAKABTAGUAYwBvAG4AZAApACwAIABJAEYAKABfAHMAIAA9ACAASQBOAFQAKABfAHMAKQAsACAAMwAsACAANAApACwAIABJAFMATgBVAE0AQgBFAFIAKABNAGkAbgB1AHQAZQApACwAIAAyACwAIABUAFIAVQBFACwAIAAxACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHUAcwBlAFAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAFwAIgAgACYAIABUAEUAWABUACgAXwBoACwAIABcACIAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHUAcwBlAFAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGIAYQBzAGkAYwBGAG8AcgBtAGEAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABcACIAIAAmACAAVABFAFgAVAAoAF8AaAAsACAAXAAiADAAMABcACIAKQAgACYAIABUAEUAWABUACgAXwBtACwAIABcACIAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAFwAIgAgACYAIABUAEUAWABUACgAXwBoACwAIABcACIAMAAwAFwAIgApACAAJgAgAFwAIgA6AFwAIgAgACYAIABUAEUAWABUACgAXwBtACwAIABcACIAMAAwAFwAIgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFQAXAAiACAAJgAgAFQARQBYAFQAKABfAGgALAAgAFwAIgAwADAAXAAiACkAIAAmACAAVABFAFgAVAAoAF8AbQAsACAAXAAiADAAMABcACIAKQAgACYAIABUAEUAWABUACgAXwBzACwAIABcACIAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAFwAIgAgACYAIABUAEUAWABUACgAXwBoACwAIABcACIAMAAwAFwAIgApACAAJgAgAFwAIgA6AFwAIgAgACYAIABUAEUAWABUACgAXwBtACwAIABcACIAMAAwAFwAIgApACAAJgAgAFwAIgA6AFwAIgAgACYAIABUAEUAWABUACgAXwBzACwAIABcACIAMAAwAFwAIgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AXwB1AHMAZQBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAA0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAFwAIgAgACYAIABUAEUAWABUACgAXwBoACwAIABcACIAMAAwAFwAIgApACAAJgAgAFQARQBYAFQAKABfAG0ALAAgAFwAIgAwADAAXAAiACkAIAAmACAAVABFAFgAVAAoAF8AcwAsACAAXAAiADAAMAAuADAAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAFwAIgAgACYAIABUAEUAWABUACgAXwBoACwAIABcACIAMAAwAFwAIgApACAAJgAgAFwAIgA6AFwAIgAgACYAIABUAEUAWABUACgAXwBtACwAIABcACIAMAAwAFwAIgApACAAJgAgAFwAIgA6AFwAIgAgACYAIABUAEUAWABUACgAXwBzACwAIABcACIAMAAwAC4AMAAwADAAXAAiACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8AVABJAE0ARQBfAFoATwBOAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAHQAaQBtAGUAIAB6AG8AbgBlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgBcAG4ARQB4AGEAbQBwAGwAZQAgAGYAbwByAG0AYQB0AHMAIAAoAG4AbwB0ACAAZQB4AGgAYQB1AHMAdABpAHYAZQApADoAIAArAGgAaAA6AG0AbQA6AHMAcwAsACAALQBoAGgAOgBtAG0ALAAgACsAaABoACwAIABaAFwAbgAjAFYAQQBMAFUARQAhACAAaQBmACAAYQBuACAAaQBuAHYAYQBsAGkAZAAgAHQAaQBtAGUAIAB6AG8AbgBlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABmAHIAbwBtACAAVQBUAEMAIABpAG4AIABtAGkAbgB1AHQAZQBzACAALQA5ADAAMAAuAC4AKwA5ADAAMABcAG4AWwBCAGEAcwBpAGMAXQAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAFIAZQB0AHUAcgBuACAAaQBuACAAYgBhAHMAaQBjACAAZgBvAHIAbQBhAHQAXABuAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABTAGUAbABlAGMAdAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAbABlAHYAZQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAAYQB1AHQAbwBtAGEAdABpAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABoAG8AdQByAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMgAgAC0AIABtAGkAbgB1AHQAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAAcwBlAGMAbwBuAGQAcwBcAG4AWwBOAG8AWgB1AGwAdQBdACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAFUAcwBlACAAKwAwADAAOgAwADAAIABpAG4AcwB0AGUAYQBkACAAbwBmACAAWgAgAGYAbwByACAAVQBUAEMAIAB0AGkAbQBlACAAegBvAG4AZQAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBGAE8AUgBNAEEAVABfAFQASQBNAEUAXwBaAE8ATgBFACAAPQAgAEwAQQBNAEIARABBACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwAsACAAWwBCAGEAcwBpAGMAXQAsACAAWwBQAHIAZQBjAGkAcwBpAG8AbgBdACwAIABbAE4AbwBaAHUAbAB1AF0ALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwApACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAIABOACgAQgBhAHMAaQBjACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAE0AQQBYACgASQBOAFQAKABOACgAUAByAGUAYwBpAHMAaQBvAG4AKQApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAYQByAFoAZQByAG8ALAAgAFIATwBVAE4ARABEAE8AVwBOACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwAgACoAIAA2ADAALAAgADAAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgATgAoAE4AbwBaAHUAbAB1ACkAIAA9ACAAMAApACAAKgAgAF8AbgBlAGEAcgBaAGUAcgBvACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFoAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAXwBaAE8ATgBFACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAUwBlAGMAcwAsACAAUgBPAFUATgBEAEQATwBXAE4AKABNAE8ARAAoAE8AZgBmAHMAZQB0AE0AaQBuAHUAdABlAHMALAAgADEAKQAgACoAIAA2ADAALAAgADAAKQAgAD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBGAG0AdAAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAUwBlAGMAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAFwAIgBoAGgAbQBtAHMAcwBcACIALAAgAFwAIgBoAGgAOgBtAG0AOgBzAHMAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAIABcACIAaABoAG0AbQBcACIALAAgAFwAIgBoAGgAOgBtAG0AXAAiACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBoAGgAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAFwAIgBoAGgAbQBtAFwAIgAsACAAXAAiAGgAaAA6AG0AbQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAFwAIgBoAGgAbQBtAHMAcwBcACIALAAgAFwAIgBoAGgAOgBtAG0AOgBzAHMAXAAiACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABTAEkARwBOACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwApACAAPAAgADAALAAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkALAAgAFwAIgArAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABBAEIAUwAoAE8AZgBmAHMAZQB0AE0AaQBuAHUAdABlAHMAKQAgAC8AIAAxADQANAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAgACYAIABUAEUAWABUACgAXwB0AGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALAAgAF8AcwBGAG0AdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAE8AUgBNAEEAVABfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgBcAG4ARQB4AGEAbQBwAGwAZQAgAGYAbwByAG0AYQB0AHMAIAAoAG4AbwB0ACAAZQB4AGgAYQB1AHMAdABpAHYAZQApADoAIABZAFkAWQBZAC0ARABEAEQALAAgAFkAWQBZAFkARABEAEQAXABuACMAVgBBAEwAVQBFACEAIABpAGYAIABhAG4AIABpAG4AdgBhAGwAaQBkACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4ATwByAGQAaQBuAGEAbAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgBcAG4AWwBCAGEAcwBpAGMAXQAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAUgBlAHQAdQByAG4AIABpAG4AIABiAGEAcwBpAGMAIABmAG8AcgBtAGEAdAAgAGUAZwAgAFkAWQBZAFkARABEAEQAXABuAFsAUwBpAGcAbgBlAGQAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEEAbAB3AGEAeQBzACAAcwBpAGcAbgAgAHkAZQBhAHIAIAB2AGEAbAB1AGUAIABlAGcAIAArAFkAWQBZAFkALQBNAE0ALQBEAEQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYATwBSAE0AQQBUAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbAAsACAAWwBCAGEAcwBpAGMAXQAsACAAWwBTAGkAZwBuAGUAZABdACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACoAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE8AcgBkAGkAbgBhAGwAKQApACwAXABuACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABPAHIAZABpAG4AYQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAE4AKABCAGEAcwBpAGMAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AZQBkAFkARQBhAHIALAAgAE4AKABTAGkAZwBuAGUAZAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAKABBAEIAUwAoAF8AeQApACAAPgA9ACAAMQAwADAAMAAwACkAIAAqACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AEYAbQB0ACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEEAQgBTACgAXwB5ACkAIAA+AD0AIAAxADAAMAAwADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArADAAMAAwADAAMAA7AFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACAAJgAgAFwAIgAwADAAMAAwADAAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuAGUAZABZAGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAKwAwADAAMAAwADsAXAAiACAAJgAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkAIAAmACAAXAAiADAAMAAwADAAOwArADAAMAAwADAAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMAA7ADAAMAAwADAAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABUAEUAWABUACgAXwB5ACwAIABfAHkARgBtAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMATwByAGQAaQBuAGEAbAAsACAAVABFAFgAVAAoAEkATgBUACgATwByAGQAaQBuAGEAbAApACwAIABcACIAMAAwADAAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAF8AcwBZAGUAYQByACAAJgAgAF8AcwBPAHIAZABpAG4AYQBsACwAIABfAHMAWQBlAGEAcgAgACYAIABcACIALQBcACIAIAAmACAAXwBzAE8AcgBkAGkAbgBhAGwAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARgBPAFIATQBBAFQAXwBXAEUARQBLAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAdwBlAGUAawAgAGQAYQB0AGUAIABhAHMAIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuAFwAbgBFAHgAYQBtAHAAbABlACAAZgBvAHIAbQBhAHQAcwAgACgAbgBvAHQAIABlAHgAaABhAHUAcwB0AGkAdgBlACkAOgAgAFkAWQBZAFkALQBXAHcAdwAtAEQALAAgAFkAWQBZAFkALQBXAHcAdwAsACAAWQBZAFkAWQBXAHcAdwBEACwAIABZAFkAWQBZAFcAdwB3AFwAbgAjAFYAQQBMAFUARQAhACAAaQBmACAAYQBuACAAaQBuAHYAYQBsAGkAZAAgAHcAZQBlAGsAIABkAGEAdABlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4AVwBlAGUAawAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABvAGYAIAB0AGgAZQAgAHkAZQBhAHIAXABuAEQAYQB5AE8AZgBXAGUAZQBrACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIAB3AGgAZQByAGUAIAAxAC4ALgA3ACAALQA+ACAATQBvAG4ALgAuAFMAdQBuACAAXABuAFsAQgBhAHMAaQBjAF0AIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAUgBlAHQAdQByAG4AIABpAG4AIABiAGEAcwBpAGMAIABmAG8AcgBtAGEAdAAgAGUAZwAgAFkAWQBZAFkAVwB3AHcARABcAG4AWwBTAGkAZwBuAGUAZABdACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABBAGwAdwBhAHkAcwAgAHMAaQBnAG4AIAB5AGUAYQByACAAdgBhAGwAdQBlACAAZQBnACAAKwBZAFkAWQBZAC0AVwB3AHcALQBEAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBGAE8AUgBNAEEAVABfAFcARQBFAEsAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAFcAZQBlAGsALAAgAEQAYQB5AE8AZgBXAGUAZQBrACwAIABbAEIAYQBzAGkAYwBdACwAIABbAFMAaQBnAG4AZQBkAF0ALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACAAKgAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAVwBlAGUAawApACkAIAAqACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQBPAGYAVwBlAGUAawApACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFcARQBFAEsAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAFcAZQBlAGsALAAgAEQAYQB5AE8AZgBXAGUAZQBrACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAE4AKABCAGEAcwBpAGMAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AZQBkAFkAZQBhAHIALAAgAE4AKABTAGkAZwBuAGUAZAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AEYAbQB0ACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQQBCAFMAKABfAHkAKQAgAD4APQAgADEAMAAwADAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAKwAwADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMAAwAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuAGUAZABZAGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMAA7ACsAMAAwADAAMABcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMAA7ADAAMAAwADAAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAWQBlAGEAcgAsACAAVABFAFgAVAAoAF8AeQAsACAAXwB5AEYAbQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAVwBlAGUAawAsACAAVABFAFgAVAAoAEkATgBUACgAVwBlAGUAawApACwAIABcACIAVwAwADAAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgARABhAHkATwBmAFcAZQBlAGsAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGIAYQBzAGkAYwBGAG8AcgBtAGEAdAAsACAAXwBzAFkAZQBhAHIAIAAmACAAXwBzAFcAZQBlAGsALAAgAF8AcwBZAGUAYQByACAAJgAgAFwAIgAtAFwAIgAgACYAIABfAHMAVwBlAGUAawApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFkAZQBhAHIAIAAmACAAXwBzAFcAZQBlAGsAIAAmACAASQBOAFQAKABEAGEAeQBPAGYAVwBlAGUAawApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACAAJgAgAFwAIgAtAFwAIgAgACYAIABfAHMAVwBlAGUAawAgACYAIABcACIALQBcACIAIAAmACAASQBOAFQAKABEAGEAeQBPAGYAVwBlAGUAawApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAE8AUgBNAEEAVABfAEkAUwBPADgANgAwADEAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAGMAbwBtAHAAbABpAGMAYQB0AGkAbwBuAHMAIABhAHMAIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuAFwAbgBFAHgAYQBtAHAAbABlACAAZgBvAHIAbQBhAHQAcwAgACgAbgBvAHQAIABlAHgAaABhAHUAcwB0AGkAdgBlACkAOgAgAFkAWQBZAFkALQBNAE0ALQBEAEQAVABoAGgAOgBtAG0AOgBzAHMALgBzAHMAcwArAGgAaAA6AG0AbQA6AHMAcwAsACAAWQBZAFkAWQAtAFcAdwB3AC0ARABUAGgAaAA6AG0AbQBaACwAIABUAGgAaABtAG0AcwBzAFwAbgAjAFYAQQBMAFUARQAhACAAaQBmACAAYQBuACAAaQBuAHYAYQBsAGkAZAAgAGQAYQB0AGUALAAgAHQAaQBtAGUAIABvAHIAIAB0AGkAbQBlACAAegBvAG4AZQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAYQB0AGUAVAB5AHAAZQAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABEAGEAdABlACAAdAB5AHAAZQAgAHIAZQBwAHIAZQBzAGUAbgB0AGUAZAAgAGkAbgAgAEQAYQB0AGUAQQByAGcAMQAgAGEAbgBkACAARABhAHQAZQBBAHIAZwAyAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAAbgBvACAAZABhAHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAxACAALQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMgAgAC0AIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAHcAZQBlAGsAIABkAGEAdABlAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAFsARABhAHQAZQBBAHIAZwAxAF0AIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABNAG8AbgB0AGgAIABvAGYAIAB5AGUAYQByACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAxACAAIAAgACAAIAAgACAAIAAgADEALgAuADEAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAFcAZQBlAGsAIABvAGYAIAB5AGUAYQByACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAzACAAIAAgACAAIAAgACAAIAAgACAAMQAuAC4ANQAzAFwAbgBbAEQAYQB0AGUAQQByAGcAMgBdACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARABhAHkAIABvAGYAIABtAG8AbgB0AGgAIAB3AGgAZQBuACAARABhAHQAZQBUAHkAcABlACAAPQAgADEAIAAgACAAIAAgACAAIAAgACAAIAAxAC4ALgAzADEAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABPAHIAZABpAG4AYQBsACAAZABhAHkAIABvAGYAIAB5AGUAYQByACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAyACAAIAAgADEALgAuADMANgA2AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAARABhAHkAIABvAGYAIAB3AGUAZQBrACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAzACAAIAAgACAAIAAgACAAIAAgACAAIAAxAC4ALgA3AFwAbgBbAEgAbwB1AHIAXQAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMAAuAC4AMgA0AFwAbgBbAE0AaQBuAHUAdABlAF0AIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMAAuAC4ANQA5AFwAbgBbAFMAZQBjAG8AbgBkAF0AIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAMAAuAC4ANQA5AC4AOQA5ADkAXABuAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0AIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABUAGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAaQBuACAAbQBpAG4AdQB0AGUAcwAgAGYAcgBvAG0AIABVAFQAQwAgAC0AOQAwADAALgAuACsAOQAwADAAXABuAFsAQgBhAHMAaQBjAF0AIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABSAGUAdAB1AHIAbgAgAGkAbgAgAGIAYQBzAGkAYwAgAGYAbwByAG0AYQB0ACAAZQBnACAAWQBZAFkAWQBNAE0ARABEAFQAMQAwADQANQArADAAOQAzADAAXABuAFsAUwBpAGcAbgBlAGQAXQAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABBAGwAdwBhAHkAcwAgAHMAaQBnAG4AIAB5AGUAYQByACAAdgBhAGwAdQBlACAAZQBnACAAKwBZAFkAWQBZAC0ATQBNAC0ARABEAFwAbgBbAFAAcgBlAGMAaQBzAGkAbwBuAF0AIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUwBlAGwAZQBjAHQAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGwAZQB2AGUAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEEAdQB0AG8AbQBhAHQAaQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADEAIAAtACAAWQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgAE0AbwBuAHQAaAAvAFcAZQBlAGsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIABEAGEAeQAvAE8AcgBkAGkAbgBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANAAgAC0AIABIAG8AdQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADUAIAAtACAATQBpAG4AdQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANgAgAC0AIABTAGUAYwBvAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA3ACAALQAgAEYAcgBhAGMAdABpAG8AbgBhAGwAXABuAFsATgBvAFQAaQBtAGUAWgBvAG4AZQBdACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABEAHIAbwBwACAAdABpAG0AZQAgAHoAbwBuAGUAIABmAHIAbwBtACAAbwB1AHQAcAB1AHQALgBcAG4AWwBOAG8AWgB1AGwAdQBdACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAFUAcwBlACAAKwAwADAAOgAwADAAIABpAG4AcwB0AGUAYQBkACAAbwBmACAAWgAgAGYAbwByACAAVQBUAEMAIAB0AGkAbQBlACAAegBvAG4AZQAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBGAE8AUgBNAEEAVABfAEkAUwBPADgANgAwADEAIAA9ACAATABBAE0AQgBEAEEAKABcAG4AIAAgACAAIABEAGEAdABlAFQAeQBwAGUALABcAG4AIAAgACAAIABbAFkAZQBhAHIAQwBFAF0ALABcAG4AIAAgACAAIABbAEQAYQB0AGUAQQByAGcAMQBdACwAXABuACAAIAAgACAAWwBEAGEAdABlAEEAcgBnADIAXQAsAFwAbgAgACAAIAAgAFsASABvAHUAcgBdACwAXABuACAAIAAgACAAWwBNAGkAbgB1AHQAZQBdACwAXABuACAAIAAgACAAWwBTAGUAYwBvAG4AZABdACwAXABuACAAIAAgACAAWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAsAFwAbgAgACAAIAAgAFsAQgBhAHMAaQBjAF0ALABcAG4AIAAgACAAIABbAFMAaQBnAG4AZQBkAF0ALABcAG4AIAAgACAAIABbAFAAcgBlAGMAaQBzAGkAbwBuAF0ALABcAG4AIAAgACAAIABbAE4AbwBUAGkAbQBlAFoAbwBuAGUAXQAsAFwAbgAgACAAIAAgAFsATgBvAFoAdQBsAHUAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAVAB5AHAAZQAsACAATABFAFQAKABfAGQAdAAsACAATQBBAFgAKABJAE4AVAAoAE4AKABEAGEAdABlAFQAeQBwAGUAKQApACwAIAAwACkALAAgAEkARgAoAF8AZAB0ACAAPgAgADMALAAgADAALAAgAF8AZAB0ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBoAGEAcwBEAGEAdABlACwAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFQAeQBwAGUAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACAAKwAgAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB0AGUAQQByAGcAMQApACAAKwAgAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB0AGUAQQByAGcAMgApACkAIAA8AD4AIAAwAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBoAGEAcwBUAGkAbQBlACwAIAAoAEkAUwBOAFUATQBCAEUAUgAoAEgAbwB1AHIAKQAgACsAIABJAFMATgBVAE0AQgBFAFIAKABNAGkAbgB1AHQAZQApACAAKwAgAEkAUwBOAFUATQBCAEUAUgAoAFMAZQBjAG8AbgBkACkAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgAF8AaABhAHMAVABpAG0AZQBaAG8AbgBlACwAIABJAFMATgBVAE0AQgBFAFIAKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBzAGgAbwB3AFQAaQBtAGUAWgBvAG4AZQAsACAATgAoAE4AbwBUAGkAbQBlAFoAbwBuAGUAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIABfAGkAcwBFAG0AcAB0AHkALAAgAF8AaABhAHMARABhAHQAZQAgACsAIABfAGgAYQBzAFQAaQBtAGUAIAArACAAKABfAGgAYQBzAFQAaQBtAGUAWgBvAG4AZQAgACoAIABfAHMAaABvAHcAVABpAG0AZQBaAG8AbgBlACkAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAEUAbQBwAHQAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBoAGEAcwBEAGEAdABlACAAKgAgAF8AaABhAHMAVABpAG0AZQBaAG8AbgBlACAAKgAgAF8AcwBoAG8AdwBUAGkAbQBlAFoAbwBuAGUAKQAgACoAIABOAE8AVAAoAF8AaABhAHMAVABpAG0AZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACwAIABNAEEAWAAoAEkATgBUACgATgAoAFAAcgBlAGMAaQBzAGkAbwBuACkAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMARABhAHQAZQAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFQAeQBwAGUAIAA9ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAwACkAIAArACAAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPgA9ACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBPAFIATQBBAFQAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAEQAYQB0AGUAQQByAGcAMQAsACAARABhAHQAZQBBAHIAZwAyACwAIABCAGEAcwBpAGMALAAgAFMAaQBnAG4AZQBkACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAQgBhAHMAaQBjACwAIABTAGkAZwBuAGUAZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBPAFIATQBBAFQAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAEQAYQB0AGUAQQByAGcAMQAsACAAXAAiAFwAIgAsACAAQgBhAHMAaQBjACwAIABTAGkAZwBuAGUAZAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBUAHkAcABlACAAPQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADAAKQAgACsAIAAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA+AD0AIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAEQAYQB0AGUAQQByAGcAMgAsACAAQgBhAHMAaQBjACwAIABTAGkAZwBuAGUAZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBPAFIATQBBAFQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABcACIAXAAiACwAIABCAGEAcwBpAGMALAAgAFMAaQBnAG4AZQBkACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFQAeQBwAGUAIAA9ACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAwACkAIAArACAAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPgA9ACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBPAFIATQBBAFQAXwBXAEUARQBLAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABEAGEAdABlAEEAcgBnADEALAAgAEQAYQB0AGUAQQByAGcAMgAsACAAQgBhAHMAaQBjACwAIABTAGkAZwBuAGUAZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBPAFIATQBBAFQAXwBXAEUARQBLAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABCAGEAcwBpAGMALAAgAFMAaQBnAG4AZQBkACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAFcARQBFAEsAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAEQAYQB0AGUAQQByAGcAMQAsACAAXAAiAFwAIgAsACAAQgBhAHMAaQBjACwAIABTAGkAZwBuAGUAZAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAC8ALwBfAGQAYQB0AGUAVAB5AHAAZQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAVABpAG0AZQAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAwACkAIAArACAAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPgA9ACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8AVABJAE0ARQAoAEgAbwB1AHIALAAgAE0AaQBuAHUAdABlACwAIABTAGUAYwBvAG4AZAAsACAAQgBhAHMAaQBjACwAIABNAEEAWAAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAAtACAAMwAsACAAMAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBUAFoATwAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADAAKQAgACsAIAAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA+AD0AIAA0ACkAKQAgACoAIABfAGgAYQBzAFQAaQBtAGUAWgBvAG4AZQAgACoAIABfAHMAaABvAHcAVABpAG0AZQBaAG8AbgBlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBUAFoAcAByAGUAYwBpAHMAaQBvAG4ALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAANQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD4APQAgADYALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8AVABJAE0ARQBfAFoATwBOAEUAKABUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALAAgAEIAYQBzAGkAYwAsACAAMAAsACAATgBvAFoAdQBsAHUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAEQAYQB0AGUAIAAmACAAXwBzAFQAaQBtAGUAIAAmACAAXwBzAFQAWgBPAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEMATwBOAFYARQBSAFQAXwBUAE8AXwBEAEEAVABFAFwAbgBcAG4AQwBvAG4AdgBlAHIAdABzACAAdABlAHgAdAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQAIAB0AG8AIABhAG4AIABFAHgAYwBlAGwAIABkAGEAdABlAC4AIABcAG4AQwBvAGwAdQBtAG4AcwA6AFwAbgAgACAAMQAgAHwAIABFAHgAYwBlAGwAIABEAGEAdABlACAAIAAgACAAIAB8ACAAZABhAHQAZQAgACAAIAAgAHwAIAAxADkAMAAwAC0AMAAxAC0AMAAxAFQAMAAwADoAMAAwAC4ALgA5ADkAOQA5AC0AMQAyAC0AMwAxAFQAMgA0ADoAMAAwAFwAbgAgACAAMgAgAHwAIABNAGkAbgB1AHQAZQBzACAAbwBmAGYAcwBlAHQAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIAAtADkAMAAwAC4ALgArADkAMAAwAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVABlAHgAdAAgACAAIAAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAB8ACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQAdABlAGQAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlAC4AXABuAFsAUwB0AHIAaQBjAHQAXQAgACAAfAAgAHMAdwBpAHQAYwBoACAAfAAgAEUAbgBmAG8AcgBjAGUAIABzAHQAcgBpAGMAdAAgAEkAUwBPACAAOAA2ADAAMQAgAHAAYQByAHMAaQBuAGcAIAByAHUAbABlAHMALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AQwBPAE4AVgBFAFIAVABfAFQATwBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABUAGUAeAB0ACwAIABbAFMAdAByAGkAYwB0AF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACwAIABMAEEATQBCAEQAQQAoAF8AZQB4AGMAZQBwAHQAaQBvAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAAgAHwAIABuAHUAbABsACAAIABFAG0AcAB0AHkAIAB0AGUAeAB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE4ALwBBACAAIAAgAFUAbgBhAGIAbABlACAAdABvACAAcABhAHIAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE4AVQBNACAAIAAgAE8AdQB0ACAAbwBmACAARQB4AGUAbAAgAGQAYQB0AGUAIAByAGEAbgBnAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIATgAvAEEAXAAiACwAIAB7ACMATgAvAEEALAAgACMATgAvAEEAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQB4AGMAZQBwAHQAaQBvAG4AIAA9ACAAXAAiAE4AVQBNAFwAIgAsACAAewAjAE4AVQBNACEALAAgACMATgBVAE0AIQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAALwAvACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgB9AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABUAGUAeAB0ACAAPQAgAFwAIgBcACIALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwB0AHIAaQBjAHQALAAgAE4AKABTAHQAcgBpAGMAdAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBsAGUAbQBlAG4AdABzACwAIABQAEEAUgBTAEUAXwBJAFMATwA4ADYAMAAxACgAVABlAHgAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBzAHQAcgBpAGMAdAAgACoAIAAoAEkATgBEAEUAWAAoAF8AZQBsAGUAbQBlAG4AdABzACwAIAAxACAALAAgADEAKQAgAD0AIABGAEEATABTAEUAKQAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAEQAYQB0AGUALAAgAEIASQBUAEEATgBEACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADIAKQAsACAANAApACAAPQAgADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABOACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADYAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AaABhAHMARABhAHQAZQAgACoAIAAoACgAXwB5AGUAYQByACAAPAAgADEAOQAwADAAKQAgACsAIAAoAF8AeQBlAGEAcgAgAD4AIAA5ADkAOQA5ACkAKQAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4AVQBNAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAVAB5AHAAZQAsACAASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlACwAIABJAEYAKABfAGgAYQBzAEQAYQB0AGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABfAGQAYQB0AGUAVAB5AHAAZQAgAD0AIAAxACwAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEQAQQBUAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AKABJAE4ARABFAFgAKABfAGUAbABlAG0AZQBuAHQAcwAsACAAMQAsACAANwApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAEkATgBEAEUAWAAoAF8AZQBsAGUAbQBlAG4AdABzACwAIAAxACwAIAA4ACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAVAB5AHAAZQAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMARABhAHQAZQAsACAARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACgAXwB5AGUAYQByACwAIABOACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADgAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARABBAFQARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AYwBEAGEAdABlACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGMARABhAHQAZQAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBjAEQAYQB0AGUALAAgADEALAAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAVAB5AHAAZQAgAD0AIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMARABhAHQAZQAsACAARgBSAE8ATQBfAFcARQBFAEsAXwBEAEEAVABFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAEkATgBEAEUAWAAoAF8AZQBsAGUAbQBlAG4AdABzACwAIAAxACwAIAA3ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AKABJAE4ARABFAFgAKABfAGUAbABlAG0AZQBuAHQAcwAsACAAMQAsACAAOAApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARABBAFQARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AYwBEAGEAdABlACwAIAAxACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGMARABhAHQAZQAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBjAEQAYQB0AGUALAAgADEALAAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAFQAaQBtAGUALAAgAEIASQBUAEEATgBEACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADIAKQAsACAAMgApACAAPQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQAsACAASQBGACgAXwBoAGEAcwBUAGkAbQBlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQASQBNAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAEkATgBEAEUAWAAoAF8AZQBsAGUAbQBlAG4AdABzACwAIAAxACwAIAAxADAAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAEkATgBEAEUAWAAoAF8AZQBsAGUAbQBlAG4AdABzACwAIAAxACwAIAAxADEAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZAB0ACwAIABfAGQAYQB0AGUAIAArACAAXwB0AGkAbQBlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAFQAWgAsACAAKABCAEkAVABBAE4ARAAoAEkATgBEAEUAWAAoAF8AZQBsAGUAbQBlAG4AdABzACwAIAAxACwAIAAyACkALAAgADEAKQAgAD0AIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8ALAAgAEkARgAoAF8AaABhAHMAVABaACwAIABJAE4ARABFAFgAKABfAGUAbABlAG0AZQBuAHQAcwAsACAAMQAsACAAMQAyACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAGQAdAAsACAAXwB0AHoAbwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEMATwBOAFYARQBSAFQAXwBGAFIATwBNAF8ARABBAFQARQBcAG4AXABuAEMAbwBuAHYAZQByAHQAcwAgAGEAbgAgAEUAeABjAGUAbAAgAGQAYQB0AGUAIAB0AG8AIABJAFMATwAgAGYAbwByAG0AYQB0AHQAZQBkACAAdABlAHgAdAAuAFwAbgBFAHgAYQBtAHAAbABlACAAZgBvAHIAbQBhAHQAcwAgACgAbgBvAHQAIABlAHgAaABhAHUAcwB0AGkAdgBlACkAOgAgAFkAWQBZAFkALQBNAE0ALQBEAEQAVABoAGgAOgBtAG0AOgBzAHMALgBzAHMAcwArAGgAaAA6AG0AbQA6AHMAcwAsACAAWQBZAFkAWQAtAFcAdwB3AC0ARABUAGgAaAA6AG0AbQBaACwAIABUAGgAaABtAG0AcwBzAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGEAdABlACAAIAAgACAAfAAgAEEAbgAgAEUAeABjAGUAbAAgAGQAYQB0AGUAIABhAG4AZAAvAG8AcgAgAHQAaQBtAGUALgBcAG4AWwBUAGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQAXQAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAZgByAG8AbQAgAFUAVABDACAALQA5ADAAMAAuAC4AKwA5ADAAMAAgAFwAbgBbAEIAYQBzAGkAYwBdACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAUgBlAHQAdQByAG4AIABpAG4AIABiAGEAcwBpAGMAIABmAG8AcgBtAGEAdAAgAGUAZwAgAFkAWQBZAFkATQBNAEQARABUAGgAaABtAG0AKwBoAGgAXABuAFsAUwBpAGcAbgBlAGQAXQAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABBAGwAdwBhAHkAcwAgAHMAaQBnAG4AIAB5AGUAYQByACAAdgBhAGwAdQBlACAAZQBnACAAKwBZAFkAWQBZAC0ATQBNAC0ARABEAFwAbgBbAFAAcgBlAGMAaQBzAGkAbwBuAF0AIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUwBlAGwAZQBjAHQAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGwAZQB2AGUAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAEEAdQB0AG8AbQBhAHQAaQBjAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADEAIAAtACAAWQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAyACAALQAgAE0AbwBuAHQAaAAvAFcAZQBlAGsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIABEAGEAeQAvAE8AcgBkAGkAbgBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANAAgAC0AIABIAG8AdQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADUAIAAtACAATQBpAG4AdQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANgAgAC0AIABTAGUAYwBvAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA3ACAALQAgAEYAcgBhAGMAdABpAG8AbgBhAGwAXABuAFsATgBvAFQAaQBtAGUAWgBvAG4AZQBdACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABEAHIAbwBwACAAdABpAG0AZQAgAHoAbwBuAGUAIABmAHIAbwBtACAAbwB1AHQAcAB1AHQALgBcAG4AWwBOAG8AWgB1AGwAdQBdACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAFUAcwBlACAAKwAwADAAOgAwADAAIABpAG4AcwB0AGUAYQBkACAAbwBmACAAWgAgAGYAbwByACAAVQBUAEMAIAB0AGkAbQBlACAAegBvAG4AZQAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBDAE8ATgBWAEUAUgBUAF8ARgBSAE8ATQBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABEAGEAdABlACwAIABbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACwAIABbAEIAYQBzAGkAYwBdACwAIABbAFMAaQBnAG4AZQBkAF0ALAAgAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAsACAAWwBOAG8AVABpAG0AZQBaAG8AbgBlAF0ALAAgAFsATgBvAFoAdQBsAHUAXQAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAdABlACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAGEAcwBEAGEAdABlACwAIABJAE4AVAAoAE4AKABEAGEAdABlACkAIAA8AD4AIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByACwAIABJAEYAKABfAGgAYQBzAEQAYQB0AGUALAAgAFkARQBBAFIAKABEAGEAdABlACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAASQBGACgAXwBoAGEAcwBEAGEAdABlACwAIABNAE8ATgBUAEgAKABEAGEAdABlACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABJAEYAKABfAGgAYQBzAEQAYQB0AGUALAAgAEQAQQBZACgARABhAHQAZQApACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AFMAZQBjADEALAAgAFIATwBVAE4ARAAoACgARABhAHQAZQAgAC0AIABJAE4AVAAoAE4AKABEAGEAdABlACkAKQApACAAKgAgADgANgA0ADAAMAAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgAsACAASQBOAFQAKABfAHQAUwBlAGMAMQAgAC8AIAAzADYAMAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AFMAZQBjADIALAAgAF8AdABTAGUAYwAxACAALQAgACgAXwBoAG8AdQByACAAKgAgADMANgAwADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlACwAIABJAE4AVAAoAF8AdABTAGUAYwAyACAALwAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQALAAgAF8AdABTAGUAYwAyACAALQAgACgAXwBtAGkAbgB1AHQAZQAgACoAIAA2ADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAEkAUwBPADgANgAwADEAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgAXwBoAGEAcwBEAGEAdABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEIAYQBzAGkAYwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFMAaQBnAG4AZQBkACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUAByAGUAYwBpAHMAaQBvAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAG8AVABpAG0AZQBaAG8AbgBlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBvAFoAdQBsAHUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbACIASQBTAE8AXwA4ADYAMAAxAC4ASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgAiACwAIgBJAFMATwBfADgANgAwADEALgBJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAiACwAIgBJAFMATwBfADgANgAwADEALgBJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQBfAFoATwBOAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ASQBTAF8AVgBBAEwASQBEAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ASQBTAF8AVgBBAEwASQBEAF8AVwBFAEUASwBfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AWQBFAEEAUgBfAEQAQQBZAF8AQwBPAFUATgBUACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAFkARQBBAFIAXwBXAEUARQBLAF8AQwBPAFUATgBUACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEQAQQBZAF8ATwBSAEQASQBOAEEATAAiACwAIgBJAFMATwBfADgANgAwADEALgBGAFIATwBNAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ARABBAFkAXwBPAEYAXwBXAEUARQBLACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEQAQQBZAF8ATwBGAF8AVwBFAEUASwBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAFcARQBFAEsAXwBOAFUATQBCAEUAUgAiACwAIgBJAFMATwBfADgANgAwADEALgBXAEUARQBLAF8ATgBVAE0AQgBFAFIAXwBGAFIATwBNAF8ATwBSAEQASQBOAEEATAAiACwAIgBJAFMATwBfADgANgAwADEALgBUAE8AXwBXAEUARQBLAF8ARABBAFQARQAiACwAIgBJAFMATwBfADgANgAwADEALgBGAFIATwBNAF8AVwBFAEUASwBfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AVgBBAEwASQBEAEEAVABFAF8AQwBIAEEAUgBBAEMAVABFAFIAUwAiACwAIgBJAFMATwBfADgANgAwADEALgBQAEEAUgBTAEUAXwBEAEEAVABFACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAFAAQQBSAFMARQBfAFQASQBNAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AUABBAFIAUwBFAF8AVABJAE0ARQBfAFoATwBOAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AUABBAFIAUwBFAF8AUABBAFIAVABTACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAFAAQQBSAFMARQBfAEkAUwBPADgANgAwADEAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ARgBPAFIATQBBAFQAXwBEAEEAVABFACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEYATwBSAE0AQQBUAF8AVABJAE0ARQAiACwAIgBJAFMATwBfADgANgAwADEALgBGAE8AUgBNAEEAVABfAFQASQBNAEUAXwBaAE8ATgBFACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEYATwBSAE0AQQBUAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ARgBPAFIATQBBAFQAXwBXAEUARQBLAF8ARABBAFQARQAiACwAIgBJAFMATwBfADgANgAwADEALgBGAE8AUgBNAEEAVABfAEkAUwBPADgANgAwADEAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AQwBPAE4AVgBFAFIAVABfAFQATwBfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AQwBPAE4AVgBFAFIAVABfAEYAUgBPAE0AXwBEAEEAVABFACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIARABNAFkAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAiAH0ALAB7ACIAcABhAHQAaAAiADoAIgAvAHAAcgBvAGoAZQBjAHQAcwAvAEkAUwBPAF8AOAA2ADAAMQAiACwAIgB0AGUAeAB0ACIAOgAiAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABJAFMATwBfADgANgAwADEAIAB2ADEAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAIAAgACAAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABUAGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAHMAdABhAG4AZABhAHIAZAAgAGQAZQBmAGkAbgBlAHMAIABhACAAdQBuAGkAdgBlAHIAcwBhAGwAIABuAG8AdABhAHQAaQBvAG4AIABvAGYAIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlAHMALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABEAGEAdABlAHMAIABhAHIAZQAgAGkAbgAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIAIABhAG4AZAAgAHQAaQBtAGUAcwAgAGEAcgBlACAAYgBhAHMAZQBkACAAbwBuACAAdABoAGUAIAAyADQAIABoAG8AdQByACAAdABpAG0AZQBrAGUAZQBwAGkAbgBnACAAcwB5AHMAdABlAG0AIAB3AGkAdABoACAAYQBuACAAIAAgACAAIAAgACMAXABuACMAIABvAHAAdABpAG8AbgBhAGwAIAB0AGkAbQBlACAAegBvAG4AZQAgAG8AZgBmAHMAZQB0ACAAZgByAG8AbQAgAFUAVABDAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABNAG8AZAB1AGwAZQAgAEQAZQBwAGUAbgBkAGUAbgBjAGkAZQBzADoAIABOAG8AbgBlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABMAG8AZwBpAGMAYQBsACAARgB1AG4AYwB0AGkAbwBuAHMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBZAEUAQQBSACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQBzAHQAcwAgAGkAZgAgAGEAIAB5AGUAYQByACAAaQBzACAAdgBhAGwAaQBkACAAZgBvAHIAIABJAFMATwAgADgANgAwADEALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAIABcAG4AIwAgAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAHkAZQBhAHIAIABpAG4AYwBsAHUAZABlAHMAIABhACAAbABlAGEAcAAgAGQAYQB5ACAAaQBuACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAYQAgAGQAYQB0AGUAIABpAHMAIAB2AGEAbABpAGQAIABmAG8AcgAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwAgAFwAbgAjACAASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAGUAcwB0AHMAIABpAGYAIABhACAAdABpAG0AZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIAAyADQAIABoAG8AdQByACAAdABpAG0AZQBrAGUAZQBwAGkAbgBnACAAcwB5AHMAdABlAG0ALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjACAAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBUAEkATQBFAF8AWgBPAE4ARQAgACAAIAAgACAAIAAgAFQAZQBzAHQAcwAgAGkAZgAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAaQBzACAAaQBuACAAdgBhAGwAaQBkACAAcgBhAG4AZwBlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAgACAAIAAgAFQAZQBzAHQAcwAgAGkAZgAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlACAAaQBzACAAdgBhAGwAaQBkACAAZgBvAHIAIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIABJAFMAXwBWAEEATABJAEQAXwBXAEUARQBLAF8ARABBAFQARQAgACAAIAAgACAAIAAgAFQAZQBzAHQAcwAgAGkAZgAgAGEAIAB3AGUAZQBrACAAZABhAHQAZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAIABcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEMAYQBsAGUAbgBkAGEAcgAgAEYAdQBuAGMAdABpAG8AbgBzACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACAAIwBcAG4AIwAgAFkARQBBAFIAXwBEAEEAWQBfAEMATwBVAE4AVAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBvAHUAbgB0ACAAbwBmACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5AHMAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIAB5AGUAYQByAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFkARQBBAFIAXwBXAEUARQBLAF8AQwBPAFUATgBUACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAYwBvAHUAbgB0ACAAbwBmACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawBzACAAaQBuACAAYQAgAGcAaQB2AGUAbgAgAHkAZQBhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEQAQQBZAF8ATwBSAEQASQBOAEEATAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbgB1AG0AYgBlAHIAIABvAGYAIABhACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIALgAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAZgByAG8AbQAgAGEAIABnAGkAdgBlAG4AIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABkAGEAdABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABmAG8AcgAgAGEAIABnAGkAdgBlAG4AIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAuACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFcARQBFAEsAXwBOAFUATQBCAEUAUgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFcARQBFAEsAXwBOAFUATQBCAEUAUgBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAbwBmACAAYQAgAGcAaQB2AGUAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFQATwBfAFcARQBFAEsAXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAASQBTAE8AIABkAGUAZgBpAG4AZQBkACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAYQBuAGQAIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgAGQAYQB0AGUALgAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYAUgBPAE0AXwBXAEUARQBLAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAZQBpAHQAaABlAHIAIABhACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlACAAbwByACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAIABmAHIAbwBtACAAYQAgAGcAaQB2AGUAbgAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdwBlAGUAawAgAGEAbgBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFAAYQByAHMAaQBuAGcAIABGAHUAbgBjAHQAaQBvAG4AcwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACAAIwBcAG4AIwAgAFYAQQBMAEkARABBAFQARQBfAEMASABBAFIAQQBDAFQARQBSAFMAIAAgACAAIAAgACAAVABlAHMAdABzACAAaQBmACAAdABlAHgAdAAgAGMAbwBuAHQAYQBpAG4AcwAgAG8AbgBsAHkAIABjAGgAYQByAGEAYwB0AGUAcgBzACAAdABoAGEAdAAgAGEAcgBlACAAdgBhAGwAaQBkACAAZgBvAHIAIABJAFMATwAgADgANgAwADEALgAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeQBlAGEAcgAsACAAbQBvAG4AdABoACAAYQBuAGQAIABkAGEAeQAgAG8AZgAgAGEAIABkAGEAdABlACAAZgByAG8AbQAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AIAAgACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAFQASQBNAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAaABvAHUAcgAsACAAbQBpAG4AdQB0AGUAIABhAG4AZAAgAHMAZQBjAG8AbgBkACAAbwBmACAAdABpAG0AZQAgAGYAcgBvAG0AIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAFQASQBNAEUAXwBaAE8ATgBFACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAFAAQQBSAFQAUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUwBwAGwAaQB0AHMAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAB0AGUAZAAgAHQAZQB4AHQAIAB2AGEAbAB1AGUAIABpAG4AdABvACAAaQBuAHQAbwAgAHIAZQBzAHAAZQBjAHQAaQB2AGUAIABwAGEAcgB0AHMAIABvAGYAIABkAGEAdABlACwAIAAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAdABpAG0AZQAgAGEAbgBkACAAdABpAG0AZQAgAHoAbwBuAGUALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAFAAQQBSAFMARQBfAEkAUwBPADgANgAwADEAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAgAGMAbwBtAHAAbABpAGMAYQB0AGkAbwBuAHMAIABmAHIAbwBtACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYAbwByAG0AYQB0AHQAaQBuAGcAIABGAHUAbgBjAHQAaQBvAG4AcwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIABkAGEAdABlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8AVABJAE0ARQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIAB0AGkAbQBlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8AVABJAE0ARQBfAFoATwBOAEUAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIAB0AGkAbQBlACAAegBvAG4AZQAgAGEAcwAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8AVwBFAEUASwBfAEQAQQBUAEUAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIAB3AGUAZQBrACAAZABhAHQAZQAgAGEAcwAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEYATwBSAE0AQQBUAF8ASQBTAE8AOAA2ADAAMQAgACAAIAAgACAAIAAgACAAIAAgACAAUgBlAHQAdQByAG4AcwAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABjAG8AbQBwAGwAaQBjAGEAdABpAG8AbgBzACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEMAbwBuAHYAZQByAHMAaQBvAG4AIABGAHUAbgBjAHQAaQBvAG4AcwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACAAIwBcAG4AIwAgAEMATwBOAFYARQBSAFQAXwBUAE8AXwBEAEEAVABFACAAIAAgACAAIAAgACAAIAAgACAAQwBvAG4AdgBlAHIAdABzACAAdABlAHgAdAAgAGkAbgAgAEkAUwBPACAAZgBvAHIAbQBhAHQAIAB0AG8AIABhAG4AIABFAHgAYwBlAGwAIABkAGEAdABlAC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgAEMATwBOAFYARQBSAFQAXwBGAFIATwBNAF8ARABBAFQARQAgACAAIAAgACAAIAAgACAAQwBvAG4AdgBlAHIAdABzACAAYQBuACAARQB4AGMAZQBsACAAZABhAHQAZQAgAHQAbwAgAEkAUwBPACAAZgBvAHIAbQBhAHQAdABlAGQAIAB0AGUAeAB0AC4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgBcAG4AXABuAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABMAE8ARwBJAEMAQQBMACAARgBVAE4AQwBUAEkATwBOAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAqAC8AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgBcAG4AXABuAFQAZQBzAHQAcwAgAGkAZgAgAGEAIAB5AGUAYQByACAAaQBzACAAdgBhAGwAaQBkACAAZgBvAHIAIABJAFMATwAgADgANgAwADEALgAgAE4AbwB0AGUAIAB0AGgAYQB0ACAAMQAgAEIAQwAgAD0AIAAwACAAQwBFACwAIAAyACAAQgBDACAAPQAgAC0AMQAgAEMARQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABiAG8AbwBsAGUAYQBuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAFsAQQBsAGwAbwB3AEQAZQBjAGkAbQBhAGwAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEEAbABsAG8AdwAgAGQAZQBjAGkAbQBhAGwAIAB2AGEAbAB1AGUAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBfAFYAQQBMAEkARABfAFkARQBBAFIAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAAWwBBAGwAbABvAHcARABlAGMAaQBtAGEAbABdACwAXABuACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACwAXABuACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACgATgAoAEEAbABsAG8AdwBEAGUAYwBpAG0AYQBsACkAIAA9ACAAMAApACAAKgAgACgAWQBlAGEAcgBDAEUAIAA8AD4AIABJAE4AVAAoAFkAZQBhAHIAQwBFACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIABBAEIAUwAoAFkAZQBhAHIAQwBFACkAIAA8ACAAMQAwADAAMAAwADAAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAF8ATABFAEEAUABfAFkARQBBAFIAXABuAFwAbgBUAGUAcwB0AHMAIABpAGYAIABhACAAeQBlAGEAcgAgAGkAbgBjAGwAdQBkAGUAcwAgAGEAIABsAGUAYQBwACAAZABhAHkAIABpAG4AIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGIAbwBvAGwAZQBhAG4AIAB8ACAAIwBWAEEATABVAEUAIQAgAGkAZgAgAG4AbwB0ACAAYQAgAHYAYQBsAGkAZAAgAHkAZQBhAHIALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE0ATwBEACgAXwB5AGUAYQByAEMARQAsACAANAAwADAAKQAgAD0AIAAwACwAIABUAFIAVQBFACwAIABJAEYAKABNAE8ARAAoAF8AeQBlAGEAcgBDAEUALAAgADEAMAAwACkAIAA9ACAAMAAsACAARgBBAEwAUwBFACwAIABNAE8ARAAoAF8AeQBlAGEAcgBDAEUALAAgADQAKQAgAD0AIAAwACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQBcAG4AXABuAFQAZQBzAHQAcwAgAGkAZgAgAGEAIABkAGEAdABlACAAaQBzACAAdgBhAGwAaQBkACAAZgBvAHIAIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByAC4AXABuAEkAZgAgAG0AbwBuAHQAaAAgAGEAbgBkACAAZABhAHkAIABtAGkAcwBzAGkAbgBnACwAIABjAG8AbgBzAGkAZABlAHIAZQBkACAAYQAgAHkAZQBhAHIAIABvAG4AbAB5ACAAZABhAHQAZQAuAFwAbgBJAGYAIABvAG4AbAB5ACAAZABhAHkAIABpAHMAIABtAGkAcwBzAGkAbgBnACwAIABjAG8AbgBzAGkAZABlAHIAZQBkACAAYQAgAHkAZQBhAHIAIABhAG4AZAAgAG0AbwBuAHQAaAAgAGQAYQB0AGUALgBcAG4ATwBuAGwAeQAgAHQAaABlACAAbABhAHMAdAAgAHAAcgBvAHYAaQBkAGUAZAAgAGUAbABlAG0AZQBuAHQAIABjAGEAbgAgAGgAYQB2AGUAIABhACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHYAYQBsAHUAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABiAG8AbwBsAGUAYQBuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAE0AbwBuAHQAaAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAE0AbwBuAHQAaAAgAG8AZgAgAHkAZQBhAHIAXABuAEQAYQB5ACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAYQB5ACAAbwBmACAAbQBvAG4AdABoAFwAbgBbAEEAbABsAE0AYQBuAGQAYQB0AG8AcgB5AF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABEAGkAcwBhAGwAbABvAHcAIABzAGgAbwByAHQAIABmAG8AcgBtAHMAOgAgAFkAZQBhAHIALAAgAFkAZQBhAHIAIABhAG4AZAAgAE0AbwBuAHQAaABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIABbAEEAbABsAE0AYQBuAGQAYQB0AG8AcgB5AF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAXwBlAGwAZQBtAGUAbgB0AHMALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABNAG8AbgB0AGgAKQApACAAKgAgAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkAIAAqACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBlAGwAZQBtAGUAbgB0AHMAIAA9ACAAMAApACAAKwAgACgAKABOACgAQQBsAGwATQBhAG4AZABhAHQAbwByAHkAKQAgADwAPgAgADAAKQAgACoAIAAoAF8AZQBsAGUAbQBlAG4AdABzACAAPAAgADMAKQApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHkAZQBhAHIAIABpAHMAIABtAGEAbgBkAGEAdABvAHIAeQAsACAAYQBuAGQAIABhAGwAbAAgAGUAbABlAG0AZQBuAHQAcwAgAG0AYQBuAGQAYQB0AG8AcgB5ACAAaQBmACAAQQBsAGwATQBhAG4AZABhAHQAbwByAHkAIABzAHcAaQB0AGMAaAAgAGkAcwAgAHMAZQB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAbABlAG0AZQBuAHQAcwAgAD0AIAAzACwAIAAvAC8AIAB5AGUAYQByACwAIABtAG8AbgB0AGgAIABhAG4AZAAgAGQAYQB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAG8AbgB0AGgAIAA8AD4AIABJAE4AVAAoAE0AbwBuAHQAaAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG0AbwBuAHQAaAAgAGMAYQBuAG4AbwB0ACAAYgBlACAAZgByAGEAYwB0AGkAbwBuAGEAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABmAG8AcgAgAG0AbwBuAHQAaAAgAHIAYQBuAGcAZQAgADEALgAuADEAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKAAoAE0AbwBuAHQAaAAgAD4APQAgADEAKQAgACoAIAAoAE0AbwBuAHQAaAAgADwAPQAgADEAMgApACkAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB5ACwAIABJAE4AVAAoAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgATQBvAG4AdABoACAAPQAgADIAKQAsACAALwAvACAARgBlAGIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAGQAYQB5ACAAPgA9ACAAMQApACAAKgAgACgAXwBkAGEAeQAgADwAPQAgACgAMgA4ACAAKwAgAE4AKABJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACkAKQApACkAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABNAG8AbgB0AGgAIAA8AD0AIAA3ACkALAAgAC8ALwAgAEoAYQBuACwAIABNAGEAcgAsACAAQQBwAHIALAAgAE0AYQB5ACwAIABKAHUAbgAsACAASgB1AGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAGQAYQB5ACAAPgA9ACAAMQApACAAKgAgACgAXwBkAGEAeQAgADwAPQAgACgAMwAwACAAKwAgAE0ATwBEACgATQBvAG4AdABoACwAIAAyACkAKQApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgATQBvAG4AdABoACAAPgA9ACAAOAApACwAIAAvAC8AIABBAHUAZwAsACAAUwBlAHAALAAgAE8AYwB0ACwAIABOAG8AdgAsACAARABlAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBkAGEAeQAgAD4APQAgADEAKQAgACoAIAAoAF8AZABhAHkAIAA8AD0AIAAoADMAMQAgAC0AIABNAE8ARAAoAE0AbwBuAHQAaAAsACAAMgApACkAKQAgADwAPgAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAbABlAG0AZQBuAHQAcwAgAD0AIAAyACwAIAAvAC8AIAB5AGUAYQByACAAYQBuAGQAIABtAG8AbgB0AGgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFkARQBBAFIAKABZAGUAYQByAEMARQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAEkATgBUACgATQBvAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAGYAbwByACAAbQBvAG4AdABoACAAcgBhAG4AZwBlACAAMQAuAC4AMQAyAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBtAG8AbgB0AGgAIAA+AD0AIAAxACkAIAAqACAAKABfAG0AbwBuAHQAaAAgADwAPQAgADEAMgApACkAIAA8AD4AIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAGwAZQBtAGUAbgB0AHMAIAA9ACAAMQAsACAALwAvACAAeQBlAGEAcgAgAG8AbgBsAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACwAIAAxACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAXABuAFwAbgBUAGUAcwB0AHMAIABpAGYAIABhACAAdABpAG0AZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIAAyADQAIABoAG8AdQByACAAdABpAG0AZQBrAGUAZQBwAGkAbgBnACAAcwB5AHMAdABlAG0ALgBcAG4ATwBuAGwAeQAgAHQAaABlACAAbABhAHMAdAAgAHAAcgBvAHYAaQBkAGUAZAAgAGUAbABlAG0AZQBuAHQAIABjAGEAbgAgAGgAYQB2AGUAIABhACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHYAYQBsAHUAZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABiAG8AbwBsAGUAYQBuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ASABvAHUAcgAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAMAAuAC4AMgA0AFwAbgBNAGkAbgB1AHQAZQAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIAAwAC4ALgA1ADkALgA5ADkAOQBcAG4AUwBlAGMAbwBuAGQAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAMAAuAC4ANQA5AC4AOQA5ADkAXABuAFsAQQBsAGwATQBhAG4AZABhAHQAbwByAHkAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEQAaQBzAGEAbABsAG8AdwAgAHMAaABvAHIAdAAgAGYAbwByAG0AcwA6ACAASABvAHUAcgAsACAASABvAHUAcgAgAGEAbgBkACAATQBpAG4AdQB0AGUAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAIAA9ACAATABBAE0AQgBEAEEAKABIAG8AdQByACwAIABNAGkAbgB1AHQAZQAsACAAUwBlAGMAbwBuAGQALAAgAFsAQQBsAGwATQBhAG4AZABhAHQAbwByAHkAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABfAGUAbABlAG0AZQBuAHQAcwAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABIAG8AdQByACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQApACAAKgAgAEkAUwBOAFUATQBCAEUAUgAoAFMAZQBjAG8AbgBkACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AaQBuAHUAdABlACkAKQAgACoAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFMAZQBjAG8AbgBkACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgAUwBlAGMAbwBuAGQAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAGUAbABlAG0AZQBuAHQAcwAgAD0AIAAwACkAIAArACAAKAAoAE4AKABBAGwAbABNAGEAbgBkAGEAdABvAHIAeQApACAAPAA+ACAAMAApACAAKgAgACgAXwBlAGwAZQBtAGUAbgB0AHMAIAA8ACAAMwApACkAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAaABvAHUAcgAgAGkAcwAgAG0AYQBuAGQAYQB0AG8AcgB5ACwAIABhAG4AZAAgAGEAbABsACAAZQBsAGUAbQBlAG4AdABzACAAbQBhAG4AZABhAHQAbwByAHkAIABpAGYAIABBAGwAbABNAGEAbgBkAGEAdABvAHIAeQAgAHMAdwBpAHQAYwBoACAAaQBzACAAcwBlAHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBsAGUAbQBlAG4AdABzACAAPQAgADMALAAgAC8ALwAgAGgAbwB1AHIALAAgAG0AaQBuAHUAdABlACwAIABzAGUAYwBvAG4AZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZABYACwAIABSAE8AVQBOAEQARABPAFcATgAoAFMAZQBjAG8AbgBkACAAKgAgADEAMAAwADAAMAAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGUAcwB0ACAAaABvAHUAcgAgAGkAcwAgAG4AbwB0ACAAZgByAGEAYwB0AGkAbwBuAGEAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABvAHUAcgAgADwAPgAgAEkATgBUACgASABvAHUAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAGgAbwB1AHIAIABpAG4AIAByAGEAbgBnAGUAIAAwAC4ALgAyADQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABIAG8AdQByACAAPgA9ACAAMAApACAAKgAgACgASABvAHUAcgAgADwAPQAgADIANAApACkAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABtAGkAbgB1AHQAZQAgAGkAcwAgAG4AbwB0ACAAZgByAGEAYwB0AGkAbwBuAGEAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATQBpAG4AdQB0AGUAIAA8AD4AIABJAE4AVAAoAE0AaQBuAHUAdABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGUAcwB0ACAAbQBpAG4AdQB0AGUAIABpAG4AIAByAGEAbgBnAGUAIAAwAC4ALgA1ADkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABNAGkAbgB1AHQAZQAgAD4APQAgADAAKQAgACoAIAAoAE0AaQBuAHUAdABlACAAPAA9ACAANQA5ACkAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAHoAZQByAG8AIABtAGkAbgB1AHQAZQAgAGEAbgBkACAAcwBlAGMAbwBuAGQAIABmAG8AcgAgADIANAAgAGgAbwB1AHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABIAG8AdQByACAAPQAgADIANAApACAAKgAgACgAKABNAGkAbgB1AHQAZQAgADwAPgAgADAAKQAgACsAIAAoAF8AcwBlAGMAbwBuAGQAWAAgADwAPgAgADAAKQApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAHMAZQBjAG8AbgBkACAAaQBuACAAcgBhAG4AZwBlACAAMAAuAC4ANQA5AC4AOQA5ADkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAHMAZQBjAG8AbgBkAFgAIAA+AD0AIAAwACkAIAAqACAAKABfAHMAZQBjAG8AbgBkAFgAIAA8ACAANgAwADAAMAAwADAAKQApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQBsAGUAbQBlAG4AdABzACAAPQAgADIALAAgAC8ALwAgAGgAbwB1AHIAIABhAG4AZAAgAG0AaQBuAHUAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlAFgALAAgAFIATwBVAE4ARABEAE8AVwBOACgATQBpAG4AdQB0AGUAIAAqACAANgAwADAAMAAwADAALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABlAHMAdAAgAGgAbwB1AHIAIABpAHMAIABuAG8AdAAgAGYAcgBhAGMAdABpAG8AbgBhAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAbwB1AHIAIAA8AD4AIABJAE4AVAAoAEgAbwB1AHIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABoAG8AdQByACAAaQBuACAAcgBhAG4AZwBlACAAMAAuAC4AMgA0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgASABvAHUAcgAgAD4APQAgADAAKQAgACoAIAAoAEgAbwB1AHIAIAA8AD0AIAAyADQAKQApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGUAcwB0ACAAegBlAHIAbwAgAG0AaQBuAHUAdABlACAAZgBvAHIAIAAyADQAIABoAG8AdQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgASABvAHUAcgAgAD0AIAAyADQAKQAgACoAIAAoAF8AbQBpAG4AdQB0AGUAWAAgADwAPgAgADAAKQApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABtAGkAbgB1AHQAZQAgAGkAbgAgAHIAYQBuAGcAZQAgADAALgAuADUAOQAuADkAOQA5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBtAGkAbgB1AHQAZQBYACAAPgA9ACAAMAApACAAKgAgACgAXwBtAGkAbgB1AHQAZQBYACAAPAAgADMANgAwADAAMAAwADAAMAApACkAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAGwAZQBtAGUAbgB0AHMAIAA9ACAAMQAsACAALwAvACAAaABvAHUAcgAgAG8AbgBsAHkAIAB0AGkAbQBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIAWAAsACAAUgBPAFUATgBEAEQATwBXAE4AKABIAG8AdQByACAAKgAgADMANgAwADAAMAAwADAAMAAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGUAcwB0ACAAaABvAHUAcgAgAGkAbgAgAHIAYQBuAGcAZQAgADAALgAuADIANABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAGgAbwB1AHIAWAAgAD4APQAgADAAKQAgACoAIAAoAF8AaABvAHUAcgBYACAAPAA9ACAAOAA2ADQAMAAwADAAMAAwADAAKQApACAAPAA+ACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMAXwBWAEEATABJAEQAXwBUAEkATQBFAF8AWgBPAE4ARQBcAG4AXABuAFQAZQBzAHQAcwAgAGkAZgAgAHQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABpAG4AIABtAGkAbgB1AHQAZQBzACAAaQBzACAAaQBuACAAdgBhAGwAaQBkACAAcgBhAG4AZwBlAC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAGIAbwBvAGwAZQBhAG4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBPAGYAZgBzAGUAdABNAGkAbgB1AHQAZQBzACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAUgBhAG4AZwBlACAAaQBzACAALQA5ADAAMAAuAC4AKwA5ADAAMAAgAC0APgAgAC0AMQA1ADoAMAAwAC4ALgArADEANQA6ADAAMABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQBfAFoATwBOAEUAIAA9ACAATABBAE0AQgBEAEEAKABPAGYAZgBzAGUAdABNAGkAbgB1AHQAZQBzACwAXABuACAAIAAgACAASQBGACgATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABPAGYAZgBzAGUAdABNAGkAbgB1AHQAZQBzACkAKQAsACAARgBBAEwAUwBFACwAIAAoACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwAgAD4APQAgAC0AOQAwADAAKQAgACoAIAAoAE8AZgBmAHMAZQB0AE0AaQBuAHUAdABlAHMAIAA8AD0AIAA5ADAAMAApACkAIAA8AD4AIAAwACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEkAUwBfAFYAQQBMAEkARABfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFAFwAbgBcAG4AVABlAHMAdABzACAAaQBmACAAYQBuACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAIABpAHMAIAB2AGEAbABpAGQAIABmAG8AcgAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIALgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIABiAG8AbwBsAGUAYQBuAC4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBPAHIAZABpAG4AYQBsACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAE8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG8AZgAgAHkAZQBhAHIAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBfAFYAQQBMAEkARABfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE8AcgBkAGkAbgBhAGwALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATwByAGQAaQBuAGEAbAApACkALABcAG4AIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsACAALwAvACAATwByAGQAaQBuAGEAbAAgAGkAcwAgAG0AYQBuAGQAYQB0AG8AcgB5AFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AcgBkAGkAbgBhAGwALAAgAEkATgBUACgATwByAGQAaQBuAGEAbAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAYQBwAEQAYQB5ACwAIABOACgASQBTAF8ATABFAEEAUABfAFkARQBBAFIAKABZAGUAYQByAEMARQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGUAcwB0ACAAZgBvAHIAIAB2AGEAbABpAGQAIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBvAHIAZABpAG4AYQBsACAAPgA9ACAAMQApACAAKgAgACgAXwBvAHIAZABpAG4AYQBsACAAPAA9ACAAKAAzADYANQAgACsAIABfAGwAZQBhAHAARABhAHkAKQApACkAIAA8AD4AIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBJAFMAXwBWAEEATABJAEQAXwBXAEUARQBLAF8ARABBAFQARQBcAG4AXABuAFQAZQBzAHQAcwAgAGkAZgAgAGEAIAB3AGUAZQBrACAAZABhAHQAZQAgAGkAcwAgAHYAYQBsAGkAZAAgAGYAbwByACAAdABoAGUAIABHAHIAZQBnAG8AcgBpAGEAbgAgAGMAYQBsAGUAbgBkAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABiAG8AbwBsAGUAYQBuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAFcAZQBlAGsAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAG8AZgAgAHQAaABlACAAeQBlAGEAcgBcAG4ARABhAHkATwBmAFcAZQBlAGsAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARABhAHkAIABvAGYAIAB0AGgAZQAgAHcAZQBlAGsAIAB3AGgAZQByAGUAIAAxAC4ALgA3ACAALQA+ACAATQBvAG4ALgAuAFMAdQBuAFwAbgBbAEQAYQB5AE8AZgBXAGUAZQBrAE0AYQBuAGQAYQB0AG8AcgB5AF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABEAGEAeQBPAGYAVwBlAGUAawAgAG0AdQBzAHQAIABiAGUAIABwAHIAbwB2AGkAZABlAGQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEkAUwBfAFYAQQBMAEkARABfAFcARQBFAEsAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAFcAZQBlAGsALAAgAEQAYQB5AE8AZgBXAGUAZQBrACwAIABbAEQAYQB5AE8AZgBXAGUAZQBrAE0AYQBuAGQAYQB0AG8AcgB5AF0ALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgAoAFkAZQBhAHIAQwBFACkAKQAgACsAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFcAZQBlAGsAKQApACwAXABuACAAIAAgACAAIAAgACAAIABGAEEATABTAEUALAAgAC8ALwAgAFkAZQBhAHIAIABhAG4AZAAgAFcAZQBlAGsAIABtAGEAbgBkAGEAdABvAHIAeQBcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwBtAG0AaQB0AEQAbwBXACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5AE8AZgBXAGUAZQBrACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAE4AKABEAGEAeQBPAGYAVwBlAGUAawBNAGEAbgBkAGEAdABvAHIAeQApACAAPAA+ACAAMAApACAAKgAgAF8AbwBtAG0AaQB0AEQAbwBXACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAIAAvAC8AIABEAGEAeQBPAGYAVwBlAGUAawBNAGEAbgBkAGEAdABvAHIAeQAgAHMAZQB0ACAAYQBuAGQAIABEAGEAeQBPAGYAVwBlAGUAawAgAGkAcwAgAG8AbQBtAGkAdABlAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABpAGYAIAB3AGUAZQBrACAAaQBuACAAcgBhAG4AZwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrACwAIABJAE4AVAAoAFcAZQBlAGsAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAKABfAHcAZQBlAGsAIAA+AD0AIAAxACkAIAAqACAAKABfAHcAZQBlAGsAIAA8AD0AIABZAEUAQQBSAF8AVwBFAEUASwBfAEMATwBVAE4AVAAoAFkAZQBhAHIAQwBFACkAKQApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwBtAG0AaQB0AEQAbwBXACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAALwAvACAAeQBlAGEAcgAgAGEAbgBkACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFcAZQBlAGsAIAA8AD4AIABfAHcAZQBlAGsALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAQQBMAFMARQAsACAALwAvACAAdwBlAGUAawAgAGgAYQBzACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHYAYQBsAHUAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAZQBzAHQAIABpAGYAIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsAIABpAG4AIAByAGEAbgBnAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABvAHcALAAgAEkATgBUACgARABhAHkATwBmAFcAZQBlAGsAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBkAG8AdwAgAD4APQAgADEAKQAgACoAIAAoAF8AZABvAHcAIAA8AD0AIAA3ACkAKQAgADwAPgAgADAAIAAvAC8AIABUAGUAcwB0ACAAZgBvAHIAIABEAGEAeQBPAGYAVwBlAGUAawAgADEALgAuADcAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAEMAQQBMAEUATgBEAEEAUgAgAEYAVQBOAEMAVABJAE8ATgBTACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAEUAQQBSAF8ARABBAFkAXwBDAE8AVQBOAFQAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABjAG8AdQBuAHQAIABvAGYAIABvAHIAZABpAG4AYQBsACAAZABhAHkAcwAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAHkAZQBhAHIALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAzADYANQAuAC4AMwA2ADYALAAgACMAVgBBAEwAVQBFACEAIABpAGYAIABuAG8AdAAgAGEAIAB2AGEAbABpAGQAIAB5AGUAYQByAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AWQBFAEEAUgBfAEQAQQBZAF8AQwBPAFUATgBUACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALABcAG4AIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFkARQBBAFIAKABZAGUAYQByAEMARQAsACAAMQApACkALAAgACMAVgBBAEwAVQBFACEALAAgAEkARgAoAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUAKQAsACAAMwA2ADYALAAgADMANgA1ACkAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBFAEEAUgBfAFcARQBFAEsAXwBDAE8AVQBOAFQAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABjAG8AdQBuAHQAIABvAGYAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrAHMAIABpAG4AIABhACAAZwBpAHYAZQBuACAAeQBlAGEAcgAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADUAMgAuAC4ANQAzACwAIAAjAFYAQQBMAFUARQAhACAAaQBmACAAbgBvAHQAIABhACAAdgBhAGwAaQBkACAAeQBlAGEAcgAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AWQBFAEEAUgBfAFcARQBFAEsAXwBDAE8AVQBOAFQAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIAQwBFACwAIABJAE4AVAAoAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwBMAGEAcwB0AEQAYQB5ACwAIABNAE8ARAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUAIAArACAASQBOAFQAKABfAHkAZQBhAHIAQwBFACAALwAgADQAKQAgAC0AIABJAE4AVAAoAF8AeQBlAGEAcgBDAEUAIAAvACAAMQAwADAAKQAgACsAIABJAE4AVAAoAF8AeQBlAGEAcgBDAEUAIAAvACAANAAwADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADcAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwBMAGEAcwB0AEQAYQB5ACAAPQAgADQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAGYAIABsAGEAcwB0ACAAZABhAHkAIABvAGYAIAB5AGUAYQByACAAaQBzACAAYQAgAFQAaAB1AHIAcwBkAGEAeQAsACAAdABoAGUAbgAgAGgAYQBzACAAYQBuACAAZQB4AHQAcgBhACAAdwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAA1ADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGEAcwB0AFkAZQBhAHIALAAgAF8AeQBlAGEAcgBDAEUAIAAtACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwBMAGEAcwB0AEQAYQB5AFAAcgBlAHYALAAgAE0ATwBEACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABhAHMAdABZAGUAYQByACAAKwAgAEkATgBUACgAXwBsAGEAcwB0AFkAZQBhAHIAIAAvACAANAApACAALQAgAEkATgBUACgAXwBsAGEAcwB0AFkAZQBhAHIAIAAvACAAMQAwADAAKQAgACsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAFQAKABfAGwAYQBzAHQAWQBlAGEAcgAgAC8AIAA0ADAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADcAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwBMAGEAcwB0AEQAYQB5AFAAcgBlAHYAIAA9ACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABpAGYAIABsAGEAcwB0ACAAZABhAHkAIABvAGYAIABwAHIAZQB2AGkAbwB1AHMAIAB5AGUAYQByACAAaQBzACAAYQAgAFcAZQBkAG4AZQBzAGQAYQB5ACwAIAB0AGgAZQBuACAAaABhAHMAIABhAG4AIABlAHgAdAByAGEAIAB3AGUAZQBrAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAA1ADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbwB0AGgAZQByAHcAaQB6AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARABBAFkAXwBPAFIARABJAE4AQQBMAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbgB1AG0AYgBlAHIAIABvAGYAIABhACAAZABhAHQAZQAgAGkAbgAgAHQAaABlACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABhAHIALgBcAG4ASQBuAHQAZQBnAGUAcgAgAHcAaQB0AGgAIAByAGEAbgBnAGUAIAAxAC4ALgAzADYANgBcAG4AIwBWAEEATABVAEUAIQAgAGkAZgAgAG4AbwB0ACAAYQAgAHYAYQBsAGkAZAAgAGQAYQB0AGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAE0AbwBuAHQAaAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATQBvAG4AdABoACAAbwBmACAAeQBlAGEAcgBcAG4ARABhAHkAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGEAeQAgAG8AZgAgAG0AbwBuAHQAaABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARABBAFkAXwBPAFIARABJAE4AQQBMACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQALAAgAHsAMAAsACAAMwAxACwAIAA1ADkALAAgADkAMAAsACAAMQAyADAALAAgADEANQAxACwAIAAxADgAMQAsACAAMgAxADIALAAgADIANAAzACwAIAAyADcAMwAsACAAMwAwADQALAAgADMAMwA0AH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAG8AbgB0AGgALAAgAEkATgBUACgATQBvAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAARABhAHkAIAArACAASQBOAEQARQBYACgAXwBtAG8AbgB0AGgATwBmAGYAcwBlAHQALAAgACwAIABfAG0AbwBuAHQAaAApACAAKwAgAEkARgAoAF8AbQBvAG4AdABoACAAPAA9ACAAMgAsACAAMAAsACAATgAoAEkAUwBfAEwARQBBAFAAXwBZAEUAQQBSACgAWQBlAGEAcgBDAEUAKQApACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHQAZQAgAGYAcgBvAG0AIABhACAAZwBpAHYAZQBuACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUALgBcAG4AIwBWAEEATABVAEUAIQAgAGkAZgAgAG4AbwB0ACAAdgBhAGwAaQBkACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUALgBcAG4AXABuAEMAbwBsAHUAbQBuAHMAOgBcAG4AIAAgADEAIAB8ACAAWQBlAGEAcgAgAEMARQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4AIAAgADIAIAB8ACAATQBvAG4AdABoACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADEALgAuADEAMgBcAG4AIAAgADMAIAB8ACAARABhAHkAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADEALgAuADMAMQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4ATwByAGQAaQBuAGEAbAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAE8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG8AZgAgAHkAZQBhAHIAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABPAHIAZABpAG4AYQBsACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAE8AcgBkAGkAbgBhAGwAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaABGAGkAcgBzAHQATwByAGQAaQBuAGEAbAAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBTAF8ATABFAEEAUABfAFkARQBBAFIAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAewAxACwAIAAzADIALAAgADYAMQAsACAAOQAyACwAIAAxADIAMgAsACAAMQA1ADMALAAgADEAOAAzACwAIAAyADEANAAsACAAMgA0ADUALAAgADIANwA1ACwAIAAzADAANgAsACAAMwAzADYAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAMQAsACAAMwAyACwAIAA2ADAALAAgADkAMQAsACAAMQAyADEALAAgADEANQAyACwAIAAxADgAMgAsACAAMgAxADMALAAgADIANAA0ACwAIAAyADcANAAsACAAMwAwADUALAAgADMAMwA1AH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBvAHIAZABpAG4AYQBsACwAIABJAE4AVAAoAE8AcgBkAGkAbgBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AbwBuAHQAaAAsACAAWABNAEEAVABDAEgAKABfAG8AcgBkAGkAbgBhAGwALAAgAF8AbQBvAG4AdABoAEYAaQByAHMAdABPAHIAZABpAG4AYQBsACwAIAAtADEALAAgAC0AMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwBmAGYAcwBlAHQALAAgAEkATgBEAEUAWAAoAF8AbQBvAG4AdABoAEYAaQByAHMAdABPAHIAZABpAG4AYQBsACwAIABfAG0AbwBuAHQAaAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAE8AcgBkAGkAbgBhAGwAIAAtACAAXwBvAGYAZgBzAGUAdAAgACsAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAWQBlAGEAcgBDAEUALAAgAF8AbQBvAG4AdABoACwAIABfAGQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEQAQQBZAF8ATwBGAF8AVwBFAEUASwBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAGQAYQB5ACAAbwBmACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAZgBvAHIAIABhACAAZwBpAHYAZQBuACAAZABhAHQAZQAuAFwAbgAgACAAMQAgAC0AIABNAG8AbgBkAGEAeQBcAG4AIAAgADIAIAAtACAAVAB1AGUAcwBkAGEAeQBcAG4AIAAgADMAIAAtACAAVwBlAGQAbgBlAHMAZABhAHkAXABuACAAIAA0ACAALQAgAFQAaAB1AHIAZABhAHkAXABuACAAIAA1ACAALQAgAEYAcgBpAGQAYQB5AFwAbgAgACAANgAgAC0AIABTAGEAdAB1AHIAZABhAHkAXABuACAAIAA3ACAALQAgAFMAdQBuAGQAYQB5AFwAbgAjAFYAQQBMAFUARQAhACAAaQBmACAAbgBvAHQAIABhACAAdgBhAGwAaQBkACAAZABhAHQAZQAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4ATQBvAG4AdABoACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABNAG8AbgB0AGgAIABvAGYAIAB5AGUAYQByAFwAbgBEAGEAeQAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAEQAYQB5ACAAbwBmACAAbQBvAG4AdABoAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBEAEEAWQBfAE8ARgBfAFcARQBFAEsAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABVAHMAaQBuAGcAIABaAGUAbABsAGUAcgAgAEMAbwBuAGcAcgB1AGUAbgBjAGUALAAgAGMAZgAuACAAaAB0AHQAcABzADoALwAvAGUAbgAuAHcAaQBrAGkAcABlAGQAaQBhAC4AbwByAGcALwB3AGkAawBpAC8AWgBlAGwAbABlAHIAJQAyADcAcwBfAGMAbwBuAGcAcgB1AGUAbgBjAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABNAGEAcAAgAG0AbwBuAHQAaABzACAATQBhAHIALgAuAEYAZQBiACAALQA+ACAAMwAuAC4AMQA0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHoAZQBsAGwAZQByAE0AbwBuAHQAaAAsACAATQBPAEQAKABJAE4AVAAoAE0AbwBuAHQAaAApACAALQAgADMALAAgADEAMgApACAAKwAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAEoAYQBuACwAIABGAGUAYgAgAGMAbwBuAHMAaQBkAGUAcgBlAGQAIABiAGUAbABvAG4AZwBpAG4AZwAgAHQAbwAgAHAAcgBlAHYAaQBvAHUAcwAgAHkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AegBlAGwAbABlAHIAWQBlAGEAcgAsACAASQBOAFQAKABZAGUAYQByAEMARQApACAALQAgAEkATgBUACgAXwB6AGUAbABsAGUAcgBNAG8AbgB0AGgAIAAvACAAMQAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAE8AZgBDAGUAbgB0ACwAIABNAE8ARAAoAF8AegBlAGwAbABlAHIAWQBlAGEAcgAsACAAMQAwADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHoAZQByAG8AQgBhAHMAZQBkAEMAZQBuAHQALAAgAEkATgBUACgAXwB6AGUAbABsAGUAcgBZAGUAYQByACAALwAgADEAMAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFoAZQBsAGwAZQByACAAQwBvAG4AZwByAHUAZQBuAGMAZQAgAGYAbwByACAARwByAGUAZwBvAHIAaQBhAG4AIABjAGEAbABlAG4AZABlAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHIAZQB0AHUAcgBuAHMAIAB3AGUAZQBrAGQAYQB5AHMAIAAwAC4ALgA2ACAALQA+ACAAUwBhAHQALgAuAEYAcgBpAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHoAZQBsAGwAZQByAFcAZQBlAGsARABhAHkALAAgAE0ATwBEACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAFQAKABEAGEAeQApACAAKwAgAEkATgBUACgAMQAzACAAKgAgACgAXwB6AGUAbABsAGUAcgBNAG8AbgB0AGgAIAArACAAMQApACAALwAgADUAKQAgACsAIABfAHkAZQBhAHIATwBmAEMAZQBuAHQAIAArACAASQBOAFQAKABfAHkAZQBhAHIATwBmAEMAZQBuAHQAIAAvACAANAApACAAKwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBUACgAXwB6AGUAcgBvAEIAYQBzAGUAZABDAGUAbgB0ACAALwAgADQAKQAgAC0AIAAyACAAKgAgAF8AegBlAHIAbwBCAGEAcwBlAGQAQwBlAG4AdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADcAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFQAcgBhAG4AcwBsAGEAdABlACAAdABvACAASQBTAE8AIABuAHUAbQBiAGUAcgBpAG4AZwAgADEALgAuADcAIAAtAD4AIABNAG8AbgAuAC4AUwB1AG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0ATwBEACgAXwB6AGUAbABsAGUAcgBXAGUAZQBrAEQAYQB5ACAAKwAgADUALAAgADcAKQAgACsAIAAxAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBEAEEAWQBfAE8ARgBfAFcARQBFAEsAXwBGAFIATwBNAF8ATwBSAEQASQBOAEEATABcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAGQAYQB5ACAAbwBmACAAdwBlAGUAawAgAG4AdQBtAGIAZQByACAAZgBvAHIAIABhACAAZwBpAHYAZQBuACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUALgBcAG4AIAAgADEAIAAtACAATQBvAG4AZABhAHkAXABuACAAIAAyACAALQAgAFQAdQBlAHMAZABhAHkAXABuACAAIAAzACAALQAgAFcAZQBkAG4AZQBzAGQAYQB5AFwAbgAgACAANAAgAC0AIABUAGgAdQByAGQAYQB5AFwAbgAgACAANQAgAC0AIABGAHIAaQBkAGEAeQBcAG4AIAAgADYAIAAtACAAUwBhAHQAdQByAGQAYQB5AFwAbgAgACAANwAgAC0AIABTAHUAbgBkAGEAeQBcAG4AIwBWAEEATABVAEUAIQAgAGkAZgAgAG4AbwB0ACAAYQAgAHYAYQBsAGkAZAAgAGQAYQB0AGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4ATwByAGQAaQBuAGEAbAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAE8AcgBkAGkAbgBhAGwAIABkAGEAeQAgAG8AZgAgAHkAZQBhAHIAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEQAQQBZAF8ATwBGAF8AVwBFAEUASwBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE8AcgBkAGkAbgBhAGwALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAHIAcwB0AEQAYQB5AE8AZgBZAGUAYQByACwAIABEAEEAWQBfAE8ARgBfAFcARQBFAEsAKABZAGUAYQByAEMARQAsACAAMQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABUAHIAYQBuAHMAbABhAHQAZQAgAHQAbwAgAEkAUwBPACAAbgB1AG0AYgBlAHIAaQBuAGcAIAAxAC4ALgA3ACAALQA+ACAATQBvAG4ALgAuAFMAdQBuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAE8ARAAoAF8AZgBpAHIAcwB0AEQAYQB5AE8AZgBZAGUAYQByACAAKwAgAEkATgBUACgATwByAGQAaQBuAGEAbAApACAALQAgADIALAAgADcAKQAgACsAIAAxAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBXAEUARQBLAF8ATgBVAE0AQgBFAFIAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABvAGYAIABhACAAZwBpAHYAZQBuACAAZABhAHQAZQAuAFwAbgBJAG4AdABlAGcAZQByACAAdwBpAHQAaAAgAHIAYQBuAGcAZQAgADEALgAuADUAMwBcAG4AIwBWAEEATABVAEUAIQAgAGkAZgAgAG4AbwB0ACAAYQAgAHYAYQBsAGkAZAAgAGQAYQB0AGUALgBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFkAZQBhAHIAQwBFACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAE0AbwBuAHQAaAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATQBvAG4AdABoACAAbwBmACAAeQBlAGEAcgBcAG4ARABhAHkAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGEAeQAgAG8AZgAgAG0AbwBuAHQAaABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AVwBFAEUASwBfAE4AVQBNAEIARQBSACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBvAHIAZABpAG4AYQBsACwAIABEAEEAWQBfAE8AUgBEAEkATgBBAEwAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkATwBmAFcAZQBlAGsALAAgAEQAQQBZAF8ATwBGAF8AVwBFAEUASwAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAG8AbQBpAG4AYQBsAFcAZQBlAGsALAAgAEkATgBUACgAKABJAE4AVAAoAF8AbwByAGQAaQBuAGEAbAApACAALQAgAF8AZABhAHkATwBmAFcAZQBlAGsAIAArACAAMQAwACkAIAAvACAANwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAG8AbQBpAG4AYQBsAFcAZQBlAGsAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGwAYQBzAHQAIAB3AGUAZQBrACAAbwBmACAAcAByAGUAdgBpAG8AdQBzACAAeQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABZAEUAQQBSAF8AVwBFAEUASwBfAEMATwBVAE4AVAAoAFkAZQBhAHIAQwBFACAALQAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABXAGUAZQBrACAAPQAgADUAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGkAZgAgAHQAaABpAHMAIAB5AGUAYQByACAAZABvAGUAcwAgAG4AbwB0ACAAaABhAHYAZQAgADUAMwAgAHcAZQBlAGsAcwAsACAAdABoAGUAbgAgAGkAcwAgAHQAaABlACAAZgBpAHIAcwB0ACAAdwBlAGUAawAgAG8AZgAgAGYAbwBsAGwAbwB3AGkAbgBnACAAeQBlAGEAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABZAEUAQQBSAF8AVwBFAEUASwBfAEMATwBVAE4AVAAoAFkAZQBhAHIAQwBFACkAIAA9ACAANQAzACwAIAA1ADMALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVwBFAEUASwBfAE4AVQBNAEIARQBSAF8ARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAdABoAGUAIABJAFMATwAgAGQAZQBmAGkAbgBlAGQAIAB3AGUAZQBrACAAbgB1AG0AYgBlAHIAIABvAGYAIABhACAAZwBpAHYAZQBuACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUALgBcAG4ASQBuAHQAZQBnAGUAcgAgAHcAaQB0AGgAIAByAGEAbgBnAGUAIAAxAC4ALgA1ADMAXABuACMAVgBBAEwAVQBFACEAIABpAGYAIABuAG8AdAAgAGEAIAB2AGEAbABpAGQAIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAuAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBPAHIAZABpAG4AYQBsACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAATwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AVwBFAEUASwBfAE4AVQBNAEIARQBSAF8ARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbAAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABPAHIAZABpAG4AYQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQBPAGYAVwBlAGUAawAsACAARABBAFkAXwBPAEYAXwBXAEUARQBLAF8ARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABXAGUAZQBrACwAIABJAE4AVAAoACgASQBOAFQAKABPAHIAZABpAG4AYQBsACkAIAAtACAAXwBkAGEAeQBPAGYAVwBlAGUAawAgACsAIAAxADAAKQAgAC8AIAA3ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AbwBtAGkAbgBhAGwAVwBlAGUAawAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbABhAHMAdAAgAHcAZQBlAGsAIABvAGYAIABwAHIAZQB2AGkAbwB1AHMAIAB5AGUAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFkARQBBAFIAXwBXAEUARQBLAF8AQwBPAFUATgBUACgAWQBlAGEAcgBDAEUAIAAtACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAG8AbQBpAG4AYQBsAFcAZQBlAGsAIAA9ACAANQAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAaQBmACAAdABoAGkAcwAgAHkAZQBhAHIAIABkAG8AZQBzACAAbgBvAHQAIABoAGEAdgBlACAANQAzACAAdwBlAGUAawBzACwAIAB0AGgAZQBuACAAaQBzACAAMQBzAHQAIAB3AGUAZQBrACAAbwBmACAAZgBvAGwAbABvAHcAaQBuAGcAIAB5AGUAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFkARQBBAFIAXwBXAEUARQBLAF8AQwBPAFUATgBUACgAWQBlAGEAcgBDAEUAKQAgAD0AIAA1ADMALAAgADUAMwAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBvAG0AaQBuAGEAbABXAGUAZQBrAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBUAE8AXwBXAEUARQBLAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAGEAbgBkACAAZABhAHkAIABvAGYAIAB3AGUAZQBrACAAZgByAG8AbQAgAGEAIABnAGkAdgBlAG4AIABkAGEAdABlAC4AIABUAGgAZQAgAHAAcgBvAHYAaQBkAGUAZAAgAGQAYQB0AGUAIABjAGEAbgAgAGkAbQBwAGwAaQBjAGkAdABsAHkAXABuAGIAZQAgAGUAaQB0AGgAZQByACAAYQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB0AGUAIABvAHIAIABvAHIAZABpAG4AaQBuAGEAbAAgAGQAYQB0AGUALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAMQAgAHwAIABZAGUAYQByACAAQwBFACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkALAAgACMAVgBBAEwAVQBFACEAIABpAGYAIABuAG8AdAAgAGEAIAB2AGEAbABpAGQAIABkAGEAdABlAFwAbgAgACAAMgAgAHwAIABXAGUAZQBrACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxAC4ALgA1ADMAXABuACAAIAAzACAAfAAgAEQAYQB5ACAAbwBmACAAdwBlAGUAawAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADEALgAuADcAIABNAG8AbgAuAC4AcwB1AG4AXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAE0AbwBuAHQAaAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABNAG8AbgB0AGgAIABvAGYAIAB0AGgAZQAgAHkAZQBhAHIALgAgAEkAZgAgAG8AbQBtAGkAdAB0AGUAZAAsACAAZABhAHkAIABpAHMAIABhAHMAcwB1AG0AZQBkACAAdABvACAAYgBlACAAbwByAGQAaQBuAGEAbAAuAFwAbgBEAGEAeQAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAARABhAHkAIABvAGYAIAB0AGgAZQAgAG0AbwBuAHQAaAAgAHcAaABlAG4AIABtAG8AbgB0AGgAIABwAHIAbwB2AGkAZABlAGQALAAgAG8AdABoAGUAcgB3AGkAcwBlACAAbwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAdABoAGUAIAB5AGUAYQByAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFQATwBfAFcARQBFAEsAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAE0AbwBuAHQAaAAsACAARABhAHkALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACwAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAHAAYQByAGEAbQBlAHQAZQByAHMAIABhAHIAZQAgAGEAIABkAGEAdABlAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABNAG8AbgB0AGgALAAgAEQAYQB5ACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAHIAYQBjAEQAYQB5ACwAIABEAGEAeQAgAC0AIABJAE4AVAAoAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAbwB3ACwAIABEAEEAWQBfAE8ARgBfAFcARQBFAEsAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB3AGUAZQBrACwAIABXAEUARQBLAF8ATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACAAKwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAKABfAHcAZQBlAGsAIAA9ACAAMQApACAAKgAgACgATQBvAG4AdABoACAAPQAgADEAMgApACwAIAAxACwAIAAoAF8AdwBlAGUAawAgAD4APQAgADUAMgApACAAKgAgACgATQBvAG4AdABoACAAPQAgADEAKQAsACAALQAxACwAIABUAFIAVQBFACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AeQBlAGEAcgBDAEUALAAgAF8AdwBlAGUAawAsACAAXwBkAG8AdwAgACsAIABfAGYAcgBhAGMARABhAHkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAcABhAHIAYQBtAGUAdABlAHIAcwAgAGEAcgBlACAAYQBuACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABEAGEAeQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgByAGEAYwBEAGEAeQAsACAARABhAHkAIAAtACAASQBOAFQAKABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAG8AdwAsACAARABBAFkAXwBPAEYAXwBXAEUARQBLAF8ARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAKABZAGUAYQByAEMARQAsACAARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdwBlAGUAawAsACAAVwBFAEUASwBfAE4AVQBNAEIARQBSAF8ARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAKABZAGUAYQByAEMARQAsACAARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgBDAEUALAAgAEkATgBUACgAWQBlAGEAcgBDAEUAKQAgACsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoACgAXwB3AGUAZQBrACAAPQAgADEAKQAgACoAIAAoAE0AbwBuAHQAaAAgAD0AIAAxADIAKQAsACAAMQAsACAAKABfAHcAZQBlAGsAIAA+AD0AIAA1ADIAKQAgACoAIAAoAE0AbwBuAHQAaAAgAD0AIAAxACkALAAgAC0AMQAsACAAVABSAFUARQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHkAZQBhAHIAQwBFACwAIABfAHcAZQBlAGsALAAgAF8AZABvAHcAIAArACAAXwBmAHIAYQBjAEQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYAUgBPAE0AXwBXAEUARQBLAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGUAaQB0AGgAZQByACAAYQAgAEcAcgBlAGcAbwByAGkAYQBuACAAYwBhAGwAZQBuAGQAYQByACAAZABhAHQAZQAgAG8AcgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlACAAZgByAG8AbQAgAGEAIABnAGkAdgBlAG4AIAB3AGUAZQBrACAAYQBuAGQAIABkAGEAeQAgAG8AZgAgAHcAZQBlAGsALgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIwBWAEEATABVAEUAIQAgAGkAZgAgAG4AbwB0ACAAYQAgAHYAYQBsAGkAZAAgAHcAZQBlAGsAIABkAGEAdABlAC4AXABuAFwAbgBSAGUAdAB1AHIAbgBPAHIAZABpAG4AYQBsACAAPQAgAEYAQQBMAFMARQBcAG4AIAAgADEAIAB8ACAAWQBlAGEAcgAgAEMARQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4AIAAgADIAIAB8ACAATQBvAG4AdABoACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADEALgAuADEAMgBcAG4AIAAgADMAIAB8ACAARABhAHkAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADEALgAuADMAMQBcAG4AUgBlAHQAdQByAG4ATwByAGQAaQBuAGEAbAAgAD0AIABUAFIAVQBFAFwAbgAgACAAMQAgAHwAIABZAGUAYQByACAAQwBFACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgAgACAAMgAgAHwAIABPAHIAZABpAG4AYQBsACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAMQAuAC4AMwA2ADYAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBXAGUAZQBrACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAG8AZgAgAHQAaABlACAAeQBlAGEAcgBcAG4ARABhAHkATwBmAFcAZQBlAGsAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIABEAGEAeQAgAG8AZgAgAHQAaABlACAAdwBlAGUAawAgAHcAaABlAHIAZQAgADEALgAuADcAIAAtAD4AIABNAG8AbgAuAC4AUwB1AG4AIABcAG4AWwBSAGUAdAB1AHIAbgBPAHIAZABpAG4AYQBsAF0AIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABSAGUAdAB1AHIAbgAgAHIAZQBzAHUAbAB0ACAAYQBzACAAYQBuACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYAUgBPAE0AXwBXAEUARQBLAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFkAZQBhAHIAQwBFACwAIABXAGUAZQBrACwAIABEAGEAeQBPAGYAVwBlAGUAawAsACAAWwBSAGUAdAB1AHIAbgBPAHIAZABpAG4AYQBsAF0ALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVwBFAEUASwBfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAAVwBlAGUAawAsACAARABhAHkATwBmAFcAZQBlAGsALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAQwBvAHIAcgBlAGMAdABpAG8AbgAsACAARABBAFkAXwBPAEYAXwBXAEUARQBLACgAWQBlAGEAcgBDAEUALAAgADEALAAgADQAKQAgACsAIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwByAGQAaQBuAGEAbABEAGEAeQAsACAASQBOAFQAKABXAGUAZQBrACkAIAAqACAANwAgACsAIABEAGEAeQBPAGYAVwBlAGUAawAgAC0AIABfAHkAQwBvAHIAcgBlAGMAdABpAG8AbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAbgB0AE8AcgBkAGkAbgBhAGwALAAgAEkATgBUACgAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAbgB0AE8AcgBkAGkAbgBhAGwAIAA8ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAHYAWQBlAGEAcgAsACAAWQBlAGEAcgBDAEUAIAAtACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQB2AFkAZQBhAHIARABhAHkAQwBvAHUAbgB0ACwAIABZAEUAQQBSAF8ARABBAFkAXwBDAE8AVQBOAFQAKABfAHAAcgBlAHYAWQBlAGEAcgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGEAZABqAHUAcwB0AGUAZABPAHIAZABpAG4AYQBsAEQAYQB5ACwAIABfAHAAcgBlAHYAWQBlAGEAcgBEAGEAeQBDAG8AdQBuAHQAIAArACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAFIAZQB0AHUAcgBuAE8AcgBkAGkAbgBhAGwAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAHAAcgBlAHYAWQBlAGEAcgAsACAAXwBhAGQAagB1AHMAdABlAGQATwByAGQAaQBuAGEAbABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAF8AcAByAGUAdgBZAGUAYQByACwAIABfAGEAZABqAHUAcwB0AGUAZABPAHIAZABpAG4AYQBsAEQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAbgB0AE8AcgBkAGkAbgBhAGwAIAA8AD0AIAAzADYANQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAFIAZQB0AHUAcgBuAE8AcgBkAGkAbgBhAGwAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAWQBlAGEAcgBDAEUALAAgAF8AbwByAGQAaQBuAGEAbABEAGEAeQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAFIATwBNAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGgAaQBzAFkAZQBhAHIARABhAHkAQwBvAHUAbgB0ACwAIABZAEUAQQBSAF8ARABBAFkAXwBDAE8AVQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAG4AdABPAHIAZABpAG4AYQBsACAAPgAgAF8AdABoAGkAcwBZAGUAYQByAEQAYQB5AEMAbwB1AG4AdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBlAHgAdABZAGUAYQByACwAIABZAGUAYQByAEMARQAgACsAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGQAagB1AHMAdABlAGQATwByAGQAaQBuAGEAbABEAGEAeQAsACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACAALQAgAF8AdABoAGkAcwBZAGUAYQByAEQAYQB5AEMAbwB1AG4AdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAFIAZQB0AHUAcgBuAE8AcgBkAGkAbgBhAGwAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwBuAGUAeAB0AFkAZQBhAHIALAAgAF8AYQBkAGoAdQBzAHQAZQBkAE8AcgBkAGkAbgBhAGwARABhAHkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBSAE8ATQBfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFACgAXwBuAGUAeAB0AFkAZQBhAHIALAAgAF8AYQBkAGoAdQBzAHQAZQBkAE8AcgBkAGkAbgBhAGwARABhAHkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABsAGEAcwB0ACAAZABhAHkAIABvAGYAIABhACAAbABlAGEAcAAgAHkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AKABSAGUAdAB1AHIAbgBPAHIAZABpAG4AYQBsACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABZAGUAYQByAEMARQAsACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAFIATwBNAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAAXwBvAHIAZABpAG4AYQBsAEQAYQB5ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAFAAQQBSAFMASQBOAEcAIABGAFUATgBDAFQASQBPAE4AUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBWAEEATABJAEQAQQBUAEUAXwBDAEgAQQBSAEEAQwBUAEUAUgBTAFwAbgBcAG4AVABlAHMAdABzACAAaQBmACAAdABlAHgAdAAgAGMAbwBuAHQAYQBpAG4AcwAgAG8AbgBsAHkAIABjAGgAYQByAGEAYwB0AGUAcgBzACAAdABoAGEAdAAgAGEAcgBlACAAdgBhAGwAaQBkACAAZgBvAHIAIABJAFMATwAgADgANgAwADEALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAYgBvAG8AbABlAGEAbgAsACAAbgB1AGwAbAAgAGkAZgAgAGUAbQBwAHQAeQAgAHMAdAByAGkAbgBnACAAcAByAG8AdgBpAGQAZQBkAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AVABlAHgAdAAgACAAIAAgACAAfAAgAHMAdAByAGkAbgBnACAAIAB8ACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQAdABlAGQAIAB0AGUAeAB0AC4AXABuAFsAUwB1AGIAcwBlAHQAXQAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFMAdQBiAHMAZQB0ACAAZgBvAHIAbQBhAHQAIAB0AG8AIABtAGEAdABjAGgAXABuACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAGQAYQB0AGUALAAgAHQAaQBtAGUAIABhAG4AZAAgAHQAaQBtAGUAegBvAG4AZQAgACAAKwAsAC0ALgAwADEAMgAzADQANQA2ADcAOAA5ADoAVABXAFoAEiIgACgAZABlAGYAYQB1AGwAdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABkAGEAdABlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACsALQAwADEAMgAzADQANQA2ADcAOAA5AFcAEiJcAG4AIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAAdABpAG0AZQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAsAC4AMAAxADIAMwA0ADUANgA3ADgAOQA6AFQAXABuACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAHQAaQBtAGUAIAB6AG8AbgBlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAtADAAMQAyADMANAA1ADYANwA4ADkAOgBaABIiXABuACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA0ACAALQAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAsAC0ALgAwADEAMgAzADQANQA2ADcAOAA5ADoAVABXABIiXABuACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA1ACAALQAgAHQAaQBtAGUAIABhAG4AZAAgAHQAaQBtAGUAIAB6AG8AbgBlACAAIAAgACAAIAAgACAAKwAsAC0ALgAwADEAMgAzADQANQA2ADcAOAA5ADoAVABaABIiXABuACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA2ACAALQAgAGQAdQByAGEAdABpAG8AbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALAAtAC4AMAAxADIAMwA0ADUANgA3ADgAOQA6AEQASABNAFAAUwBUAFcAWQBcAG4AIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADcAIAAtACAAaQBuAHQAZQByAHYAYQBsACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAArACwALQAuAC8AMAAxADIAMwA0ADUANgA3ADgAOQA6AEQASABNAFAAUwBUAFcAWQBaABIiXABuACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA4ACAALQAgAGYAdQBsAGwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKwAsAC0ALgAvADAAMQAyADMANAA1ADYANwA4ADkAOgBEAEgATQBQAFIAUwBUAFcAWQBaABIiXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFYAQQBMAEkARABBAFQARQBfAEMASABBAFIAQQBDAFQARQBSAFMAIAA9ACAATABBAE0AQgBEAEEAKABUAGUAeAB0ACwAIABbAFMAdQBiAHMAZQB0AF0ALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAFQAZQB4AHQAIAA9ACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAGQAeAAsACAASQBOAFQAKABOACgAUwB1AGIAcwBlAHQAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgBTAGUAdAAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAZAB4ACAAPAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGQAYQB0AGUALAAgAHQAaQBtAGUAIABhAG4AZAAgAHQAaQBtAGUAIAB6AG8AbgBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArACwALQAuADAAMQAyADMANAA1ADYANwA4ADkAOgBUAFcAWgBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBkAHgAIAA9ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGQAYQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsALQAwADEAMgAzADQANQA2ADcAOAA5AFcAXAAiACAAJgAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAZAB4ACAAPQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAB0AGkAbQBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgAsAC4AMAAxADIAMwA0ADUANgA3ADgAOQA6AFQAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAGQAeAAgAD0AIAAzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAdABpAG0AZQAgAHoAbwBuAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsALQAwADEAMgAzADQANQA2ADcAOAA5ADoAWgBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBkAHgAIAA9ACAANAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsALAAtAC4AMAAxADIAMwA0ADUANgA3ADgAOQA6AFQAVwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBkAHgAIAA9ACAANQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHQAaQBtAGUAIABhAG4AZAAgAHQAaQBtAGUAIAB6AG8AbgBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArACwALQAuADAAMQAyADMANAA1ADYANwA4ADkAOgBUAFoAXAAiACAAJgAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAZAB4ACAAPQAgADYALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABkAHUAcgBhAHQAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACwALQAuADAAMQAyADMANAA1ADYANwA4ADkAOgBEAEgATQBQAFMAVABXAFkAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAGQAeAAgAD0AIAA3ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAaQBuAHQAZQByAHYAYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArACwALQAuAC8AMAAxADIAMwA0ADUANgA3ADgAOQA6AEQASABNAFAAUwBUAFcAWQBaAFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAGQAeAAgAD4APQAgADgALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABmAHUAbABsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArACwALQAuAC8AMAAxADIAMwA0ADUANgA3ADgAOQA6AEQASABNAFAAUgBTAFQAVwBZAFoAXAAiACAAJgAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHMAYwBhAHAAZQBUAGUAeAB0ACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAUwBVAEIAUwBUAEkAVABVAFQARQAoAFQAZQB4AHQALAAgAFwAIgAmAFwAIgAsACAAXAAiACYAYQBtAHAAOwBcACIAKQAsACAAXAAiADwAXAAiACwAIABcACIAJgBsAHQAOwBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHgAbQBsACwAIABcACIAPAB0AD4APABzAD4AXAAiACAAJgAgAF8AZQBzAGMAYQBwAGUAVABlAHgAdAAgACYAIABcACIAPAAvAHMAPgA8AC8AdAA+AFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHgAcABhAHQAaAAsACAAXAAiAC8ALwBzAFsAdAByAGEAbgBzAGwAYQB0AGUAKAAuACwAJwBcACIAIAAmACAAXwBjAGgAYQByAFMAZQB0ACAAJgAgAFwAIgAnACwAJwAnACkAPQAnACcAXQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMARQBSAFIATwBSACgARgBJAEwAVABFAFIAWABNAEwAKABfAHgAbQBsACwAIABfAHgAcABhAHQAaAApACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHkAZQBhAHIALAAgAG0AbwBuAHQAaAAgAGEAbgBkACAAZABhAHkAIABvAGYAIABhACAAZABhAHQAZQAgAGYAcgBvAG0AIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuAFwAbgBOAG8AdABlACAAWQBZAFkAWQBNAE0AIABpAHMAIABpAG4AdgBhAGwAaQBkACwAIABkAHUAZQAgAHQAbwAgAGMAbwBsAGwAaQBzAGkAbwBuACAAdwBpAHQAaAAgAHQAcgB1AG4AYwBhAHQAZQBkACAAZgBvAHIAbQBhAHQAIABZAFkATQBNAEQARAAgAGkAbgAgAGUAYQByAGwAaQBlAHIAIAB2AGUAcgBzAGkAbwBuAHMAIABvAGYAIABJAFMATwAgADgANgAwADEALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAMQAgAHwAIABJAFMATwBDAG8AbQBwAGwAaQBhAG4AdAAgAHwAIABiAG8AbwBsAGUAYQBuACAAfAAgAEYAbABhAGcAIABpAGYAIABjAG8AbQBwAGwAaQBhAG4AdAAgAHQAbwAgAEkAUwBPACAAOAA2ADAAMQAgAHMAdABhAG4AZABhAHIAZABcAG4AIAAgADIAIAB8ACAAUAByAGUAYwBpAHMAaQBvAG4AIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAwACAALQAgAGkAbgB2AGEAbABpAGQAIAB2AGEAbAB1AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMQAgAC0AIAB5AGUAYQByAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADIAIAAtACAAbQBvAG4AdABoAC8AdwBlAGUAawBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAzACAALQAgAGQAYQB5AFwAbgAgACAAMwAgAHwAIABGAG8AcgBtAGEAdAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADEAIAAtACAAYgBhAHMAaQBjAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADIAIAAtACAAZQB4AHQAZQBuAGQAZQBkAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADMAIAAtACAAYwBvAG4AcwBpAHMAdABlAG4AdAAgAHcAaQB0AGgAIABiAGEAcwBpAGMAIABvAHIAIABlAHgAdABlAG4AZABlAGQAXABuACAAIAA0ACAAfAAgAEQAYQB0AGUAVAB5AHAAZQAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMQAgAC0AIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADIAIAAtACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMwAgAC0AIAB3AGUAZQBrACAAZABhAHQAZQBcAG4AIAAgADUAIAB8ACAAWQBlAGEAcgAgAEMARQAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuACAAIAA2ACAAfAAgAEQAYQB0AGUAQQByAGcAMQAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATQBvAG4AdABoACAAMQAuAC4AMQAyACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAxAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAEUAbQBwAHQAeQAgAHcAaABlAG4AIABEAGEAdABlAFQAeQBwAGUAIAA9ACAAMgBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABXAGUAZQBrACAAMQAuAC4ANQAzACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAzAFwAbgAgACAANwAgAHwAIABEAGEAdABlAEEAcgBnADIAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEQAYQB5ACAAMQAuAC4AMwAxACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAxAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE8AcgBkAGkAbgBhAGwAIAAxAC4ALgAzADYANgAgAHcAaABlAG4AIABEAGEAdABlAFQAeQBwAGUAIAA9ACAAMgBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABEAGEAeQAgAG8AZgAgAFcAZQBlAGsAIAAxAC4ALgA3ACAALQA+ACAATQBvAG4ALgAuAFMAdQBuACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAzAFwAbgAgACAAIAAgACAAIAAgACAAXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFQAZQB4AHQAIAAgACAAIAAgACAAIAAgAHwAIABzAHQAcgBpAG4AZwAgAHwAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAB0AGUAZAAgAGQAYQB0AGUALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAfAAgAEUAeABhAG0AcABsAGUAIABmAG8AcgBtAGEAdABzADoAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgAHwAIAArAFkAWQBZAFkAWQAtAE0ATQAtAEQARAAsACAALQBZAFkAWQBZAC0ATQBNAC0ARABEACwAIABZAFkAWQBZAC0ATQBNAC0ARABEACwAIABZAFkAWQBZAC0ATQBNACwAIABZAFkAWQBZAE0ATQBEAEQALAAgAFkAWQBZAFkAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABUAGUAeAB0ACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBsAHUAbQBuAHMAOgAgAEgAYQBzAGgALAAgAFAAcgBlAGMAaQBzAGkAbwBuACwAIABGAG8AcgBtAGEAdAAsACAARABhAHQAZQBUAHkAcABlACwAIABZAGUAYQByAEwAZQBuACwAIABEAGEAdABlAEEAcgBnADEAUABvAHMALAAgAEQAYQB0AGUAQQByAGcAMQBMAGUAbgAsACAARABhAHQAZQBBAHIAZwAyAEwAZQBuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAdwBoAGUAcgBlACAASABhAHMAaAAgAD0AIAAoAEwARQBOACAAKgAgADQAMAA5ADYAKQAgACsAIAAoAEgAeQBwAGgAZQBuAFAAbwBzACAAKgAgADIANQA2ACkAIAArACAAKABIAHkAcABoAGUAbgAyAFAAbwBzACAAKgAgADEANgApACAAKwAgAFcAUABvAHMAIABcAG4AIAAgACAAIAAgACAAIAAgAF8AZgBtAHQASABhAHMAaABUAGEAYgBsAGUALAAgAHsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEANgAzADgANAAsACAAMQAsACAAMwAsACAAMQAsACAANAAsACAAMAAsACAAMAAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyADAANAA4ADAALAAgADEALAAgADMALAAgADEALAAgADUALAAgADAALAAgADAALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgA4ADYANwAyACwAIAAzACwAIAAxACwAIAAyACwAIAA0ACwAIAAwACwAIAAwACwAIAAzADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIAOAA2ADcANwAsACAAMgAsACAAMQAsACAAMwAsACAANAAsACAANgAsACAAMgAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyADkAOQA1ADIALAAgADIALAAgADIALAAgADEALAAgADQALAAgADYALAAgADIALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwAyADcANgA4ACwAIAAzACwAIAAxACwAIAAxACwAIAA0ACwAIAA1ACwAIAAyACwAIAAyADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMAMgA3ADcAMwAsACAAMwAsACAAMQAsACAAMwAsACAANAAsACAANgAsACAAMgAsACAAMQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADIANwA3ADQALAAgADIALAAgADEALAAgADMALAAgADUALAAgADcALAAgADIALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwA0ADAANAA4ACwAIAAzACwAIAAyACwAIAAyACwAIAA0ACwAIAAwACwAIAAwACwAIAAzADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMANAAwADUANAAsACAAMgAsACAAMgAsACAAMwAsACAANAAsACAANwAsACAAMgAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADQAMwAwADQALAAgADIALAAgADIALAAgADEALAAgADUALAAgADcALAAgADIALAAgADAAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwA2ADgANgA0ACwAIAAzACwAIAAxACwAIAAxACwAIAA1ACwAIAA2ACwAIAAyACwAIAAyADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMANgA4ADcAMAAsACAAMwAsACAAMQAsACAAMwAsACAANQAsACAANwAsACAAMgAsACAAMQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADgANAAwADAALAAgADMALAAgADIALAAgADIALAAgADUALAAgADAALAAgADAALAAgADMAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwA4ADQAMAA3ACwAIAAyACwAIAAyACwAIAAzACwAIAA1ACwAIAA4ACwAIAAyACwAIAAwADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADQAMgAzADYAOAAsACAAMwAsACAAMgAsACAAMQAsACAANAAsACAANgAsACAAMgAsACAAMgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAA0ADIAMwA5ADAALAAgADMALAAgADIALAAgADMALAAgADQALAAgADcALAAgADIALAAgADEAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAANAA2ADcAMwA2ACwAIAAzACwAIAAyACwAIAAxACwAIAA1ACwAIAA3ACwAIAAyACwAIAAyADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADQANgA3ADUAOQAsACAAMwAsACAAMgAsACAAMwAsACAANQAsACAAOAAsACAAMgAsACAAMQBcAG4AIAAgACAAIAAgACAAIAAgAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAsACAATABBAE0AQgBEAEEAKABfAGUAeABjAGUAcAB0AGkAbwBuACwAIABbAF8AcAByAGUAYwBpAHMAaQBvAG4AXQAsACAAWwBfAGUAeAB0AGUAbgBkAGUAZABdACwAIABbAF8AZABhAHQAZQBUAHkAcABlAF0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgACAAfAAgAHMAdAByAGkAbgBnACAAIAB8ACAAbgB1AGwAbAAgACAARQBtAHAAdAB5ACAAdABlAHgAdABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAATgAvAEEAIAAgACAAVQBuAGEAYgBsAGUAIAB0AG8AIABwAGEAcgBzAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAFYAQQBMAFUARQAgAEkAbgB2AGEAbABpAGQAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUAByAGUAYwBpAHMAaQBvAG4AIABvAGYAIABwAGEAcgBzAGUAZAAgAHYAYQBsAHUAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABfAGUAeAB0AGUAbgBkAGUAZAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABQAGEAcgBzAGUAZAAgAGUAeAB0AGUAbgBkAGUAZAAgAGYAbwByAG0AYQB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABfAGQAYQB0AGUAVAB5AHAAZQAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABDAGEAbABlAG4AZABhAHIAIABkAGEAdABlACwAIABvAHIAZABpAG4AYQBsACAAZABhAHQAZQAsACAAbwByACAAdwBlAGUAawAgAGQAYQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIATgAvAEEAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AEYAQQBMAFMARQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIAVgBBAEwAVQBFAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABGAEEATABTAEUALAAgADAALAAgAE4AKABfAGUAeAB0AGUAbgBkAGUAZAApACwAIABOACgAXwBkAGEAdABlAFQAeQBwAGUAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIABcACIAXAAiACwAIABcACIAXAAiAH0AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAEYAQQBMAFMARQAsACAAMAAsACAATgAoAF8AZQB4AHQAZQBuAGQAZQBkACkALAAgAE4AKABfAGQAYQB0AGUAVAB5AHAAZQApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgAFwAIgBcACIAfQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAC8ALwBfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABGAEEATABTAEUALAAgADAALAAgAE4AKABfAGUAeAB0AGUAbgBkAGUAZAApACwAIABOACgAXwBkAGEAdABlAFQAeQBwAGUAKQAsACAAewAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhACwAIAAjAFYAQQBMAFUARQAhAH0AKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAFwAIgBcACIAfQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABJAEYAKABUAGUAeAB0ACAAPQAgAFwAIgBcACIALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAFYAQQBMAEkARABBAFQARQBfAEMASABBAFIAQQBDAFQARQBSAFMAKABUAGUAeAB0ACwAIAAxACkAKQAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAUwBpAGcAbgAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAEYAVAAoAFQAZQB4AHQALAAgADEAKQAgAD0AIABcACIAKwBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUARgBUACgAVABlAHgAdAAsACAAMQApACAAPQAgAFwAIgAtAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFUATgBJAEMATwBEAEUAKABMAEUARgBUACgAVABlAHgAdAAsACAAMQApACkAIAA9ACAAOAA3ADIAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAFMAaQBnAG4ALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBGAFQAKABUAGUAeAB0ACwAIAAxACkAIAA9ACAAXAAiAC0AXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABVAE4ASQBDAE8ARABFACgATABFAEYAVAAoAFQAZQB4AHQALAAgADEAKQApACAAPQAgADgANwAyADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4ALAAgAEwARQBOACgAVABlAHgAdAApACAALQAgAE4AKABfAGgAYQBzAFMAaQBnAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAEQAYQB0AGUALAAgAEkARgAoAF8AaABhAHMAUwBpAGcAbgAsACAAUgBJAEcASABUACgAVABlAHgAdAAsACAAXwBsAGUAbgApACwAIABUAGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8ASAB5AHAAaAAxAFAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgAtAFwAIgAsACAAXwBzAEQAYQB0AGUAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEgAeQBwAGgAMgBQAG8AcwAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIALQBcACIALAAgAF8AcwBEAGEAdABlACwAIABfAEgAeQBwAGgAMQBQAG8AcwAgACsAIAAxACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBXAHAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgBXAFwAIgAsACAAXwBzAEQAYQB0AGUAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAGgALAAgACgAXwBsAGUAbgAgACoAIAA0ADAAOQA2ACkAIAArACAAKABfAEgAeQBwAGgAMQBQAG8AcwAgACoAIAAyADUANgApACAAKwAgACgAXwBIAHkAcABoADIAUABvAHMAIAAqACAAMQA2ACkAIAArACAAXwBXAHAAbwBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAGgATABrAHUAcAAsACAASQBGAE4AQQAoAFgATQBBAFQAQwBIACgAXwBoAGEAcwBoACwAIABDAEgATwBPAFMARQBDAE8ATABTACgAXwBmAG0AdABIAGEAcwBoAFQAYQBiAGwAZQAsACAAMQApACwAIAAwACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBoAGEAcwBoAEwAawB1AHAAIAA9ACAAMAAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGUAZgBuACwAIABDAEgATwBPAFMARQBSAE8AVwBTACgAXwBmAG0AdABIAGEAcwBoAFQAYQBiAGwAZQAsACAAXwBoAGEAcwBoAEwAawB1AHAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAdABlAG4AZABlAGQALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFQAeQBwAGUALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AGUAYQByAEMARQAsACAAXwB5AGUAYQByAFMAaQBnAG4AIAAqACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8AcwBEAGEAdABlACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADUAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAQQByAGcAMQAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA8ACAAMgApACAAKwAgACgASQBOAEQARQBYACgAXwBkAGUAZgBuACwAIAAxACwAIAA2ACkAIAA9ACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABWAEEATABVAEUAKABNAEkARAAoAF8AcwBEAGEAdABlACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADYAKQAsACAASQBOAEQARQBYACgAXwBkAGUAZgBuACwAIAAxACwAIAA3ACkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAQQByAGcAMgAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPAAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAF8AcwBEAGEAdABlACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADgAKQApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdgBhAGwAaQBkACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFQAeQBwAGUAIAA9ACAAMQAsACAASQBTAF8AVgBBAEwASQBEAF8ARABBAFQARQAoAF8AeQBlAGEAcgBDAEUALAAgAF8AZABBAHIAZwAxACwAIABfAGQAQQByAGcAMgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAVAB5AHAAZQAgAD0AIAAyACwAIABJAFMAXwBWAEEATABJAEQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAF8AeQBlAGEAcgBDAEUALAAgAF8AZABBAHIAZwAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBUAHkAcABlACAAPQAgADMALAAgAEkAUwBfAFYAQQBMAEkARABfAFcARQBFAEsAXwBEAEEAVABFACgAXwB5AGUAYQByAEMARQAsACAAXwBkAEEAcgBnADEALAAgAF8AZABBAHIAZwAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAFQAUgBVAEUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AdgBhAGwAaQBkACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFQAUgBVAEUALAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAF8AZQB4AHQAZQBuAGQAZQBkACwAIABfAGQAYQB0AGUAVAB5AHAAZQAsACAAXwB5AGUAYQByAEMARQAsACAAXwBkAEEAcgBnADEALAAgAF8AZABBAHIAZwAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBWAEEATABVAEUAXAAiACwAIABfAHAAcgBlAGMAaQBzAGkAbwBuACwAIABfAGUAeAB0AGUAbgBkAGUAZAAsACAAXwBkAGEAdABlAFQAeQBwAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBQAEEAUgBTAEUAXwBUAEkATQBFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAaABvAHUAcgAsACAAbQBpAG4AdQB0AGUAIABhAG4AZAAgAHMAZQBjAG8AbgBkACAAbwBmACAAdABpAG0AZQAgAGYAcgBvAG0AIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAIAAxACAAfAAgAEkAUwBPAEMAbwBtAHAAbABpAGEAbgB0ACAAfAAgAGIAbwBvAGwAZQBhAG4AIAB8ACAARgBsAGEAZwAgAGkAZgAgAGMAbwBtAHAAbABpAGEAbgB0ACAAdABvACAASQBTAE8AIAA4ADYAMAAxACAAcwB0AGEAbgBkAGEAcgBkAFwAbgAgACAAMgAgAHwAIABQAHIAZQBjAGkAcwBpAG8AbgAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADAAIAAtACAAaQBuAHYAYQBsAGkAZAAgAHYAYQBsAHUAZQBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAxACAALQAgAGgAbwB1AHIAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMgAgAC0AIABtAGkAbgB1AHQAZQBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAzACAALQAgAGkAbgB0AGUAZwBlAHIAIABzAGUAYwBvAG4AZABcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAA0ACAALQAgAHMAZQBjAG8AbgBkACAAMAAuADAAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAANQAgAC0AIABzAGUAYwBvAG4AZAAgADAALgAwADAAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAANgAgAC0AIABzAGUAYwBvAG4AZAAgADAALgAwADAAMABcAG4AIAAgADMAIAB8ACAARgBvAHIAbQBhAHQAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxACAALQAgAGIAYQBzAGkAYwBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAyACAALQAgAGUAeAB0AGUAbgBkAGUAZABcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAzACAALQAgAGMAbwBuAHMAaQBzAHQAZQBuAHQAIAB3AGkAdABoACAAYgBhAHMAaQBjACAAbwByACAAZQB4AHQAZQBuAGQAZQBkAFwAbgAgACAANAAgAHwAIABIAG8AdQByACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADAALgAuADIANABcAG4AIAAgADUAIAB8ACAATQBpAG4AdQB0AGUAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAwAC4ALgA1ADkAXABuACAAIAA2ACAAfAAgAFMAZQBjAG8AbgBkACAAIAAgACAAIAAgACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAMAAuAC4ANQA5AC4AOQA5ADkAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBUAGUAeAB0ACAAIAAgACAAIAAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAB8ACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQAdABlAGQAIAB0AGkAbQBlAC4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgAHwAIABFAHgAYQBtAHAAbABlACAAZgBvAHIAbQBhAHQAcwA6AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAAVABoAGgAOgBtAG0AOgBzAHMALgBzAHMAcwAsACAAVABoAGgAOgBtAG0AOgBzAHMALAAgAFQAaABoAG0AbQAsACAAVABoAGgAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAFAAQQBSAFMARQBfAFQASQBNAEUAIAA9ACAATABBAE0AQgBEAEEAKABUAGUAeAB0ACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBsAHUAbQBuAHMAOgAgAEgAYQBzAGgALAAgAFAAcgBlAGMAaQBzAGkAbwBuACwAIABGAG8AcgBtAGEAdAAsACAATQBpAG4AdQB0AGUAUABvAHMALAAgAFMAZQBjAG8AbgBkAEwAZQBuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAdwBoAGUAcgBlACAASABhAHMAaAAgAD0AIAAoAEwARQBOACAAKgAgADQAMAA5ADYAKQAgACsAIAAoAEMAbwBsAG8AbgAxAFAAbwBzACAAKgAgADIANQA2ACkAIAArACAAKABDAG8AbABvAG4AMgBQAG8AcwAgACoAIAAxADYAKQAgACsAIABEAGUAYwBpAG0AYQBsAFAAbwBzACAAXABuACAAIAAgACAAIAAgACAAIABfAGYAbQB0AEgAYQBzAGgAVABhAGIAbABlACwAIAB7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAA4ADEAOQAyACwAIAAxACwAIAAzACwAIAAwACwAIAAwADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEANgAzADgANAAsACAAMgAsACAAMQAsACAAMwAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyADQANQA3ADYALAAgADMALAAgADEALAAgADMALAAgADIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwAyADcANwA1ACwAIAA0ACwAIAAxACwAIAAzACwAIAA0ADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMANgA4ADcAMQAsACAANQAsACAAMQAsACAAMwAsACAANQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAA0ADAAOQA2ADcALAAgADYALAAgADEALAAgADMALAAgADYAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAxADIANAA4ACwAIAAyACwAIAAyACwAIAA0ACwAIAAwADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMAMwA2ADMAMgAsACAAMwAsACAAMgAsACAANAAsACAAMgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAA0ADEAOAAzADMALAAgADQALAAgADIALAAgADQALAAgADQAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAANAA1ADkAMgA5ACwAIAA1ACwAIAAyACwAIAA0ACwAIAA1ADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMAAwADIANQAsACAANgAsACAAMgAsACAANAAsACAANgBcAG4AIAAgACAAIAAgACAAIAAgAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAsACAATABBAE0AQgBEAEEAKABfAGUAeABjAGUAcAB0AGkAbwBuACwAIABbAF8AcAByAGUAYwBpAHMAaQBvAG4AXQAsACAAWwBfAGUAeAB0AGUAbgBkAGUAZABdACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAF8AZQB4AGMAZQBwAHQAaQBvAG4AIAAgAHwAIABzAHQAcgBpAG4AZwAgACAAfAAgAG4AdQBsAGwAIAAgAEUAbQBwAHQAeQAgAHQAZQB4AHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE4ALwBBACAAIAAgAFUAbgBhAGIAbABlACAAdABvACAAcABhAHIAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABWAEEATABVAEUAIABJAG4AdgBhAGwAaQBkACAAdgBhAGwAdQBlAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFAAcgBlAGMAaQBzAGkAbwBuACAAbwBmACAAcABhAHIAcwBlAGQAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAdABlAG4AZABlAGQAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUABhAHIAcwBlAGQAIABlAHgAdABlAG4AZABlAGQAIABmAG8AcgBtAGEAdABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBOAC8AQQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsARgBBAEwAUwBFACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBWAEEATABVAEUAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAEYAQQBMAFMARQAsACAAMAAsACAATgAoAF8AZQB4AHQAZQBuAGQAZQBkACkALAAgAHsAIwBWAEEATABVAEUAIQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABGAEEATABTAEUALAAgADAALAAgAE4AKABfAGUAeAB0AGUAbgBkAGUAZAApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgAFwAIgBcACIAfQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALAAgAC8ALwBfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABGAEEATABTAEUALAAgADAALAAgAE4AKABfAGUAeAB0AGUAbgBkAGUAZAApACwAIAB7ACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEALAAgACMAVgBBAEwAVQBFACEAfQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBBAHIAcgBhAHkALAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHgAdAAgAD0AIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIAZQBtAG8AdgBlAGQALAAgAFIARQBEAFUAQwBFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBoAGEAcgBBAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABfAGEAYwBjACwAIABfAGMAdQByAHIALAAgAFMAVQBCAFMAVABJAFQAVQBUAEUAKABfAGEAYwBjACwAIABfAGMAdQByAHIALAAgAFwAIgBcACIAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAE4AKABUAGUAeAB0ACkAIAAtACAATABFAE4AKABfAHIAZQBtAG8AdgBlAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEYAaQBuAGQATgB0AGgAQwBoAGEAcgBQAG8AcwAsACAATABBAE0AQgBEAEEAKABDAGgAYQByAHMALAAgAFQAZQB4AHQALAAgAE4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAQwBvAHUAbgB0ACwAIABMAEUATgAoAEMAaABhAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuACwAIABJAE4AVAAoAE4AKABOACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABfAGMAaABhAHIAQwBvAHUAbgB0ACAAPQAgADAAKQAgACsAIAAoAF8AbgAgAD0AIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgBzACwAIABNAEkARAAoAEMAaABhAHIAcwAsACAAUwBFAFEAVQBFAE4AQwBFACgAMQAsACAAXwBjAGgAYQByAEMAbwB1AG4AdAApACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAGkAbgBkAEMAbwB1AG4AdAAsACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMAKABfAGMAaABhAHIAcwAsACAAVABlAHgAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAG4AZABDAG8AdQBuAHQAIAA8ACAAQQBCAFMAKABfAG4AKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbgB0AGgAIABjAGEAbgAgAGMAbwB1AG4AdAAgAGYAcgBvAG0AIABlAG4AZAAgAGIAYQBjAGsAdwBhAHIAZABzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAHQAaAAsACAASQBGACgAXwBuACAAPgAgADAALAAgAF8AbgAsACAAXwBmAGkAbgBkAEMAbwB1AG4AdAAgACsAIABfAG4AIAArACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AdABoAFAAbwBzACwAIABSAEUARABVAEMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEEATQBCAEQAQQAoAF8AYQBjAGMALAAgAF8AYwB1AHIAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGMAYwAgADwAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAtADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBlAHgAdABQAG8AcwBDAGgAYQByAHMALAAgAEkARgBFAFIAUgBPAFIAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAEkATgBEACgAXwBjAGgAYQByAHMALAAgAFQAZQB4AHQALAAgAF8AYQBjAGMAIAArACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AZQB4AHQAUABvAHMALAAgAE0ASQBOACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAEwAVABFAFIAKABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACAAPgAgADAALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAG4AZQB4AHQAUABvAHMAIAA9ACAAMAAsACAALQAxACwAIABfAG4AZQB4AHQAUABvAHMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE0AQQBYACgAXwBuAHQAaABQAG8AcwAsACAAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABUAGUAeAB0ACAAPQAgAFwAIgBcACIALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAFYAQQBMAEkARABBAFQARQBfAEMASABBAFIAQQBDAFQARQBSAFMAKABUAGUAeAB0ACwAIAAyACkAKQAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AVABwAG8AcwAsACAASQBGAEUAUgBSAE8AUgAoAEYASQBOAEQAKABcACIAVABcACIALAAgAFQAZQB4AHQAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAFQAcABvAHMAIAA+ACAAMQAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAE4ALwBBAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFQAaQBtAGUALAAgAEkARgAoAF8AVABwAG8AcwAgAD0AIAAxACwAIABSAEkARwBIAFQAKABUAGUAeAB0ACwAIABMAEUATgAoAFQAZQB4AHQAKQAgAC0AIAAxACkALAAgAFQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4ALAAgAEwARQBOACgAXwBzAFQAaQBtAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGwAbwBuADEAUABvAHMALAAgAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXAAiADoAXAAiACwAIABfAHMAVABpAG0AZQApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAbwBsAG8AbgAyAFAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgA6AFwAIgAsACAAXwBzAFQAaQBtAGUALAAgAF8AYwBvAGwAbwBuADEAUABvAHMAIAArACAAMQApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAZQBjAGkAbQBhAGwAUABvAHMALAAgAGYAbgBGAGkAbgBkAE4AdABoAEMAaABhAHIAUABvAHMAKABcACIALgAsAFwAIgAsACAAXwBzAFQAaQBtAGUALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAaAAsACAAKABfAGwAZQBuACAAKgAgADQAMAA5ADYAKQAgACsAIAAoAF8AYwBvAGwAbwBuADEAUABvAHMAIAAqACAAMgA1ADYAKQAgACsAIAAoAF8AYwBvAGwAbwBuADIAUABvAHMAIAAqACAAMQA2ACkAIAArACAAXwBkAGUAYwBpAG0AYQBsAFAAbwBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAGEAcwBoAEwAawB1AHAALAAgAEkARgBOAEEAKABYAE0AQQBUAEMASAAoAF8AaABhAHMAaAAsACAAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAF8AZgBtAHQASABhAHMAaABUAGEAYgBsAGUALAAgADEAKQAsACAAMAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGgAYQBzAGgATABrAHUAcAAgAD0AIAAwACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIATgAvAEEAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGYAbgAsACAAQwBIAE8ATwBTAEUAUgBPAFcAUwAoAF8AZgBtAHQASABhAHMAaABUAGEAYgBsAGUALAAgAF8AaABhAHMAaABMAGsAdQBwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAsACAASQBOAEQARQBYACgAXwBkAGUAZgBuACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAdABlAG4AZABlAGQALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgAsACAAVgBBAEwAVQBFACgATABFAEYAVAAoAF8AcwBUAGkAbQBlACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0AaQBuAHUAdABlACwAIABJAEYAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPAAgADIALAAgAFwAIgBcACIALAAgAFYAQQBMAFUARQAoAE0ASQBEACgAXwBzAFQAaQBtAGUALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAANAApACwAIAAyACkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMATABlAG4ALAAgAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAANQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBlAGMAbwBuAGQALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgADwAIAAzACwAIABcACIAXAAiACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVgBBAEwAVQBFACgAUgBJAEcASABUACgAXwBzAFQAaQBtAGUALAAgAF8AcwBlAGMATABlAG4AKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAALwAvACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD4AIAAzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAYwBhAG4AbwB0ACAAYQBzAHMAdQBtAGUAIABWAEEATABVAEUAIABmAHUAbgBjAHQAaQBvAG4AIAB3AGkAbABsACAAdQBzAGUAIABkAGUAYwBpAG0AYQBsACAAYwBoAGEAcgBhAGMAdABlAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAHcAaABlAG4AIABFAHgAYwBlAGwAIABoAGEAcwAgAG4AbwBuAC0AZQBuAGcAbABpAHMAaAAgAFIAZQBnAGkAbwBuAGEAbAAgAHMAZQB0AHQAaQBuAGcAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFMAZQBjACwAIABSAEkARwBIAFQAKABfAHMAVABpAG0AZQAsACAAXwBzAGUAYwBMAGUAbgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBuAHQAUwBlAGMALAAgAFYAQQBMAFUARQAoAEwARQBGAFQAKABfAHMAUwBlAGMALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgByAGEAYwBTAGUAYwAsACAAVgBBAEwAVQBFACgAUgBJAEcASABUACgAXwBzAFMAZQBjACwAIABfAHMAZQBjAEwAZQBuACAALQAgADMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGMAaQBtAGEAbABCAGEAcwBlACwAIABJAE4ARABFAFgAKAB7ADEAMAAsACAAMQAwADAALAAgADEAMAAwADAAfQAsACAAMQAgACwAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAC0AIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAG4AdABTAGUAYwAgACsAIAAoAF8AZgByAGEAYwBTAGUAYwAgAC8AIABfAGQAZQBjAGkAbQBhAGwAQgBhAHMAZQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAKABfAGgAbwB1AHIALAAgAF8AbQBpAG4AdQB0AGUALAAgAF8AcwBlAGMAbwBuAGQAKQApACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIAVgBBAEwAVQBFAFwAIgAsACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAsACAAXwBlAHgAdABlAG4AZABlAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAKABfAFQAcABvAHMAIAA9ACAAMQApACwAIABfAHAAcgBlAGMAaQBzAGkAbwBuACwAIABfAGUAeAB0AGUAbgBkAGUAZAAsACAAXwBoAG8AdQByACwAIABfAG0AaQBuAHUAdABlACwAIABfAHMAZQBjAG8AbgBkACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFAAQQBSAFMARQBfAFQASQBNAEUAXwBaAE8ATgBFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAHQAaABlACAAdABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAMQAgAHwAIABJAFMATwBDAG8AbQBwAGwAaQBhAG4AdAAgACAAfAAgAGIAbwBvAGwAZQBhAG4AIAB8ACAARgBsAGEAZwAgAGkAZgAgAGMAbwBtAHAAbABpAGEAbgB0ACAAdABvACAASQBTAE8AIAA4ADYAMAAxACAAcwB0AGEAbgBkAGEAcgBkAFwAbgAgACAAMgAgAHwAIABQAHIAZQBjAGkAcwBpAG8AbgAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMAAgAC0AIABpAG4AdgBhAGwAaQBkACAAdgBhAGwAdQBlAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMQAgAC0AIABoAG8AdQByAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMgAgAC0AIABtAGkAbgB1AHQAZQBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADMAIAAtACAAcwBlAGMAbwBuAGQAXABuACAAIAAzACAAfAAgAEYAbwByAG0AYQB0ACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxACAALQAgAGIAYQBzAGkAYwBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADIAIAAtACAAZQB4AHQAZQBuAGQAZQBkAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMwAgAC0AIABjAG8AbgBzAGkAcwB0AGUAbgB0ACAAdwBpAHQAaAAgAGIAYQBzAGkAYwAgAG8AcgAgAGUAeAB0AGUAbgBkAGUAZABcAG4AIAAgADUAIAB8ACAATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAC0AOQAwADAALgAuACsAOQAwADAAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBUAGUAeAB0ACAAIAAgACAAIAAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAB8ACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQAdABlAGQAIAB0AGkAbQBlACAAegBvAG4AZQAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAB8ACAARQB4AGEAbQBwAGwAZQAgAGYAbwByAG0AYQB0AHMAOgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAfAAgACsAaABoADoAbQBtACwAIAArAGgAaABtAG0ALAAgAC0AaABoACwAIABaAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBQAEEAUgBTAEUAXwBUAEkATQBFAF8AWgBPAE4ARQAgAD0AIABMAEEATQBCAEQAQQAoAFQAZQB4AHQALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAQwBvAGwAdQBtAG4AcwA6ACAASABhAHMAaAAsACAAUAByAGUAYwBpAHMAaQBvAG4ALAAgAEUAeAB0AGUAbgBkAGUAZAAsACAAWgAsACAATQBpAG4AUABvAHMAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAB3AGgAZQByAGUAIABoAGEAcwBoACAAPQAgAEwARQBOACAAKgAgADEAMAAyADQAIAArACAAWgBvAG4AbAB5ACAAKgAgADUAMQAyACAAKwAgAEwAYQBzAHQAUwBpAGcAbgBQAG8AcwBBAHQAMQAgACoAMgA1ADYAIAArACAAQwBvAGwAbwBuADEAUABvAHMAIAAqACAAMQA2ACAAKwAgAEMAbwBsAG8AbgAyAFAAbwBzAFwAbgAgACAAIAAgACAAIAAgACAAXwBmAG0AdABIAGEAcwBoAFQAYQBiAGwAZQAsACAAewBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQA1ADMANgAsACAAMwAsACAAMwAsACAAMQAsACAAMAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAzADMAMgA4ACwAIAAxACwAIAAzACwAIAAwACwAIAAwADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADUAMwA3ADYALAAgADIALAAgADEALAAgADAALAAgADQAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAANgA0ADYANAAsACAAMgAsACAAMgAsACAAMAAsACAANQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAA3ADQAMgA0ACwAIAAzACwAIAAxACwAIAAwACwAIAA0ADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADkANQA0ADMALAAgADMALAAgADIALAAgADAALAAgADUAXABuACAAIAAgACAAIAAgACAAIAB9ACwAXABuACAAIAAgACAAIAAgACAAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4ALAAgAEwAQQBNAEIARABBACgAXwBlAHgAYwBlAHAAdABpAG8AbgAsACAAWwBfAGUAeAB0AGUAbgBkAGUAZABdACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAF8AZQB4AGMAZQBwAHQAaQBvAG4AIAAgAHwAIABzAHQAcgBpAG4AZwAgACAAfAAgAG4AdQBsAGwAIAAgAEUAbQBwAHQAeQAgAHQAZQB4AHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE4ALwBBACAAIAAgAFUAbgBhAGIAbABlACAAdABvACAAcABhAHIAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABWAEEATABVAEUAIABJAG4AdgBhAGwAaQBkACAAdgBhAGwAdQBlAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAF8AZQB4AHQAZQBuAGQAZQBkACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFAAYQByAHMAZQBkACAAZQB4AHQAZQBuAGQAZQBkACAAZgBvAHIAbQBhAHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIATgAvAEEAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AEYAQQBMAFMARQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIAVgBBAEwAVQBFAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABGAEEATABTAEUALAAgADAALAAgAE4AKABfAGUAeAB0AGUAbgBkAGUAZAApACwAIAB7ACMAVgBBAEwAVQBFACEAfQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBDAG8AdQBuAHQAQwBoAGEAcgBzACwAIABMAEEATQBCAEQAQQAoAEMAaABhAHIAQQByAHIAYQB5ACwAIABUAGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQAIAA9ACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwByAGUAbQBvAHYAZQBkACwAIABSAEUARABVAEMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEMAaABhAHIAQQByAHIAYQB5ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwAQQBNAEIARABBACgAXwBhAGMAYwAsACAAXwBjAHUAcgByACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAXwBhAGMAYwAsACAAXwBjAHUAcgByACwAIABcACIAXAAiACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBOACgAVABlAHgAdAApACAALQAgAEwARQBOACgAXwByAGUAbQBvAHYAZQBkACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBGAGkAbgBkAE4AdABoAEMAaABhAHIAUABvAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBzACwAIABUAGUAeAB0ACwAIABOACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByAEMAbwB1AG4AdAAsACAATABFAE4AKABDAGgAYQByAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgAsACAASQBOAFQAKABOACgATgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBjAGgAYQByAEMAbwB1AG4AdAAgAD0AIAAwACkAIAArACAAKABfAG4AIAA9ACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAaABhAHIAcwAsACAATQBJAEQAKABDAGgAYQByAHMALAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AYwBoAGEAcgBDAG8AdQBuAHQAKQAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAG4AZABDAG8AdQBuAHQALAAgAGYAbgBDAG8AdQBuAHQAQwBoAGEAcgBzACgAXwBjAGgAYQByAHMALAAgAFQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAaQBuAGQAQwBvAHUAbgB0ACAAPAAgAEEAQgBTACgAXwBuACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG4AdABoACAAYwBhAG4AIABjAG8AdQBuAHQAIABmAHIAbwBtACAAZQBuAGQAIABiAGEAYwBrAHcAYQByAGQAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgB0AGgALAAgAEkARgAoAF8AbgAgAD4AIAAwACwAIABfAG4ALAAgAF8AZgBpAG4AZABDAG8AdQBuAHQAIAArACAAXwBuACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAHQAaABQAG8AcwAsACAAUgBFAEQAVQBDAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAUQBVAEUATgBDAEUAKAAxACwAIABfAG4AdABoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABfAGEAYwBjACwAIABfAGMAdQByAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYQBjAGMAIAA8ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABJAEYARQBSAFIATwBSACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAE4ARAAoAF8AYwBoAGEAcgBzACwAIABUAGUAeAB0ACwAIABfAGEAYwBjACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAeAB0AFAAbwBzACwAIABNAEkATgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBMAFQARQBSACgAXwBuAGUAeAB0AFAAbwBzAEMAaABhAHIAcwAsACAAXwBuAGUAeAB0AFAAbwBzAEMAaABhAHIAcwAgAD4AIAAwACwAIAAwACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBuAGUAeAB0AFAAbwBzACAAPQAgADAALAAgAC0AMQAsACAAXwBuAGUAeAB0AFAAbwBzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABNAEEAWAAoAF8AbgB0AGgAUABvAHMALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFQAZQB4AHQAIAA9ACAAXAAiAFwAIgAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4ATwBUACgAVgBBAEwASQBEAEEAVABFAF8AQwBIAEEAUgBBAEMAVABFAFIAUwAoAFQAZQB4AHQALAAgADMAKQApACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIATgAvAEEAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgAsACAATABFAE4AKABUAGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AWgBvAG4AbAB5ACwAIABOACgAKABfAGwAZQBuACAAPQAgADEAKQAgACoAIAAoAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXAAiAFoAXAAiACwAIABUAGUAeAB0ACkALAAgADAAKQAgAD0AIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGEAcwB0AFMAaQBnAG4AUABvAHMAQQB0ADEALAAgAE4AKABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiACsALQBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAsACAAVABlAHgAdAAsACAALQAxACkAIAA9ACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGMAbwBsAG8AbgAxAFAAbwBzACwAIABJAEYARQBSAFIATwBSACgARgBJAE4ARAAoAFwAIgA6AFwAIgAsACAAVABlAHgAdAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBvAGwAbwBuADIAUABvAHMALAAgAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXAAiADoAXAAiACwAIABUAGUAeAB0ACwAIABfAGMAbwBsAG8AbgAxAFAAbwBzACAAKwAgADEAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAGgALAAgACgAXwBsAGUAbgAgACoAIAAxADAAMgA0ACkAIAArACAAKABfAFoAbwBuAGwAeQAgACoAIAA1ADEAMgApACAAKwAgACgAXwBsAGEAcwB0AFMAaQBnAG4AUABvAHMAQQB0ADEAIAAqACAAMgA1ADYAKQAgACsAIAAoAF8AYwBvAGwAbwBuADEAUABvAHMAIAAqACAAMQA2ACkAIAArACAAXwBjAG8AbABvAG4AMgBQAG8AcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAGEAcwBoAEwAawB1AHAALAAgAEkARgBOAEEAKABYAE0AQQBUAEMASAAoAF8AaABhAHMAaAAsACAAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAF8AZgBtAHQASABhAHMAaABUAGEAYgBsAGUALAAgADEAKQAsACAAMAApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AaABhAHMAaABMAGsAdQBwACAAPQAgADAALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBOAC8AQQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABlAGYAbgAsACAAQwBIAE8ATwBTAEUAUgBPAFcAUwAoAF8AZgBtAHQASABhAHMAaABUAGEAYgBsAGUALAAgAF8AaABhAHMAaABMAGsAdQBwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZQB4AHQAZQBuAGQAZQBkACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkATgBEAEUAWAAoAF8AZABlAGYAbgAsACAAMQAsACAANAApACAAPgAgADAALAAgAC8ALwAgAFoAIABvAG4AbAB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABUAFIAVQBFACwAIABfAHAAcgBlAGMAaQBzAGkAbwBuACwAIABfAGUAeAB0AGUAbgBkAGUAZAAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4ALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAEYAVAAoAFQAZQB4AHQALAAgADEAKQAgAD0AIABcACIALQBcACIALAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFUATgBJAEMATwBEAEUAKABMAEUARgBUACgAVABlAHgAdAAsACAAMQApACkAIAA9ACAAOAA3ADIAMgAsACAALQAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAMQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAbwB1AHIALAAgAF8AcwBpAGcAbgAgACoAIABWAEEATABVAEUAKABNAEkARAAoAFQAZQB4AHQALAAgADIALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUALAAgAEkARgAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA8ACAAMgAsACAAXAAiAFwAIgAsACAAVgBBAEwAVQBFACgATQBJAEQAKABUAGUAeAB0ACwAIABJAE4ARABFAFgAKABfAGQAZQBmAG4ALAAgADEALAAgADUAKQAsACAAMgApACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkACwAIABJAEYAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPAAgADMALAAgAFwAIgBcACIALAAgAFYAQQBMAFUARQAoAFIASQBHAEgAVAAoAFQAZQB4AHQALAAgADIAKQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwBNAGkAbgB1AHQAZQBzACwAIABJAE4AVAAoACgATgAoAF8AaABvAHUAcgApACAAKgAgADMANgAwADAAKQAgACsAIAAoAE4AKABfAG0AaQBuAHUAdABlACkAIAAqACAANgAwACkAIAArACAATgAoAF8AcwBlAGMAbwBuAGQAKQApACAALwAgADYAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAXwBaAE8ATgBFACgAXwB0AHoAbwBNAGkAbgB1AHQAZQBzACkAKQAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAFYAQQBMAFUARQBcACIALAAgAF8AZQB4AHQAZQBuAGQAZQBkACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFQAUgBVAEUALAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAF8AZQB4AHQAZQBuAGQAZQBkACwAIABfAHQAegBvAE0AaQBuAHUAdABlAHMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8AUABBAFIAVABTAFwAbgBcAG4AUwBwAGwAaQB0AHMAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAB0AGUAZAAgAHQAZQB4AHQAIAB2AGEAbAB1AGUAIABpAG4AdABvACAAaQBuAHQAbwAgAHIAZQBzAHAAZQBjAHQAaQB2AGUAIABwAGEAcgB0AHMAIABvAGYAIABkAGEAdABlACwAIAB0AGkAbQBlACAAYQBuAGQAIAB0AGkAbQBlACAAegBvAG4AZQAuAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAIAAxACAAfAAgAEkAUwBPAEMAbwBtAHAAbABpAGEAbgB0ACAAfAAgAGIAbwBvAGwAZQBhAG4AIAB8ACAARgBsAGEAZwAgAGkAZgAgAGMAbwBtAHAAbABpAGEAbgB0ACAAdABvACAASQBTAE8AIAA4ADYAMAAxACAAcwB0AGEAbgBkAGEAcgBkAFwAbgAgACAAMgAgAHwAIABQAGEAcgB0AHMAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEIAaQB0AGYAbABhAGcAIABvAGYAIABwAGEAcgB0AHMAIAAwAC4ALgA3AFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADAAeAAwADQAIAAtACAAZABhAHQAZQBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAwAHgAMAAyACAALQAgAHQAaQBtAGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMAB4ADAAMQAgAC0AIAB0AGkAbQBlACAAegBvAG4AZQBcAG4AIAAgADMAIAB8ACAARABhAHQAZQAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAAgAHwAXABuACAAIAA0ACAAfAAgAFQAaQBtAGUAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdAByAGkAbgBnACAAIAB8AFwAbgAgACAANQAgAHwAIABUAGkAbQBlACAAWgBvAG4AZQAgACAAIAAgAHwAIABzAHQAcgBpAG4AZwAgACAAfABcAG4AIAAgACAAIAAgACAAXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFQAZQB4AHQAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdAByAGkAbgBnACAAfAAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AHQAZQBkACAAdgBhAGwAdQBlACAAZgBvAHIAIABkAGEAdABlACwAIAB0AGkAbQBlACAAbwByACAAdABpAG0AZQAgAHoAbwBuAGUALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4AUABBAFIAUwBFAF8AUABBAFIAVABTACAAPQAgAEwAQQBNAEIARABBACgAVABlAHgAdAAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAsACAATABBAE0AQgBEAEEAKABfAGUAeABjAGUAcAB0AGkAbwBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAF8AZQB4AGMAZQBwAHQAaQBvAG4AIAAgAHwAIABzAHQAcgBpAG4AZwAgACAAfAAgAG4AdQBsAGwAIAAgAEUAbQBwAHQAeQAgAHQAZQB4AHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE4ALwBBACAAIAAgAFUAbgBhAGIAbABlACAAdABvACAAcABhAHIAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBOAC8AQQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AEYAQQBMAFMARQAsACAAMAAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAewBcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiACwAIABcACIAXAAiAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEMAbwB1AG4AdABDAGgAYQByAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBBAHIAcgBhAHkALAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABlAHgAdAAgAD0AIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHIAZQBtAG8AdgBlAGQALAAgAFIARQBEAFUAQwBFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAZQB4AHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBoAGEAcgBBAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABfAGEAYwBjACwAIABfAGMAdQByAHIALAAgAFMAVQBCAFMAVABJAFQAVQBUAEUAKABfAGEAYwBjACwAIABfAGMAdQByAHIALAAgAFwAIgBcACIAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAE4AKABUAGUAeAB0ACkAIAAtACAATABFAE4AKABfAHIAZQBtAG8AdgBlAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBGAGkAbgBkAE4AdABoAEMAaABhAHIAUABvAHMALAAgAEwAQQBNAEIARABBACgAQwBoAGEAcgBzACwAIABUAGUAeAB0ACwAIABOACwAIABbAFMAdABhAHIAdABQAG8AcwBdACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAE4AKABTAHQAYQByAHQAUABvAHMAKQAgAD4AIABMAEUATgAoAFQAZQB4AHQAKQAsACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGYAcgBvAG0AUABvAHMALAAgAEkARgAoAE4AKABTAHQAYQByAHQAUABvAHMAKQAgADwAPQAgADAALAAgADAALAAgAE4AKABTAHQAYQByAHQAUABvAHMAKQAgAC0AIAAxACkALAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGUAeAB0ACwAIABJAEYAKABfAGYAcgBvAG0AUABvAHMAIAA9ACAAMAAsACAAVABlAHgAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAEkARwBIAFQAKABUAGUAeAB0ACwAIABMAEUATgAoAFQAZQB4AHQAKQAgAC0AIABfAGYAcgBvAG0AUABvAHMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBoAGEAcgBDAG8AdQBuAHQALAAgAEwARQBOACgAQwBoAGEAcgBzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgAsACAASQBOAFQAKABOACgATgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoACgAXwBjAGgAYQByAEMAbwB1AG4AdAAgAD0AIAAwACkAIAArACAAKABfAG4AIAA9ACAAMAApACwAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBjAGgAYQByAHMALAAgAE0ASQBEACgAQwBoAGEAcgBzACwAIABTAEUAUQBVAEUATgBDAEUAKAAxACwAIABfAGMAaABhAHIAQwBvAHUAbgB0ACkALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZgBpAG4AZABDAG8AdQBuAHQALAAgAGYAbgBDAG8AdQBuAHQAQwBoAGEAcgBzACgAXwBjAGgAYQByAHMALAAgAF8AdABlAHgAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBmAGkAbgBkAEMAbwB1AG4AdAAgADwAIABBAEIAUwAoAF8AbgApACwAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABuAHQAaAAgAGMAYQBuACAAYwBvAHUAbgB0ACAAZgByAG8AbQAgAGUAbgBkACAAYgBhAGMAawB3AGEAcgBkAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgB0AGgALAAgAEkARgAoAF8AbgAgAD4AIAAwACwAIABfAG4ALAAgAF8AZgBpAG4AZABDAG8AdQBuAHQAIAArACAAXwBuACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AdABoAFAAbwBzACwAIABSAEUARABVAEMARQAoADAALAAgAFMARQBRAFUARQBOAEMARQAoADEALAAgAF8AbgB0AGgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwAQQBNAEIARABBACgAXwBhAGMAYwAsACAAXwBjAHUAcgByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGEAYwBjACAAPAAgADAALAAgAC0AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBlAHgAdABQAG8AcwBDAGgAYQByAHMALAAgAEkARgBFAFIAUgBPAFIAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYASQBOAEQAKABfAGMAaABhAHIAcwAsACAAXwB0AGUAeAB0ACwAIABfAGEAYwBjACAAKwAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAeAB0AFAAbwBzACwAIABNAEkATgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBJAEwAVABFAFIAKABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACwAIABfAG4AZQB4AHQAUABvAHMAQwBoAGEAcgBzACAAPgAgADAALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBuAGUAeAB0AFAAbwBzACAAPQAgADAALAAgAC0AMQAsACAAXwBuAGUAeAB0AFAAbwBzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBuAHQAaABQAG8AcwAgAD4AIAAwACwAIABfAG4AdABoAFAAbwBzACAAKwAgAF8AZgByAG8AbQBQAG8AcwAgACwAIAAwACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAMQAgAC0AIABUACAAZgBpAHIAcwB0ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAgAD0AIABBAHQAIABmAGkAcgBzAHQAIABwAG8AcwBpAHQAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACAAPQAgAEEAZgB0AGUAcgAgAGYAaQByAHMAdAAgAHAAbwBzAGkAdABpAG8AbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgADIAIAAtACAAVABaACAAbQBhAHIAawBlAHIAIABhAGYAdABlAHIAIABUACAAIAAgADAAIAA9ACAATgBvACAAcwBpAGcAbgAgAG8AcgAgAFoAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACAAPQAgAEYAaQByAHMAdAAgAHAAbwBzAGkAdABpAG8AbgAgAGYAbwBsAGwAbwB3AGkAbgBnACAAVABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIAIAA9ACAAQQBmAHQAZQByACAAZgBpAHIAcwB0ACAAcABvAHMAaQB0AGkAbwBuACAAZgBvAGwAbABvAHcAaQBuAGcAIABUAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAMwAgAC0AIABQAGEAcgB0AHMAIABiAGkAdAAgAGYAbABhAGcAIAAgACAAIAAgACAAMAB4ADAANAAgAC0AIABEAGEAdABlAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAB4ADAAMgAgAC0AIABUAGkAbQBlAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAB4ADAAMQAgAC0AIABUAGkAbQBlACAAWgBvAG4AZQBcAG4AIAAgACAAIAAgACAAIAAgAFcAaQB0AGgAVABfAEwAbwBnAGkAYwAsACAAewBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsACAAMAAsACAAMgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACwAIAAxACwAIAAxADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEALAAgADIALAAgADMAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAsACAAMAAsACAANgA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAIAAxACwAIAA1ADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIALAAgADIALAAgADcAXABuACAAIAAgACAAIAAgACAAIAB9ACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAMQAgAC0AIABUAFoAIABtAGEAcgBrAGUAcgAgAGYAaQByAHMAdAAgACAAIAAgACAAMAAgAD0AIABOAG8AIABzAGkAZwBuACAAbwByACAAWgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEAIAA9ACAARgBpAHIAcwB0ACAAcABvAHMAaQB0AGkAbwBuAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAgAD0AIABBAGYAdABlAHIAIABmAGkAcgBzAHQAIABwAG8AcwBpAHQAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAAyACAALQAgAFQAWgAgAG0AYQByAGsAZQByACAAaQBzACAAWgAgACgAYgBvAG8AbABlAGEAbgApAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAMwAgAC0AIABIAGEAcwAgAEMAbwBsAG8AbgAgACgAYgBvAG8AbABlAGEAbgApAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAANAAgAC0AIABUAGkAbQBlACAAYwBvAG4AZABpAHQAaQBvAG4AcwAgACgAYgBvAG8AbABlAGEAbgApAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAANQAgAC0AIABQAGEAcgB0AHMAIABiAGkAdAAgAGYAbABhAGcAIAAgACAAIAAgACAAMAB4ADAANAAgAC0AIABEAGEAdABlAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAB4ADAAMgAgAC0AIABUAGkAbQBlAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAB4ADAAMQAgAC0AIABUAGkAbQBlACAAWgBvAG4AZQBcAG4AIAAgACAAIAAgACAAIAAgAFcAaQB0AGgAbwB1AHQAVABfAEwAbwBnAGkAYwAsACAAewBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsACAAMAAsACAAMAAsACAAMAAsACAANAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAIAAwACwAIAAwACwAIAAxACwAIAAyADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALAAgADAALAAgADEALAAgADAALAAgADIAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsACAAMAAsACAAMAAsACAAMAAsACAANAA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACwAIAAwACwAIAAwACwAIAAxACwAIAAxADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADEALAAgADAALAAgADEALAAgADAALAAgADEAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsACAAMQAsACAAMAAsACAAMAAsACAAMQA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAIAAwACwAIAAwACwAIAAwACwAIAA0ADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIALAAgADAALAAgADAALAAgADEALAAgADMAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAsACAAMAAsACAAMQAsACAAMAAsACAAMwA7AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAyACwAIAAwACwAIAAxACwAIAAxACwAIAAzADsAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADIALAAgADEALAAgADAALAAgADEALAAgADMAOwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAsACAAMQAsACAAMQAsACAAMAAsACAAMwBcAG4AIAAgACAAIAAgACAAIAAgAH0ALABcAG4AXABuACAAIAAgACAAIAAgACAAIABmAG4AVwBpAHQAaABUAF8AUABhAHIAdABzAEwAZQBuACwAIABMAEEATQBCAEQAQQAoAF8AVABwAG8AcwAsACAAXwBUAGYAaQByAHMAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbABlAG4ALAAgAEwARQBOACgAVABlAHgAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGYAdABlAHIAVAAsACAAUgBJAEcASABUACgAVABlAHgAdAAsACAAXwBsAGUAbgAgAC0AIABfAFQAcABvAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AVABaAG0AYQByAGsAZQByAFAAbwBzACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiAFoAKwAtAFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAIABfAGEAZgB0AGUAcgBUACwAIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFQAWgBtAGEAcgBrAEYAaQByAHMAdAAsACAASQBGACgAXwBUAFoAbQBhAHIAawBlAHIAUABvAHMAIAA+ACAAMQAsACAAMgAsACAAXwBUAFoAbQBhAHIAawBlAHIAUABvAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABzAEYAbABhAGcALAAgAEYASQBMAFQARQBSACgAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAFcAaQB0AGgAVABfAEwAbwBnAGkAYwAsACAAMwApACwAIAAoAEMASABPAE8AUwBFAEMATwBMAFMAKABXAGkAdABoAFQAXwBMAG8AZwBpAGMALAAgADEAKQAgAD0AIABfAFQAZgBpAHIAcwB0ACkAIAAqACAAKABDAEgATwBPAFMARQBDAE8ATABTACgAVwBpAHQAaABUAF8ATABvAGcAaQBjACwAIAAyACkAIAA9ACAAXwBUAFoAbQBhAHIAawBGAGkAcgBzAHQAKQAsACAAIwBOAC8AQQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgASQBTAE4AQQAoAF8AcABhAHIAdABzAEYAbABhAGcAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKAAjAE4ALwBBACwAIAAwACwAIAAwACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBMAGUAbgAsACAAXwBUAHAAbwBzACAALQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlAEwAZQBuACwAIABJAEYAKABCAEkAVABBAE4ARAAoAF8AcABhAHIAdABzAEYAbABhAGcALAAgADIAKQAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAQgBJAFQAQQBOAEQAKABfAHAAYQByAHQAcwBGAGwAYQBnACwAIAAxACkAIAA9ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBUAFoAbQBhAHIAawBlAHIAUABvAHMAIAAtACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgAgAC0AIABfAFQAcABvAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoATABlAG4ALAAgAF8AbABlAG4AIAAtACAAXwBUAHAAbwBzACAALQAgAF8AdABpAG0AZQBMAGUAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AcABhAHIAdABzAEYAbABhAGcALAAgAF8AZABhAHQAZQBMAGUAbgAsACAAXwB0AGkAbQBlAEwAZQBuACwAIABfAHQAegBMAGUAbgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBXAGkAdABoAG8AdQB0AFQAXwBQAGEAcgB0AHMATABlAG4ALAAgAEwAQQBNAEIARABBACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgAsACAATABFAE4AKABUAGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFQAWgBtAGEAcgBrAFAAbwBzACwAIABmAG4ARgBpAG4AZABOAHQAaABDAGgAYQByAFAAbwBzACgAXAAiAFoAKwAtAFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACwAIABUAGUAeAB0ACwAIAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AVABaAG0AYQByAGsARgBpAHIAcwB0ACwAIABJAEYAKABfAFQAWgBtAGEAcgBrAFAAbwBzACAAPgAgADEALAAgADIALAAgAF8AVABaAG0AYQByAGsAUABvAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AVABaAG0AYQByAGsASQBzAFoALAAgAEkARgAoAF8AVABaAG0AYQByAGsAUABvAHMAIAA+ACAAMAAsACAATgAoAEMATwBEAEUAKABNAEkARAAoAFQAZQB4AHQALAAgAF8AVABaAG0AYQByAGsAUABvAHMALAAgADEAKQApACAAPQAgADkAMAApACwAIAAwACkALAAgAC8ALwAgAEMATwBEAEUAKABcACIAWgBcACIAKQAgAD0AIAA5ADAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAEgAYQBzAEMAbwBsAG8AbgAsACAATgAoAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXAAiADoAXAAiACwAIABUAGUAeAB0ACkALAAgADAAKQAgAD4AIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuAEIAZQBmAG8AcgBlAFQAWgAsACAASQBGACgAXwBUAFoAbQBhAHIAawBGAGkAcgBzAHQAIAA9ACAAMAAsACAAXwBsAGUAbgAsACAAXwBUAFoAbQBhAHIAawBQAG8AcwAgAC0AIAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUAQwBvAG4AZABpAHQAaQBvAG4AYQBsACwAIABJAEYAKABfAFQAWgBtAGEAcgBrAEYAaQByAHMAdAAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGwAZQBuAEEAZgB0AGUAcgBUAFoALAAgAF8AbABlAG4AIAAtACAAXwBUAFoAbQBhAHIAawBQAG8AcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAF8AbABlAG4AQQBmAHQAZQByAFQAWgAgAD0AIAAyACwAIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBsAGUAbgBBAGYAdABlAHIAVABaACAAPQAgADYALAAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAF8AbABlAG4AQgBlAGYAbwByAGUAVABaACAAPQAgADIAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBtAGEAdABjAGgALAAgACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAEMASABPAE8AUwBFAEMATwBMAFMAKABXAGkAdABoAG8AdQB0AFQAXwBMAG8AZwBpAGMALAAgADEAKQAgAD0AIABfAFQAWgBtAGEAcgBrAEYAaQByAHMAdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKgAgACgAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAFcAaQB0AGgAbwB1AHQAVABfAEwAbwBnAGkAYwAsACAAMgApACAAPQAgAF8AVABaAG0AYQByAGsASQBzAFoAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACoAIAAoAEMASABPAE8AUwBFAEMATwBMAFMAKABXAGkAdABoAG8AdQB0AFQAXwBMAG8AZwBpAGMALAAgADMAKQAgAD0AIABfAEgAYQBzAEMAbwBsAG8AbgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKgAgACgAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAFcAaQB0AGgAbwB1AHQAVABfAEwAbwBnAGkAYwAsACAANAApACAAPQAgAF8AdABpAG0AZQBDAG8AbgBkAGkAdABpAG8AbgBhAGwAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABzAEYAbABhAGcALAAgAEYASQBMAFQARQBSACgAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAFcAaQB0AGgAbwB1AHQAVABfAEwAbwBnAGkAYwAsACAANQApACwAIABfAG0AYQB0AGMAaAAsACAAIwBOAC8AQQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAEwAZQBuACwAIABJAEYAKABCAEkAVABBAE4ARAAoAF8AcABhAHIAdABzAEYAbABhAGcALAAgADQAKQAgAD0AIAA0ACwAIABfAGwAZQBuACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAaQBtAGUATABlAG4ALAAgAEkARgAoAEIASQBUAEEATgBEACgAXwBwAGEAcgB0AHMARgBsAGEAZwAsACAAMgApACAAPQAgADIALAAgAF8AbABlAG4AQgBlAGYAbwByAGUAVABaACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBMAGUAbgAsACAASQBGACgAQgBJAFQAQQBOAEQAKABfAHAAYQByAHQAcwBGAGwAYQBnACwAIAAxACkAIAA9ACAAMQAsACAAXwBsAGUAbgAgAC0AIABfAFQAWgBtAGEAcgBrAFAAbwBzACAAKwAgADEALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXwBwAGEAcgB0AHMARgBsAGEAZwAsACAAXwBkAGEAdABlAEwAZQBuACwAIABfAHQAaQBtAGUATABlAG4ALAAgAF8AdAB6AEwAZQBuACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAVABlAHgAdAAgAD0AIABcACIAXAAiACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgATgBPAFQAKABWAEEATABJAEQAQQBUAEUAXwBDAEgAQQBSAEEAQwBUAEUAUgBTACgAVABlAHgAdAAsACAAMAApACkALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBOAC8AQQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAFQAcABvAHMALAAgAEkARgBFAFIAUgBPAFIAKABGAEkATgBEACgAXAAiAFQAXAAiACwAIABUAGUAeAB0ACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBUAHAAbwBzACAAPQAgAEwARQBOACgAVABlAHgAdAApACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIATgAvAEEAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAFQALAAgAEkARgAoAF8AVABwAG8AcwAgAD4AIAAxACwAIAAyACwAIABfAFQAcABvAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABzAEwAZQBuACwAIABJAEYAKABfAGgAYQBzAFQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGYAbgBXAGkAdABoAFQAXwBQAGEAcgB0AHMATABlAG4AKABfAFQAcABvAHMALAAgAF8AaABhAHMAVAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABmAG4AVwBpAHQAaABvAHUAdABUAF8AUABhAHIAdABzAEwAZQBuACgAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAGEAcgB0AHMARgBsAGEAZwAsACAASQBOAEQARQBYACgAXwBwAGEAcgB0AHMATABlAG4ALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBOAEEAKABfAHAAYQByAHQAcwBGAGwAYQBnACkALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBOAC8AQQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBpAHMAbwBDAG8AbQBwAGwAaQBhAG4AdAAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAYQByAHQAcwBGAGwAYQBnACAAPQAgADEALAAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABzAEYAbABhAGcAIAA9ACAANQAsACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAGEAcgB0AHMARgBsAGEAZwAgAD0AIAA0ACwAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAAKABfAGgAYQBzAFQAIAA+ACAAMAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBQAGEAcgB0ACwAIABJAEYAKABCAEkAVABBAE4ARAAoAF8AcABhAHIAdABzAEYAbABhAGcALAAgADQAKQAgAD0AIAA0ACwAIABMAEUARgBUACgAVABlAHgAdAAsACAASQBOAEQARQBYACgAXwBwAGEAcgB0AHMATABlAG4ALAAgADEALAAgADIAKQApACwAIABcACIAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlAFAAYQByAHQALAAgAEkARgAoAEIASQBUAEEATgBEACgAXwBwAGEAcgB0AHMARgBsAGEAZwAsACAAMgApACAAPQAgADIALAAgAFwAIgBUAFwAIgAgACYAIABNAEkARAAoAFQAZQB4AHQALAAgAF8AVABwAG8AcwAgACsAIAAxACwAIABJAE4ARABFAFgAKABfAHAAYQByAHQAcwBMAGUAbgAsACAAMQAsACAAMwApACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBQAGEAcgB0ACwAIABJAEYAKABCAEkAVABBAE4ARAAoAF8AcABhAHIAdABzAEYAbABhAGcALAAgADEAKQAgAD0AIAAxACwAIABSAEkARwBIAFQAKABUAGUAeAB0ACwAIABJAE4ARABFAFgAKABfAHAAYQByAHQAcwBMAGUAbgAsACAAMQAsACAANAApACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AaQBzAG8AQwBvAG0AcABsAGkAYQBuAHQALAAgAF8AcABhAHIAdABzAEYAbABhAGcALAAgAF8AZABhAHQAZQBQAGEAcgB0ACwAIABfAHQAaQBtAGUAUABhAHIAdAAsACAAXwB0AHoAUABhAHIAdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AUABBAFIAUwBFAF8ASQBTAE8AOAA2ADAAMQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUAIABjAG8AbQBwAGwAaQBjAGEAdABpAG8AbgBzACAAbwBmACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAgADEAIAB8ACAASQBTAE8AQwBvAG0AcABsAGkAYQBuAHQAIAAgACAAfAAgAGIAbwBvAGwAZQBhAG4AIAB8ACAARgBsAGEAZwAgAGkAZgAgAGMAbwBtAHAAbABpAGEAbgB0ACAAdABvACAASQBTAE8AIAA4ADYAMAAxACAAcwB0AGEAbgBkAGEAcgBkAFwAbgAgACAAMgAgAHwAIABQAGEAcgB0AHMAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABCAGkAdABmAGwAYQBnACAAbwBmACAAcABhAHIAdABzACAAMAAuAC4ANwBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMAB4ADAANAAgAC0AIABkAGEAdABlAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAwAHgAMAAyACAALQAgAHQAaQBtAGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADAAeAAwADEAIAAtACAAdABpAG0AZQAgAHoAbwBuAGUAXABuACAAIAAzACAAfAAgAFAAcgBlAGMAaQBzAGkAbwBuACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADEAIAAtACAAeQBlAGEAcgBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMgAgAC0AIABtAG8AbgB0AGgALwB3AGUAZQBrAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAzACAALQAgAGQAYQB5AFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAA0ACAALQAgAGgAbwB1AHIAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADUAIAAtACAAbQBpAG4AdQB0AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADYAIAAtACAAaQBuAHQAZQBnAGUAcgAgAHMAZQBjAG8AbgBkAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAA3ACAALQAgAHMAZQBjAG8AbgBkACAAMAAuADAAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADgAIAAtACAAcwBlAGMAbwBuAGQAIAAwAC4AMAAwAFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAA5ACAALQAgAHMAZQBjAG8AbgBkACAAMAAuADAAMAAwAFwAbgAgACAANAAgAHwAIABGAG8AcgBtAGEAdAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxACAALQAgAGIAYQBzAGkAYwBcAG4AIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAMgAgAC0AIABlAHgAdABlAG4AZABlAGQAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADMAIAAtACAAYwBvAG4AcwBpAHMAdABlAG4AdAAgAHcAaQB0AGgAIABiAGEAcwBpAGMAIABvAHIAIABlAHgAdABlAG4AZABlAGQAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADQAIAAtACAAbQBpAHgAZQBkAFwAbgAgACAANQAgAHwAIABEAGEAdABlACAAVAB5AHAAZQAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAwACAALQAgAG4AbwAgAGQAYQB0AGUAIABwAHIAZQBzAGUAbgB0AFwAbgAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAxACAALQAgAGMAYQBsAGUAbgBkAGEAcgAgAGQAYQB0AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADIAIAAtACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAXABuACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgADMAIAAtACAAdwBlAGUAawAgAGQAYQB0AGUAXABuACAAIAA2ACAAfAAgAFkAZQBhAHIAIABDAEUAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4AIAAgADcAIAB8ACAATQBvAG4AdABoACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMQAuAC4AMQAyAFwAbgAgACAAIAAgAHwAIABXAGUAZQBrACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIAAxAC4ALgA1ADMAXABuACAAIAA4ACAAfAAgAEQAYQB5ACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADEALgAuADMAMQBcAG4AIAAgACAAIAB8ACAATwByAGQAaQBuAGEAbAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMQAuAC4AMwA2ADYAXABuACAAIAAgACAAfAAgAEQAYQB5ACAAbwBmACAAVwBlAGUAawAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADEALgAuADcAIAAtAD4AIABNAG8AbgAuAC4AUwB1AG4AXABuACAAIAA5ACAAfAAgAEgAbwB1AHIAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADAALgAuADIANABcAG4AIAAxADAAIAB8ACAATQBpAG4AdQB0AGUAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMAAuAC4ANQA5AFwAbgAgADEAMQAgAHwAIABTAGUAYwBvAG4AZAAgACAAIAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIAAwAC4ALgA1ADkALgA5ADkAOQBcAG4AIAAxADIAIAB8ACAATQBpAG4AdQB0AGUAcwAgAE8AZgBmAHMAZQB0ACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAALQA5ADAAMAAuAC4AKwA5ADAAMABcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAFQAZQB4AHQAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdAByAGkAbgBnACAAfAAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AHQAZQBkACAAZABhAHQAZQAgAGEAbgBkACAAdABpAG0AZQAuAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgAHwAIABFAHgAYQBtAHAAbABlACAAZgBvAHIAbQBhAHQAcwA6AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgAHwAIAArAFkAWQBZAFkAWQAtAE0ATQAtAEQARABUAGgAaAA6AG0AbQA6AHMAcwAuAHMAcwBzACsAaABoADoAbQBtADoAcwBzACwAIABZAFkAWQBZAC0ATQBNAC0ARABEAFQAaABoADoAbQBtAC0AaABoACwAIABZAFkAWQBZAC0AVwB3AHcALQBEAFQAaABoADoAbQBtAFoAXABuAFsAQQBsAGwAbwB3AE0AaQB4AGUAZABGAG8AcgBtAGEAdABdACAAfAAgAHMAdwBpAHQAYwBoACAAfAAgAEEAbABsAG8AdwAgAGEAIABtAGkAeAAgAG8AZgAgAGIAYQBzAGkAYwAgAGEAbgBkACAAZQB4AHQAZQBuAGQAZQBkACAAZgBvAHIAbQBhAHQAcwAgAHcAaQB0AGgAIABuAG8AIABlAGYAZgBlAGMAdAAgAG8AbgAgAEkAUwBPACAAYwBvAG0AcABsAGkAYQBuAGMAZQAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBQAEEAUgBTAEUAXwBJAFMATwA4ADYAMAAxACAAPQAgAEwAQQBNAEIARABBACgAVABlAHgAdAAsACAAWwBBAGwAbABvAHcATQBpAHgAZQBkAEYAbwByAG0AYQB0AF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACwAIABMAEEATQBCAEQAQQAoAF8AZQB4AGMAZQBwAHQAaQBvAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgACAAIAB8ACAAcwB0AHIAaQBuAGcAIAAgAHwAIABuAHUAbABsACAAIABFAG0AcAB0AHkAIAB0AGUAeAB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAE4ALwBBACAAIAAgAFUAbgBhAGIAbABlACAAdABvACAAcABhAHIAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBOAC8AQQBcACIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB7AEYAQQBMAFMARQAsACAAMAAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHsAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgB9AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIABmAG4AUABhAHIAdABzAEYAbABhAGcALAAgAEwAQQBNAEIARABBACgAXwBwAEQAYQB0AGUALAAgAF8AcABUAGkAbQBlACwAIABfAHAAVABaACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFAAYQByAHQALAAgAE4AKABJAE4ARABFAFgAKABfAHAARABhAHQAZQAsACAAMQAsACAAMQApACkAIAAqACAANAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBQAGEAcgB0ACwAIABOACgASQBOAEQARQBYACgAXwBwAFQAaQBtAGUALAAgADEALAAgADEAKQApACAAKgAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAegBQAGEAcgB0ACwAIABOACgASQBOAEQARQBYACgAXwBwAFQAWgAsACAAMQAsACAAMQApACkAIAAqACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBQAGEAcgB0ACAAKwAgAF8AdABpAG0AZQBQAGEAcgB0ACAAKwAgAF8AdAB6AFAAYQByAHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBJAFMATwBWAGEAbAB1AGUAQwBvAG0AcABsAGkAYQBuAGMAZQAsACAATABBAE0AQgBEAEEAKABfAHAARABhAHQAZQAsACAAXwBwAFQAaQBtAGUALAAgAF8AcABUAFoALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUASQBTAE8AQwBvAG0AcABsAGkAYQBuAHQALAAgAEkARgAoAEkATgBEAEUAWAAoAF8AcABEAGEAdABlACwAIAAxACwAIAAxACkAIAA9ACAAXAAiAFwAIgAsACAAVABSAFUARQAsACAASQBOAEQARQBYACgAXwBwAEQAYQB0AGUALAAgADEALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlAEkAUwBPAEMAbwBtAHAAbABpAGEAbgB0ACwAIABJAEYAKABJAE4ARABFAFgAKABfAHAAVABpAG0AZQAsACAAMQAsACAAMQApACAAPQAgAFwAIgBcACIALAAgAFQAUgBVAEUALAAgAEkATgBEAEUAWAAoAF8AcABUAGkAbQBlACwAIAAxACwAIAAxACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AEkAUwBPAEMAbwBtAHAAbABpAGEAbgB0ACwAIABJAEYAKABJAE4ARABFAFgAKABfAHAAVABaACwAIAAxACwAIAAxACkAIAA9ACAAXAAiAFwAIgAsACAAVABSAFUARQAsACAASQBOAEQARQBYACgAXwBwAFQAWgAsACAAMQAsACAAMQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AZABhAHQAZQBJAFMATwBDAG8AbQBwAGwAaQBhAG4AdAAgACoAIABfAHQAaQBtAGUASQBTAE8AQwBvAG0AcABsAGkAYQBuAHQAIAAqACAAXwB0AHoASQBTAE8AQwBvAG0AcABsAGkAYQBuAHQAKQAgADwAPgAgADAAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAZgBuAEkAUwBPAEYAbwByAG0AYQB0AEMAbwBtAHAAbABpAGEAbgBjAGUALAAgAEwAQQBNAEIARABBACgAXwBwAEQAYQB0AGUALAAgAF8AcABUAGkAbQBlACwAIABfAHAAVABaACwAIABfAGEAbABsAG8AdwBNAGkAeABlAGQARgBvAHIAbQBhAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAQwBvAGwAdQBtAG4AcwAgAE8AdQB0ADoAIABJAFMATwBDAG8AbQBwAGwAaQBhAG4AdAAsACAAUgBlAHMAbwBsAHYAZQBkAEYAbwByAG0AYQB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBGAG0AdAAsACAATgAoAEkATgBEAEUAWAAoAF8AcABEAGEAdABlACwAIAAxACwAIAAzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBGAG0AdAAsACAATgAoAEkATgBEAEUAWAAoAF8AcABUAGkAbQBlACwAIAAxACwAIAAzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdAB6AG8ARgBtAHQALAAgAE4AKABJAE4ARABFAFgAKABfAHAAVABaACwAIAAxACwAIAAzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcgBlAHMAbwBsAHYAZQBGAG0AdAAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBkAGEAdABlAEYAbQB0ACAAPQAgADMAKQAgACoAIAAoAF8AdABpAG0AZQBGAG0AdAAgAD0AIAAwACkAIAAqACAAKABfAHQAegBvAEYAbQB0ACAAPQAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbwBuAGwAeQAgAGQAYQB0AGUAIABwAHIAbwB2AGkAZABlAGQALAAgAGMAbwBuAHMAaQBzAHQAZQBuAHQAIAB3AGkAdABoACAAYgBhAHMAaQBjACAAbwByACAAZQB4AHQAZQBuAGQAZQBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBkAGEAdABlAEYAbQB0ACAAPQAgADAAKQAgACoAIAAoAF8AdABpAG0AZQBGAG0AdAAgAD0AIAAzACkAIAAqACAAKABfAHQAegBvAEYAbQB0ACAAPQAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbwBuAGwAeQAgAHQAaQBtAGUAIABwAHIAbwB2AGkAZABlAGQALAAgAGMAbwBuAHMAaQBzAHQAZQBuAHQAIAB3AGkAdABoACAAYgBhAHMAaQBjACAAbwByACAAZQB4AHQAZQBuAGQAZQBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMwAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBkAGEAdABlAEYAbQB0ACAAPQAgADAAKQAgACoAIAAoAF8AdABpAG0AZQBGAG0AdAAgAD0AIAAwACkAIAAqACAAKABfAHQAegBvAEYAbQB0ACAAPQAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbwBuAGwAeQAgAHQAaQBtAGUAIAB6AG8AbgBlACAAcAByAG8AdgBpAGQAZQBkACwAIABjAG8AbgBzAGkAcwB0AGUAbgB0ACAAdwBpAHQAaAAgAGIAYQBzAGkAYwAgAG8AcgAgAGUAeAB0AGUAbgBkAGUAZABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADMALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AZABhAHQAZQBGAG0AdAAgADwAPgAgADIAKQAgACoAIAAoAF8AdABpAG0AZQBGAG0AdAAgADwAPgAgADIAKQAgACoAIAAoAF8AdAB6AG8ARgBtAHQAIAA8AD4AIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAGEAbABsACAAYgBhAHMAaQBjACAAZgBvAHIAbQBhAHQAIAB3AGgAZQByAGUAIABwAHIAZQBzAGUAbgB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABfAGQAYQB0AGUARgBtAHQAIAA8AD4AIAAxACkAIAAqACAAKABfAHQAaQBtAGUARgBtAHQAIAA8AD4AIAAxACkAIAAqACAAKABfAHQAegBvAEYAbQB0ACAAPAA+ACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABhAGwAbAAgAGUAeAB0AGUAbgBkAGUAZAAgAGYAbwByAG0AYQB0ACAAdwBoAGUAcgBlACAAcAByAGUAcwBlAG4AdAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMgAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG0AaQB4AGUAZAAgAGYAbwByAG0AYQB0AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAANABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBmAG8AcgBtAGEAdABDAG8AbQBwAGwAaQBhAG4AdAAsACAASQBGACgAXwBhAGwAbABvAHcATQBpAHgAZQBkAEYAbwByAG0AYQB0ACwAIAAxACwAIABOACgAXwByAGUAcwBvAGwAdgBlAEYAbQB0ACAAPAAgADQAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABfAGYAbwByAG0AYQB0AEMAbwBtAHAAbABpAGEAbgB0ACwAIABfAHIAZQBzAG8AbAB2AGUARgBtAHQAKQAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGYAbgBJAFMATwBQAHIAZQBjAGkAcwBpAG8AbgBDAG8AbQBwAGwAaQBhAG4AYwBlACwAIABMAEEATQBCAEQAQQAoAF8AcABEAGEAdABlACwAIABfAHAAVABpAG0AZQAsACAAXwBwAFQAWgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABDAG8AbAB1AG0AbgBzACAATwB1AHQAOgAgAEkAUwBPAEMAbwBtAHAAbABpAGEAbgB0ACwAIABQAHIAZQBjAGkAcwBpAG8AbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAUAByAGUAYwAsACAATgAoAEkATgBEAEUAWAAoAF8AcABEAGEAdABlACwAIAAxACwAIAAyACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBQAHIAZQBjACwAIABOACgASQBOAEQARQBYACgAXwBwAFQAaQBtAGUALAAgADEALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAUAByAGUAYwAsACAATgAoAEkATgBEAEUAWAAoAF8AcABUAFoALAAgADEALAAgADIAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBQAHIAZQBjACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwB0AGkAbQBlAFAAcgBlAGMAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AdAB6AFAAcgBlAGMAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABGAEEATABTAEUALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABUAFIAVQBFACwAIABfAHQAegBQAHIAZQBjACAAKwAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABUAFIAVQBFACwAIABfAHQAaQBtAGUAUAByAGUAYwAgACsAIAAzACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBQAHIAZQBjACAAPAAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKAAoAF8AdABpAG0AZQBQAHIAZQBjACAAPQAgADAAKQAsACAAXwBkAGEAdABlAFAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsACAALwAvACAAXwBkAGEAdABlAFAAcgBlAGMAIAA9ACAAMwAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFQAUgBVAEUALAAgAF8AdABpAG0AZQBQAHIAZQBjACAAKwAgADMAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABUAGUAeAB0ACAAPQAgAFwAIgBcACIALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABhAHIAdABzACwAIABQAEEAUgBTAEUAXwBQAEEAUgBUAFMAKABUAGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOACgASQBOAEQARQBYACgAXwBwAGEAcgB0AHMALAAgADEALAAgADIAKQApACAAPQAgADAALAAgAGYAbgBFAHgAYwBlAHAAdABpAG8AbgAoAFwAIgBOAC8AQQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBhAGwAbABvAHcATQBpAHgAZQBkAEYAbwByAG0AYQB0ACwAIABOACgAQQBsAGwAbwB3AE0AaQB4AGUAZABGAG8AcgBtAGEAdAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAcwBvAFAAYQByAHQAcwBDAG8AbQBwAGwAaQBhAG4AYwBlACwAIABOACgASQBOAEQARQBYACgAXwBwAGEAcgB0AHMALAAgADEALAAgADEAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABEAGEAdABlACwAIABQAEEAUgBTAEUAXwBEAEEAVABFACgASQBOAEQARQBYACgAXwBwAGEAcgB0AHMALAAgADEALAAgADMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABUAGkAbQBlACwAIABQAEEAUgBTAEUAXwBUAEkATQBFACgASQBOAEQARQBYACgAXwBwAGEAcgB0AHMALAAgADEALAAgADQAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcABUAFoALAAgAFAAQQBSAFMARQBfAFQASQBNAEUAXwBaAE8ATgBFACgASQBOAEQARQBYACgAXwBwAGEAcgB0AHMALAAgADEALAAgADUAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAG8AVgBhAGwAdQBlAEMAbwBtAHAAbABpAGEAbgBjAGUALAAgAGYAbgBJAFMATwBWAGEAbAB1AGUAQwBvAG0AcABsAGkAYQBuAGMAZQAoAF8AcABEAGEAdABlACwAIABfAHAAVABpAG0AZQAsACAAXwBwAFQAWgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAG8ARgBvAHIAbQBhAHQAQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAZgBuAEkAUwBPAEYAbwByAG0AYQB0AEMAbwBtAHAAbABpAGEAbgBjAGUAKABfAHAARABhAHQAZQAsACAAXwBwAFQAaQBtAGUALAAgAF8AcABUAFoALAAgAF8AYQBsAGwAbwB3AE0AaQB4AGUAZABGAG8AcgBtAGEAdAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaQBzAG8AUAByAGUAYwBpAHMAaQBvAG4AQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAZgBuAEkAUwBPAFAAcgBlAGMAaQBzAGkAbwBuAEMAbwBtAHAAbABpAGEAbgBjAGUAKABfAHAARABhAHQAZQAsACAAXwBwAFQAaQBtAGUALAAgAF8AcABUAFoAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AdQB0AEkAUwBPAGMAbwBtAHAAbABpAGEAbgBjAGUALAAgACgAXwBpAHMAbwBWAGEAbAB1AGUAQwBvAG0AcABsAGkAYQBuAGMAZQAgACoAIABfAGkAcwBvAFAAYQByAHQAcwBDAG8AbQBwAGwAaQBhAG4AYwBlACAAKgAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARgBvAHIAbQBhAHQAQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAMQAsACAAMQApACAAKgAgAEkATgBEAEUAWAAoAF8AaQBzAG8AUAByAGUAYwBpAHMAaQBvAG4AQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAMQAsACAAMQApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwB1AHQARABhAHQAZQBUAHkAcABlACwAIABOACgASQBOAEQARQBYACgAXwBwAEQAYQB0AGUALAAgADEALAAgADQAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwB1AHQARABhAHQAZQAsACAARABSAE8AUAAoAF8AcABEAGEAdABlACwAIAAsACAANAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwB1AHQAVABpAG0AZQAsACAARABSAE8AUAAoAF8AcABUAGkAbQBlACwAIAAsACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbwB1AHQAVABaACwAIABEAFIATwBQACgAXwBwAFQAWgAsACAALAAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG8AdQB0AFAAYQByAHQAcwBGAGwAYQBnACwAIABmAG4AUABhAHIAdABzAEYAbABhAGcAKABfAHAARABhAHQAZQAsACAAXwBwAFQAaQBtAGUALAAgAF8AcABUAFoAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AbwB1AHQASQBTAE8AYwBvAG0AcABsAGkAYQBuAGMAZQAsACAAXwBvAHUAdABQAGEAcgB0AHMARgBsAGEAZwAsACAASQBOAEQARQBYACgAXwBpAHMAbwBQAHIAZQBjAGkAcwBpAG8AbgBDAG8AbQBwAGwAaQBhAG4AYwBlACwAIAAxACwAIAAyACkALAAgAEkATgBEAEUAWAAoAF8AaQBzAG8ARgBvAHIAbQBhAHQAQwBvAG0AcABsAGkAYQBuAGMAZQAsACAAMQAsACAAMgApACwAIABfAG8AdQB0AEQAYQB0AGUAVAB5AHAAZQAsACAAXwBvAHUAdABEAGEAdABlACwAIABfAG8AdQB0AFQAaQBtAGUALAAgAF8AbwB1AHQAVABaACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAEYATwBSAE0AQQBUAFQASQBOAEcAIABGAFUATgBDAFQASQBPAE4AUwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAE8AUgBNAEEAVABfAEQAQQBUAEUAXABuAFwAbgBSAGUAdAB1AHIAbgBzACAAYQAgAGQAYQB0AGUAIABhAHMAIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuAFwAbgBFAHgAYQBtAHAAbABlACAAZgBvAHIAbQBhAHQAcwAgACgAbgBvAHQAIABlAHgAaABhAHUAcwB0AGkAdgBlACkAOgAgACsAWQBZAFkAWQBZAC0ATQBNAC0ARABEACwAIABZAFkAWQBZAC0ATQBNAC0ARABEACwAIABZAFkAWQBZAC0ATQBNACwAIAArAFkAWQBZAFkATQBNACwAIABZAFkAWQBZAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgACMAVgBBAEwAVQBFACEAIABpAGYAIABhAG4AIABpAG4AdgBhAGwAaQBkACAAZABhAHQAZQAgAG8AcgAgAGEAbQBiAGkAZwB1AG8AdQBzACAAYgBhAHMAaQBjACAAZgBvAHIAbQBhAHQALgAgAGUAZwAgADIAMAAyADMAMAA1AFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAWQBlAGEAcgAgAGkAbgAgAEMAbwBtAG0AbwBuACAARQByAGEAIAAtADkAOQA5ADkAOQAuAC4AKwA5ADkAOQA5ADkAXABuAFsATQBvAG4AdABoAF0AIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAE0AbwBuAHQAaAAgAG8AZgAgAHQAaABlACAAeQBlAGEAcgBcAG4AWwBEAGEAeQBdACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARABhAHkAIABvAGYAIAB0AGgAZQAgAG0AbwBuAHQAaABcAG4AWwBCAGEAcwBpAGMAXQAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAUgBlAHQAdQByAG4AIABpAG4AIABiAGEAcwBpAGMAIABmAG8AcgBtAGEAdAAgAGUAZwAgAFkAWQBZAFkATQBNAEQARABcAG4AWwBTAGkAZwBuAGUAZABdACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQQBsAHcAYQB5AHMAIABzAGkAZwBuACAAeQBlAGEAcgAgAHYAYQBsAHUAZQAgAGUAZwAgACsAWQBZAFkAWQAtAE0ATQAtAEQARABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARgBPAFIATQBBAFQAXwBEAEEAVABFACAAPQAgAEwAQQBNAEIARABBACgAWQBlAGEAcgBDAEUALAAgAFsATQBvAG4AdABoAF0ALAAgAFsARABhAHkAXQAsACAAWwBCAGEAcwBpAGMAXQAsACAAWwBTAGkAZwBuAGUAZABdACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACoAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkAIAAqACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQApACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAATQBvAG4AdABoACwAIABEAGEAeQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAIABOACgAQgBhAHMAaQBjACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuAGUAZABZAGUAYQByACwAIABOACgAUwBpAGcAbgBlAGQAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5ACkAKQAgACoAIABfAGIAYQBzAGkAYwBGAG8AcgBtAGEAdAAsACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5ACwAIABJAE4AVAAoAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AEYAbQB0ACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEEAQgBTACgAXwB5ACkAIAA+AD0AIAAxADAAMAAwADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArADAAMAAwADAAMAA7AFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACAAJgAgAFwAIgAwADAAMAAwADAAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuAGUAZABZAGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAKwAwADAAMAAwADsAXAAiACAAJgAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkAIAAmACAAXAAiADAAMAAwADAAOwArADAAMAAwADAAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMAA7ADAAMAAwADAAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABUAEUAWABUACgAXwB5ACwAIABfAHkARgBtAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AbwBuAHQAaAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAWQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMATQBvAG4AdABoACwAIABUAEUAWABUACgASQBOAFQAKABNAG8AbgB0AGgAKQAsACAAXAAiADAAMABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgARABhAHkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAIABfAHMAWQBlAGEAcgAgACYAIABfAHMATQBvAG4AdABoACwAIABfAHMAWQBlAGEAcgAgACYAIABcACIALQBcACIAIAAmACAAXwBzAE0AbwBuAHQAaAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAEQAYQB5ACwAIABUAEUAWABUACgASQBOAFQAKABEAGEAeQApACwAIABcACIAMAAwAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGIAYQBzAGkAYwBGAG8AcgBtAGEAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFkAZQBhAHIAIAAmACAAXwBzAE0AbwBuAHQAaAAgACYAIABfAHMARABhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACAAJgAgAFwAIgAtAFwAIgAgACYAIABfAHMATQBvAG4AdABoACAAJgAgAFwAIgAtAFwAIgAgACYAIABfAHMARABhAHkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARgBPAFIATQBBAFQAXwBUAEkATQBFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIAB0AGkAbQBlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgBcAG4ARQB4AGEAbQBwAGwAZQAgAGYAbwByAG0AYQB0AHMAIAAoAG4AbwB0ACAAZQB4AGgAYQB1AHMAdABpAHYAZQApADoAIABUAGgAaAA6AG0AbQA6AHMAcwAuAHMAcwBzACwAIABUAGgAaAA6AG0AbQA6AHMAcwAsACAAVABoAGgAOgBtAG0ALAAgAFQAaABoAG0AbQBzAHMALAAgAFQAaABoAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgACMAVgBBAEwAVQBFACEAIABpAGYAIABhAG4AIABpAG4AdgBhAGwAaQBkACAAdABpAG0AZQBcAG4AXABuAFAAYQByAGEAbQBlAHQAZQByAHMAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEgAbwB1AHIAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADAALgAuADIANABcAG4ATQBpAG4AdQB0AGUAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAMAAuAC4ANQA5AFwAbgBTAGUAYwBvAG4AZAAgACAAIAAgACAAIAB8ACAAZABlAGMAaQBtAGEAbAAgAHwAIAAwAC4ALgA1ADkALgA5ADkAOQBcAG4AWwBCAGEAcwBpAGMAXQAgACAAIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAUgBlAHQAdQByAG4AIABpAG4AIABiAGEAcwBpAGMAIABmAG8AcgBtAGEAdABcAG4AWwBQAHIAZQBjAGkAcwBpAG8AbgBdACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAAUwBlAGwAZQBjAHQAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGwAZQB2AGUAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAAYQB1AHQAbwBtAGEAdABpAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAxACAALQAgAGgAbwB1AHIAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAAbQBpAG4AdQB0AGUAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAAaQBuAHQAZQBnAGUAcgAgAHMAZQBjAG8AbgBkAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA0ACAALQAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIABzAGUAYwBvAG4AZABzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBGAE8AUgBNAEEAVABfAFQASQBNAEUAIAA9ACAATABBAE0AQgBEAEEAKABIAG8AdQByACwAIABNAGkAbgB1AHQAZQAsACAAUwBlAGMAbwBuAGQALAAgAFsAQgBhAHMAaQBjAF0ALAAgAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABIAG8AdQByACkAKQAgACoAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE0AaQBuAHUAdABlACkAKQAgACoAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFMAZQBjAG8AbgBkACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQAoAEgAbwB1AHIALAAgAE0AaQBuAHUAdABlACwAIABTAGUAYwBvAG4AZAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBWAEEATABVAEUAIQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAIABOACgAQgBhAHMAaQBjACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzACwAIABSAE8AVQBOAEQARABPAFcATgAoAE4AKABTAGUAYwBvAG4AZAApACwAIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG0ALAAgAEkATgBUACgATgAoAE0AaQBuAHUAdABlACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaAAsACAASQBOAFQAKABOACgASABvAHUAcgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACwAIABNAEEAWAAoAEkATgBUACgATgAoAFAAcgBlAGMAaQBzAGkAbwBuACkAKQAsACAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBQAHIAZQBjAGkAcwBpAG8AbgAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgBTACgASQBTAE4AVQBNAEIARQBSACgAUwBlAGMAbwBuAGQAKQAsACAASQBGACgAXwBzACAAPQAgAEkATgBUACgAXwBzACkALAAgADMALAAgADQAKQAsACAASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQAsACAAMgAsACAAVABSAFUARQAsACAAMQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABcACIAIAAmACAAVABFAFgAVAAoAF8AaAAsACAAXAAiADAAMABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB1AHMAZQBQAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFQAXAAiACAAJgAgAFQARQBYAFQAKABfAGgALAAgAFwAIgAwADAAXAAiACkAIAAmACAAVABFAFgAVAAoAF8AbQAsACAAXAAiADAAMABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABcACIAIAAmACAAVABFAFgAVAAoAF8AaAAsACAAXAAiADAAMABcACIAKQAgACYAIABcACIAOgBcACIAIAAmACAAVABFAFgAVAAoAF8AbQAsACAAXAAiADAAMABcACIAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdQBzAGUAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBUAFwAIgAgACYAIABUAEUAWABUACgAXwBoACwAIABcACIAMAAwAFwAIgApACAAJgAgAFQARQBYAFQAKABfAG0ALAAgAFwAIgAwADAAXAAiACkAIAAmACAAVABFAFgAVAAoAF8AcwAsACAAXAAiADAAMABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABcACIAIAAmACAAVABFAFgAVAAoAF8AaAAsACAAXAAiADAAMABcACIAKQAgACYAIABcACIAOgBcACIAIAAmACAAVABFAFgAVAAoAF8AbQAsACAAXAAiADAAMABcACIAKQAgACYAIABcACIAOgBcACIAIAAmACAAVABFAFgAVAAoAF8AcwAsACAAXAAiADAAMABcACIAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvAF8AdQBzAGUAUAByAGUAYwBpAHMAaQBvAG4AIAA9ACAANABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFQAUgBVAEUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGIAYQBzAGkAYwBGAG8AcgBtAGEAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABcACIAIAAmACAAVABFAFgAVAAoAF8AaAAsACAAXAAiADAAMABcACIAKQAgACYAIABUAEUAWABUACgAXwBtACwAIABcACIAMAAwAFwAIgApACAAJgAgAFQARQBYAFQAKABfAHMALAAgAFwAIgAwADAALgAwADAAMABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAVABcACIAIAAmACAAVABFAFgAVAAoAF8AaAAsACAAXAAiADAAMABcACIAKQAgACYAIABcACIAOgBcACIAIAAmACAAVABFAFgAVAAoAF8AbQAsACAAXAAiADAAMABcACIAKQAgACYAIABcACIAOgBcACIAIAAmACAAVABFAFgAVAAoAF8AcwAsACAAXAAiADAAMAAuADAAMAAwAFwAIgApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAE8AUgBNAEEAVABfAFQASQBNAEUAXwBaAE8ATgBFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAIAB0AGkAbQBlACAAegBvAG4AZQAgAGEAcwAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AXABuAEUAeABhAG0AcABsAGUAIABmAG8AcgBtAGEAdABzACAAKABuAG8AdAAgAGUAeABoAGEAdQBzAHQAaQB2AGUAKQA6ACAAKwBoAGgAOgBtAG0AOgBzAHMALAAgAC0AaABoADoAbQBtACwAIAArAGgAaAAsACAAWgBcAG4AXABuAE8AdQB0AHAAdQB0AFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgADEAIAB8ACAAdABlAHgAdAAgAHwAIAAjAFYAQQBMAFUARQAhACAAaQBmACAAYQBuACAAaQBuAHYAYQBsAGkAZAAgAHQAaQBtAGUAIAB6AG8AbgBlAFwAbgBcAG4AUABhAHIAYQBtAGUAdABlAHIAcwBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAFQAaQBtAGUAIAB6AG8AbgBlACAAbwBmAGYAcwBlAHQAIABmAHIAbwBtACAAVQBUAEMAIABpAG4AIABtAGkAbgB1AHQAZQBzACAALQA5ADAAMAAuAC4AKwA5ADAAMABcAG4AWwBCAGEAcwBpAGMAXQAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAFIAZQB0AHUAcgBuACAAaQBuACAAYgBhAHMAaQBjACAAZgBvAHIAbQBhAHQAXABuAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABTAGUAbABlAGMAdAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAbABlAHYAZQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAAYQB1AHQAbwBtAGEAdABpAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABoAG8AdQByAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMgAgAC0AIABtAGkAbgB1AHQAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAAcwBlAGMAbwBuAGQAcwBcAG4AWwBOAG8AWgB1AGwAdQBdACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAFUAcwBlACAAKwAwADAAOgAwADAAIABpAG4AcwB0AGUAYQBkACAAbwBmACAAWgAgAGYAbwByACAAVQBUAEMAIAB0AGkAbQBlACAAegBvAG4AZQAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBGAE8AUgBNAEEAVABfAFQASQBNAEUAXwBaAE8ATgBFACAAPQAgAEwAQQBNAEIARABBACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwAsACAAWwBCAGEAcwBpAGMAXQAsACAAWwBQAHIAZQBjAGkAcwBpAG8AbgBdACwAIABbAE4AbwBaAHUAbAB1AF0ALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAE4AVQBNAEIARQBSACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwApACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBcACIALABcAG4AIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAIABOACgAQgBhAHMAaQBjACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAE0AQQBYACgASQBOAFQAKABOACgAUAByAGUAYwBpAHMAaQBvAG4AKQApACwAIAAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBuAGUAYQByAFoAZQByAG8ALAAgAFIATwBVAE4ARABEAE8AVwBOACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwAgACoAIAA2ADAALAAgADAAKQAgAD0AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgATgAoAE4AbwBaAHUAbAB1ACkAIAA9ACAAMAApACAAKgAgAF8AbgBlAGEAcgBaAGUAcgBvACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFoAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAXwBaAE8ATgBFACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAUwBlAGMAcwAsACAAUgBPAFUATgBEAEQATwBXAE4AKABNAE8ARAAoAE8AZgBmAHMAZQB0AE0AaQBuAHUAdABlAHMALAAgADEAKQAgACoAIAA2ADAALAAgADAAKQAgAD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBGAG0AdAAsACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAUwBlAGMAcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAFwAIgBoAGgAbQBtAHMAcwBcACIALAAgAFwAIgBoAGgAOgBtAG0AOgBzAHMAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAIABcACIAaABoAG0AbQBcACIALAAgAFwAIgBoAGgAOgBtAG0AXAAiACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBoAGgAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAFwAIgBoAGgAbQBtAFwAIgAsACAAXAAiAGgAaAA6AG0AbQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAFwAIgBoAGgAbQBtAHMAcwBcACIALAAgAFwAIgBoAGgAOgBtAG0AOgBzAHMAXAAiACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuACwAIABJAEYAKABTAEkARwBOACgATwBmAGYAcwBlAHQATQBpAG4AdQB0AGUAcwApACAAPAAgADAALAAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkALAAgAFwAIgArAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AdABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABBAEIAUwAoAE8AZgBmAHMAZQB0AE0AaQBuAHUAdABlAHMAKQAgAC8AIAAxADQANAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgAgACYAIABUAEUAWABUACgAXwB0AGkAbQBlAFoAbwBuAGUATwBmAGYAcwBlAHQALAAgAF8AcwBGAG0AdAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBGAE8AUgBNAEEAVABfAE8AUgBEAEkATgBBAEwAXwBEAEEAVABFAFwAbgBcAG4AUgBlAHQAdQByAG4AcwAgAGEAbgAgAG8AcgBkAGkAbgBhAGwAIABkAGEAdABlACAAYQBzACAAdABlAHgAdAAgAGkAbgAgAHQAaABlACAASQBTAE8AIAA4ADYAMAAxACAAZgBvAHIAbQBhAHQALgBcAG4ARQB4AGEAbQBwAGwAZQAgAGYAbwByAG0AYQB0AHMAIAAoAG4AbwB0ACAAZQB4AGgAYQB1AHMAdABpAHYAZQApADoAIABZAFkAWQBZAC0ARABEAEQALAAgAFkAWQBZAFkARABEAEQAXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAHQAZQB4AHQAIAB8ACMAVgBBAEwAVQBFACEAIABpAGYAIABhAG4AIABpAG4AdgBhAGwAaQBkACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABZAGUAYQByACAAaQBuACAAQwBvAG0AbQBvAG4AIABFAHIAYQAgAC0AOQA5ADkAOQA5AC4ALgArADkAOQA5ADkAOQBcAG4ATwByAGQAaQBuAGEAbAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgBcAG4AWwBCAGEAcwBpAGMAXQAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAUgBlAHQAdQByAG4AIABpAG4AIABiAGEAcwBpAGMAIABmAG8AcgBtAGEAdAAgAGUAZwAgAFkAWQBZAFkARABEAEQAXABuAFsAUwBpAGcAbgBlAGQAXQAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEEAbAB3AGEAeQBzACAAcwBpAGcAbgAgAHkAZQBhAHIAIAB2AGEAbAB1AGUAIABlAGcAIAArAFkAWQBZAFkALQBNAE0ALQBEAEQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYATwBSAE0AQQBUAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAATwByAGQAaQBuAGEAbAAsACAAWwBCAGEAcwBpAGMAXQAsACAAWwBTAGkAZwBuAGUAZABdACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFkAZQBhAHIAQwBFACkAKQAgACoAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAE8AcgBkAGkAbgBhAGwAKQApACwAXABuACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMAXwBWAEEATABJAEQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABPAHIAZABpAG4AYQBsACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAjAFYAQQBMAFUARQAhACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAE4AKABCAGEAcwBpAGMAKQAgADwAPgAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AZQBkAFkARQBhAHIALAAgAE4AKABTAGkAZwBuAGUAZAApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQAsACAASQBOAFQAKABZAGUAYQByAEMARQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAKABBAEIAUwAoAF8AeQApACAAPgA9ACAAMQAwADAAMAAwACkAIAAqACAAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5AEYAbQB0ACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEEAQgBTACgAXwB5ACkAIAA+AD0AIAAxADAAMAAwADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArADAAMAAwADAAMAA7AFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACAAJgAgAFwAIgAwADAAMAAwADAAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGkAZwBuAGUAZABZAGUAYQByACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAKwAwADAAMAAwADsAXAAiACAAJgAgAFUATgBJAEMASABBAFIAKAA4ADcAMgAyACkAIAAmACAAXAAiADAAMAAwADAAOwArADAAMAAwADAAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiADAAMAAwADAAOwBcACIAIAAmACAAVQBOAEkAQwBIAEEAUgAoADgANwAyADIAKQAgACYAIABcACIAMAAwADAAMAA7ADAAMAAwADAAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABUAEUAWABUACgAXwB5ACwAIABfAHkARgBtAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMATwByAGQAaQBuAGEAbAAsACAAVABFAFgAVAAoAEkATgBUACgATwByAGQAaQBuAGEAbAApACwAIABcACIAMAAwADAAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBiAGEAcwBpAGMARgBvAHIAbQBhAHQALAAgAF8AcwBZAGUAYQByACAAJgAgAF8AcwBPAHIAZABpAG4AYQBsACwAIABfAHMAWQBlAGEAcgAgACYAIABcACIALQBcACIAIAAmACAAXwBzAE8AcgBkAGkAbgBhAGwAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4ARgBPAFIATQBBAFQAXwBXAEUARQBLAF8ARABBAFQARQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABhACAAdwBlAGUAawAgAGQAYQB0AGUAIABhAHMAIAB0AGUAeAB0ACAAaQBuACAAdABoAGUAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAAuAFwAbgBFAHgAYQBtAHAAbABlACAAZgBvAHIAbQBhAHQAcwAgACgAbgBvAHQAIABlAHgAaABhAHUAcwB0AGkAdgBlACkAOgAgAFkAWQBZAFkALQBXAHcAdwAtAEQALAAgAFkAWQBZAFkALQBXAHcAdwAsACAAWQBZAFkAWQBXAHcAdwBEACwAIABZAFkAWQBZAFcAdwB3AFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAMQAgAHwAIAB0AGUAeAB0ACAAfAAgACMAVgBBAEwAVQBFACEAIABpAGYAIABhAG4AIABpAG4AdgBhAGwAaQBkACAAdwBlAGUAawAgAGQAYQB0AGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBZAGUAYQByAEMARQAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBXAGUAZQBrACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEkAUwBPACAAZABlAGYAaQBuAGUAZAAgAHcAZQBlAGsAIABuAHUAbQBiAGUAcgAgAG8AZgAgAHQAaABlACAAeQBlAGEAcgBcAG4ARABhAHkATwBmAFcAZQBlAGsAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABEAGEAeQAgAG8AZgAgAHQAaABlACAAdwBlAGUAawAgAHcAaABlAHIAZQAgADEALgAuADcAIAAtAD4AIABNAG8AbgAuAC4AUwB1AG4AIABcAG4AWwBCAGEAcwBpAGMAXQAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABSAGUAdAB1AHIAbgAgAGkAbgAgAGIAYQBzAGkAYwAgAGYAbwByAG0AYQB0ACAAZQBnACAAWQBZAFkAWQBXAHcAdwBEAFwAbgBbAFMAaQBnAG4AZQBkAF0AIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEEAbAB3AGEAeQBzACAAcwBpAGcAbgAgAHkAZQBhAHIAIAB2AGEAbAB1AGUAIABlAGcAIAArAFkAWQBZAFkALQBXAHcAdwAtAEQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEYATwBSAE0AQQBUAF8AVwBFAEUASwBfAEQAQQBUAEUAIAA9ACAATABBAE0AQgBEAEEAKABZAGUAYQByAEMARQAsACAAVwBlAGUAawAsACAARABhAHkATwBmAFcAZQBlAGsALAAgAFsAQgBhAHMAaQBjAF0ALAAgAFsAUwBpAGcAbgBlAGQAXQAsAFwAbgAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABZAGUAYQByAEMARQApACkAIAAqACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABXAGUAZQBrACkAKQAgACoAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB5AE8AZgBXAGUAZQBrACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4ATwBUACgASQBTAF8AVgBBAEwASQBEAF8AVwBFAEUASwBfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAAVwBlAGUAawAsACAARABhAHkATwBmAFcAZQBlAGsAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGIAYQBzAGkAYwBGAG8AcgBtAGEAdAAsACAATgAoAEIAYQBzAGkAYwApACAAPAA+ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBpAGcAbgBlAGQAWQBlAGEAcgAsACAATgAoAFMAaQBnAG4AZQBkACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB5ACwAIABJAE4AVAAoAFkAZQBhAHIAQwBFACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkARgBtAHQALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABBAEIAUwAoAF8AeQApACAAPgA9ACAAMQAwADAAMAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgArADAAMAAwADAAMAA7AFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACAAJgAgAFwAIgAwADAAMAAwADAAXAAiACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAaQBnAG4AZQBkAFkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiACsAMAAwADAAMAA7AFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACAAJgAgAFwAIgAwADAAMAAwADsAKwAwADAAMAAwAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABSAFUARQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAMAAwADAAMAA7AFwAIgAgACYAIABVAE4ASQBDAEgAQQBSACgAOAA3ADIAMgApACAAJgAgAFwAIgAwADAAMAAwADsAMAAwADAAMABcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBZAGUAYQByACwAIABUAEUAWABUACgAXwB5ACwAIABfAHkARgBtAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBXAGUAZQBrACwAIABUAEUAWABUACgASQBOAFQAKABXAGUAZQBrACkALAAgAFwAIgBXADAAMABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgBPAFQAKABJAFMATgBVAE0AQgBFAFIAKABEAGEAeQBPAGYAVwBlAGUAawApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAF8AYgBhAHMAaQBjAEYAbwByAG0AYQB0ACwAIABfAHMAWQBlAGEAcgAgACYAIABfAHMAVwBlAGUAawAsACAAXwBzAFkAZQBhAHIAIAAmACAAXAAiAC0AXAAiACAAJgAgAF8AcwBXAGUAZQBrACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGIAYQBzAGkAYwBGAG8AcgBtAGEAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAWQBlAGEAcgAgACYAIABfAHMAVwBlAGUAawAgACYAIABJAE4AVAAoAEQAYQB5AE8AZgBXAGUAZQBrACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFkAZQBhAHIAIAAmACAAXAAiAC0AXAAiACAAJgAgAF8AcwBXAGUAZQBrACAAJgAgAFwAIgAtAFwAIgAgACYAIABJAE4AVAAoAEQAYQB5AE8AZgBXAGUAZQBrACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuAEYATwBSAE0AQQBUAF8ASQBTAE8AOAA2ADAAMQBcAG4AXABuAFIAZQB0AHUAcgBuAHMAIABkAGEAdABlACAAYQBuAGQAIAB0AGkAbQBlACAAYwBvAG0AcABsAGkAYwBhAHQAaQBvAG4AcwAgAGEAcwAgAHQAZQB4AHQAIABpAG4AIAB0AGgAZQAgAEkAUwBPACAAOAA2ADAAMQAgAGYAbwByAG0AYQB0AC4AXABuAEUAeABhAG0AcABsAGUAIABmAG8AcgBtAGEAdABzACAAKABuAG8AdAAgAGUAeABoAGEAdQBzAHQAaQB2AGUAKQA6ACAAWQBZAFkAWQAtAE0ATQAtAEQARABUAGgAaAA6AG0AbQA6AHMAcwAuAHMAcwBzACsAaABoADoAbQBtADoAcwBzACwAIABZAFkAWQBZAC0AVwB3AHcALQBEAFQAaABoADoAbQBtAFoALAAgAFQAaABoAG0AbQBzAHMAXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAHQAZQB4AHQAIAB8ACAAIwBWAEEATABVAEUAIQAgAGkAZgAgAGEAbgAgAGkAbgB2AGEAbABpAGQAIABkAGEAdABlACwAIAB0AGkAbQBlACAAbwByACAAdABpAG0AZQAgAHoAbwBuAGUAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBEAGEAdABlAFQAeQBwAGUAIAAgACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAARABhAHQAZQAgAHQAeQBwAGUAIAByAGUAcAByAGUAcwBlAG4AdABlAGQAIABpAG4AIABEAGEAdABlAEEAcgBnADEAIABhAG4AZAAgAEQAYQB0AGUAQQByAGcAMgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAwACAALQAgAG4AbwAgAGQAYQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABjAGEAbABlAG4AZABhAHIAIABkAGEAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAAbwByAGQAaQBuAGEAbAAgAGQAYQB0AGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMwAgAC0AIAB3AGUAZQBrACAAZABhAHQAZQBcAG4AWQBlAGEAcgBDAEUAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFkAZQBhAHIAIABpAG4AIABDAG8AbQBtAG8AbgAgAEUAcgBhACAALQA5ADkAOQA5ADkALgAuACsAOQA5ADkAOQA5AFwAbgBbAEQAYQB0AGUAQQByAGcAMQBdACAAIAAgACAAIAAgACAAfAAgAGkAbgB0AGUAZwBlAHIAIAB8ACAATQBvAG4AdABoACAAbwBmACAAeQBlAGEAcgAgAHcAaABlAG4AIABEAGEAdABlAFQAeQBwAGUAIAA9ACAAMQAgACAAIAAgACAAIAAgACAAIAAxAC4ALgAxADIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIABXAGUAZQBrACAAbwBmACAAeQBlAGEAcgAgAHcAaABlAG4AIABEAGEAdABlAFQAeQBwAGUAIAA9ACAAMwAgACAAIAAgACAAIAAgACAAIAAgADEALgAuADUAMwBcAG4AWwBEAGEAdABlAEEAcgBnADIAXQAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAEQAYQB5ACAAbwBmACAAbQBvAG4AdABoACAAdwBoAGUAbgAgAEQAYQB0AGUAVAB5AHAAZQAgAD0AIAAxACAAIAAgACAAIAAgACAAIAAgACAAMQAuAC4AMwAxAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAATwByAGQAaQBuAGEAbAAgAGQAYQB5ACAAbwBmACAAeQBlAGEAcgAgAHcAaABlAG4AIABEAGEAdABlAFQAeQBwAGUAIAA9ACAAMgAgACAAIAAxAC4ALgAzADYANgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgAEQAYQB5ACAAbwBmACAAdwBlAGUAawAgAHcAaABlAG4AIABEAGEAdABlAFQAeQBwAGUAIAA9ACAAMwAgACAAIAAgACAAIAAgACAAIAAgACAAMQAuAC4ANwBcAG4AWwBIAG8AdQByAF0AIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADAALgAuADIANABcAG4AWwBNAGkAbgB1AHQAZQBdACAAIAAgACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgADAALgAuADUAOQBcAG4AWwBTAGUAYwBvAG4AZABdACAAIAAgACAAIAAgACAAIAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgADAALgAuADUAOQAuADkAOQA5AFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMAIAAtADkAMAAwAC4ALgArADkAMAAwAFwAbgBbAEIAYQBzAGkAYwBdACAAIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAUgBlAHQAdQByAG4AIABpAG4AIABiAGEAcwBpAGMAIABmAG8AcgBtAGEAdAAgAGUAZwAgAFkAWQBZAFkATQBNAEQARABUADEAMAA0ADUAKwAwADkAMwAwAFwAbgBbAFMAaQBnAG4AZQBkAF0AIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAQQBsAHcAYQB5AHMAIABzAGkAZwBuACAAeQBlAGEAcgAgAHYAYQBsAHUAZQAgAGUAZwAgACsAWQBZAFkAWQAtAE0ATQAtAEQARABcAG4AWwBQAHIAZQBjAGkAcwBpAG8AbgBdACAAIAAgACAAIAAgAHwAIABpAG4AdABlAGcAZQByACAAfAAgAFMAZQBsAGUAYwB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABsAGUAdgBlAGwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMAAgAC0AIABBAHUAdABvAG0AYQB0AGkAYwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAxACAALQAgAFkAZQBhAHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMgAgAC0AIABNAG8AbgB0AGgALwBXAGUAZQBrAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADMAIAAtACAARABhAHkALwBPAHIAZABpAG4AYQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADQAIAAtACAASABvAHUAcgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA1ACAALQAgAE0AaQBuAHUAdABlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADYAIAAtACAAUwBlAGMAbwBuAGQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANwAgAC0AIABGAHIAYQBjAHQAaQBvAG4AYQBsAFwAbgBbAE4AbwBUAGkAbQBlAFoAbwBuAGUAXQAgACAAIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAARAByAG8AcAAgAHQAaQBtAGUAIAB6AG8AbgBlACAAZgByAG8AbQAgAG8AdQB0AHAAdQB0AC4AXABuAFsATgBvAFoAdQBsAHUAXQAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABVAHMAZQAgACsAMAAwADoAMAAwACAAaQBuAHMAdABlAGEAZAAgAG8AZgAgAFoAIABmAG8AcgAgAFUAVABDACAAdABpAG0AZQAgAHoAbwBuAGUALgBcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtACoALwBcAG4ARgBPAFIATQBBAFQAXwBJAFMATwA4ADYAMAAxACAAPQAgAEwAQQBNAEIARABBACgAXABuACAAIAAgACAARABhAHQAZQBUAHkAcABlACwAXABuACAAIAAgACAAWwBZAGUAYQByAEMARQBdACwAXABuACAAIAAgACAAWwBEAGEAdABlAEEAcgBnADEAXQAsAFwAbgAgACAAIAAgAFsARABhAHQAZQBBAHIAZwAyAF0ALABcAG4AIAAgACAAIABbAEgAbwB1AHIAXQAsAFwAbgAgACAAIAAgAFsATQBpAG4AdQB0AGUAXQAsAFwAbgAgACAAIAAgAFsAUwBlAGMAbwBuAGQAXQAsAFwAbgAgACAAIAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALABcAG4AIAAgACAAIABbAEIAYQBzAGkAYwBdACwAXABuACAAIAAgACAAWwBTAGkAZwBuAGUAZABdACwAXABuACAAIAAgACAAWwBQAHIAZQBjAGkAcwBpAG8AbgBdACwAXABuACAAIAAgACAAWwBOAG8AVABpAG0AZQBaAG8AbgBlAF0ALABcAG4AIAAgACAAIABbAE4AbwBaAHUAbAB1AF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAXwBkAGEAdABlAFQAeQBwAGUALAAgAEwARQBUACgAXwBkAHQALAAgAE0AQQBYACgASQBOAFQAKABOACgARABhAHQAZQBUAHkAcABlACkAKQAsACAAMAApACwAIABJAEYAKABfAGQAdAAgAD4AIAAzACwAIAAwACwAIABfAGQAdAApACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AaABhAHMARABhAHQAZQAsACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBUAHkAcABlACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgASQBTAE4AVQBNAEIARQBSACgAWQBlAGEAcgBDAEUAKQAgACsAIABJAFMATgBVAE0AQgBFAFIAKABEAGEAdABlAEEAcgBnADEAKQAgACsAIABJAFMATgBVAE0AQgBFAFIAKABEAGEAdABlAEEAcgBnADIAKQApACAAPAA+ACAAMABcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AaABhAHMAVABpAG0AZQAsACAAKABJAFMATgBVAE0AQgBFAFIAKABIAG8AdQByACkAIAArACAASQBTAE4AVQBNAEIARQBSACgATQBpAG4AdQB0AGUAKQAgACsAIABJAFMATgBVAE0AQgBFAFIAKABTAGUAYwBvAG4AZAApACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIABfAGgAYQBzAFQAaQBtAGUAWgBvAG4AZQAsACAASQBTAE4AVQBNAEIARQBSACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AcwBoAG8AdwBUAGkAbQBlAFoAbwBuAGUALAAgAE4AKABOAG8AVABpAG0AZQBaAG8AbgBlACkAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBpAHMARQBtAHAAdAB5ACwAIABfAGgAYQBzAEQAYQB0AGUAIAArACAAXwBoAGEAcwBUAGkAbQBlACAAKwAgACgAXwBoAGEAcwBUAGkAbQBlAFoAbwBuAGUAIAAqACAAXwBzAGgAbwB3AFQAaQBtAGUAWgBvAG4AZQApACAAPQAgADAALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGkAcwBFAG0AcAB0AHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AaABhAHMARABhAHQAZQAgACoAIABfAGgAYQBzAFQAaQBtAGUAWgBvAG4AZQAgACoAIABfAHMAaABvAHcAVABpAG0AZQBaAG8AbgBlACkAIAAqACAATgBPAFQAKABfAGgAYQBzAFQAaQBtAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAVgBBAEwAVQBFACEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAsACAATQBBAFgAKABJAE4AVAAoAE4AKABQAHIAZQBjAGkAcwBpAG8AbgApACkALAAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAEQAYQB0AGUALAAgAEkARgBTACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBUAHkAcABlACAAPQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMAApACAAKwAgACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD4APQAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABEAGEAdABlAEEAcgBnADEALAAgAEQAYQB0AGUAQQByAGcAMgAsACAAQgBhAHMAaQBjACwAIABTAGkAZwBuAGUAZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBPAFIATQBBAFQAXwBEAEEAVABFACgAWQBlAGEAcgBDAEUALAAgAFwAIgBcACIALAAgAFwAIgBcACIALAAgAEIAYQBzAGkAYwAsACAAUwBpAGcAbgBlAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABEAGEAdABlAEEAcgBnADEALAAgAFwAIgBcACIALAAgAEIAYQBzAGkAYwAsACAAUwBpAGcAbgBlAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUAVAB5AHAAZQAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAwACkAIAArACAAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPgA9ACAAMwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBPAFIATQBBAFQAXwBPAFIARABJAE4AQQBMAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABEAGEAdABlAEEAcgBnADIALAAgAEIAYQBzAGkAYwAsACAAUwBpAGcAbgBlAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAAXAAiAFwAIgAsACAAQgBhAHMAaQBjACwAIABTAGkAZwBuAGUAZAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBUAHkAcABlACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMAApACAAKwAgACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD4APQAgADMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8AVwBFAEUASwBfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAARABhAHQAZQBBAHIAZwAxACwAIABEAGEAdABlAEEAcgBnADIALAAgAEIAYQBzAGkAYwAsACAAUwBpAGcAbgBlAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8AVwBFAEUASwBfAEQAQQBUAEUAKABZAGUAYQByAEMARQAsACAAXAAiAFwAIgAsACAAXAAiAFwAIgAsACAAQgBhAHMAaQBjACwAIABTAGkAZwBuAGUAZAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAyACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARgBPAFIATQBBAFQAXwBXAEUARQBLAF8ARABBAFQARQAoAFkAZQBhAHIAQwBFACwAIABEAGEAdABlAEEAcgBnADEALAAgAFwAIgBcACIALAAgAEIAYQBzAGkAYwAsACAAUwBpAGcAbgBlAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAAvAC8AXwBkAGEAdABlAFQAeQBwAGUAIAA9ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcACIAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAFQAaQBtAGUALAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA9ACAAMAApACAAKwAgACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD4APQAgADQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAFQASQBNAEUAKABIAG8AdQByACwAIABNAGkAbgB1AHQAZQAsACAAUwBlAGMAbwBuAGQALAAgAEIAYQBzAGkAYwAsACAATQBBAFgAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAALQAgADMALAAgADAAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAIgBcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAVABaAE8ALAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoACgAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAAwACkAIAArACAAKABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPgA9ACAANAApACkAIAAqACAAXwBoAGEAcwBUAGkAbQBlAFoAbwBuAGUAIAAqACAAXwBzAGgAbwB3AFQAaQBtAGUAWgBvAG4AZQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AVABaAHAAcgBlAGMAaQBzAGkAbwBuACwAIABJAEYAUwAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBwAHIAZQBjAGkAcwBpAG8AbgAgAD0AIAA0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHAAcgBlAGMAaQBzAGkAbwBuACAAPQAgADUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcAByAGUAYwBpAHMAaQBvAG4AIAA+AD0AIAA2ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABGAE8AUgBNAEEAVABfAFQASQBNAEUAXwBaAE8ATgBFACgAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAIABCAGEAcwBpAGMALAAgADAALAAgAE4AbwBaAHUAbAB1ACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXAAiAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AcwBEAGEAdABlACAAJgAgAF8AcwBUAGkAbQBlACAAJgAgAF8AcwBUAFoATwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAC8AKgAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAXABuACMAIABDAE8ATgBWAEUAUgBTAEkATwBOACAARgBVAE4AQwBUAEkATwBOAFMAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACMAXABuACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAqAC8AXABuAFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AQwBPAE4AVgBFAFIAVABfAFQATwBfAEQAQQBUAEUAXABuAFwAbgBDAG8AbgB2AGUAcgB0AHMAIAB0AGUAeAB0ACAAaQBuACAASQBTAE8AIABmAG8AcgBtAGEAdAAgAHQAbwAgAGEAbgAgAEUAeABjAGUAbAAgAGQAYQB0AGUALgAgAFwAbgBcAG4ATwB1AHQAcAB1AHQAXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAIAAxACAAfAAgAEUAeABjAGUAbAAgAEQAYQB0AGUAIAAgACAAIAAgAHwAIABkAGEAdABlACAAIAAgACAAfAAgADEAOQAwADAALQAwADEALQAwADEAVAAwADAAOgAwADAALgAuADkAOQA5ADkALQAxADIALQAzADEAVAAyADQAOgAwADAAXABuACAAIAAyACAAfAAgAE0AaQBuAHUAdABlAHMAIABvAGYAZgBzAGUAdAAgAHwAIABkAGUAYwBpAG0AYQBsACAAfAAgAC0AOQAwADAALgAuACsAOQAwADAAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBUAGUAeAB0ACAAIAAgACAAIAAgAHwAIABzAHQAcgBpAG4AZwAgAHwAIABJAFMATwAgADgANgAwADEAIABmAG8AcgBtAGEAdAB0AGUAZAAgAGQAYQB0AGUAIABhAG4AZAAgAHQAaQBtAGUALgBcAG4AWwBTAHQAcgBpAGMAdABdACAAIAB8ACAAcwB3AGkAdABjAGgAIAB8ACAARQBuAGYAbwByAGMAZQAgAHMAdAByAGkAYwB0ACAASQBTAE8AIAA4ADYAMAAxACAAcABhAHIAcwBpAG4AZwAgAHIAdQBsAGUAcwAuAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AKgAvAFwAbgBDAE8ATgBWAEUAUgBUAF8AVABPAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAFQAZQB4AHQALAAgAFsAUwB0AHIAaQBjAHQAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4ALAAgAEwAQQBNAEIARABBACgAXwBlAHgAYwBlAHAAdABpAG8AbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABfAGUAeABjAGUAcAB0AGkAbwBuACAAIAAgAHwAIABzAHQAcgBpAG4AZwAgACAAfAAgAG4AdQBsAGwAIAAgAEUAbQBwAHQAeQAgAHQAZQB4AHQAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAATgAvAEEAIAAgACAAVQBuAGEAYgBsAGUAIAB0AG8AIABwAGEAcgBzAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAATgBVAE0AIAAgACAATwB1AHQAIABvAGYAIABFAHgAZQBsACAAZABhAHQAZQAgAHIAYQBuAGcAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGAFMAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBOAC8AQQBcACIALAAgAHsAIwBOAC8AQQAsACAAIwBOAC8AQQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAHgAYwBlAHAAdABpAG8AbgAgAD0AIABcACIATgBVAE0AXAAiACwAIAB7ACMATgBVAE0AIQAsACAAIwBOAFUATQAhAH0ALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAVQBFACwAIAAvAC8AIABfAGUAeABjAGUAcAB0AGkAbwBuACAAPQAgAFwAIgBcACIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAewBcACIAXAAiACwAIABcACIAXAAiAH0AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFQAZQB4AHQAIAA9ACAAXAAiAFwAIgAsACAAZgBuAEUAeABjAGUAcAB0AGkAbwBuACgAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAHQAcgBpAGMAdAAsACAATgAoAFMAdAByAGkAYwB0ACkAIAA8AD4AIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBlAGwAZQBtAGUAbgB0AHMALAAgAFAAQQBSAFMARQBfAEkAUwBPADgANgAwADEAKABUAGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABfAHMAdAByAGkAYwB0ACAAKgAgACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEAIAAsACAAMQApACAAPQAgAEYAQQBMAFMARQApACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIATgAvAEEAXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMARABhAHQAZQAsACAAQgBJAFQAQQBOAEQAKABJAE4ARABFAFgAKABfAGUAbABlAG0AZQBuAHQAcwAsACAAMQAsACAAMgApACwAIAA0ACkAIAA9ACAANAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAE4AKABJAE4ARABFAFgAKABfAGUAbABlAG0AZQBuAHQAcwAsACAAMQAsACAANgApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAXwBoAGEAcwBEAGEAdABlACAAKgAgACgAKABfAHkAZQBhAHIAIAA8ACAAMQA5ADAAMAApACAAKwAgACgAXwB5AGUAYQByACAAPgAgADkAOQA5ADkAKQApACwAIABmAG4ARQB4AGMAZQBwAHQAaQBvAG4AKABcACIATgBVAE0AXAAiACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABMAEUAVAAoACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBUAHkAcABlACwAIABJAE4ARABFAFgAKABfAGUAbABlAG0AZQBuAHQAcwAsACAAMQAsACAANQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGQAYQB0AGUALAAgAEkARgAoAF8AaABhAHMARABhAHQAZQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAUwAoAF8AZABhAHQAZQBUAHkAcABlACAAPQAgADEALAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAARABBAFQARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAEkATgBEAEUAWAAoAF8AZQBsAGUAbQBlAG4AdABzACwAIAAxACwAIAA3ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADgAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBUAHkAcABlACAAPQAgADIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBEAGEAdABlACwAIABGAFIATwBNAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAKABfAHkAZQBhAHIALAAgAE4AKABJAE4ARABFAFgAKABfAGUAbABlAG0AZQBuAHQAcwAsACAAMQAsACAAOAApACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAEEAVABFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBjAEQAYQB0AGUALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AYwBEAGEAdABlACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGMARABhAHQAZQAsACAAMQAsACAAMwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHQAZQBUAHkAcABlACAAPQAgADMALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AYwBEAGEAdABlACwAIABGAFIATwBNAF8AVwBFAEUASwBfAEQAQQBUAEUAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADcAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAATgAoAEkATgBEAEUAWAAoAF8AZQBsAGUAbQBlAG4AdABzACwAIAAxACwAIAA4ACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABEAEEAVABFACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXwBjAEQAYQB0AGUALAAgADEALAAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAF8AYwBEAGEAdABlACwAIAAxACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAE4ARABFAFgAKABfAGMARABhAHQAZQAsACAAMQAsACAAMwApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAVABpAG0AZQAsACAAQgBJAFQAQQBOAEQAKABJAE4ARABFAFgAKABfAGUAbABlAG0AZQBuAHQAcwAsACAAMQAsACAAMgApACwAIAAyACkAIAA9ACAAMgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AGkAbQBlACwAIABJAEYAKABfAGgAYQBzAFQAaQBtAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABJAE0ARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AKABJAE4ARABFAFgAKABfAGUAbABlAG0AZQBuAHQAcwAsACAAMQAsACAAOQApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADEAMAApACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADEAMQApACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAHQALAAgAF8AZABhAHQAZQAgACsAIABfAHQAaQBtAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABhAHMAVABaACwAIAAoAEIASQBUAEEATgBEACgASQBOAEQARQBYACgAXwBlAGwAZQBtAGUAbgB0AHMALAAgADEALAAgADIAKQAsACAAMQApACAAPQAgADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwB0AHoAbwAsACAASQBGACgAXwBoAGEAcwBUAFoALAAgAEkATgBEAEUAWAAoAF8AZQBsAGUAbQBlAG4AdABzACwAIAAxACwAIAAxADIAKQAsACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAF8AZAB0ACwAIABfAHQAegBvACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AQwBPAE4AVgBFAFIAVABfAEYAUgBPAE0AXwBEAEEAVABFAFwAbgBcAG4AQwBvAG4AdgBlAHIAdABzACAAYQBuACAARQB4AGMAZQBsACAAZABhAHQAZQAgAHQAbwAgAEkAUwBPACAAZgBvAHIAbQBhAHQAdABlAGQAIAB0AGUAeAB0AC4AXABuAEUAeABhAG0AcABsAGUAIABmAG8AcgBtAGEAdABzACAAKABuAG8AdAAgAGUAeABoAGEAdQBzAHQAaQB2AGUAKQA6ACAAWQBZAFkAWQAtAE0ATQAtAEQARABUAGgAaAA6AG0AbQA6AHMAcwAuAHMAcwBzACsAaABoADoAbQBtADoAcwBzACwAIABZAFkAWQBZAC0AVwB3AHcALQBEAFQAaABoADoAbQBtAFoALAAgAFQAaABoAG0AbQBzAHMAXABuAFwAbgBPAHUAdABwAHUAdABcAG4ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAxACAAfAAgAHQAZQB4AHQAIAB8ACAAbgB1AGwAbAAgAGkAZgAgAGEAIABkAGEAdABlACAAaQBzACAAbgBvAHQAIABwAHIAbwB2AGkAZABlAGQAXABuAFwAbgBQAGEAcgBhAG0AZQB0AGUAcgBzAFwAbgAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgBEAGEAdABlACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgAGQAYQB0AGUAIAAgACAAIAB8ACAAQQBuACAARQB4AGMAZQBsACAAZABhAHQAZQAgAGEAbgBkAC8AbwByACAAdABpAG0AZQAuAFwAbgBbAFQAaQBtAGUAWgBvAG4AZQBPAGYAZgBzAGUAdABdACAAfAAgAGQAZQBjAGkAbQBhAGwAIAB8ACAAVABpAG0AZQAgAHoAbwBuAGUAIABvAGYAZgBzAGUAdAAgAGkAbgAgAG0AaQBuAHUAdABlAHMAIABmAHIAbwBtACAAVQBUAEMAIAAtADkAMAAwAC4ALgArADkAMAAwACAAXABuAFsAQgBhAHMAaQBjAF0AIAAgACAAIAAgACAAIAAgACAAIAB8ACAAcwB3AGkAdABjAGgAIAAgAHwAIABSAGUAdAB1AHIAbgAgAGkAbgAgAGIAYQBzAGkAYwAgAGYAbwByAG0AYQB0ACAAZQBnACAAWQBZAFkAWQBNAE0ARABEAFQAaABoAG0AbQArAGgAaABcAG4AWwBTAGkAZwBuAGUAZABdACAAIAAgACAAIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEEAbAB3AGEAeQBzACAAcwBpAGcAbgAgAHkAZQBhAHIAIAB2AGEAbAB1AGUAIABlAGcAIAArAFkAWQBZAFkALQBNAE0ALQBEAEQAXABuAFsAUAByAGUAYwBpAHMAaQBvAG4AXQAgACAAIAAgACAAIAB8ACAAaQBuAHQAZQBnAGUAcgAgAHwAIABTAGUAbABlAGMAdAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAbABlAHYAZQBsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADAAIAAtACAAQQB1AHQAbwBtAGEAdABpAGMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAMQAgAC0AIABZAGUAYQByAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADIAIAAtACAATQBvAG4AdABoAC8AVwBlAGUAawBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAzACAALQAgAEQAYQB5AC8ATwByAGQAaQBuAGEAbABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA0ACAALQAgAEgAbwB1AHIAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAANQAgAC0AIABNAGkAbgB1AHQAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHwAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAA2ACAALQAgAFMAZQBjAG8AbgBkAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAfAAgACAAIAAgACAAIAAgACAAIAB8ACAAIAAgADcAIAAtACAARgByAGEAYwB0AGkAbwBuAGEAbABcAG4AWwBOAG8AVABpAG0AZQBaAG8AbgBlAF0AIAAgACAAIAAgAHwAIABzAHcAaQB0AGMAaAAgACAAfAAgAEQAcgBvAHAAIAB0AGkAbQBlACAAegBvAG4AZQAgAGYAcgBvAG0AIABvAHUAdABwAHUAdAAuAFwAbgBbAE4AbwBaAHUAbAB1AF0AIAAgACAAIAAgACAAIAAgACAAfAAgAHMAdwBpAHQAYwBoACAAIAB8ACAAVQBzAGUAIAArADAAMAA6ADAAMAAgAGkAbgBzAHQAZQBhAGQAIABvAGYAIABaACAAZgBvAHIAIABVAFQAQwAgAHQAaQBtAGUAIAB6AG8AbgBlAC4AXABuAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAqAC8AXABuAEMATwBOAFYARQBSAFQAXwBGAFIATwBNAF8ARABBAFQARQAgAD0AIABMAEEATQBCAEQAQQAoAEQAYQB0AGUALAAgAFsAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0AF0ALAAgAFsAQgBhAHMAaQBjAF0ALAAgAFsAUwBpAGcAbgBlAGQAXQAsACAAWwBQAHIAZQBjAGkAcwBpAG8AbgBdACwAIABbAE4AbwBUAGkAbQBlAFoAbwBuAGUAXQAsACAAWwBOAG8AWgB1AGwAdQBdACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAEQAYQB0AGUAKQApACwAXABuACAAIAAgACAAIAAgACAAIABcACIAXAAiACwAXABuACAAIAAgACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAGgAYQBzAEQAYQB0AGUALAAgAEkATgBUACgATgAoAEQAYQB0AGUAKQAgADwAPgAgADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHkAZQBhAHIALAAgAEkARgAoAF8AaABhAHMARABhAHQAZQAsACAAWQBFAEEAUgAoAEQAYQB0AGUAKQAsACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAIABJAEYAKABfAGgAYQBzAEQAYQB0AGUALAAgAE0ATwBOAFQASAAoAEQAYQB0AGUAKQAsACAAXAAiAFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AZABhAHkALAAgAEkARgAoAF8AaABhAHMARABhAHQAZQAsACAARABBAFkAKABEAGEAdABlACkALAAgAFwAIgBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAUwBlAGMAMQAsACAAUgBPAFUATgBEACgAKABEAGEAdABlACAALQAgAEkATgBUACgATgAoAEQAYQB0AGUAKQApACkAIAAqACAAOAA2ADQAMAAwACwAIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBoAG8AdQByACwAIABJAE4AVAAoAF8AdABTAGUAYwAxACAALwAgADMANgAwADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHQAUwBlAGMAMgAsACAAXwB0AFMAZQBjADEAIAAtACAAKABfAGgAbwB1AHIAIAAqACAAMwA2ADAAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUALAAgAEkATgBUACgAXwB0AFMAZQBjADIAIAAvACAANgAwACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBzAGUAYwBvAG4AZAAsACAAXwB0AFMAZQBjADIAIAAtACAAKABfAG0AaQBuAHUAdABlACAAKgAgADYAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEYATwBSAE0AQQBUAF8ASQBTAE8AOAA2ADAAMQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AKABfAGgAYQBzAEQAYQB0AGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AeQBlAGEAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBvAG4AdABoACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAXwBkAGEAeQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AaABvAHUAcgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbQBpAG4AdQB0AGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAHMAZQBjAG8AbgBkACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAVABpAG0AZQBaAG8AbgBlAE8AZgBmAHMAZQB0ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAQgBhAHMAaQBjACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUwBpAGcAbgBlAGQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABQAHIAZQBjAGkAcwBpAG8AbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAE4AbwBUAGkAbQBlAFoAbwBuAGUALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABOAG8AWgB1AGwAdQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwBcAG4AIwAgAEUATgBEACAASQBTAE8AXwA4ADYAMAAxACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIwBcAG4AIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACMAIwAjACoALwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbACIASQBTAE8AXwA4ADYAMAAxAC4ASQBTAF8AVgBBAEwASQBEAF8AWQBFAEEAUgAiACwAIgBJAFMATwBfADgANgAwADEALgBJAFMAXwBMAEUAQQBQAF8AWQBFAEEAUgAiACwAIgBJAFMATwBfADgANgAwADEALgBJAFMAXwBWAEEATABJAEQAXwBEAEEAVABFACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEkAUwBfAFYAQQBMAEkARABfAFQASQBNAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ASQBTAF8AVgBBAEwASQBEAF8AVABJAE0ARQBfAFoATwBOAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ASQBTAF8AVgBBAEwASQBEAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ASQBTAF8AVgBBAEwASQBEAF8AVwBFAEUASwBfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AWQBFAEEAUgBfAEQAQQBZAF8AQwBPAFUATgBUACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAFkARQBBAFIAXwBXAEUARQBLAF8AQwBPAFUATgBUACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEQAQQBZAF8ATwBSAEQASQBOAEEATAAiACwAIgBJAFMATwBfADgANgAwADEALgBGAFIATwBNAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ARABBAFkAXwBPAEYAXwBXAEUARQBLACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEQAQQBZAF8ATwBGAF8AVwBFAEUASwBfAEYAUgBPAE0AXwBPAFIARABJAE4AQQBMACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAFcARQBFAEsAXwBOAFUATQBCAEUAUgAiACwAIgBJAFMATwBfADgANgAwADEALgBXAEUARQBLAF8ATgBVAE0AQgBFAFIAXwBGAFIATwBNAF8ATwBSAEQASQBOAEEATAAiACwAIgBJAFMATwBfADgANgAwADEALgBUAE8AXwBXAEUARQBLAF8ARABBAFQARQAiACwAIgBJAFMATwBfADgANgAwADEALgBGAFIATwBNAF8AVwBFAEUASwBfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AVgBBAEwASQBEAEEAVABFAF8AQwBIAEEAUgBBAEMAVABFAFIAUwAiACwAIgBJAFMATwBfADgANgAwADEALgBQAEEAUgBTAEUAXwBEAEEAVABFACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAFAAQQBSAFMARQBfAFQASQBNAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AUABBAFIAUwBFAF8AVABJAE0ARQBfAFoATwBOAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AUABBAFIAUwBFAF8AUABBAFIAVABTACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAFAAQQBSAFMARQBfAEkAUwBPADgANgAwADEAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ARgBPAFIATQBBAFQAXwBEAEEAVABFACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEYATwBSAE0AQQBUAF8AVABJAE0ARQAiACwAIgBJAFMATwBfADgANgAwADEALgBGAE8AUgBNAEEAVABfAFQASQBNAEUAXwBaAE8ATgBFACIALAAiAEkAUwBPAF8AOAA2ADAAMQAuAEYATwBSAE0AQQBUAF8ATwBSAEQASQBOAEEATABfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4ARgBPAFIATQBBAFQAXwBXAEUARQBLAF8ARABBAFQARQAiACwAIgBJAFMATwBfADgANgAwADEALgBGAE8AUgBNAEEAVABfAEkAUwBPADgANgAwADEAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AQwBPAE4AVgBFAFIAVABfAFQATwBfAEQAQQBUAEUAIgAsACIASQBTAE8AXwA4ADYAMAAxAC4AQwBPAE4AVgBFAFIAVABfAEYAUgBPAE0AXwBEAEEAVABFACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIARABNAFkAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>